<commit_message>
fix list parser runtime bug
</commit_message>
<xml_diff>
--- a/example/config/BasicItem_Common.xlsx
+++ b/example/config/BasicItem_Common.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\Go\configTool-src\src\github.com\Blizzardx\ConfigProtocol\example\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\porject\GoConfigTool\src\github.com\Blizzardx\ConfigProtocol\example\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143384FB-3388-4D58-BE11-4CC934E7C949}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="-225" windowWidth="19440" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5280" yWindow="-225" windowWidth="19440" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="67">
   <si>
     <t>道具图标：直接调用美术资源图名</t>
   </si>
@@ -263,11 +262,6 @@
   </si>
   <si>
     <t>{"type":"int32",
-"name":"LimitNum"}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"type":"int32",
 "name":"Acauire"}</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -301,11 +295,20 @@
 "name":"quality1"}</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
+  <si>
+    <t>{"type":"int32",
+"name":"LimitNum","isList":true}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>999|2054|1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3193,823 +3196,823 @@
     </xf>
   </cellXfs>
   <cellStyles count="817">
-    <cellStyle name="20% - 强调文字颜色 1 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 11" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 12" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 13" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 14" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 15" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 16" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 17" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 18" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 19" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 20" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 3" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 4" xfId="14" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 5" xfId="15" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 6" xfId="16" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 7" xfId="17" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 8" xfId="18" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 9" xfId="19" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 10" xfId="20" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 11" xfId="21" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 12" xfId="22" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 13" xfId="23" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 14" xfId="24" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 15" xfId="25" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 16" xfId="26" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 17" xfId="27" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 18" xfId="28" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 19" xfId="29" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 20" xfId="31" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 3" xfId="32" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 4" xfId="33" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 5" xfId="34" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 6" xfId="35" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 7" xfId="36" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 8" xfId="37" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 9" xfId="38" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 10" xfId="39" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 11" xfId="40" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 12" xfId="41" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 13" xfId="42" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 14" xfId="43" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 15" xfId="44" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 16" xfId="45" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 17" xfId="46" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 18" xfId="47" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 19" xfId="48" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 20" xfId="50" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 3" xfId="51" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 4" xfId="52" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 5" xfId="53" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 6" xfId="54" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 7" xfId="55" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 8" xfId="56" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 9" xfId="57" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 10" xfId="58" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 11" xfId="59" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 12" xfId="60" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 13" xfId="61" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 14" xfId="62" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 15" xfId="63" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 16" xfId="64" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 17" xfId="65" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 18" xfId="66" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 19" xfId="67" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 2" xfId="68" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 20" xfId="69" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 3" xfId="70" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 4" xfId="71" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 5" xfId="72" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 6" xfId="73" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 7" xfId="74" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 8" xfId="75" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 9" xfId="76" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 10" xfId="77" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 11" xfId="78" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 12" xfId="79" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 13" xfId="80" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 14" xfId="81" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 15" xfId="82" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 16" xfId="83" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 17" xfId="84" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 18" xfId="85" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 19" xfId="86" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 20" xfId="88" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 3" xfId="89" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 4" xfId="90" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 5" xfId="91" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 6" xfId="92" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 7" xfId="93" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 8" xfId="94" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 9" xfId="95" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 10" xfId="96" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 11" xfId="97" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 12" xfId="98" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 13" xfId="99" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 14" xfId="100" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 15" xfId="101" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 16" xfId="102" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 17" xfId="103" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 18" xfId="104" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 19" xfId="105" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 2" xfId="106" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 20" xfId="107" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 3" xfId="108" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 4" xfId="109" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 5" xfId="110" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 6" xfId="111" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 7" xfId="112" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 8" xfId="113" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 9" xfId="114" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 10" xfId="115" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 11" xfId="116" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 12" xfId="117" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 13" xfId="118" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 14" xfId="119" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 15" xfId="120" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 16" xfId="121" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 17" xfId="122" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 18" xfId="123" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 19" xfId="124" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 2" xfId="125" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 20" xfId="126" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 3" xfId="127" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 4" xfId="128" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 5" xfId="129" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 6" xfId="130" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 7" xfId="131" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 8" xfId="132" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 9" xfId="133" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 10" xfId="134" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 11" xfId="135" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 12" xfId="136" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 13" xfId="137" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 14" xfId="138" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 15" xfId="139" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 16" xfId="140" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 17" xfId="141" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 18" xfId="142" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 19" xfId="143" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 2" xfId="144" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 20" xfId="145" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 3" xfId="146" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 4" xfId="147" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 5" xfId="148" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 6" xfId="149" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 7" xfId="150" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 8" xfId="151" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 9" xfId="152" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 10" xfId="153" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 11" xfId="154" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 12" xfId="155" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 13" xfId="156" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 14" xfId="157" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 15" xfId="158" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 16" xfId="159" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 17" xfId="160" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 18" xfId="161" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 19" xfId="162" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 2" xfId="163" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 20" xfId="164" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 3" xfId="165" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 4" xfId="166" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 5" xfId="167" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 6" xfId="168" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 7" xfId="169" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 8" xfId="170" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 9" xfId="171" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 10" xfId="172" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 11" xfId="173" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 12" xfId="174" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 13" xfId="175" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 14" xfId="176" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 15" xfId="177" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 16" xfId="178" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 17" xfId="179" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 18" xfId="180" xr:uid="{00000000-0005-0000-0000-0000B3000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 19" xfId="181" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 2" xfId="182" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 20" xfId="183" xr:uid="{00000000-0005-0000-0000-0000B6000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 3" xfId="184" xr:uid="{00000000-0005-0000-0000-0000B7000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 4" xfId="185" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 5" xfId="186" xr:uid="{00000000-0005-0000-0000-0000B9000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 6" xfId="187" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 7" xfId="188" xr:uid="{00000000-0005-0000-0000-0000BB000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 8" xfId="189" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 9" xfId="190" xr:uid="{00000000-0005-0000-0000-0000BD000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 10" xfId="191" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 11" xfId="192" xr:uid="{00000000-0005-0000-0000-0000BF000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 12" xfId="193" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 13" xfId="194" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 14" xfId="195" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 15" xfId="196" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 16" xfId="197" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 17" xfId="198" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 18" xfId="199" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 19" xfId="200" xr:uid="{00000000-0005-0000-0000-0000C7000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 2" xfId="201" xr:uid="{00000000-0005-0000-0000-0000C8000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 20" xfId="202" xr:uid="{00000000-0005-0000-0000-0000C9000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 3" xfId="203" xr:uid="{00000000-0005-0000-0000-0000CA000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 4" xfId="204" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 5" xfId="205" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 6" xfId="206" xr:uid="{00000000-0005-0000-0000-0000CD000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 7" xfId="207" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 8" xfId="208" xr:uid="{00000000-0005-0000-0000-0000CF000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 9" xfId="209" xr:uid="{00000000-0005-0000-0000-0000D0000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 10" xfId="210" xr:uid="{00000000-0005-0000-0000-0000D1000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 11" xfId="211" xr:uid="{00000000-0005-0000-0000-0000D2000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 12" xfId="212" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 13" xfId="213" xr:uid="{00000000-0005-0000-0000-0000D4000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 14" xfId="214" xr:uid="{00000000-0005-0000-0000-0000D5000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 15" xfId="215" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 16" xfId="216" xr:uid="{00000000-0005-0000-0000-0000D7000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 17" xfId="217" xr:uid="{00000000-0005-0000-0000-0000D8000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 18" xfId="218" xr:uid="{00000000-0005-0000-0000-0000D9000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 19" xfId="219" xr:uid="{00000000-0005-0000-0000-0000DA000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 2" xfId="220" xr:uid="{00000000-0005-0000-0000-0000DB000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 20" xfId="221" xr:uid="{00000000-0005-0000-0000-0000DC000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 3" xfId="222" xr:uid="{00000000-0005-0000-0000-0000DD000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 4" xfId="223" xr:uid="{00000000-0005-0000-0000-0000DE000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 5" xfId="224" xr:uid="{00000000-0005-0000-0000-0000DF000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 6" xfId="225" xr:uid="{00000000-0005-0000-0000-0000E0000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 7" xfId="226" xr:uid="{00000000-0005-0000-0000-0000E1000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 8" xfId="227" xr:uid="{00000000-0005-0000-0000-0000E2000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 9" xfId="228" xr:uid="{00000000-0005-0000-0000-0000E3000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 10" xfId="229" xr:uid="{00000000-0005-0000-0000-0000E4000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 11" xfId="230" xr:uid="{00000000-0005-0000-0000-0000E5000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 12" xfId="231" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 13" xfId="232" xr:uid="{00000000-0005-0000-0000-0000E7000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 14" xfId="233" xr:uid="{00000000-0005-0000-0000-0000E8000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 15" xfId="234" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 16" xfId="235" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 17" xfId="236" xr:uid="{00000000-0005-0000-0000-0000EB000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 18" xfId="237" xr:uid="{00000000-0005-0000-0000-0000EC000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 19" xfId="238" xr:uid="{00000000-0005-0000-0000-0000ED000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 2" xfId="239" xr:uid="{00000000-0005-0000-0000-0000EE000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 20" xfId="240" xr:uid="{00000000-0005-0000-0000-0000EF000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 3" xfId="241" xr:uid="{00000000-0005-0000-0000-0000F0000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 4" xfId="242" xr:uid="{00000000-0005-0000-0000-0000F1000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 5" xfId="243" xr:uid="{00000000-0005-0000-0000-0000F2000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 6" xfId="244" xr:uid="{00000000-0005-0000-0000-0000F3000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 7" xfId="245" xr:uid="{00000000-0005-0000-0000-0000F4000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 8" xfId="246" xr:uid="{00000000-0005-0000-0000-0000F5000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 9" xfId="247" xr:uid="{00000000-0005-0000-0000-0000F6000000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 10" xfId="248" xr:uid="{00000000-0005-0000-0000-0000F7000000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 11" xfId="249" xr:uid="{00000000-0005-0000-0000-0000F8000000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 12" xfId="250" xr:uid="{00000000-0005-0000-0000-0000F9000000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 13" xfId="251" xr:uid="{00000000-0005-0000-0000-0000FA000000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 14" xfId="252" xr:uid="{00000000-0005-0000-0000-0000FB000000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 15" xfId="253" xr:uid="{00000000-0005-0000-0000-0000FC000000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 16" xfId="254" xr:uid="{00000000-0005-0000-0000-0000FD000000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 17" xfId="255" xr:uid="{00000000-0005-0000-0000-0000FE000000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 18" xfId="256" xr:uid="{00000000-0005-0000-0000-0000FF000000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 19" xfId="257" xr:uid="{00000000-0005-0000-0000-000000010000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 2" xfId="258" xr:uid="{00000000-0005-0000-0000-000001010000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 20" xfId="259" xr:uid="{00000000-0005-0000-0000-000002010000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 3" xfId="260" xr:uid="{00000000-0005-0000-0000-000003010000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 4" xfId="261" xr:uid="{00000000-0005-0000-0000-000004010000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 5" xfId="262" xr:uid="{00000000-0005-0000-0000-000005010000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 6" xfId="263" xr:uid="{00000000-0005-0000-0000-000006010000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 7" xfId="264" xr:uid="{00000000-0005-0000-0000-000007010000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 8" xfId="265" xr:uid="{00000000-0005-0000-0000-000008010000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 9" xfId="266" xr:uid="{00000000-0005-0000-0000-000009010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 10" xfId="267" xr:uid="{00000000-0005-0000-0000-00000A010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 11" xfId="268" xr:uid="{00000000-0005-0000-0000-00000B010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 12" xfId="269" xr:uid="{00000000-0005-0000-0000-00000C010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 13" xfId="270" xr:uid="{00000000-0005-0000-0000-00000D010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 14" xfId="271" xr:uid="{00000000-0005-0000-0000-00000E010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 15" xfId="272" xr:uid="{00000000-0005-0000-0000-00000F010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 16" xfId="273" xr:uid="{00000000-0005-0000-0000-000010010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 17" xfId="274" xr:uid="{00000000-0005-0000-0000-000011010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 18" xfId="275" xr:uid="{00000000-0005-0000-0000-000012010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 19" xfId="276" xr:uid="{00000000-0005-0000-0000-000013010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 2" xfId="277" xr:uid="{00000000-0005-0000-0000-000014010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 20" xfId="278" xr:uid="{00000000-0005-0000-0000-000015010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 3" xfId="279" xr:uid="{00000000-0005-0000-0000-000016010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 4" xfId="280" xr:uid="{00000000-0005-0000-0000-000017010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 5" xfId="281" xr:uid="{00000000-0005-0000-0000-000018010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 6" xfId="282" xr:uid="{00000000-0005-0000-0000-000019010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 7" xfId="283" xr:uid="{00000000-0005-0000-0000-00001A010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 8" xfId="284" xr:uid="{00000000-0005-0000-0000-00001B010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 9" xfId="285" xr:uid="{00000000-0005-0000-0000-00001C010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 10" xfId="286" xr:uid="{00000000-0005-0000-0000-00001D010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 11" xfId="287" xr:uid="{00000000-0005-0000-0000-00001E010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 12" xfId="288" xr:uid="{00000000-0005-0000-0000-00001F010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 13" xfId="289" xr:uid="{00000000-0005-0000-0000-000020010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 14" xfId="290" xr:uid="{00000000-0005-0000-0000-000021010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 15" xfId="291" xr:uid="{00000000-0005-0000-0000-000022010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 16" xfId="292" xr:uid="{00000000-0005-0000-0000-000023010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 17" xfId="293" xr:uid="{00000000-0005-0000-0000-000024010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 18" xfId="294" xr:uid="{00000000-0005-0000-0000-000025010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 19" xfId="295" xr:uid="{00000000-0005-0000-0000-000026010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 2" xfId="296" xr:uid="{00000000-0005-0000-0000-000027010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 20" xfId="297" xr:uid="{00000000-0005-0000-0000-000028010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 3" xfId="298" xr:uid="{00000000-0005-0000-0000-000029010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 4" xfId="299" xr:uid="{00000000-0005-0000-0000-00002A010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 5" xfId="300" xr:uid="{00000000-0005-0000-0000-00002B010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 6" xfId="301" xr:uid="{00000000-0005-0000-0000-00002C010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 7" xfId="302" xr:uid="{00000000-0005-0000-0000-00002D010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 8" xfId="303" xr:uid="{00000000-0005-0000-0000-00002E010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 9" xfId="304" xr:uid="{00000000-0005-0000-0000-00002F010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 10" xfId="305" xr:uid="{00000000-0005-0000-0000-000030010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 11" xfId="306" xr:uid="{00000000-0005-0000-0000-000031010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 12" xfId="307" xr:uid="{00000000-0005-0000-0000-000032010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 13" xfId="308" xr:uid="{00000000-0005-0000-0000-000033010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 14" xfId="309" xr:uid="{00000000-0005-0000-0000-000034010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 15" xfId="310" xr:uid="{00000000-0005-0000-0000-000035010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 16" xfId="311" xr:uid="{00000000-0005-0000-0000-000036010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 17" xfId="312" xr:uid="{00000000-0005-0000-0000-000037010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 18" xfId="313" xr:uid="{00000000-0005-0000-0000-000038010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 19" xfId="314" xr:uid="{00000000-0005-0000-0000-000039010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 2" xfId="315" xr:uid="{00000000-0005-0000-0000-00003A010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 20" xfId="316" xr:uid="{00000000-0005-0000-0000-00003B010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 3" xfId="317" xr:uid="{00000000-0005-0000-0000-00003C010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 4" xfId="318" xr:uid="{00000000-0005-0000-0000-00003D010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 5" xfId="319" xr:uid="{00000000-0005-0000-0000-00003E010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 6" xfId="320" xr:uid="{00000000-0005-0000-0000-00003F010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 7" xfId="321" xr:uid="{00000000-0005-0000-0000-000040010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 8" xfId="322" xr:uid="{00000000-0005-0000-0000-000041010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 9" xfId="323" xr:uid="{00000000-0005-0000-0000-000042010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 10" xfId="324" xr:uid="{00000000-0005-0000-0000-000043010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 11" xfId="325" xr:uid="{00000000-0005-0000-0000-000044010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 12" xfId="326" xr:uid="{00000000-0005-0000-0000-000045010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 13" xfId="327" xr:uid="{00000000-0005-0000-0000-000046010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 14" xfId="328" xr:uid="{00000000-0005-0000-0000-000047010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 15" xfId="329" xr:uid="{00000000-0005-0000-0000-000048010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 16" xfId="330" xr:uid="{00000000-0005-0000-0000-000049010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 17" xfId="331" xr:uid="{00000000-0005-0000-0000-00004A010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 18" xfId="332" xr:uid="{00000000-0005-0000-0000-00004B010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 19" xfId="333" xr:uid="{00000000-0005-0000-0000-00004C010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 2" xfId="334" xr:uid="{00000000-0005-0000-0000-00004D010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 20" xfId="335" xr:uid="{00000000-0005-0000-0000-00004E010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 3" xfId="336" xr:uid="{00000000-0005-0000-0000-00004F010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 4" xfId="337" xr:uid="{00000000-0005-0000-0000-000050010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 5" xfId="338" xr:uid="{00000000-0005-0000-0000-000051010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 6" xfId="339" xr:uid="{00000000-0005-0000-0000-000052010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 7" xfId="340" xr:uid="{00000000-0005-0000-0000-000053010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 8" xfId="341" xr:uid="{00000000-0005-0000-0000-000054010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 9" xfId="342" xr:uid="{00000000-0005-0000-0000-000055010000}"/>
+    <cellStyle name="20% - 强调文字颜色 1 10" xfId="1"/>
+    <cellStyle name="20% - 强调文字颜色 1 11" xfId="2"/>
+    <cellStyle name="20% - 强调文字颜色 1 12" xfId="3"/>
+    <cellStyle name="20% - 强调文字颜色 1 13" xfId="4"/>
+    <cellStyle name="20% - 强调文字颜色 1 14" xfId="5"/>
+    <cellStyle name="20% - 强调文字颜色 1 15" xfId="6"/>
+    <cellStyle name="20% - 强调文字颜色 1 16" xfId="7"/>
+    <cellStyle name="20% - 强调文字颜色 1 17" xfId="8"/>
+    <cellStyle name="20% - 强调文字颜色 1 18" xfId="9"/>
+    <cellStyle name="20% - 强调文字颜色 1 19" xfId="10"/>
+    <cellStyle name="20% - 强调文字颜色 1 2" xfId="11"/>
+    <cellStyle name="20% - 强调文字颜色 1 20" xfId="12"/>
+    <cellStyle name="20% - 强调文字颜色 1 3" xfId="13"/>
+    <cellStyle name="20% - 强调文字颜色 1 4" xfId="14"/>
+    <cellStyle name="20% - 强调文字颜色 1 5" xfId="15"/>
+    <cellStyle name="20% - 强调文字颜色 1 6" xfId="16"/>
+    <cellStyle name="20% - 强调文字颜色 1 7" xfId="17"/>
+    <cellStyle name="20% - 强调文字颜色 1 8" xfId="18"/>
+    <cellStyle name="20% - 强调文字颜色 1 9" xfId="19"/>
+    <cellStyle name="20% - 强调文字颜色 2 10" xfId="20"/>
+    <cellStyle name="20% - 强调文字颜色 2 11" xfId="21"/>
+    <cellStyle name="20% - 强调文字颜色 2 12" xfId="22"/>
+    <cellStyle name="20% - 强调文字颜色 2 13" xfId="23"/>
+    <cellStyle name="20% - 强调文字颜色 2 14" xfId="24"/>
+    <cellStyle name="20% - 强调文字颜色 2 15" xfId="25"/>
+    <cellStyle name="20% - 强调文字颜色 2 16" xfId="26"/>
+    <cellStyle name="20% - 强调文字颜色 2 17" xfId="27"/>
+    <cellStyle name="20% - 强调文字颜色 2 18" xfId="28"/>
+    <cellStyle name="20% - 强调文字颜色 2 19" xfId="29"/>
+    <cellStyle name="20% - 强调文字颜色 2 2" xfId="30"/>
+    <cellStyle name="20% - 强调文字颜色 2 20" xfId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2 3" xfId="32"/>
+    <cellStyle name="20% - 强调文字颜色 2 4" xfId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2 5" xfId="34"/>
+    <cellStyle name="20% - 强调文字颜色 2 6" xfId="35"/>
+    <cellStyle name="20% - 强调文字颜色 2 7" xfId="36"/>
+    <cellStyle name="20% - 强调文字颜色 2 8" xfId="37"/>
+    <cellStyle name="20% - 强调文字颜色 2 9" xfId="38"/>
+    <cellStyle name="20% - 强调文字颜色 3 10" xfId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3 11" xfId="40"/>
+    <cellStyle name="20% - 强调文字颜色 3 12" xfId="41"/>
+    <cellStyle name="20% - 强调文字颜色 3 13" xfId="42"/>
+    <cellStyle name="20% - 强调文字颜色 3 14" xfId="43"/>
+    <cellStyle name="20% - 强调文字颜色 3 15" xfId="44"/>
+    <cellStyle name="20% - 强调文字颜色 3 16" xfId="45"/>
+    <cellStyle name="20% - 强调文字颜色 3 17" xfId="46"/>
+    <cellStyle name="20% - 强调文字颜色 3 18" xfId="47"/>
+    <cellStyle name="20% - 强调文字颜色 3 19" xfId="48"/>
+    <cellStyle name="20% - 强调文字颜色 3 2" xfId="49"/>
+    <cellStyle name="20% - 强调文字颜色 3 20" xfId="50"/>
+    <cellStyle name="20% - 强调文字颜色 3 3" xfId="51"/>
+    <cellStyle name="20% - 强调文字颜色 3 4" xfId="52"/>
+    <cellStyle name="20% - 强调文字颜色 3 5" xfId="53"/>
+    <cellStyle name="20% - 强调文字颜色 3 6" xfId="54"/>
+    <cellStyle name="20% - 强调文字颜色 3 7" xfId="55"/>
+    <cellStyle name="20% - 强调文字颜色 3 8" xfId="56"/>
+    <cellStyle name="20% - 强调文字颜色 3 9" xfId="57"/>
+    <cellStyle name="20% - 强调文字颜色 4 10" xfId="58"/>
+    <cellStyle name="20% - 强调文字颜色 4 11" xfId="59"/>
+    <cellStyle name="20% - 强调文字颜色 4 12" xfId="60"/>
+    <cellStyle name="20% - 强调文字颜色 4 13" xfId="61"/>
+    <cellStyle name="20% - 强调文字颜色 4 14" xfId="62"/>
+    <cellStyle name="20% - 强调文字颜色 4 15" xfId="63"/>
+    <cellStyle name="20% - 强调文字颜色 4 16" xfId="64"/>
+    <cellStyle name="20% - 强调文字颜色 4 17" xfId="65"/>
+    <cellStyle name="20% - 强调文字颜色 4 18" xfId="66"/>
+    <cellStyle name="20% - 强调文字颜色 4 19" xfId="67"/>
+    <cellStyle name="20% - 强调文字颜色 4 2" xfId="68"/>
+    <cellStyle name="20% - 强调文字颜色 4 20" xfId="69"/>
+    <cellStyle name="20% - 强调文字颜色 4 3" xfId="70"/>
+    <cellStyle name="20% - 强调文字颜色 4 4" xfId="71"/>
+    <cellStyle name="20% - 强调文字颜色 4 5" xfId="72"/>
+    <cellStyle name="20% - 强调文字颜色 4 6" xfId="73"/>
+    <cellStyle name="20% - 强调文字颜色 4 7" xfId="74"/>
+    <cellStyle name="20% - 强调文字颜色 4 8" xfId="75"/>
+    <cellStyle name="20% - 强调文字颜色 4 9" xfId="76"/>
+    <cellStyle name="20% - 强调文字颜色 5 10" xfId="77"/>
+    <cellStyle name="20% - 强调文字颜色 5 11" xfId="78"/>
+    <cellStyle name="20% - 强调文字颜色 5 12" xfId="79"/>
+    <cellStyle name="20% - 强调文字颜色 5 13" xfId="80"/>
+    <cellStyle name="20% - 强调文字颜色 5 14" xfId="81"/>
+    <cellStyle name="20% - 强调文字颜色 5 15" xfId="82"/>
+    <cellStyle name="20% - 强调文字颜色 5 16" xfId="83"/>
+    <cellStyle name="20% - 强调文字颜色 5 17" xfId="84"/>
+    <cellStyle name="20% - 强调文字颜色 5 18" xfId="85"/>
+    <cellStyle name="20% - 强调文字颜色 5 19" xfId="86"/>
+    <cellStyle name="20% - 强调文字颜色 5 2" xfId="87"/>
+    <cellStyle name="20% - 强调文字颜色 5 20" xfId="88"/>
+    <cellStyle name="20% - 强调文字颜色 5 3" xfId="89"/>
+    <cellStyle name="20% - 强调文字颜色 5 4" xfId="90"/>
+    <cellStyle name="20% - 强调文字颜色 5 5" xfId="91"/>
+    <cellStyle name="20% - 强调文字颜色 5 6" xfId="92"/>
+    <cellStyle name="20% - 强调文字颜色 5 7" xfId="93"/>
+    <cellStyle name="20% - 强调文字颜色 5 8" xfId="94"/>
+    <cellStyle name="20% - 强调文字颜色 5 9" xfId="95"/>
+    <cellStyle name="20% - 强调文字颜色 6 10" xfId="96"/>
+    <cellStyle name="20% - 强调文字颜色 6 11" xfId="97"/>
+    <cellStyle name="20% - 强调文字颜色 6 12" xfId="98"/>
+    <cellStyle name="20% - 强调文字颜色 6 13" xfId="99"/>
+    <cellStyle name="20% - 强调文字颜色 6 14" xfId="100"/>
+    <cellStyle name="20% - 强调文字颜色 6 15" xfId="101"/>
+    <cellStyle name="20% - 强调文字颜色 6 16" xfId="102"/>
+    <cellStyle name="20% - 强调文字颜色 6 17" xfId="103"/>
+    <cellStyle name="20% - 强调文字颜色 6 18" xfId="104"/>
+    <cellStyle name="20% - 强调文字颜色 6 19" xfId="105"/>
+    <cellStyle name="20% - 强调文字颜色 6 2" xfId="106"/>
+    <cellStyle name="20% - 强调文字颜色 6 20" xfId="107"/>
+    <cellStyle name="20% - 强调文字颜色 6 3" xfId="108"/>
+    <cellStyle name="20% - 强调文字颜色 6 4" xfId="109"/>
+    <cellStyle name="20% - 强调文字颜色 6 5" xfId="110"/>
+    <cellStyle name="20% - 强调文字颜色 6 6" xfId="111"/>
+    <cellStyle name="20% - 强调文字颜色 6 7" xfId="112"/>
+    <cellStyle name="20% - 强调文字颜色 6 8" xfId="113"/>
+    <cellStyle name="20% - 强调文字颜色 6 9" xfId="114"/>
+    <cellStyle name="40% - 强调文字颜色 1 10" xfId="115"/>
+    <cellStyle name="40% - 强调文字颜色 1 11" xfId="116"/>
+    <cellStyle name="40% - 强调文字颜色 1 12" xfId="117"/>
+    <cellStyle name="40% - 强调文字颜色 1 13" xfId="118"/>
+    <cellStyle name="40% - 强调文字颜色 1 14" xfId="119"/>
+    <cellStyle name="40% - 强调文字颜色 1 15" xfId="120"/>
+    <cellStyle name="40% - 强调文字颜色 1 16" xfId="121"/>
+    <cellStyle name="40% - 强调文字颜色 1 17" xfId="122"/>
+    <cellStyle name="40% - 强调文字颜色 1 18" xfId="123"/>
+    <cellStyle name="40% - 强调文字颜色 1 19" xfId="124"/>
+    <cellStyle name="40% - 强调文字颜色 1 2" xfId="125"/>
+    <cellStyle name="40% - 强调文字颜色 1 20" xfId="126"/>
+    <cellStyle name="40% - 强调文字颜色 1 3" xfId="127"/>
+    <cellStyle name="40% - 强调文字颜色 1 4" xfId="128"/>
+    <cellStyle name="40% - 强调文字颜色 1 5" xfId="129"/>
+    <cellStyle name="40% - 强调文字颜色 1 6" xfId="130"/>
+    <cellStyle name="40% - 强调文字颜色 1 7" xfId="131"/>
+    <cellStyle name="40% - 强调文字颜色 1 8" xfId="132"/>
+    <cellStyle name="40% - 强调文字颜色 1 9" xfId="133"/>
+    <cellStyle name="40% - 强调文字颜色 2 10" xfId="134"/>
+    <cellStyle name="40% - 强调文字颜色 2 11" xfId="135"/>
+    <cellStyle name="40% - 强调文字颜色 2 12" xfId="136"/>
+    <cellStyle name="40% - 强调文字颜色 2 13" xfId="137"/>
+    <cellStyle name="40% - 强调文字颜色 2 14" xfId="138"/>
+    <cellStyle name="40% - 强调文字颜色 2 15" xfId="139"/>
+    <cellStyle name="40% - 强调文字颜色 2 16" xfId="140"/>
+    <cellStyle name="40% - 强调文字颜色 2 17" xfId="141"/>
+    <cellStyle name="40% - 强调文字颜色 2 18" xfId="142"/>
+    <cellStyle name="40% - 强调文字颜色 2 19" xfId="143"/>
+    <cellStyle name="40% - 强调文字颜色 2 2" xfId="144"/>
+    <cellStyle name="40% - 强调文字颜色 2 20" xfId="145"/>
+    <cellStyle name="40% - 强调文字颜色 2 3" xfId="146"/>
+    <cellStyle name="40% - 强调文字颜色 2 4" xfId="147"/>
+    <cellStyle name="40% - 强调文字颜色 2 5" xfId="148"/>
+    <cellStyle name="40% - 强调文字颜色 2 6" xfId="149"/>
+    <cellStyle name="40% - 强调文字颜色 2 7" xfId="150"/>
+    <cellStyle name="40% - 强调文字颜色 2 8" xfId="151"/>
+    <cellStyle name="40% - 强调文字颜色 2 9" xfId="152"/>
+    <cellStyle name="40% - 强调文字颜色 3 10" xfId="153"/>
+    <cellStyle name="40% - 强调文字颜色 3 11" xfId="154"/>
+    <cellStyle name="40% - 强调文字颜色 3 12" xfId="155"/>
+    <cellStyle name="40% - 强调文字颜色 3 13" xfId="156"/>
+    <cellStyle name="40% - 强调文字颜色 3 14" xfId="157"/>
+    <cellStyle name="40% - 强调文字颜色 3 15" xfId="158"/>
+    <cellStyle name="40% - 强调文字颜色 3 16" xfId="159"/>
+    <cellStyle name="40% - 强调文字颜色 3 17" xfId="160"/>
+    <cellStyle name="40% - 强调文字颜色 3 18" xfId="161"/>
+    <cellStyle name="40% - 强调文字颜色 3 19" xfId="162"/>
+    <cellStyle name="40% - 强调文字颜色 3 2" xfId="163"/>
+    <cellStyle name="40% - 强调文字颜色 3 20" xfId="164"/>
+    <cellStyle name="40% - 强调文字颜色 3 3" xfId="165"/>
+    <cellStyle name="40% - 强调文字颜色 3 4" xfId="166"/>
+    <cellStyle name="40% - 强调文字颜色 3 5" xfId="167"/>
+    <cellStyle name="40% - 强调文字颜色 3 6" xfId="168"/>
+    <cellStyle name="40% - 强调文字颜色 3 7" xfId="169"/>
+    <cellStyle name="40% - 强调文字颜色 3 8" xfId="170"/>
+    <cellStyle name="40% - 强调文字颜色 3 9" xfId="171"/>
+    <cellStyle name="40% - 强调文字颜色 4 10" xfId="172"/>
+    <cellStyle name="40% - 强调文字颜色 4 11" xfId="173"/>
+    <cellStyle name="40% - 强调文字颜色 4 12" xfId="174"/>
+    <cellStyle name="40% - 强调文字颜色 4 13" xfId="175"/>
+    <cellStyle name="40% - 强调文字颜色 4 14" xfId="176"/>
+    <cellStyle name="40% - 强调文字颜色 4 15" xfId="177"/>
+    <cellStyle name="40% - 强调文字颜色 4 16" xfId="178"/>
+    <cellStyle name="40% - 强调文字颜色 4 17" xfId="179"/>
+    <cellStyle name="40% - 强调文字颜色 4 18" xfId="180"/>
+    <cellStyle name="40% - 强调文字颜色 4 19" xfId="181"/>
+    <cellStyle name="40% - 强调文字颜色 4 2" xfId="182"/>
+    <cellStyle name="40% - 强调文字颜色 4 20" xfId="183"/>
+    <cellStyle name="40% - 强调文字颜色 4 3" xfId="184"/>
+    <cellStyle name="40% - 强调文字颜色 4 4" xfId="185"/>
+    <cellStyle name="40% - 强调文字颜色 4 5" xfId="186"/>
+    <cellStyle name="40% - 强调文字颜色 4 6" xfId="187"/>
+    <cellStyle name="40% - 强调文字颜色 4 7" xfId="188"/>
+    <cellStyle name="40% - 强调文字颜色 4 8" xfId="189"/>
+    <cellStyle name="40% - 强调文字颜色 4 9" xfId="190"/>
+    <cellStyle name="40% - 强调文字颜色 5 10" xfId="191"/>
+    <cellStyle name="40% - 强调文字颜色 5 11" xfId="192"/>
+    <cellStyle name="40% - 强调文字颜色 5 12" xfId="193"/>
+    <cellStyle name="40% - 强调文字颜色 5 13" xfId="194"/>
+    <cellStyle name="40% - 强调文字颜色 5 14" xfId="195"/>
+    <cellStyle name="40% - 强调文字颜色 5 15" xfId="196"/>
+    <cellStyle name="40% - 强调文字颜色 5 16" xfId="197"/>
+    <cellStyle name="40% - 强调文字颜色 5 17" xfId="198"/>
+    <cellStyle name="40% - 强调文字颜色 5 18" xfId="199"/>
+    <cellStyle name="40% - 强调文字颜色 5 19" xfId="200"/>
+    <cellStyle name="40% - 强调文字颜色 5 2" xfId="201"/>
+    <cellStyle name="40% - 强调文字颜色 5 20" xfId="202"/>
+    <cellStyle name="40% - 强调文字颜色 5 3" xfId="203"/>
+    <cellStyle name="40% - 强调文字颜色 5 4" xfId="204"/>
+    <cellStyle name="40% - 强调文字颜色 5 5" xfId="205"/>
+    <cellStyle name="40% - 强调文字颜色 5 6" xfId="206"/>
+    <cellStyle name="40% - 强调文字颜色 5 7" xfId="207"/>
+    <cellStyle name="40% - 强调文字颜色 5 8" xfId="208"/>
+    <cellStyle name="40% - 强调文字颜色 5 9" xfId="209"/>
+    <cellStyle name="40% - 强调文字颜色 6 10" xfId="210"/>
+    <cellStyle name="40% - 强调文字颜色 6 11" xfId="211"/>
+    <cellStyle name="40% - 强调文字颜色 6 12" xfId="212"/>
+    <cellStyle name="40% - 强调文字颜色 6 13" xfId="213"/>
+    <cellStyle name="40% - 强调文字颜色 6 14" xfId="214"/>
+    <cellStyle name="40% - 强调文字颜色 6 15" xfId="215"/>
+    <cellStyle name="40% - 强调文字颜色 6 16" xfId="216"/>
+    <cellStyle name="40% - 强调文字颜色 6 17" xfId="217"/>
+    <cellStyle name="40% - 强调文字颜色 6 18" xfId="218"/>
+    <cellStyle name="40% - 强调文字颜色 6 19" xfId="219"/>
+    <cellStyle name="40% - 强调文字颜色 6 2" xfId="220"/>
+    <cellStyle name="40% - 强调文字颜色 6 20" xfId="221"/>
+    <cellStyle name="40% - 强调文字颜色 6 3" xfId="222"/>
+    <cellStyle name="40% - 强调文字颜色 6 4" xfId="223"/>
+    <cellStyle name="40% - 强调文字颜色 6 5" xfId="224"/>
+    <cellStyle name="40% - 强调文字颜色 6 6" xfId="225"/>
+    <cellStyle name="40% - 强调文字颜色 6 7" xfId="226"/>
+    <cellStyle name="40% - 强调文字颜色 6 8" xfId="227"/>
+    <cellStyle name="40% - 强调文字颜色 6 9" xfId="228"/>
+    <cellStyle name="60% - 强调文字颜色 1 10" xfId="229"/>
+    <cellStyle name="60% - 强调文字颜色 1 11" xfId="230"/>
+    <cellStyle name="60% - 强调文字颜色 1 12" xfId="231"/>
+    <cellStyle name="60% - 强调文字颜色 1 13" xfId="232"/>
+    <cellStyle name="60% - 强调文字颜色 1 14" xfId="233"/>
+    <cellStyle name="60% - 强调文字颜色 1 15" xfId="234"/>
+    <cellStyle name="60% - 强调文字颜色 1 16" xfId="235"/>
+    <cellStyle name="60% - 强调文字颜色 1 17" xfId="236"/>
+    <cellStyle name="60% - 强调文字颜色 1 18" xfId="237"/>
+    <cellStyle name="60% - 强调文字颜色 1 19" xfId="238"/>
+    <cellStyle name="60% - 强调文字颜色 1 2" xfId="239"/>
+    <cellStyle name="60% - 强调文字颜色 1 20" xfId="240"/>
+    <cellStyle name="60% - 强调文字颜色 1 3" xfId="241"/>
+    <cellStyle name="60% - 强调文字颜色 1 4" xfId="242"/>
+    <cellStyle name="60% - 强调文字颜色 1 5" xfId="243"/>
+    <cellStyle name="60% - 强调文字颜色 1 6" xfId="244"/>
+    <cellStyle name="60% - 强调文字颜色 1 7" xfId="245"/>
+    <cellStyle name="60% - 强调文字颜色 1 8" xfId="246"/>
+    <cellStyle name="60% - 强调文字颜色 1 9" xfId="247"/>
+    <cellStyle name="60% - 强调文字颜色 2 10" xfId="248"/>
+    <cellStyle name="60% - 强调文字颜色 2 11" xfId="249"/>
+    <cellStyle name="60% - 强调文字颜色 2 12" xfId="250"/>
+    <cellStyle name="60% - 强调文字颜色 2 13" xfId="251"/>
+    <cellStyle name="60% - 强调文字颜色 2 14" xfId="252"/>
+    <cellStyle name="60% - 强调文字颜色 2 15" xfId="253"/>
+    <cellStyle name="60% - 强调文字颜色 2 16" xfId="254"/>
+    <cellStyle name="60% - 强调文字颜色 2 17" xfId="255"/>
+    <cellStyle name="60% - 强调文字颜色 2 18" xfId="256"/>
+    <cellStyle name="60% - 强调文字颜色 2 19" xfId="257"/>
+    <cellStyle name="60% - 强调文字颜色 2 2" xfId="258"/>
+    <cellStyle name="60% - 强调文字颜色 2 20" xfId="259"/>
+    <cellStyle name="60% - 强调文字颜色 2 3" xfId="260"/>
+    <cellStyle name="60% - 强调文字颜色 2 4" xfId="261"/>
+    <cellStyle name="60% - 强调文字颜色 2 5" xfId="262"/>
+    <cellStyle name="60% - 强调文字颜色 2 6" xfId="263"/>
+    <cellStyle name="60% - 强调文字颜色 2 7" xfId="264"/>
+    <cellStyle name="60% - 强调文字颜色 2 8" xfId="265"/>
+    <cellStyle name="60% - 强调文字颜色 2 9" xfId="266"/>
+    <cellStyle name="60% - 强调文字颜色 3 10" xfId="267"/>
+    <cellStyle name="60% - 强调文字颜色 3 11" xfId="268"/>
+    <cellStyle name="60% - 强调文字颜色 3 12" xfId="269"/>
+    <cellStyle name="60% - 强调文字颜色 3 13" xfId="270"/>
+    <cellStyle name="60% - 强调文字颜色 3 14" xfId="271"/>
+    <cellStyle name="60% - 强调文字颜色 3 15" xfId="272"/>
+    <cellStyle name="60% - 强调文字颜色 3 16" xfId="273"/>
+    <cellStyle name="60% - 强调文字颜色 3 17" xfId="274"/>
+    <cellStyle name="60% - 强调文字颜色 3 18" xfId="275"/>
+    <cellStyle name="60% - 强调文字颜色 3 19" xfId="276"/>
+    <cellStyle name="60% - 强调文字颜色 3 2" xfId="277"/>
+    <cellStyle name="60% - 强调文字颜色 3 20" xfId="278"/>
+    <cellStyle name="60% - 强调文字颜色 3 3" xfId="279"/>
+    <cellStyle name="60% - 强调文字颜色 3 4" xfId="280"/>
+    <cellStyle name="60% - 强调文字颜色 3 5" xfId="281"/>
+    <cellStyle name="60% - 强调文字颜色 3 6" xfId="282"/>
+    <cellStyle name="60% - 强调文字颜色 3 7" xfId="283"/>
+    <cellStyle name="60% - 强调文字颜色 3 8" xfId="284"/>
+    <cellStyle name="60% - 强调文字颜色 3 9" xfId="285"/>
+    <cellStyle name="60% - 强调文字颜色 4 10" xfId="286"/>
+    <cellStyle name="60% - 强调文字颜色 4 11" xfId="287"/>
+    <cellStyle name="60% - 强调文字颜色 4 12" xfId="288"/>
+    <cellStyle name="60% - 强调文字颜色 4 13" xfId="289"/>
+    <cellStyle name="60% - 强调文字颜色 4 14" xfId="290"/>
+    <cellStyle name="60% - 强调文字颜色 4 15" xfId="291"/>
+    <cellStyle name="60% - 强调文字颜色 4 16" xfId="292"/>
+    <cellStyle name="60% - 强调文字颜色 4 17" xfId="293"/>
+    <cellStyle name="60% - 强调文字颜色 4 18" xfId="294"/>
+    <cellStyle name="60% - 强调文字颜色 4 19" xfId="295"/>
+    <cellStyle name="60% - 强调文字颜色 4 2" xfId="296"/>
+    <cellStyle name="60% - 强调文字颜色 4 20" xfId="297"/>
+    <cellStyle name="60% - 强调文字颜色 4 3" xfId="298"/>
+    <cellStyle name="60% - 强调文字颜色 4 4" xfId="299"/>
+    <cellStyle name="60% - 强调文字颜色 4 5" xfId="300"/>
+    <cellStyle name="60% - 强调文字颜色 4 6" xfId="301"/>
+    <cellStyle name="60% - 强调文字颜色 4 7" xfId="302"/>
+    <cellStyle name="60% - 强调文字颜色 4 8" xfId="303"/>
+    <cellStyle name="60% - 强调文字颜色 4 9" xfId="304"/>
+    <cellStyle name="60% - 强调文字颜色 5 10" xfId="305"/>
+    <cellStyle name="60% - 强调文字颜色 5 11" xfId="306"/>
+    <cellStyle name="60% - 强调文字颜色 5 12" xfId="307"/>
+    <cellStyle name="60% - 强调文字颜色 5 13" xfId="308"/>
+    <cellStyle name="60% - 强调文字颜色 5 14" xfId="309"/>
+    <cellStyle name="60% - 强调文字颜色 5 15" xfId="310"/>
+    <cellStyle name="60% - 强调文字颜色 5 16" xfId="311"/>
+    <cellStyle name="60% - 强调文字颜色 5 17" xfId="312"/>
+    <cellStyle name="60% - 强调文字颜色 5 18" xfId="313"/>
+    <cellStyle name="60% - 强调文字颜色 5 19" xfId="314"/>
+    <cellStyle name="60% - 强调文字颜色 5 2" xfId="315"/>
+    <cellStyle name="60% - 强调文字颜色 5 20" xfId="316"/>
+    <cellStyle name="60% - 强调文字颜色 5 3" xfId="317"/>
+    <cellStyle name="60% - 强调文字颜色 5 4" xfId="318"/>
+    <cellStyle name="60% - 强调文字颜色 5 5" xfId="319"/>
+    <cellStyle name="60% - 强调文字颜色 5 6" xfId="320"/>
+    <cellStyle name="60% - 强调文字颜色 5 7" xfId="321"/>
+    <cellStyle name="60% - 强调文字颜色 5 8" xfId="322"/>
+    <cellStyle name="60% - 强调文字颜色 5 9" xfId="323"/>
+    <cellStyle name="60% - 强调文字颜色 6 10" xfId="324"/>
+    <cellStyle name="60% - 强调文字颜色 6 11" xfId="325"/>
+    <cellStyle name="60% - 强调文字颜色 6 12" xfId="326"/>
+    <cellStyle name="60% - 强调文字颜色 6 13" xfId="327"/>
+    <cellStyle name="60% - 强调文字颜色 6 14" xfId="328"/>
+    <cellStyle name="60% - 强调文字颜色 6 15" xfId="329"/>
+    <cellStyle name="60% - 强调文字颜色 6 16" xfId="330"/>
+    <cellStyle name="60% - 强调文字颜色 6 17" xfId="331"/>
+    <cellStyle name="60% - 强调文字颜色 6 18" xfId="332"/>
+    <cellStyle name="60% - 强调文字颜色 6 19" xfId="333"/>
+    <cellStyle name="60% - 强调文字颜色 6 2" xfId="334"/>
+    <cellStyle name="60% - 强调文字颜色 6 20" xfId="335"/>
+    <cellStyle name="60% - 强调文字颜色 6 3" xfId="336"/>
+    <cellStyle name="60% - 强调文字颜色 6 4" xfId="337"/>
+    <cellStyle name="60% - 强调文字颜色 6 5" xfId="338"/>
+    <cellStyle name="60% - 强调文字颜色 6 6" xfId="339"/>
+    <cellStyle name="60% - 强调文字颜色 6 7" xfId="340"/>
+    <cellStyle name="60% - 强调文字颜色 6 8" xfId="341"/>
+    <cellStyle name="60% - 强调文字颜色 6 9" xfId="342"/>
     <cellStyle name="标题" xfId="343" builtinId="15" customBuiltin="1"/>
     <cellStyle name="标题 1" xfId="344" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="标题 1 10" xfId="345" xr:uid="{00000000-0005-0000-0000-000058010000}"/>
-    <cellStyle name="标题 1 11" xfId="346" xr:uid="{00000000-0005-0000-0000-000059010000}"/>
-    <cellStyle name="标题 1 12" xfId="347" xr:uid="{00000000-0005-0000-0000-00005A010000}"/>
-    <cellStyle name="标题 1 13" xfId="348" xr:uid="{00000000-0005-0000-0000-00005B010000}"/>
-    <cellStyle name="标题 1 14" xfId="349" xr:uid="{00000000-0005-0000-0000-00005C010000}"/>
-    <cellStyle name="标题 1 15" xfId="350" xr:uid="{00000000-0005-0000-0000-00005D010000}"/>
-    <cellStyle name="标题 1 16" xfId="351" xr:uid="{00000000-0005-0000-0000-00005E010000}"/>
-    <cellStyle name="标题 1 17" xfId="352" xr:uid="{00000000-0005-0000-0000-00005F010000}"/>
-    <cellStyle name="标题 1 18" xfId="353" xr:uid="{00000000-0005-0000-0000-000060010000}"/>
-    <cellStyle name="标题 1 19" xfId="354" xr:uid="{00000000-0005-0000-0000-000061010000}"/>
-    <cellStyle name="标题 1 2" xfId="355" xr:uid="{00000000-0005-0000-0000-000062010000}"/>
-    <cellStyle name="标题 1 20" xfId="356" xr:uid="{00000000-0005-0000-0000-000063010000}"/>
-    <cellStyle name="标题 1 3" xfId="357" xr:uid="{00000000-0005-0000-0000-000064010000}"/>
-    <cellStyle name="标题 1 4" xfId="358" xr:uid="{00000000-0005-0000-0000-000065010000}"/>
-    <cellStyle name="标题 1 5" xfId="359" xr:uid="{00000000-0005-0000-0000-000066010000}"/>
-    <cellStyle name="标题 1 6" xfId="360" xr:uid="{00000000-0005-0000-0000-000067010000}"/>
-    <cellStyle name="标题 1 7" xfId="361" xr:uid="{00000000-0005-0000-0000-000068010000}"/>
-    <cellStyle name="标题 1 8" xfId="362" xr:uid="{00000000-0005-0000-0000-000069010000}"/>
-    <cellStyle name="标题 1 9" xfId="363" xr:uid="{00000000-0005-0000-0000-00006A010000}"/>
-    <cellStyle name="标题 10" xfId="364" xr:uid="{00000000-0005-0000-0000-00006B010000}"/>
-    <cellStyle name="标题 11" xfId="365" xr:uid="{00000000-0005-0000-0000-00006C010000}"/>
-    <cellStyle name="标题 12" xfId="366" xr:uid="{00000000-0005-0000-0000-00006D010000}"/>
-    <cellStyle name="标题 13" xfId="367" xr:uid="{00000000-0005-0000-0000-00006E010000}"/>
-    <cellStyle name="标题 14" xfId="368" xr:uid="{00000000-0005-0000-0000-00006F010000}"/>
-    <cellStyle name="标题 15" xfId="369" xr:uid="{00000000-0005-0000-0000-000070010000}"/>
-    <cellStyle name="标题 16" xfId="370" xr:uid="{00000000-0005-0000-0000-000071010000}"/>
-    <cellStyle name="标题 17" xfId="371" xr:uid="{00000000-0005-0000-0000-000072010000}"/>
-    <cellStyle name="标题 18" xfId="372" xr:uid="{00000000-0005-0000-0000-000073010000}"/>
-    <cellStyle name="标题 19" xfId="373" xr:uid="{00000000-0005-0000-0000-000074010000}"/>
+    <cellStyle name="标题 1 10" xfId="345"/>
+    <cellStyle name="标题 1 11" xfId="346"/>
+    <cellStyle name="标题 1 12" xfId="347"/>
+    <cellStyle name="标题 1 13" xfId="348"/>
+    <cellStyle name="标题 1 14" xfId="349"/>
+    <cellStyle name="标题 1 15" xfId="350"/>
+    <cellStyle name="标题 1 16" xfId="351"/>
+    <cellStyle name="标题 1 17" xfId="352"/>
+    <cellStyle name="标题 1 18" xfId="353"/>
+    <cellStyle name="标题 1 19" xfId="354"/>
+    <cellStyle name="标题 1 2" xfId="355"/>
+    <cellStyle name="标题 1 20" xfId="356"/>
+    <cellStyle name="标题 1 3" xfId="357"/>
+    <cellStyle name="标题 1 4" xfId="358"/>
+    <cellStyle name="标题 1 5" xfId="359"/>
+    <cellStyle name="标题 1 6" xfId="360"/>
+    <cellStyle name="标题 1 7" xfId="361"/>
+    <cellStyle name="标题 1 8" xfId="362"/>
+    <cellStyle name="标题 1 9" xfId="363"/>
+    <cellStyle name="标题 10" xfId="364"/>
+    <cellStyle name="标题 11" xfId="365"/>
+    <cellStyle name="标题 12" xfId="366"/>
+    <cellStyle name="标题 13" xfId="367"/>
+    <cellStyle name="标题 14" xfId="368"/>
+    <cellStyle name="标题 15" xfId="369"/>
+    <cellStyle name="标题 16" xfId="370"/>
+    <cellStyle name="标题 17" xfId="371"/>
+    <cellStyle name="标题 18" xfId="372"/>
+    <cellStyle name="标题 19" xfId="373"/>
     <cellStyle name="标题 2" xfId="374" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="标题 2 10" xfId="375" xr:uid="{00000000-0005-0000-0000-000076010000}"/>
-    <cellStyle name="标题 2 11" xfId="376" xr:uid="{00000000-0005-0000-0000-000077010000}"/>
-    <cellStyle name="标题 2 12" xfId="377" xr:uid="{00000000-0005-0000-0000-000078010000}"/>
-    <cellStyle name="标题 2 13" xfId="378" xr:uid="{00000000-0005-0000-0000-000079010000}"/>
-    <cellStyle name="标题 2 14" xfId="379" xr:uid="{00000000-0005-0000-0000-00007A010000}"/>
-    <cellStyle name="标题 2 15" xfId="380" xr:uid="{00000000-0005-0000-0000-00007B010000}"/>
-    <cellStyle name="标题 2 16" xfId="381" xr:uid="{00000000-0005-0000-0000-00007C010000}"/>
-    <cellStyle name="标题 2 17" xfId="382" xr:uid="{00000000-0005-0000-0000-00007D010000}"/>
-    <cellStyle name="标题 2 18" xfId="383" xr:uid="{00000000-0005-0000-0000-00007E010000}"/>
-    <cellStyle name="标题 2 19" xfId="384" xr:uid="{00000000-0005-0000-0000-00007F010000}"/>
-    <cellStyle name="标题 2 2" xfId="385" xr:uid="{00000000-0005-0000-0000-000080010000}"/>
-    <cellStyle name="标题 2 20" xfId="386" xr:uid="{00000000-0005-0000-0000-000081010000}"/>
-    <cellStyle name="标题 2 3" xfId="387" xr:uid="{00000000-0005-0000-0000-000082010000}"/>
-    <cellStyle name="标题 2 4" xfId="388" xr:uid="{00000000-0005-0000-0000-000083010000}"/>
-    <cellStyle name="标题 2 5" xfId="389" xr:uid="{00000000-0005-0000-0000-000084010000}"/>
-    <cellStyle name="标题 2 6" xfId="390" xr:uid="{00000000-0005-0000-0000-000085010000}"/>
-    <cellStyle name="标题 2 7" xfId="391" xr:uid="{00000000-0005-0000-0000-000086010000}"/>
-    <cellStyle name="标题 2 8" xfId="392" xr:uid="{00000000-0005-0000-0000-000087010000}"/>
-    <cellStyle name="标题 2 9" xfId="393" xr:uid="{00000000-0005-0000-0000-000088010000}"/>
-    <cellStyle name="标题 20" xfId="394" xr:uid="{00000000-0005-0000-0000-000089010000}"/>
-    <cellStyle name="标题 21" xfId="395" xr:uid="{00000000-0005-0000-0000-00008A010000}"/>
-    <cellStyle name="标题 22" xfId="396" xr:uid="{00000000-0005-0000-0000-00008B010000}"/>
-    <cellStyle name="标题 23" xfId="397" xr:uid="{00000000-0005-0000-0000-00008C010000}"/>
+    <cellStyle name="标题 2 10" xfId="375"/>
+    <cellStyle name="标题 2 11" xfId="376"/>
+    <cellStyle name="标题 2 12" xfId="377"/>
+    <cellStyle name="标题 2 13" xfId="378"/>
+    <cellStyle name="标题 2 14" xfId="379"/>
+    <cellStyle name="标题 2 15" xfId="380"/>
+    <cellStyle name="标题 2 16" xfId="381"/>
+    <cellStyle name="标题 2 17" xfId="382"/>
+    <cellStyle name="标题 2 18" xfId="383"/>
+    <cellStyle name="标题 2 19" xfId="384"/>
+    <cellStyle name="标题 2 2" xfId="385"/>
+    <cellStyle name="标题 2 20" xfId="386"/>
+    <cellStyle name="标题 2 3" xfId="387"/>
+    <cellStyle name="标题 2 4" xfId="388"/>
+    <cellStyle name="标题 2 5" xfId="389"/>
+    <cellStyle name="标题 2 6" xfId="390"/>
+    <cellStyle name="标题 2 7" xfId="391"/>
+    <cellStyle name="标题 2 8" xfId="392"/>
+    <cellStyle name="标题 2 9" xfId="393"/>
+    <cellStyle name="标题 20" xfId="394"/>
+    <cellStyle name="标题 21" xfId="395"/>
+    <cellStyle name="标题 22" xfId="396"/>
+    <cellStyle name="标题 23" xfId="397"/>
     <cellStyle name="标题 3" xfId="398" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="标题 3 10" xfId="399" xr:uid="{00000000-0005-0000-0000-00008E010000}"/>
-    <cellStyle name="标题 3 11" xfId="400" xr:uid="{00000000-0005-0000-0000-00008F010000}"/>
-    <cellStyle name="标题 3 12" xfId="401" xr:uid="{00000000-0005-0000-0000-000090010000}"/>
-    <cellStyle name="标题 3 13" xfId="402" xr:uid="{00000000-0005-0000-0000-000091010000}"/>
-    <cellStyle name="标题 3 14" xfId="403" xr:uid="{00000000-0005-0000-0000-000092010000}"/>
-    <cellStyle name="标题 3 15" xfId="404" xr:uid="{00000000-0005-0000-0000-000093010000}"/>
-    <cellStyle name="标题 3 16" xfId="405" xr:uid="{00000000-0005-0000-0000-000094010000}"/>
-    <cellStyle name="标题 3 17" xfId="406" xr:uid="{00000000-0005-0000-0000-000095010000}"/>
-    <cellStyle name="标题 3 18" xfId="407" xr:uid="{00000000-0005-0000-0000-000096010000}"/>
-    <cellStyle name="标题 3 19" xfId="408" xr:uid="{00000000-0005-0000-0000-000097010000}"/>
-    <cellStyle name="标题 3 2" xfId="409" xr:uid="{00000000-0005-0000-0000-000098010000}"/>
-    <cellStyle name="标题 3 20" xfId="410" xr:uid="{00000000-0005-0000-0000-000099010000}"/>
-    <cellStyle name="标题 3 3" xfId="411" xr:uid="{00000000-0005-0000-0000-00009A010000}"/>
-    <cellStyle name="标题 3 4" xfId="412" xr:uid="{00000000-0005-0000-0000-00009B010000}"/>
-    <cellStyle name="标题 3 5" xfId="413" xr:uid="{00000000-0005-0000-0000-00009C010000}"/>
-    <cellStyle name="标题 3 6" xfId="414" xr:uid="{00000000-0005-0000-0000-00009D010000}"/>
-    <cellStyle name="标题 3 7" xfId="415" xr:uid="{00000000-0005-0000-0000-00009E010000}"/>
-    <cellStyle name="标题 3 8" xfId="416" xr:uid="{00000000-0005-0000-0000-00009F010000}"/>
-    <cellStyle name="标题 3 9" xfId="417" xr:uid="{00000000-0005-0000-0000-0000A0010000}"/>
+    <cellStyle name="标题 3 10" xfId="399"/>
+    <cellStyle name="标题 3 11" xfId="400"/>
+    <cellStyle name="标题 3 12" xfId="401"/>
+    <cellStyle name="标题 3 13" xfId="402"/>
+    <cellStyle name="标题 3 14" xfId="403"/>
+    <cellStyle name="标题 3 15" xfId="404"/>
+    <cellStyle name="标题 3 16" xfId="405"/>
+    <cellStyle name="标题 3 17" xfId="406"/>
+    <cellStyle name="标题 3 18" xfId="407"/>
+    <cellStyle name="标题 3 19" xfId="408"/>
+    <cellStyle name="标题 3 2" xfId="409"/>
+    <cellStyle name="标题 3 20" xfId="410"/>
+    <cellStyle name="标题 3 3" xfId="411"/>
+    <cellStyle name="标题 3 4" xfId="412"/>
+    <cellStyle name="标题 3 5" xfId="413"/>
+    <cellStyle name="标题 3 6" xfId="414"/>
+    <cellStyle name="标题 3 7" xfId="415"/>
+    <cellStyle name="标题 3 8" xfId="416"/>
+    <cellStyle name="标题 3 9" xfId="417"/>
     <cellStyle name="标题 4" xfId="418" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="标题 4 10" xfId="419" xr:uid="{00000000-0005-0000-0000-0000A2010000}"/>
-    <cellStyle name="标题 4 11" xfId="420" xr:uid="{00000000-0005-0000-0000-0000A3010000}"/>
-    <cellStyle name="标题 4 12" xfId="421" xr:uid="{00000000-0005-0000-0000-0000A4010000}"/>
-    <cellStyle name="标题 4 13" xfId="422" xr:uid="{00000000-0005-0000-0000-0000A5010000}"/>
-    <cellStyle name="标题 4 14" xfId="423" xr:uid="{00000000-0005-0000-0000-0000A6010000}"/>
-    <cellStyle name="标题 4 15" xfId="424" xr:uid="{00000000-0005-0000-0000-0000A7010000}"/>
-    <cellStyle name="标题 4 16" xfId="425" xr:uid="{00000000-0005-0000-0000-0000A8010000}"/>
-    <cellStyle name="标题 4 17" xfId="426" xr:uid="{00000000-0005-0000-0000-0000A9010000}"/>
-    <cellStyle name="标题 4 18" xfId="427" xr:uid="{00000000-0005-0000-0000-0000AA010000}"/>
-    <cellStyle name="标题 4 19" xfId="428" xr:uid="{00000000-0005-0000-0000-0000AB010000}"/>
-    <cellStyle name="标题 4 2" xfId="429" xr:uid="{00000000-0005-0000-0000-0000AC010000}"/>
-    <cellStyle name="标题 4 20" xfId="430" xr:uid="{00000000-0005-0000-0000-0000AD010000}"/>
-    <cellStyle name="标题 4 3" xfId="431" xr:uid="{00000000-0005-0000-0000-0000AE010000}"/>
-    <cellStyle name="标题 4 4" xfId="432" xr:uid="{00000000-0005-0000-0000-0000AF010000}"/>
-    <cellStyle name="标题 4 5" xfId="433" xr:uid="{00000000-0005-0000-0000-0000B0010000}"/>
-    <cellStyle name="标题 4 6" xfId="434" xr:uid="{00000000-0005-0000-0000-0000B1010000}"/>
-    <cellStyle name="标题 4 7" xfId="435" xr:uid="{00000000-0005-0000-0000-0000B2010000}"/>
-    <cellStyle name="标题 4 8" xfId="436" xr:uid="{00000000-0005-0000-0000-0000B3010000}"/>
-    <cellStyle name="标题 4 9" xfId="437" xr:uid="{00000000-0005-0000-0000-0000B4010000}"/>
-    <cellStyle name="标题 5" xfId="438" xr:uid="{00000000-0005-0000-0000-0000B5010000}"/>
-    <cellStyle name="标题 6" xfId="439" xr:uid="{00000000-0005-0000-0000-0000B6010000}"/>
-    <cellStyle name="标题 7" xfId="440" xr:uid="{00000000-0005-0000-0000-0000B7010000}"/>
-    <cellStyle name="标题 8" xfId="441" xr:uid="{00000000-0005-0000-0000-0000B8010000}"/>
-    <cellStyle name="标题 9" xfId="442" xr:uid="{00000000-0005-0000-0000-0000B9010000}"/>
+    <cellStyle name="标题 4 10" xfId="419"/>
+    <cellStyle name="标题 4 11" xfId="420"/>
+    <cellStyle name="标题 4 12" xfId="421"/>
+    <cellStyle name="标题 4 13" xfId="422"/>
+    <cellStyle name="标题 4 14" xfId="423"/>
+    <cellStyle name="标题 4 15" xfId="424"/>
+    <cellStyle name="标题 4 16" xfId="425"/>
+    <cellStyle name="标题 4 17" xfId="426"/>
+    <cellStyle name="标题 4 18" xfId="427"/>
+    <cellStyle name="标题 4 19" xfId="428"/>
+    <cellStyle name="标题 4 2" xfId="429"/>
+    <cellStyle name="标题 4 20" xfId="430"/>
+    <cellStyle name="标题 4 3" xfId="431"/>
+    <cellStyle name="标题 4 4" xfId="432"/>
+    <cellStyle name="标题 4 5" xfId="433"/>
+    <cellStyle name="标题 4 6" xfId="434"/>
+    <cellStyle name="标题 4 7" xfId="435"/>
+    <cellStyle name="标题 4 8" xfId="436"/>
+    <cellStyle name="标题 4 9" xfId="437"/>
+    <cellStyle name="标题 5" xfId="438"/>
+    <cellStyle name="标题 6" xfId="439"/>
+    <cellStyle name="标题 7" xfId="440"/>
+    <cellStyle name="标题 8" xfId="441"/>
+    <cellStyle name="标题 9" xfId="442"/>
     <cellStyle name="差" xfId="443" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="差 10" xfId="444" xr:uid="{00000000-0005-0000-0000-0000BB010000}"/>
-    <cellStyle name="差 11" xfId="445" xr:uid="{00000000-0005-0000-0000-0000BC010000}"/>
-    <cellStyle name="差 12" xfId="446" xr:uid="{00000000-0005-0000-0000-0000BD010000}"/>
-    <cellStyle name="差 13" xfId="447" xr:uid="{00000000-0005-0000-0000-0000BE010000}"/>
-    <cellStyle name="差 14" xfId="448" xr:uid="{00000000-0005-0000-0000-0000BF010000}"/>
-    <cellStyle name="差 15" xfId="449" xr:uid="{00000000-0005-0000-0000-0000C0010000}"/>
-    <cellStyle name="差 16" xfId="450" xr:uid="{00000000-0005-0000-0000-0000C1010000}"/>
-    <cellStyle name="差 17" xfId="451" xr:uid="{00000000-0005-0000-0000-0000C2010000}"/>
-    <cellStyle name="差 18" xfId="452" xr:uid="{00000000-0005-0000-0000-0000C3010000}"/>
-    <cellStyle name="差 19" xfId="453" xr:uid="{00000000-0005-0000-0000-0000C4010000}"/>
-    <cellStyle name="差 2" xfId="454" xr:uid="{00000000-0005-0000-0000-0000C5010000}"/>
-    <cellStyle name="差 20" xfId="455" xr:uid="{00000000-0005-0000-0000-0000C6010000}"/>
-    <cellStyle name="差 3" xfId="456" xr:uid="{00000000-0005-0000-0000-0000C7010000}"/>
-    <cellStyle name="差 4" xfId="457" xr:uid="{00000000-0005-0000-0000-0000C8010000}"/>
-    <cellStyle name="差 5" xfId="458" xr:uid="{00000000-0005-0000-0000-0000C9010000}"/>
-    <cellStyle name="差 6" xfId="459" xr:uid="{00000000-0005-0000-0000-0000CA010000}"/>
-    <cellStyle name="差 7" xfId="460" xr:uid="{00000000-0005-0000-0000-0000CB010000}"/>
-    <cellStyle name="差 8" xfId="461" xr:uid="{00000000-0005-0000-0000-0000CC010000}"/>
-    <cellStyle name="差 9" xfId="462" xr:uid="{00000000-0005-0000-0000-0000CD010000}"/>
+    <cellStyle name="差 10" xfId="444"/>
+    <cellStyle name="差 11" xfId="445"/>
+    <cellStyle name="差 12" xfId="446"/>
+    <cellStyle name="差 13" xfId="447"/>
+    <cellStyle name="差 14" xfId="448"/>
+    <cellStyle name="差 15" xfId="449"/>
+    <cellStyle name="差 16" xfId="450"/>
+    <cellStyle name="差 17" xfId="451"/>
+    <cellStyle name="差 18" xfId="452"/>
+    <cellStyle name="差 19" xfId="453"/>
+    <cellStyle name="差 2" xfId="454"/>
+    <cellStyle name="差 20" xfId="455"/>
+    <cellStyle name="差 3" xfId="456"/>
+    <cellStyle name="差 4" xfId="457"/>
+    <cellStyle name="差 5" xfId="458"/>
+    <cellStyle name="差 6" xfId="459"/>
+    <cellStyle name="差 7" xfId="460"/>
+    <cellStyle name="差 8" xfId="461"/>
+    <cellStyle name="差 9" xfId="462"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 10" xfId="463" xr:uid="{00000000-0005-0000-0000-0000CF010000}"/>
-    <cellStyle name="常规 11" xfId="464" xr:uid="{00000000-0005-0000-0000-0000D0010000}"/>
-    <cellStyle name="常规 12" xfId="465" xr:uid="{00000000-0005-0000-0000-0000D1010000}"/>
-    <cellStyle name="常规 13" xfId="466" xr:uid="{00000000-0005-0000-0000-0000D2010000}"/>
-    <cellStyle name="常规 14" xfId="467" xr:uid="{00000000-0005-0000-0000-0000D3010000}"/>
-    <cellStyle name="常规 15" xfId="468" xr:uid="{00000000-0005-0000-0000-0000D4010000}"/>
-    <cellStyle name="常规 16" xfId="469" xr:uid="{00000000-0005-0000-0000-0000D5010000}"/>
-    <cellStyle name="常规 17" xfId="470" xr:uid="{00000000-0005-0000-0000-0000D6010000}"/>
-    <cellStyle name="常规 18" xfId="471" xr:uid="{00000000-0005-0000-0000-0000D7010000}"/>
-    <cellStyle name="常规 19" xfId="472" xr:uid="{00000000-0005-0000-0000-0000D8010000}"/>
-    <cellStyle name="常规 2" xfId="473" xr:uid="{00000000-0005-0000-0000-0000D9010000}"/>
-    <cellStyle name="常规 2 2" xfId="474" xr:uid="{00000000-0005-0000-0000-0000DA010000}"/>
-    <cellStyle name="常规 20" xfId="475" xr:uid="{00000000-0005-0000-0000-0000DB010000}"/>
-    <cellStyle name="常规 3" xfId="476" xr:uid="{00000000-0005-0000-0000-0000DC010000}"/>
-    <cellStyle name="常规 4" xfId="477" xr:uid="{00000000-0005-0000-0000-0000DD010000}"/>
-    <cellStyle name="常规 5" xfId="478" xr:uid="{00000000-0005-0000-0000-0000DE010000}"/>
-    <cellStyle name="常规 6" xfId="479" xr:uid="{00000000-0005-0000-0000-0000DF010000}"/>
-    <cellStyle name="常规 7" xfId="480" xr:uid="{00000000-0005-0000-0000-0000E0010000}"/>
-    <cellStyle name="常规 8" xfId="481" xr:uid="{00000000-0005-0000-0000-0000E1010000}"/>
-    <cellStyle name="常规 9" xfId="482" xr:uid="{00000000-0005-0000-0000-0000E2010000}"/>
+    <cellStyle name="常规 10" xfId="463"/>
+    <cellStyle name="常规 11" xfId="464"/>
+    <cellStyle name="常规 12" xfId="465"/>
+    <cellStyle name="常规 13" xfId="466"/>
+    <cellStyle name="常规 14" xfId="467"/>
+    <cellStyle name="常规 15" xfId="468"/>
+    <cellStyle name="常规 16" xfId="469"/>
+    <cellStyle name="常规 17" xfId="470"/>
+    <cellStyle name="常规 18" xfId="471"/>
+    <cellStyle name="常规 19" xfId="472"/>
+    <cellStyle name="常规 2" xfId="473"/>
+    <cellStyle name="常规 2 2" xfId="474"/>
+    <cellStyle name="常规 20" xfId="475"/>
+    <cellStyle name="常规 3" xfId="476"/>
+    <cellStyle name="常规 4" xfId="477"/>
+    <cellStyle name="常规 5" xfId="478"/>
+    <cellStyle name="常规 6" xfId="479"/>
+    <cellStyle name="常规 7" xfId="480"/>
+    <cellStyle name="常规 8" xfId="481"/>
+    <cellStyle name="常规 9" xfId="482"/>
     <cellStyle name="好" xfId="483" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="好 10" xfId="484" xr:uid="{00000000-0005-0000-0000-0000E4010000}"/>
-    <cellStyle name="好 11" xfId="485" xr:uid="{00000000-0005-0000-0000-0000E5010000}"/>
-    <cellStyle name="好 12" xfId="486" xr:uid="{00000000-0005-0000-0000-0000E6010000}"/>
-    <cellStyle name="好 13" xfId="487" xr:uid="{00000000-0005-0000-0000-0000E7010000}"/>
-    <cellStyle name="好 14" xfId="488" xr:uid="{00000000-0005-0000-0000-0000E8010000}"/>
-    <cellStyle name="好 15" xfId="489" xr:uid="{00000000-0005-0000-0000-0000E9010000}"/>
-    <cellStyle name="好 16" xfId="490" xr:uid="{00000000-0005-0000-0000-0000EA010000}"/>
-    <cellStyle name="好 17" xfId="491" xr:uid="{00000000-0005-0000-0000-0000EB010000}"/>
-    <cellStyle name="好 18" xfId="492" xr:uid="{00000000-0005-0000-0000-0000EC010000}"/>
-    <cellStyle name="好 19" xfId="493" xr:uid="{00000000-0005-0000-0000-0000ED010000}"/>
-    <cellStyle name="好 2" xfId="494" xr:uid="{00000000-0005-0000-0000-0000EE010000}"/>
-    <cellStyle name="好 20" xfId="495" xr:uid="{00000000-0005-0000-0000-0000EF010000}"/>
-    <cellStyle name="好 3" xfId="496" xr:uid="{00000000-0005-0000-0000-0000F0010000}"/>
-    <cellStyle name="好 4" xfId="497" xr:uid="{00000000-0005-0000-0000-0000F1010000}"/>
-    <cellStyle name="好 5" xfId="498" xr:uid="{00000000-0005-0000-0000-0000F2010000}"/>
-    <cellStyle name="好 6" xfId="499" xr:uid="{00000000-0005-0000-0000-0000F3010000}"/>
-    <cellStyle name="好 7" xfId="500" xr:uid="{00000000-0005-0000-0000-0000F4010000}"/>
-    <cellStyle name="好 8" xfId="501" xr:uid="{00000000-0005-0000-0000-0000F5010000}"/>
-    <cellStyle name="好 9" xfId="502" xr:uid="{00000000-0005-0000-0000-0000F6010000}"/>
+    <cellStyle name="好 10" xfId="484"/>
+    <cellStyle name="好 11" xfId="485"/>
+    <cellStyle name="好 12" xfId="486"/>
+    <cellStyle name="好 13" xfId="487"/>
+    <cellStyle name="好 14" xfId="488"/>
+    <cellStyle name="好 15" xfId="489"/>
+    <cellStyle name="好 16" xfId="490"/>
+    <cellStyle name="好 17" xfId="491"/>
+    <cellStyle name="好 18" xfId="492"/>
+    <cellStyle name="好 19" xfId="493"/>
+    <cellStyle name="好 2" xfId="494"/>
+    <cellStyle name="好 20" xfId="495"/>
+    <cellStyle name="好 3" xfId="496"/>
+    <cellStyle name="好 4" xfId="497"/>
+    <cellStyle name="好 5" xfId="498"/>
+    <cellStyle name="好 6" xfId="499"/>
+    <cellStyle name="好 7" xfId="500"/>
+    <cellStyle name="好 8" xfId="501"/>
+    <cellStyle name="好 9" xfId="502"/>
     <cellStyle name="汇总" xfId="503" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="汇总 10" xfId="504" xr:uid="{00000000-0005-0000-0000-0000F8010000}"/>
-    <cellStyle name="汇总 11" xfId="505" xr:uid="{00000000-0005-0000-0000-0000F9010000}"/>
-    <cellStyle name="汇总 12" xfId="506" xr:uid="{00000000-0005-0000-0000-0000FA010000}"/>
-    <cellStyle name="汇总 13" xfId="507" xr:uid="{00000000-0005-0000-0000-0000FB010000}"/>
-    <cellStyle name="汇总 14" xfId="508" xr:uid="{00000000-0005-0000-0000-0000FC010000}"/>
-    <cellStyle name="汇总 15" xfId="509" xr:uid="{00000000-0005-0000-0000-0000FD010000}"/>
-    <cellStyle name="汇总 16" xfId="510" xr:uid="{00000000-0005-0000-0000-0000FE010000}"/>
-    <cellStyle name="汇总 17" xfId="511" xr:uid="{00000000-0005-0000-0000-0000FF010000}"/>
-    <cellStyle name="汇总 18" xfId="512" xr:uid="{00000000-0005-0000-0000-000000020000}"/>
-    <cellStyle name="汇总 19" xfId="513" xr:uid="{00000000-0005-0000-0000-000001020000}"/>
-    <cellStyle name="汇总 2" xfId="514" xr:uid="{00000000-0005-0000-0000-000002020000}"/>
-    <cellStyle name="汇总 20" xfId="515" xr:uid="{00000000-0005-0000-0000-000003020000}"/>
-    <cellStyle name="汇总 3" xfId="516" xr:uid="{00000000-0005-0000-0000-000004020000}"/>
-    <cellStyle name="汇总 4" xfId="517" xr:uid="{00000000-0005-0000-0000-000005020000}"/>
-    <cellStyle name="汇总 5" xfId="518" xr:uid="{00000000-0005-0000-0000-000006020000}"/>
-    <cellStyle name="汇总 6" xfId="519" xr:uid="{00000000-0005-0000-0000-000007020000}"/>
-    <cellStyle name="汇总 7" xfId="520" xr:uid="{00000000-0005-0000-0000-000008020000}"/>
-    <cellStyle name="汇总 8" xfId="521" xr:uid="{00000000-0005-0000-0000-000009020000}"/>
-    <cellStyle name="汇总 9" xfId="522" xr:uid="{00000000-0005-0000-0000-00000A020000}"/>
+    <cellStyle name="汇总 10" xfId="504"/>
+    <cellStyle name="汇总 11" xfId="505"/>
+    <cellStyle name="汇总 12" xfId="506"/>
+    <cellStyle name="汇总 13" xfId="507"/>
+    <cellStyle name="汇总 14" xfId="508"/>
+    <cellStyle name="汇总 15" xfId="509"/>
+    <cellStyle name="汇总 16" xfId="510"/>
+    <cellStyle name="汇总 17" xfId="511"/>
+    <cellStyle name="汇总 18" xfId="512"/>
+    <cellStyle name="汇总 19" xfId="513"/>
+    <cellStyle name="汇总 2" xfId="514"/>
+    <cellStyle name="汇总 20" xfId="515"/>
+    <cellStyle name="汇总 3" xfId="516"/>
+    <cellStyle name="汇总 4" xfId="517"/>
+    <cellStyle name="汇总 5" xfId="518"/>
+    <cellStyle name="汇总 6" xfId="519"/>
+    <cellStyle name="汇总 7" xfId="520"/>
+    <cellStyle name="汇总 8" xfId="521"/>
+    <cellStyle name="汇总 9" xfId="522"/>
     <cellStyle name="计算" xfId="523" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="计算 10" xfId="524" xr:uid="{00000000-0005-0000-0000-00000C020000}"/>
-    <cellStyle name="计算 11" xfId="525" xr:uid="{00000000-0005-0000-0000-00000D020000}"/>
-    <cellStyle name="计算 12" xfId="526" xr:uid="{00000000-0005-0000-0000-00000E020000}"/>
-    <cellStyle name="计算 13" xfId="527" xr:uid="{00000000-0005-0000-0000-00000F020000}"/>
-    <cellStyle name="计算 14" xfId="528" xr:uid="{00000000-0005-0000-0000-000010020000}"/>
-    <cellStyle name="计算 15" xfId="529" xr:uid="{00000000-0005-0000-0000-000011020000}"/>
-    <cellStyle name="计算 16" xfId="530" xr:uid="{00000000-0005-0000-0000-000012020000}"/>
-    <cellStyle name="计算 17" xfId="531" xr:uid="{00000000-0005-0000-0000-000013020000}"/>
-    <cellStyle name="计算 18" xfId="532" xr:uid="{00000000-0005-0000-0000-000014020000}"/>
-    <cellStyle name="计算 19" xfId="533" xr:uid="{00000000-0005-0000-0000-000015020000}"/>
-    <cellStyle name="计算 2" xfId="534" xr:uid="{00000000-0005-0000-0000-000016020000}"/>
-    <cellStyle name="计算 20" xfId="535" xr:uid="{00000000-0005-0000-0000-000017020000}"/>
-    <cellStyle name="计算 3" xfId="536" xr:uid="{00000000-0005-0000-0000-000018020000}"/>
-    <cellStyle name="计算 4" xfId="537" xr:uid="{00000000-0005-0000-0000-000019020000}"/>
-    <cellStyle name="计算 5" xfId="538" xr:uid="{00000000-0005-0000-0000-00001A020000}"/>
-    <cellStyle name="计算 6" xfId="539" xr:uid="{00000000-0005-0000-0000-00001B020000}"/>
-    <cellStyle name="计算 7" xfId="540" xr:uid="{00000000-0005-0000-0000-00001C020000}"/>
-    <cellStyle name="计算 8" xfId="541" xr:uid="{00000000-0005-0000-0000-00001D020000}"/>
-    <cellStyle name="计算 9" xfId="542" xr:uid="{00000000-0005-0000-0000-00001E020000}"/>
+    <cellStyle name="计算 10" xfId="524"/>
+    <cellStyle name="计算 11" xfId="525"/>
+    <cellStyle name="计算 12" xfId="526"/>
+    <cellStyle name="计算 13" xfId="527"/>
+    <cellStyle name="计算 14" xfId="528"/>
+    <cellStyle name="计算 15" xfId="529"/>
+    <cellStyle name="计算 16" xfId="530"/>
+    <cellStyle name="计算 17" xfId="531"/>
+    <cellStyle name="计算 18" xfId="532"/>
+    <cellStyle name="计算 19" xfId="533"/>
+    <cellStyle name="计算 2" xfId="534"/>
+    <cellStyle name="计算 20" xfId="535"/>
+    <cellStyle name="计算 3" xfId="536"/>
+    <cellStyle name="计算 4" xfId="537"/>
+    <cellStyle name="计算 5" xfId="538"/>
+    <cellStyle name="计算 6" xfId="539"/>
+    <cellStyle name="计算 7" xfId="540"/>
+    <cellStyle name="计算 8" xfId="541"/>
+    <cellStyle name="计算 9" xfId="542"/>
     <cellStyle name="检查单元格" xfId="543" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="检查单元格 10" xfId="544" xr:uid="{00000000-0005-0000-0000-000020020000}"/>
-    <cellStyle name="检查单元格 11" xfId="545" xr:uid="{00000000-0005-0000-0000-000021020000}"/>
-    <cellStyle name="检查单元格 12" xfId="546" xr:uid="{00000000-0005-0000-0000-000022020000}"/>
-    <cellStyle name="检查单元格 13" xfId="547" xr:uid="{00000000-0005-0000-0000-000023020000}"/>
-    <cellStyle name="检查单元格 14" xfId="548" xr:uid="{00000000-0005-0000-0000-000024020000}"/>
-    <cellStyle name="检查单元格 15" xfId="549" xr:uid="{00000000-0005-0000-0000-000025020000}"/>
-    <cellStyle name="检查单元格 16" xfId="550" xr:uid="{00000000-0005-0000-0000-000026020000}"/>
-    <cellStyle name="检查单元格 17" xfId="551" xr:uid="{00000000-0005-0000-0000-000027020000}"/>
-    <cellStyle name="检查单元格 18" xfId="552" xr:uid="{00000000-0005-0000-0000-000028020000}"/>
-    <cellStyle name="检查单元格 19" xfId="553" xr:uid="{00000000-0005-0000-0000-000029020000}"/>
-    <cellStyle name="检查单元格 2" xfId="554" xr:uid="{00000000-0005-0000-0000-00002A020000}"/>
-    <cellStyle name="检查单元格 20" xfId="555" xr:uid="{00000000-0005-0000-0000-00002B020000}"/>
-    <cellStyle name="检查单元格 3" xfId="556" xr:uid="{00000000-0005-0000-0000-00002C020000}"/>
-    <cellStyle name="检查单元格 4" xfId="557" xr:uid="{00000000-0005-0000-0000-00002D020000}"/>
-    <cellStyle name="检查单元格 5" xfId="558" xr:uid="{00000000-0005-0000-0000-00002E020000}"/>
-    <cellStyle name="检查单元格 6" xfId="559" xr:uid="{00000000-0005-0000-0000-00002F020000}"/>
-    <cellStyle name="检查单元格 7" xfId="560" xr:uid="{00000000-0005-0000-0000-000030020000}"/>
-    <cellStyle name="检查单元格 8" xfId="561" xr:uid="{00000000-0005-0000-0000-000031020000}"/>
-    <cellStyle name="检查单元格 9" xfId="562" xr:uid="{00000000-0005-0000-0000-000032020000}"/>
+    <cellStyle name="检查单元格 10" xfId="544"/>
+    <cellStyle name="检查单元格 11" xfId="545"/>
+    <cellStyle name="检查单元格 12" xfId="546"/>
+    <cellStyle name="检查单元格 13" xfId="547"/>
+    <cellStyle name="检查单元格 14" xfId="548"/>
+    <cellStyle name="检查单元格 15" xfId="549"/>
+    <cellStyle name="检查单元格 16" xfId="550"/>
+    <cellStyle name="检查单元格 17" xfId="551"/>
+    <cellStyle name="检查单元格 18" xfId="552"/>
+    <cellStyle name="检查单元格 19" xfId="553"/>
+    <cellStyle name="检查单元格 2" xfId="554"/>
+    <cellStyle name="检查单元格 20" xfId="555"/>
+    <cellStyle name="检查单元格 3" xfId="556"/>
+    <cellStyle name="检查单元格 4" xfId="557"/>
+    <cellStyle name="检查单元格 5" xfId="558"/>
+    <cellStyle name="检查单元格 6" xfId="559"/>
+    <cellStyle name="检查单元格 7" xfId="560"/>
+    <cellStyle name="检查单元格 8" xfId="561"/>
+    <cellStyle name="检查单元格 9" xfId="562"/>
     <cellStyle name="解释性文本" xfId="563" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="解释性文本 10" xfId="564" xr:uid="{00000000-0005-0000-0000-000034020000}"/>
-    <cellStyle name="解释性文本 11" xfId="565" xr:uid="{00000000-0005-0000-0000-000035020000}"/>
-    <cellStyle name="解释性文本 12" xfId="566" xr:uid="{00000000-0005-0000-0000-000036020000}"/>
-    <cellStyle name="解释性文本 13" xfId="567" xr:uid="{00000000-0005-0000-0000-000037020000}"/>
-    <cellStyle name="解释性文本 14" xfId="568" xr:uid="{00000000-0005-0000-0000-000038020000}"/>
-    <cellStyle name="解释性文本 15" xfId="569" xr:uid="{00000000-0005-0000-0000-000039020000}"/>
-    <cellStyle name="解释性文本 16" xfId="570" xr:uid="{00000000-0005-0000-0000-00003A020000}"/>
-    <cellStyle name="解释性文本 17" xfId="571" xr:uid="{00000000-0005-0000-0000-00003B020000}"/>
-    <cellStyle name="解释性文本 18" xfId="572" xr:uid="{00000000-0005-0000-0000-00003C020000}"/>
-    <cellStyle name="解释性文本 19" xfId="573" xr:uid="{00000000-0005-0000-0000-00003D020000}"/>
-    <cellStyle name="解释性文本 2" xfId="574" xr:uid="{00000000-0005-0000-0000-00003E020000}"/>
-    <cellStyle name="解释性文本 20" xfId="575" xr:uid="{00000000-0005-0000-0000-00003F020000}"/>
-    <cellStyle name="解释性文本 3" xfId="576" xr:uid="{00000000-0005-0000-0000-000040020000}"/>
-    <cellStyle name="解释性文本 4" xfId="577" xr:uid="{00000000-0005-0000-0000-000041020000}"/>
-    <cellStyle name="解释性文本 5" xfId="578" xr:uid="{00000000-0005-0000-0000-000042020000}"/>
-    <cellStyle name="解释性文本 6" xfId="579" xr:uid="{00000000-0005-0000-0000-000043020000}"/>
-    <cellStyle name="解释性文本 7" xfId="580" xr:uid="{00000000-0005-0000-0000-000044020000}"/>
-    <cellStyle name="解释性文本 8" xfId="581" xr:uid="{00000000-0005-0000-0000-000045020000}"/>
-    <cellStyle name="解释性文本 9" xfId="582" xr:uid="{00000000-0005-0000-0000-000046020000}"/>
+    <cellStyle name="解释性文本 10" xfId="564"/>
+    <cellStyle name="解释性文本 11" xfId="565"/>
+    <cellStyle name="解释性文本 12" xfId="566"/>
+    <cellStyle name="解释性文本 13" xfId="567"/>
+    <cellStyle name="解释性文本 14" xfId="568"/>
+    <cellStyle name="解释性文本 15" xfId="569"/>
+    <cellStyle name="解释性文本 16" xfId="570"/>
+    <cellStyle name="解释性文本 17" xfId="571"/>
+    <cellStyle name="解释性文本 18" xfId="572"/>
+    <cellStyle name="解释性文本 19" xfId="573"/>
+    <cellStyle name="解释性文本 2" xfId="574"/>
+    <cellStyle name="解释性文本 20" xfId="575"/>
+    <cellStyle name="解释性文本 3" xfId="576"/>
+    <cellStyle name="解释性文本 4" xfId="577"/>
+    <cellStyle name="解释性文本 5" xfId="578"/>
+    <cellStyle name="解释性文本 6" xfId="579"/>
+    <cellStyle name="解释性文本 7" xfId="580"/>
+    <cellStyle name="解释性文本 8" xfId="581"/>
+    <cellStyle name="解释性文本 9" xfId="582"/>
     <cellStyle name="警告文本" xfId="583" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="警告文本 10" xfId="584" xr:uid="{00000000-0005-0000-0000-000048020000}"/>
-    <cellStyle name="警告文本 11" xfId="585" xr:uid="{00000000-0005-0000-0000-000049020000}"/>
-    <cellStyle name="警告文本 12" xfId="586" xr:uid="{00000000-0005-0000-0000-00004A020000}"/>
-    <cellStyle name="警告文本 13" xfId="587" xr:uid="{00000000-0005-0000-0000-00004B020000}"/>
-    <cellStyle name="警告文本 14" xfId="588" xr:uid="{00000000-0005-0000-0000-00004C020000}"/>
-    <cellStyle name="警告文本 15" xfId="589" xr:uid="{00000000-0005-0000-0000-00004D020000}"/>
-    <cellStyle name="警告文本 16" xfId="590" xr:uid="{00000000-0005-0000-0000-00004E020000}"/>
-    <cellStyle name="警告文本 17" xfId="591" xr:uid="{00000000-0005-0000-0000-00004F020000}"/>
-    <cellStyle name="警告文本 18" xfId="592" xr:uid="{00000000-0005-0000-0000-000050020000}"/>
-    <cellStyle name="警告文本 19" xfId="593" xr:uid="{00000000-0005-0000-0000-000051020000}"/>
-    <cellStyle name="警告文本 2" xfId="594" xr:uid="{00000000-0005-0000-0000-000052020000}"/>
-    <cellStyle name="警告文本 20" xfId="595" xr:uid="{00000000-0005-0000-0000-000053020000}"/>
-    <cellStyle name="警告文本 3" xfId="596" xr:uid="{00000000-0005-0000-0000-000054020000}"/>
-    <cellStyle name="警告文本 4" xfId="597" xr:uid="{00000000-0005-0000-0000-000055020000}"/>
-    <cellStyle name="警告文本 5" xfId="598" xr:uid="{00000000-0005-0000-0000-000056020000}"/>
-    <cellStyle name="警告文本 6" xfId="599" xr:uid="{00000000-0005-0000-0000-000057020000}"/>
-    <cellStyle name="警告文本 7" xfId="600" xr:uid="{00000000-0005-0000-0000-000058020000}"/>
-    <cellStyle name="警告文本 8" xfId="601" xr:uid="{00000000-0005-0000-0000-000059020000}"/>
-    <cellStyle name="警告文本 9" xfId="602" xr:uid="{00000000-0005-0000-0000-00005A020000}"/>
+    <cellStyle name="警告文本 10" xfId="584"/>
+    <cellStyle name="警告文本 11" xfId="585"/>
+    <cellStyle name="警告文本 12" xfId="586"/>
+    <cellStyle name="警告文本 13" xfId="587"/>
+    <cellStyle name="警告文本 14" xfId="588"/>
+    <cellStyle name="警告文本 15" xfId="589"/>
+    <cellStyle name="警告文本 16" xfId="590"/>
+    <cellStyle name="警告文本 17" xfId="591"/>
+    <cellStyle name="警告文本 18" xfId="592"/>
+    <cellStyle name="警告文本 19" xfId="593"/>
+    <cellStyle name="警告文本 2" xfId="594"/>
+    <cellStyle name="警告文本 20" xfId="595"/>
+    <cellStyle name="警告文本 3" xfId="596"/>
+    <cellStyle name="警告文本 4" xfId="597"/>
+    <cellStyle name="警告文本 5" xfId="598"/>
+    <cellStyle name="警告文本 6" xfId="599"/>
+    <cellStyle name="警告文本 7" xfId="600"/>
+    <cellStyle name="警告文本 8" xfId="601"/>
+    <cellStyle name="警告文本 9" xfId="602"/>
     <cellStyle name="链接单元格" xfId="603" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="链接单元格 10" xfId="604" xr:uid="{00000000-0005-0000-0000-00005C020000}"/>
-    <cellStyle name="链接单元格 11" xfId="605" xr:uid="{00000000-0005-0000-0000-00005D020000}"/>
-    <cellStyle name="链接单元格 12" xfId="606" xr:uid="{00000000-0005-0000-0000-00005E020000}"/>
-    <cellStyle name="链接单元格 13" xfId="607" xr:uid="{00000000-0005-0000-0000-00005F020000}"/>
-    <cellStyle name="链接单元格 14" xfId="608" xr:uid="{00000000-0005-0000-0000-000060020000}"/>
-    <cellStyle name="链接单元格 15" xfId="609" xr:uid="{00000000-0005-0000-0000-000061020000}"/>
-    <cellStyle name="链接单元格 16" xfId="610" xr:uid="{00000000-0005-0000-0000-000062020000}"/>
-    <cellStyle name="链接单元格 17" xfId="611" xr:uid="{00000000-0005-0000-0000-000063020000}"/>
-    <cellStyle name="链接单元格 18" xfId="612" xr:uid="{00000000-0005-0000-0000-000064020000}"/>
-    <cellStyle name="链接单元格 19" xfId="613" xr:uid="{00000000-0005-0000-0000-000065020000}"/>
-    <cellStyle name="链接单元格 2" xfId="614" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
-    <cellStyle name="链接单元格 20" xfId="615" xr:uid="{00000000-0005-0000-0000-000067020000}"/>
-    <cellStyle name="链接单元格 3" xfId="616" xr:uid="{00000000-0005-0000-0000-000068020000}"/>
-    <cellStyle name="链接单元格 4" xfId="617" xr:uid="{00000000-0005-0000-0000-000069020000}"/>
-    <cellStyle name="链接单元格 5" xfId="618" xr:uid="{00000000-0005-0000-0000-00006A020000}"/>
-    <cellStyle name="链接单元格 6" xfId="619" xr:uid="{00000000-0005-0000-0000-00006B020000}"/>
-    <cellStyle name="链接单元格 7" xfId="620" xr:uid="{00000000-0005-0000-0000-00006C020000}"/>
-    <cellStyle name="链接单元格 8" xfId="621" xr:uid="{00000000-0005-0000-0000-00006D020000}"/>
-    <cellStyle name="链接单元格 9" xfId="622" xr:uid="{00000000-0005-0000-0000-00006E020000}"/>
-    <cellStyle name="强调文字颜色 1 10" xfId="623" xr:uid="{00000000-0005-0000-0000-00006F020000}"/>
-    <cellStyle name="强调文字颜色 1 11" xfId="624" xr:uid="{00000000-0005-0000-0000-000070020000}"/>
-    <cellStyle name="强调文字颜色 1 12" xfId="625" xr:uid="{00000000-0005-0000-0000-000071020000}"/>
-    <cellStyle name="强调文字颜色 1 13" xfId="626" xr:uid="{00000000-0005-0000-0000-000072020000}"/>
-    <cellStyle name="强调文字颜色 1 14" xfId="627" xr:uid="{00000000-0005-0000-0000-000073020000}"/>
-    <cellStyle name="强调文字颜色 1 15" xfId="628" xr:uid="{00000000-0005-0000-0000-000074020000}"/>
-    <cellStyle name="强调文字颜色 1 16" xfId="629" xr:uid="{00000000-0005-0000-0000-000075020000}"/>
-    <cellStyle name="强调文字颜色 1 17" xfId="630" xr:uid="{00000000-0005-0000-0000-000076020000}"/>
-    <cellStyle name="强调文字颜色 1 18" xfId="631" xr:uid="{00000000-0005-0000-0000-000077020000}"/>
-    <cellStyle name="强调文字颜色 1 19" xfId="632" xr:uid="{00000000-0005-0000-0000-000078020000}"/>
-    <cellStyle name="强调文字颜色 1 2" xfId="633" xr:uid="{00000000-0005-0000-0000-000079020000}"/>
-    <cellStyle name="强调文字颜色 1 20" xfId="634" xr:uid="{00000000-0005-0000-0000-00007A020000}"/>
-    <cellStyle name="强调文字颜色 1 3" xfId="635" xr:uid="{00000000-0005-0000-0000-00007B020000}"/>
-    <cellStyle name="强调文字颜色 1 4" xfId="636" xr:uid="{00000000-0005-0000-0000-00007C020000}"/>
-    <cellStyle name="强调文字颜色 1 5" xfId="637" xr:uid="{00000000-0005-0000-0000-00007D020000}"/>
-    <cellStyle name="强调文字颜色 1 6" xfId="638" xr:uid="{00000000-0005-0000-0000-00007E020000}"/>
-    <cellStyle name="强调文字颜色 1 7" xfId="639" xr:uid="{00000000-0005-0000-0000-00007F020000}"/>
-    <cellStyle name="强调文字颜色 1 8" xfId="640" xr:uid="{00000000-0005-0000-0000-000080020000}"/>
-    <cellStyle name="强调文字颜色 1 9" xfId="641" xr:uid="{00000000-0005-0000-0000-000081020000}"/>
-    <cellStyle name="强调文字颜色 2 10" xfId="642" xr:uid="{00000000-0005-0000-0000-000082020000}"/>
-    <cellStyle name="强调文字颜色 2 11" xfId="643" xr:uid="{00000000-0005-0000-0000-000083020000}"/>
-    <cellStyle name="强调文字颜色 2 12" xfId="644" xr:uid="{00000000-0005-0000-0000-000084020000}"/>
-    <cellStyle name="强调文字颜色 2 13" xfId="645" xr:uid="{00000000-0005-0000-0000-000085020000}"/>
-    <cellStyle name="强调文字颜色 2 14" xfId="646" xr:uid="{00000000-0005-0000-0000-000086020000}"/>
-    <cellStyle name="强调文字颜色 2 15" xfId="647" xr:uid="{00000000-0005-0000-0000-000087020000}"/>
-    <cellStyle name="强调文字颜色 2 16" xfId="648" xr:uid="{00000000-0005-0000-0000-000088020000}"/>
-    <cellStyle name="强调文字颜色 2 17" xfId="649" xr:uid="{00000000-0005-0000-0000-000089020000}"/>
-    <cellStyle name="强调文字颜色 2 18" xfId="650" xr:uid="{00000000-0005-0000-0000-00008A020000}"/>
-    <cellStyle name="强调文字颜色 2 19" xfId="651" xr:uid="{00000000-0005-0000-0000-00008B020000}"/>
-    <cellStyle name="强调文字颜色 2 2" xfId="652" xr:uid="{00000000-0005-0000-0000-00008C020000}"/>
-    <cellStyle name="强调文字颜色 2 20" xfId="653" xr:uid="{00000000-0005-0000-0000-00008D020000}"/>
-    <cellStyle name="强调文字颜色 2 3" xfId="654" xr:uid="{00000000-0005-0000-0000-00008E020000}"/>
-    <cellStyle name="强调文字颜色 2 4" xfId="655" xr:uid="{00000000-0005-0000-0000-00008F020000}"/>
-    <cellStyle name="强调文字颜色 2 5" xfId="656" xr:uid="{00000000-0005-0000-0000-000090020000}"/>
-    <cellStyle name="强调文字颜色 2 6" xfId="657" xr:uid="{00000000-0005-0000-0000-000091020000}"/>
-    <cellStyle name="强调文字颜色 2 7" xfId="658" xr:uid="{00000000-0005-0000-0000-000092020000}"/>
-    <cellStyle name="强调文字颜色 2 8" xfId="659" xr:uid="{00000000-0005-0000-0000-000093020000}"/>
-    <cellStyle name="强调文字颜色 2 9" xfId="660" xr:uid="{00000000-0005-0000-0000-000094020000}"/>
-    <cellStyle name="强调文字颜色 3 10" xfId="661" xr:uid="{00000000-0005-0000-0000-000095020000}"/>
-    <cellStyle name="强调文字颜色 3 11" xfId="662" xr:uid="{00000000-0005-0000-0000-000096020000}"/>
-    <cellStyle name="强调文字颜色 3 12" xfId="663" xr:uid="{00000000-0005-0000-0000-000097020000}"/>
-    <cellStyle name="强调文字颜色 3 13" xfId="664" xr:uid="{00000000-0005-0000-0000-000098020000}"/>
-    <cellStyle name="强调文字颜色 3 14" xfId="665" xr:uid="{00000000-0005-0000-0000-000099020000}"/>
-    <cellStyle name="强调文字颜色 3 15" xfId="666" xr:uid="{00000000-0005-0000-0000-00009A020000}"/>
-    <cellStyle name="强调文字颜色 3 16" xfId="667" xr:uid="{00000000-0005-0000-0000-00009B020000}"/>
-    <cellStyle name="强调文字颜色 3 17" xfId="668" xr:uid="{00000000-0005-0000-0000-00009C020000}"/>
-    <cellStyle name="强调文字颜色 3 18" xfId="669" xr:uid="{00000000-0005-0000-0000-00009D020000}"/>
-    <cellStyle name="强调文字颜色 3 19" xfId="670" xr:uid="{00000000-0005-0000-0000-00009E020000}"/>
-    <cellStyle name="强调文字颜色 3 2" xfId="671" xr:uid="{00000000-0005-0000-0000-00009F020000}"/>
-    <cellStyle name="强调文字颜色 3 20" xfId="672" xr:uid="{00000000-0005-0000-0000-0000A0020000}"/>
-    <cellStyle name="强调文字颜色 3 3" xfId="673" xr:uid="{00000000-0005-0000-0000-0000A1020000}"/>
-    <cellStyle name="强调文字颜色 3 4" xfId="674" xr:uid="{00000000-0005-0000-0000-0000A2020000}"/>
-    <cellStyle name="强调文字颜色 3 5" xfId="675" xr:uid="{00000000-0005-0000-0000-0000A3020000}"/>
-    <cellStyle name="强调文字颜色 3 6" xfId="676" xr:uid="{00000000-0005-0000-0000-0000A4020000}"/>
-    <cellStyle name="强调文字颜色 3 7" xfId="677" xr:uid="{00000000-0005-0000-0000-0000A5020000}"/>
-    <cellStyle name="强调文字颜色 3 8" xfId="678" xr:uid="{00000000-0005-0000-0000-0000A6020000}"/>
-    <cellStyle name="强调文字颜色 3 9" xfId="679" xr:uid="{00000000-0005-0000-0000-0000A7020000}"/>
-    <cellStyle name="强调文字颜色 4 10" xfId="680" xr:uid="{00000000-0005-0000-0000-0000A8020000}"/>
-    <cellStyle name="强调文字颜色 4 11" xfId="681" xr:uid="{00000000-0005-0000-0000-0000A9020000}"/>
-    <cellStyle name="强调文字颜色 4 12" xfId="682" xr:uid="{00000000-0005-0000-0000-0000AA020000}"/>
-    <cellStyle name="强调文字颜色 4 13" xfId="683" xr:uid="{00000000-0005-0000-0000-0000AB020000}"/>
-    <cellStyle name="强调文字颜色 4 14" xfId="684" xr:uid="{00000000-0005-0000-0000-0000AC020000}"/>
-    <cellStyle name="强调文字颜色 4 15" xfId="685" xr:uid="{00000000-0005-0000-0000-0000AD020000}"/>
-    <cellStyle name="强调文字颜色 4 16" xfId="686" xr:uid="{00000000-0005-0000-0000-0000AE020000}"/>
-    <cellStyle name="强调文字颜色 4 17" xfId="687" xr:uid="{00000000-0005-0000-0000-0000AF020000}"/>
-    <cellStyle name="强调文字颜色 4 18" xfId="688" xr:uid="{00000000-0005-0000-0000-0000B0020000}"/>
-    <cellStyle name="强调文字颜色 4 19" xfId="689" xr:uid="{00000000-0005-0000-0000-0000B1020000}"/>
-    <cellStyle name="强调文字颜色 4 2" xfId="690" xr:uid="{00000000-0005-0000-0000-0000B2020000}"/>
-    <cellStyle name="强调文字颜色 4 20" xfId="691" xr:uid="{00000000-0005-0000-0000-0000B3020000}"/>
-    <cellStyle name="强调文字颜色 4 3" xfId="692" xr:uid="{00000000-0005-0000-0000-0000B4020000}"/>
-    <cellStyle name="强调文字颜色 4 4" xfId="693" xr:uid="{00000000-0005-0000-0000-0000B5020000}"/>
-    <cellStyle name="强调文字颜色 4 5" xfId="694" xr:uid="{00000000-0005-0000-0000-0000B6020000}"/>
-    <cellStyle name="强调文字颜色 4 6" xfId="695" xr:uid="{00000000-0005-0000-0000-0000B7020000}"/>
-    <cellStyle name="强调文字颜色 4 7" xfId="696" xr:uid="{00000000-0005-0000-0000-0000B8020000}"/>
-    <cellStyle name="强调文字颜色 4 8" xfId="697" xr:uid="{00000000-0005-0000-0000-0000B9020000}"/>
-    <cellStyle name="强调文字颜色 4 9" xfId="698" xr:uid="{00000000-0005-0000-0000-0000BA020000}"/>
-    <cellStyle name="强调文字颜色 5 10" xfId="699" xr:uid="{00000000-0005-0000-0000-0000BB020000}"/>
-    <cellStyle name="强调文字颜色 5 11" xfId="700" xr:uid="{00000000-0005-0000-0000-0000BC020000}"/>
-    <cellStyle name="强调文字颜色 5 12" xfId="701" xr:uid="{00000000-0005-0000-0000-0000BD020000}"/>
-    <cellStyle name="强调文字颜色 5 13" xfId="702" xr:uid="{00000000-0005-0000-0000-0000BE020000}"/>
-    <cellStyle name="强调文字颜色 5 14" xfId="703" xr:uid="{00000000-0005-0000-0000-0000BF020000}"/>
-    <cellStyle name="强调文字颜色 5 15" xfId="704" xr:uid="{00000000-0005-0000-0000-0000C0020000}"/>
-    <cellStyle name="强调文字颜色 5 16" xfId="705" xr:uid="{00000000-0005-0000-0000-0000C1020000}"/>
-    <cellStyle name="强调文字颜色 5 17" xfId="706" xr:uid="{00000000-0005-0000-0000-0000C2020000}"/>
-    <cellStyle name="强调文字颜色 5 18" xfId="707" xr:uid="{00000000-0005-0000-0000-0000C3020000}"/>
-    <cellStyle name="强调文字颜色 5 19" xfId="708" xr:uid="{00000000-0005-0000-0000-0000C4020000}"/>
-    <cellStyle name="强调文字颜色 5 2" xfId="709" xr:uid="{00000000-0005-0000-0000-0000C5020000}"/>
-    <cellStyle name="强调文字颜色 5 20" xfId="710" xr:uid="{00000000-0005-0000-0000-0000C6020000}"/>
-    <cellStyle name="强调文字颜色 5 3" xfId="711" xr:uid="{00000000-0005-0000-0000-0000C7020000}"/>
-    <cellStyle name="强调文字颜色 5 4" xfId="712" xr:uid="{00000000-0005-0000-0000-0000C8020000}"/>
-    <cellStyle name="强调文字颜色 5 5" xfId="713" xr:uid="{00000000-0005-0000-0000-0000C9020000}"/>
-    <cellStyle name="强调文字颜色 5 6" xfId="714" xr:uid="{00000000-0005-0000-0000-0000CA020000}"/>
-    <cellStyle name="强调文字颜色 5 7" xfId="715" xr:uid="{00000000-0005-0000-0000-0000CB020000}"/>
-    <cellStyle name="强调文字颜色 5 8" xfId="716" xr:uid="{00000000-0005-0000-0000-0000CC020000}"/>
-    <cellStyle name="强调文字颜色 5 9" xfId="717" xr:uid="{00000000-0005-0000-0000-0000CD020000}"/>
-    <cellStyle name="强调文字颜色 6 10" xfId="718" xr:uid="{00000000-0005-0000-0000-0000CE020000}"/>
-    <cellStyle name="强调文字颜色 6 11" xfId="719" xr:uid="{00000000-0005-0000-0000-0000CF020000}"/>
-    <cellStyle name="强调文字颜色 6 12" xfId="720" xr:uid="{00000000-0005-0000-0000-0000D0020000}"/>
-    <cellStyle name="强调文字颜色 6 13" xfId="721" xr:uid="{00000000-0005-0000-0000-0000D1020000}"/>
-    <cellStyle name="强调文字颜色 6 14" xfId="722" xr:uid="{00000000-0005-0000-0000-0000D2020000}"/>
-    <cellStyle name="强调文字颜色 6 15" xfId="723" xr:uid="{00000000-0005-0000-0000-0000D3020000}"/>
-    <cellStyle name="强调文字颜色 6 16" xfId="724" xr:uid="{00000000-0005-0000-0000-0000D4020000}"/>
-    <cellStyle name="强调文字颜色 6 17" xfId="725" xr:uid="{00000000-0005-0000-0000-0000D5020000}"/>
-    <cellStyle name="强调文字颜色 6 18" xfId="726" xr:uid="{00000000-0005-0000-0000-0000D6020000}"/>
-    <cellStyle name="强调文字颜色 6 19" xfId="727" xr:uid="{00000000-0005-0000-0000-0000D7020000}"/>
-    <cellStyle name="强调文字颜色 6 2" xfId="728" xr:uid="{00000000-0005-0000-0000-0000D8020000}"/>
-    <cellStyle name="强调文字颜色 6 20" xfId="729" xr:uid="{00000000-0005-0000-0000-0000D9020000}"/>
-    <cellStyle name="强调文字颜色 6 3" xfId="730" xr:uid="{00000000-0005-0000-0000-0000DA020000}"/>
-    <cellStyle name="强调文字颜色 6 4" xfId="731" xr:uid="{00000000-0005-0000-0000-0000DB020000}"/>
-    <cellStyle name="强调文字颜色 6 5" xfId="732" xr:uid="{00000000-0005-0000-0000-0000DC020000}"/>
-    <cellStyle name="强调文字颜色 6 6" xfId="733" xr:uid="{00000000-0005-0000-0000-0000DD020000}"/>
-    <cellStyle name="强调文字颜色 6 7" xfId="734" xr:uid="{00000000-0005-0000-0000-0000DE020000}"/>
-    <cellStyle name="强调文字颜色 6 8" xfId="735" xr:uid="{00000000-0005-0000-0000-0000DF020000}"/>
-    <cellStyle name="强调文字颜色 6 9" xfId="736" xr:uid="{00000000-0005-0000-0000-0000E0020000}"/>
+    <cellStyle name="链接单元格 10" xfId="604"/>
+    <cellStyle name="链接单元格 11" xfId="605"/>
+    <cellStyle name="链接单元格 12" xfId="606"/>
+    <cellStyle name="链接单元格 13" xfId="607"/>
+    <cellStyle name="链接单元格 14" xfId="608"/>
+    <cellStyle name="链接单元格 15" xfId="609"/>
+    <cellStyle name="链接单元格 16" xfId="610"/>
+    <cellStyle name="链接单元格 17" xfId="611"/>
+    <cellStyle name="链接单元格 18" xfId="612"/>
+    <cellStyle name="链接单元格 19" xfId="613"/>
+    <cellStyle name="链接单元格 2" xfId="614"/>
+    <cellStyle name="链接单元格 20" xfId="615"/>
+    <cellStyle name="链接单元格 3" xfId="616"/>
+    <cellStyle name="链接单元格 4" xfId="617"/>
+    <cellStyle name="链接单元格 5" xfId="618"/>
+    <cellStyle name="链接单元格 6" xfId="619"/>
+    <cellStyle name="链接单元格 7" xfId="620"/>
+    <cellStyle name="链接单元格 8" xfId="621"/>
+    <cellStyle name="链接单元格 9" xfId="622"/>
+    <cellStyle name="强调文字颜色 1 10" xfId="623"/>
+    <cellStyle name="强调文字颜色 1 11" xfId="624"/>
+    <cellStyle name="强调文字颜色 1 12" xfId="625"/>
+    <cellStyle name="强调文字颜色 1 13" xfId="626"/>
+    <cellStyle name="强调文字颜色 1 14" xfId="627"/>
+    <cellStyle name="强调文字颜色 1 15" xfId="628"/>
+    <cellStyle name="强调文字颜色 1 16" xfId="629"/>
+    <cellStyle name="强调文字颜色 1 17" xfId="630"/>
+    <cellStyle name="强调文字颜色 1 18" xfId="631"/>
+    <cellStyle name="强调文字颜色 1 19" xfId="632"/>
+    <cellStyle name="强调文字颜色 1 2" xfId="633"/>
+    <cellStyle name="强调文字颜色 1 20" xfId="634"/>
+    <cellStyle name="强调文字颜色 1 3" xfId="635"/>
+    <cellStyle name="强调文字颜色 1 4" xfId="636"/>
+    <cellStyle name="强调文字颜色 1 5" xfId="637"/>
+    <cellStyle name="强调文字颜色 1 6" xfId="638"/>
+    <cellStyle name="强调文字颜色 1 7" xfId="639"/>
+    <cellStyle name="强调文字颜色 1 8" xfId="640"/>
+    <cellStyle name="强调文字颜色 1 9" xfId="641"/>
+    <cellStyle name="强调文字颜色 2 10" xfId="642"/>
+    <cellStyle name="强调文字颜色 2 11" xfId="643"/>
+    <cellStyle name="强调文字颜色 2 12" xfId="644"/>
+    <cellStyle name="强调文字颜色 2 13" xfId="645"/>
+    <cellStyle name="强调文字颜色 2 14" xfId="646"/>
+    <cellStyle name="强调文字颜色 2 15" xfId="647"/>
+    <cellStyle name="强调文字颜色 2 16" xfId="648"/>
+    <cellStyle name="强调文字颜色 2 17" xfId="649"/>
+    <cellStyle name="强调文字颜色 2 18" xfId="650"/>
+    <cellStyle name="强调文字颜色 2 19" xfId="651"/>
+    <cellStyle name="强调文字颜色 2 2" xfId="652"/>
+    <cellStyle name="强调文字颜色 2 20" xfId="653"/>
+    <cellStyle name="强调文字颜色 2 3" xfId="654"/>
+    <cellStyle name="强调文字颜色 2 4" xfId="655"/>
+    <cellStyle name="强调文字颜色 2 5" xfId="656"/>
+    <cellStyle name="强调文字颜色 2 6" xfId="657"/>
+    <cellStyle name="强调文字颜色 2 7" xfId="658"/>
+    <cellStyle name="强调文字颜色 2 8" xfId="659"/>
+    <cellStyle name="强调文字颜色 2 9" xfId="660"/>
+    <cellStyle name="强调文字颜色 3 10" xfId="661"/>
+    <cellStyle name="强调文字颜色 3 11" xfId="662"/>
+    <cellStyle name="强调文字颜色 3 12" xfId="663"/>
+    <cellStyle name="强调文字颜色 3 13" xfId="664"/>
+    <cellStyle name="强调文字颜色 3 14" xfId="665"/>
+    <cellStyle name="强调文字颜色 3 15" xfId="666"/>
+    <cellStyle name="强调文字颜色 3 16" xfId="667"/>
+    <cellStyle name="强调文字颜色 3 17" xfId="668"/>
+    <cellStyle name="强调文字颜色 3 18" xfId="669"/>
+    <cellStyle name="强调文字颜色 3 19" xfId="670"/>
+    <cellStyle name="强调文字颜色 3 2" xfId="671"/>
+    <cellStyle name="强调文字颜色 3 20" xfId="672"/>
+    <cellStyle name="强调文字颜色 3 3" xfId="673"/>
+    <cellStyle name="强调文字颜色 3 4" xfId="674"/>
+    <cellStyle name="强调文字颜色 3 5" xfId="675"/>
+    <cellStyle name="强调文字颜色 3 6" xfId="676"/>
+    <cellStyle name="强调文字颜色 3 7" xfId="677"/>
+    <cellStyle name="强调文字颜色 3 8" xfId="678"/>
+    <cellStyle name="强调文字颜色 3 9" xfId="679"/>
+    <cellStyle name="强调文字颜色 4 10" xfId="680"/>
+    <cellStyle name="强调文字颜色 4 11" xfId="681"/>
+    <cellStyle name="强调文字颜色 4 12" xfId="682"/>
+    <cellStyle name="强调文字颜色 4 13" xfId="683"/>
+    <cellStyle name="强调文字颜色 4 14" xfId="684"/>
+    <cellStyle name="强调文字颜色 4 15" xfId="685"/>
+    <cellStyle name="强调文字颜色 4 16" xfId="686"/>
+    <cellStyle name="强调文字颜色 4 17" xfId="687"/>
+    <cellStyle name="强调文字颜色 4 18" xfId="688"/>
+    <cellStyle name="强调文字颜色 4 19" xfId="689"/>
+    <cellStyle name="强调文字颜色 4 2" xfId="690"/>
+    <cellStyle name="强调文字颜色 4 20" xfId="691"/>
+    <cellStyle name="强调文字颜色 4 3" xfId="692"/>
+    <cellStyle name="强调文字颜色 4 4" xfId="693"/>
+    <cellStyle name="强调文字颜色 4 5" xfId="694"/>
+    <cellStyle name="强调文字颜色 4 6" xfId="695"/>
+    <cellStyle name="强调文字颜色 4 7" xfId="696"/>
+    <cellStyle name="强调文字颜色 4 8" xfId="697"/>
+    <cellStyle name="强调文字颜色 4 9" xfId="698"/>
+    <cellStyle name="强调文字颜色 5 10" xfId="699"/>
+    <cellStyle name="强调文字颜色 5 11" xfId="700"/>
+    <cellStyle name="强调文字颜色 5 12" xfId="701"/>
+    <cellStyle name="强调文字颜色 5 13" xfId="702"/>
+    <cellStyle name="强调文字颜色 5 14" xfId="703"/>
+    <cellStyle name="强调文字颜色 5 15" xfId="704"/>
+    <cellStyle name="强调文字颜色 5 16" xfId="705"/>
+    <cellStyle name="强调文字颜色 5 17" xfId="706"/>
+    <cellStyle name="强调文字颜色 5 18" xfId="707"/>
+    <cellStyle name="强调文字颜色 5 19" xfId="708"/>
+    <cellStyle name="强调文字颜色 5 2" xfId="709"/>
+    <cellStyle name="强调文字颜色 5 20" xfId="710"/>
+    <cellStyle name="强调文字颜色 5 3" xfId="711"/>
+    <cellStyle name="强调文字颜色 5 4" xfId="712"/>
+    <cellStyle name="强调文字颜色 5 5" xfId="713"/>
+    <cellStyle name="强调文字颜色 5 6" xfId="714"/>
+    <cellStyle name="强调文字颜色 5 7" xfId="715"/>
+    <cellStyle name="强调文字颜色 5 8" xfId="716"/>
+    <cellStyle name="强调文字颜色 5 9" xfId="717"/>
+    <cellStyle name="强调文字颜色 6 10" xfId="718"/>
+    <cellStyle name="强调文字颜色 6 11" xfId="719"/>
+    <cellStyle name="强调文字颜色 6 12" xfId="720"/>
+    <cellStyle name="强调文字颜色 6 13" xfId="721"/>
+    <cellStyle name="强调文字颜色 6 14" xfId="722"/>
+    <cellStyle name="强调文字颜色 6 15" xfId="723"/>
+    <cellStyle name="强调文字颜色 6 16" xfId="724"/>
+    <cellStyle name="强调文字颜色 6 17" xfId="725"/>
+    <cellStyle name="强调文字颜色 6 18" xfId="726"/>
+    <cellStyle name="强调文字颜色 6 19" xfId="727"/>
+    <cellStyle name="强调文字颜色 6 2" xfId="728"/>
+    <cellStyle name="强调文字颜色 6 20" xfId="729"/>
+    <cellStyle name="强调文字颜色 6 3" xfId="730"/>
+    <cellStyle name="强调文字颜色 6 4" xfId="731"/>
+    <cellStyle name="强调文字颜色 6 5" xfId="732"/>
+    <cellStyle name="强调文字颜色 6 6" xfId="733"/>
+    <cellStyle name="强调文字颜色 6 7" xfId="734"/>
+    <cellStyle name="强调文字颜色 6 8" xfId="735"/>
+    <cellStyle name="强调文字颜色 6 9" xfId="736"/>
     <cellStyle name="适中" xfId="737" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="适中 10" xfId="738" xr:uid="{00000000-0005-0000-0000-0000E2020000}"/>
-    <cellStyle name="适中 11" xfId="739" xr:uid="{00000000-0005-0000-0000-0000E3020000}"/>
-    <cellStyle name="适中 12" xfId="740" xr:uid="{00000000-0005-0000-0000-0000E4020000}"/>
-    <cellStyle name="适中 13" xfId="741" xr:uid="{00000000-0005-0000-0000-0000E5020000}"/>
-    <cellStyle name="适中 14" xfId="742" xr:uid="{00000000-0005-0000-0000-0000E6020000}"/>
-    <cellStyle name="适中 15" xfId="743" xr:uid="{00000000-0005-0000-0000-0000E7020000}"/>
-    <cellStyle name="适中 16" xfId="744" xr:uid="{00000000-0005-0000-0000-0000E8020000}"/>
-    <cellStyle name="适中 17" xfId="745" xr:uid="{00000000-0005-0000-0000-0000E9020000}"/>
-    <cellStyle name="适中 18" xfId="746" xr:uid="{00000000-0005-0000-0000-0000EA020000}"/>
-    <cellStyle name="适中 19" xfId="747" xr:uid="{00000000-0005-0000-0000-0000EB020000}"/>
-    <cellStyle name="适中 2" xfId="748" xr:uid="{00000000-0005-0000-0000-0000EC020000}"/>
-    <cellStyle name="适中 20" xfId="749" xr:uid="{00000000-0005-0000-0000-0000ED020000}"/>
-    <cellStyle name="适中 3" xfId="750" xr:uid="{00000000-0005-0000-0000-0000EE020000}"/>
-    <cellStyle name="适中 4" xfId="751" xr:uid="{00000000-0005-0000-0000-0000EF020000}"/>
-    <cellStyle name="适中 5" xfId="752" xr:uid="{00000000-0005-0000-0000-0000F0020000}"/>
-    <cellStyle name="适中 6" xfId="753" xr:uid="{00000000-0005-0000-0000-0000F1020000}"/>
-    <cellStyle name="适中 7" xfId="754" xr:uid="{00000000-0005-0000-0000-0000F2020000}"/>
-    <cellStyle name="适中 8" xfId="755" xr:uid="{00000000-0005-0000-0000-0000F3020000}"/>
-    <cellStyle name="适中 9" xfId="756" xr:uid="{00000000-0005-0000-0000-0000F4020000}"/>
+    <cellStyle name="适中 10" xfId="738"/>
+    <cellStyle name="适中 11" xfId="739"/>
+    <cellStyle name="适中 12" xfId="740"/>
+    <cellStyle name="适中 13" xfId="741"/>
+    <cellStyle name="适中 14" xfId="742"/>
+    <cellStyle name="适中 15" xfId="743"/>
+    <cellStyle name="适中 16" xfId="744"/>
+    <cellStyle name="适中 17" xfId="745"/>
+    <cellStyle name="适中 18" xfId="746"/>
+    <cellStyle name="适中 19" xfId="747"/>
+    <cellStyle name="适中 2" xfId="748"/>
+    <cellStyle name="适中 20" xfId="749"/>
+    <cellStyle name="适中 3" xfId="750"/>
+    <cellStyle name="适中 4" xfId="751"/>
+    <cellStyle name="适中 5" xfId="752"/>
+    <cellStyle name="适中 6" xfId="753"/>
+    <cellStyle name="适中 7" xfId="754"/>
+    <cellStyle name="适中 8" xfId="755"/>
+    <cellStyle name="适中 9" xfId="756"/>
     <cellStyle name="输出" xfId="757" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="输出 10" xfId="758" xr:uid="{00000000-0005-0000-0000-0000F6020000}"/>
-    <cellStyle name="输出 11" xfId="759" xr:uid="{00000000-0005-0000-0000-0000F7020000}"/>
-    <cellStyle name="输出 12" xfId="760" xr:uid="{00000000-0005-0000-0000-0000F8020000}"/>
-    <cellStyle name="输出 13" xfId="761" xr:uid="{00000000-0005-0000-0000-0000F9020000}"/>
-    <cellStyle name="输出 14" xfId="762" xr:uid="{00000000-0005-0000-0000-0000FA020000}"/>
-    <cellStyle name="输出 15" xfId="763" xr:uid="{00000000-0005-0000-0000-0000FB020000}"/>
-    <cellStyle name="输出 16" xfId="764" xr:uid="{00000000-0005-0000-0000-0000FC020000}"/>
-    <cellStyle name="输出 17" xfId="765" xr:uid="{00000000-0005-0000-0000-0000FD020000}"/>
-    <cellStyle name="输出 18" xfId="766" xr:uid="{00000000-0005-0000-0000-0000FE020000}"/>
-    <cellStyle name="输出 19" xfId="767" xr:uid="{00000000-0005-0000-0000-0000FF020000}"/>
-    <cellStyle name="输出 2" xfId="768" xr:uid="{00000000-0005-0000-0000-000000030000}"/>
-    <cellStyle name="输出 20" xfId="769" xr:uid="{00000000-0005-0000-0000-000001030000}"/>
-    <cellStyle name="输出 3" xfId="770" xr:uid="{00000000-0005-0000-0000-000002030000}"/>
-    <cellStyle name="输出 4" xfId="771" xr:uid="{00000000-0005-0000-0000-000003030000}"/>
-    <cellStyle name="输出 5" xfId="772" xr:uid="{00000000-0005-0000-0000-000004030000}"/>
-    <cellStyle name="输出 6" xfId="773" xr:uid="{00000000-0005-0000-0000-000005030000}"/>
-    <cellStyle name="输出 7" xfId="774" xr:uid="{00000000-0005-0000-0000-000006030000}"/>
-    <cellStyle name="输出 8" xfId="775" xr:uid="{00000000-0005-0000-0000-000007030000}"/>
-    <cellStyle name="输出 9" xfId="776" xr:uid="{00000000-0005-0000-0000-000008030000}"/>
+    <cellStyle name="输出 10" xfId="758"/>
+    <cellStyle name="输出 11" xfId="759"/>
+    <cellStyle name="输出 12" xfId="760"/>
+    <cellStyle name="输出 13" xfId="761"/>
+    <cellStyle name="输出 14" xfId="762"/>
+    <cellStyle name="输出 15" xfId="763"/>
+    <cellStyle name="输出 16" xfId="764"/>
+    <cellStyle name="输出 17" xfId="765"/>
+    <cellStyle name="输出 18" xfId="766"/>
+    <cellStyle name="输出 19" xfId="767"/>
+    <cellStyle name="输出 2" xfId="768"/>
+    <cellStyle name="输出 20" xfId="769"/>
+    <cellStyle name="输出 3" xfId="770"/>
+    <cellStyle name="输出 4" xfId="771"/>
+    <cellStyle name="输出 5" xfId="772"/>
+    <cellStyle name="输出 6" xfId="773"/>
+    <cellStyle name="输出 7" xfId="774"/>
+    <cellStyle name="输出 8" xfId="775"/>
+    <cellStyle name="输出 9" xfId="776"/>
     <cellStyle name="输入" xfId="777" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="输入 10" xfId="778" xr:uid="{00000000-0005-0000-0000-00000A030000}"/>
-    <cellStyle name="输入 11" xfId="779" xr:uid="{00000000-0005-0000-0000-00000B030000}"/>
-    <cellStyle name="输入 12" xfId="780" xr:uid="{00000000-0005-0000-0000-00000C030000}"/>
-    <cellStyle name="输入 13" xfId="781" xr:uid="{00000000-0005-0000-0000-00000D030000}"/>
-    <cellStyle name="输入 14" xfId="782" xr:uid="{00000000-0005-0000-0000-00000E030000}"/>
-    <cellStyle name="输入 15" xfId="783" xr:uid="{00000000-0005-0000-0000-00000F030000}"/>
-    <cellStyle name="输入 16" xfId="784" xr:uid="{00000000-0005-0000-0000-000010030000}"/>
-    <cellStyle name="输入 17" xfId="785" xr:uid="{00000000-0005-0000-0000-000011030000}"/>
-    <cellStyle name="输入 18" xfId="786" xr:uid="{00000000-0005-0000-0000-000012030000}"/>
-    <cellStyle name="输入 19" xfId="787" xr:uid="{00000000-0005-0000-0000-000013030000}"/>
-    <cellStyle name="输入 2" xfId="788" xr:uid="{00000000-0005-0000-0000-000014030000}"/>
-    <cellStyle name="输入 20" xfId="789" xr:uid="{00000000-0005-0000-0000-000015030000}"/>
-    <cellStyle name="输入 3" xfId="790" xr:uid="{00000000-0005-0000-0000-000016030000}"/>
-    <cellStyle name="输入 4" xfId="791" xr:uid="{00000000-0005-0000-0000-000017030000}"/>
-    <cellStyle name="输入 5" xfId="792" xr:uid="{00000000-0005-0000-0000-000018030000}"/>
-    <cellStyle name="输入 6" xfId="793" xr:uid="{00000000-0005-0000-0000-000019030000}"/>
-    <cellStyle name="输入 7" xfId="794" xr:uid="{00000000-0005-0000-0000-00001A030000}"/>
-    <cellStyle name="输入 8" xfId="795" xr:uid="{00000000-0005-0000-0000-00001B030000}"/>
-    <cellStyle name="输入 9" xfId="796" xr:uid="{00000000-0005-0000-0000-00001C030000}"/>
+    <cellStyle name="输入 10" xfId="778"/>
+    <cellStyle name="输入 11" xfId="779"/>
+    <cellStyle name="输入 12" xfId="780"/>
+    <cellStyle name="输入 13" xfId="781"/>
+    <cellStyle name="输入 14" xfId="782"/>
+    <cellStyle name="输入 15" xfId="783"/>
+    <cellStyle name="输入 16" xfId="784"/>
+    <cellStyle name="输入 17" xfId="785"/>
+    <cellStyle name="输入 18" xfId="786"/>
+    <cellStyle name="输入 19" xfId="787"/>
+    <cellStyle name="输入 2" xfId="788"/>
+    <cellStyle name="输入 20" xfId="789"/>
+    <cellStyle name="输入 3" xfId="790"/>
+    <cellStyle name="输入 4" xfId="791"/>
+    <cellStyle name="输入 5" xfId="792"/>
+    <cellStyle name="输入 6" xfId="793"/>
+    <cellStyle name="输入 7" xfId="794"/>
+    <cellStyle name="输入 8" xfId="795"/>
+    <cellStyle name="输入 9" xfId="796"/>
     <cellStyle name="注释" xfId="797" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="注释 10" xfId="798" xr:uid="{00000000-0005-0000-0000-00001E030000}"/>
-    <cellStyle name="注释 11" xfId="799" xr:uid="{00000000-0005-0000-0000-00001F030000}"/>
-    <cellStyle name="注释 12" xfId="800" xr:uid="{00000000-0005-0000-0000-000020030000}"/>
-    <cellStyle name="注释 13" xfId="801" xr:uid="{00000000-0005-0000-0000-000021030000}"/>
-    <cellStyle name="注释 14" xfId="802" xr:uid="{00000000-0005-0000-0000-000022030000}"/>
-    <cellStyle name="注释 15" xfId="803" xr:uid="{00000000-0005-0000-0000-000023030000}"/>
-    <cellStyle name="注释 16" xfId="804" xr:uid="{00000000-0005-0000-0000-000024030000}"/>
-    <cellStyle name="注释 17" xfId="805" xr:uid="{00000000-0005-0000-0000-000025030000}"/>
-    <cellStyle name="注释 18" xfId="806" xr:uid="{00000000-0005-0000-0000-000026030000}"/>
-    <cellStyle name="注释 19" xfId="807" xr:uid="{00000000-0005-0000-0000-000027030000}"/>
-    <cellStyle name="注释 2" xfId="808" xr:uid="{00000000-0005-0000-0000-000028030000}"/>
-    <cellStyle name="注释 20" xfId="809" xr:uid="{00000000-0005-0000-0000-000029030000}"/>
-    <cellStyle name="注释 3" xfId="810" xr:uid="{00000000-0005-0000-0000-00002A030000}"/>
-    <cellStyle name="注释 4" xfId="811" xr:uid="{00000000-0005-0000-0000-00002B030000}"/>
-    <cellStyle name="注释 5" xfId="812" xr:uid="{00000000-0005-0000-0000-00002C030000}"/>
-    <cellStyle name="注释 6" xfId="813" xr:uid="{00000000-0005-0000-0000-00002D030000}"/>
-    <cellStyle name="注释 7" xfId="814" xr:uid="{00000000-0005-0000-0000-00002E030000}"/>
-    <cellStyle name="注释 8" xfId="815" xr:uid="{00000000-0005-0000-0000-00002F030000}"/>
-    <cellStyle name="注释 9" xfId="816" xr:uid="{00000000-0005-0000-0000-000030030000}"/>
+    <cellStyle name="注释 10" xfId="798"/>
+    <cellStyle name="注释 11" xfId="799"/>
+    <cellStyle name="注释 12" xfId="800"/>
+    <cellStyle name="注释 13" xfId="801"/>
+    <cellStyle name="注释 14" xfId="802"/>
+    <cellStyle name="注释 15" xfId="803"/>
+    <cellStyle name="注释 16" xfId="804"/>
+    <cellStyle name="注释 17" xfId="805"/>
+    <cellStyle name="注释 18" xfId="806"/>
+    <cellStyle name="注释 19" xfId="807"/>
+    <cellStyle name="注释 2" xfId="808"/>
+    <cellStyle name="注释 20" xfId="809"/>
+    <cellStyle name="注释 3" xfId="810"/>
+    <cellStyle name="注释 4" xfId="811"/>
+    <cellStyle name="注释 5" xfId="812"/>
+    <cellStyle name="注释 6" xfId="813"/>
+    <cellStyle name="注释 7" xfId="814"/>
+    <cellStyle name="注释 8" xfId="815"/>
+    <cellStyle name="注释 9" xfId="816"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -4025,7 +4028,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4100,23 +4103,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4152,23 +4138,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4344,11 +4313,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4367,7 +4336,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="81" x14ac:dyDescent="0.15">
@@ -4379,28 +4348,28 @@
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>57</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="J2" s="9" t="s">
-        <v>61</v>
-      </c>
       <c r="K2" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.15">
@@ -4451,8 +4420,8 @@
       <c r="E4">
         <v>10</v>
       </c>
-      <c r="F4">
-        <v>999</v>
+      <c r="F4" s="10" t="s">
+        <v>66</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>19</v>
@@ -5389,7 +5358,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5403,7 +5372,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
add new type (color & date time )
</commit_message>
<xml_diff>
--- a/example/config/BasicItem_Common.xlsx
+++ b/example/config/BasicItem_Common.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\porject\GoConfigTool\src\github.com\Blizzardx\ConfigProtocol\example\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\Go\configTool-src\src\github.com\Blizzardx\ConfigProtocol\example\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1C91DC-4233-4C16-9FE1-5C7787CE5434}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="-225" windowWidth="19440" windowHeight="13740"/>
+    <workbookView xWindow="5280" yWindow="-225" windowWidth="19440" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="125">
   <si>
     <t>道具图标：直接调用美术资源图名</t>
   </si>
@@ -304,11 +305,195 @@
     <t>999|2054|1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
+  <si>
+    <t>2018-08-13 00:00:00</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:01</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:02</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:03</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:04</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:05</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:06</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:07</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:08</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:09</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:10</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:11</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:12</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:13</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:14</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:15</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:16</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:17</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:18</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:19</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:20</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:21</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:22</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:23</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:24</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:25</t>
+  </si>
+  <si>
+    <t>2018-08-13 00:00:26</t>
+  </si>
+  <si>
+    <t>{"type":"time",
+"name":"showTime",
+"min": "2018-08-13 00:00:00","max": "2018-08-13 00:00:30"}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"type":"time",
+"name":"endTime"}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"type":"color",
+"name":"textColor"}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>#00ff00</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>#00ff01</t>
+  </si>
+  <si>
+    <t>#00ff02</t>
+  </si>
+  <si>
+    <t>#00ff03</t>
+  </si>
+  <si>
+    <t>#00ff04</t>
+  </si>
+  <si>
+    <t>#00ff05</t>
+  </si>
+  <si>
+    <t>#00ff06</t>
+  </si>
+  <si>
+    <t>#00ff07</t>
+  </si>
+  <si>
+    <t>#00ff08</t>
+  </si>
+  <si>
+    <t>#00ff09</t>
+  </si>
+  <si>
+    <t>#00ff10</t>
+  </si>
+  <si>
+    <t>#00ff11</t>
+  </si>
+  <si>
+    <t>#00ff12</t>
+  </si>
+  <si>
+    <t>#00ff13</t>
+  </si>
+  <si>
+    <t>#00ff14</t>
+  </si>
+  <si>
+    <t>#00ff15</t>
+  </si>
+  <si>
+    <t>#00ff16</t>
+  </si>
+  <si>
+    <t>#00ff17</t>
+  </si>
+  <si>
+    <t>#00ff18</t>
+  </si>
+  <si>
+    <t>#00ff19</t>
+  </si>
+  <si>
+    <t>#00ff20</t>
+  </si>
+  <si>
+    <t>#00ff21</t>
+  </si>
+  <si>
+    <t>#00ff22</t>
+  </si>
+  <si>
+    <t>#00ff23</t>
+  </si>
+  <si>
+    <t>#00ff24</t>
+  </si>
+  <si>
+    <t>#00ff25</t>
+  </si>
+  <si>
+    <t>#00ff26</t>
+  </si>
+  <si>
+    <t>12</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3160,7 +3345,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3194,825 +3379,828 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="817">
-    <cellStyle name="20% - 强调文字颜色 1 10" xfId="1"/>
-    <cellStyle name="20% - 强调文字颜色 1 11" xfId="2"/>
-    <cellStyle name="20% - 强调文字颜色 1 12" xfId="3"/>
-    <cellStyle name="20% - 强调文字颜色 1 13" xfId="4"/>
-    <cellStyle name="20% - 强调文字颜色 1 14" xfId="5"/>
-    <cellStyle name="20% - 强调文字颜色 1 15" xfId="6"/>
-    <cellStyle name="20% - 强调文字颜色 1 16" xfId="7"/>
-    <cellStyle name="20% - 强调文字颜色 1 17" xfId="8"/>
-    <cellStyle name="20% - 强调文字颜色 1 18" xfId="9"/>
-    <cellStyle name="20% - 强调文字颜色 1 19" xfId="10"/>
-    <cellStyle name="20% - 强调文字颜色 1 2" xfId="11"/>
-    <cellStyle name="20% - 强调文字颜色 1 20" xfId="12"/>
-    <cellStyle name="20% - 强调文字颜色 1 3" xfId="13"/>
-    <cellStyle name="20% - 强调文字颜色 1 4" xfId="14"/>
-    <cellStyle name="20% - 强调文字颜色 1 5" xfId="15"/>
-    <cellStyle name="20% - 强调文字颜色 1 6" xfId="16"/>
-    <cellStyle name="20% - 强调文字颜色 1 7" xfId="17"/>
-    <cellStyle name="20% - 强调文字颜色 1 8" xfId="18"/>
-    <cellStyle name="20% - 强调文字颜色 1 9" xfId="19"/>
-    <cellStyle name="20% - 强调文字颜色 2 10" xfId="20"/>
-    <cellStyle name="20% - 强调文字颜色 2 11" xfId="21"/>
-    <cellStyle name="20% - 强调文字颜色 2 12" xfId="22"/>
-    <cellStyle name="20% - 强调文字颜色 2 13" xfId="23"/>
-    <cellStyle name="20% - 强调文字颜色 2 14" xfId="24"/>
-    <cellStyle name="20% - 强调文字颜色 2 15" xfId="25"/>
-    <cellStyle name="20% - 强调文字颜色 2 16" xfId="26"/>
-    <cellStyle name="20% - 强调文字颜色 2 17" xfId="27"/>
-    <cellStyle name="20% - 强调文字颜色 2 18" xfId="28"/>
-    <cellStyle name="20% - 强调文字颜色 2 19" xfId="29"/>
-    <cellStyle name="20% - 强调文字颜色 2 2" xfId="30"/>
-    <cellStyle name="20% - 强调文字颜色 2 20" xfId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2 3" xfId="32"/>
-    <cellStyle name="20% - 强调文字颜色 2 4" xfId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2 5" xfId="34"/>
-    <cellStyle name="20% - 强调文字颜色 2 6" xfId="35"/>
-    <cellStyle name="20% - 强调文字颜色 2 7" xfId="36"/>
-    <cellStyle name="20% - 强调文字颜色 2 8" xfId="37"/>
-    <cellStyle name="20% - 强调文字颜色 2 9" xfId="38"/>
-    <cellStyle name="20% - 强调文字颜色 3 10" xfId="39"/>
-    <cellStyle name="20% - 强调文字颜色 3 11" xfId="40"/>
-    <cellStyle name="20% - 强调文字颜色 3 12" xfId="41"/>
-    <cellStyle name="20% - 强调文字颜色 3 13" xfId="42"/>
-    <cellStyle name="20% - 强调文字颜色 3 14" xfId="43"/>
-    <cellStyle name="20% - 强调文字颜色 3 15" xfId="44"/>
-    <cellStyle name="20% - 强调文字颜色 3 16" xfId="45"/>
-    <cellStyle name="20% - 强调文字颜色 3 17" xfId="46"/>
-    <cellStyle name="20% - 强调文字颜色 3 18" xfId="47"/>
-    <cellStyle name="20% - 强调文字颜色 3 19" xfId="48"/>
-    <cellStyle name="20% - 强调文字颜色 3 2" xfId="49"/>
-    <cellStyle name="20% - 强调文字颜色 3 20" xfId="50"/>
-    <cellStyle name="20% - 强调文字颜色 3 3" xfId="51"/>
-    <cellStyle name="20% - 强调文字颜色 3 4" xfId="52"/>
-    <cellStyle name="20% - 强调文字颜色 3 5" xfId="53"/>
-    <cellStyle name="20% - 强调文字颜色 3 6" xfId="54"/>
-    <cellStyle name="20% - 强调文字颜色 3 7" xfId="55"/>
-    <cellStyle name="20% - 强调文字颜色 3 8" xfId="56"/>
-    <cellStyle name="20% - 强调文字颜色 3 9" xfId="57"/>
-    <cellStyle name="20% - 强调文字颜色 4 10" xfId="58"/>
-    <cellStyle name="20% - 强调文字颜色 4 11" xfId="59"/>
-    <cellStyle name="20% - 强调文字颜色 4 12" xfId="60"/>
-    <cellStyle name="20% - 强调文字颜色 4 13" xfId="61"/>
-    <cellStyle name="20% - 强调文字颜色 4 14" xfId="62"/>
-    <cellStyle name="20% - 强调文字颜色 4 15" xfId="63"/>
-    <cellStyle name="20% - 强调文字颜色 4 16" xfId="64"/>
-    <cellStyle name="20% - 强调文字颜色 4 17" xfId="65"/>
-    <cellStyle name="20% - 强调文字颜色 4 18" xfId="66"/>
-    <cellStyle name="20% - 强调文字颜色 4 19" xfId="67"/>
-    <cellStyle name="20% - 强调文字颜色 4 2" xfId="68"/>
-    <cellStyle name="20% - 强调文字颜色 4 20" xfId="69"/>
-    <cellStyle name="20% - 强调文字颜色 4 3" xfId="70"/>
-    <cellStyle name="20% - 强调文字颜色 4 4" xfId="71"/>
-    <cellStyle name="20% - 强调文字颜色 4 5" xfId="72"/>
-    <cellStyle name="20% - 强调文字颜色 4 6" xfId="73"/>
-    <cellStyle name="20% - 强调文字颜色 4 7" xfId="74"/>
-    <cellStyle name="20% - 强调文字颜色 4 8" xfId="75"/>
-    <cellStyle name="20% - 强调文字颜色 4 9" xfId="76"/>
-    <cellStyle name="20% - 强调文字颜色 5 10" xfId="77"/>
-    <cellStyle name="20% - 强调文字颜色 5 11" xfId="78"/>
-    <cellStyle name="20% - 强调文字颜色 5 12" xfId="79"/>
-    <cellStyle name="20% - 强调文字颜色 5 13" xfId="80"/>
-    <cellStyle name="20% - 强调文字颜色 5 14" xfId="81"/>
-    <cellStyle name="20% - 强调文字颜色 5 15" xfId="82"/>
-    <cellStyle name="20% - 强调文字颜色 5 16" xfId="83"/>
-    <cellStyle name="20% - 强调文字颜色 5 17" xfId="84"/>
-    <cellStyle name="20% - 强调文字颜色 5 18" xfId="85"/>
-    <cellStyle name="20% - 强调文字颜色 5 19" xfId="86"/>
-    <cellStyle name="20% - 强调文字颜色 5 2" xfId="87"/>
-    <cellStyle name="20% - 强调文字颜色 5 20" xfId="88"/>
-    <cellStyle name="20% - 强调文字颜色 5 3" xfId="89"/>
-    <cellStyle name="20% - 强调文字颜色 5 4" xfId="90"/>
-    <cellStyle name="20% - 强调文字颜色 5 5" xfId="91"/>
-    <cellStyle name="20% - 强调文字颜色 5 6" xfId="92"/>
-    <cellStyle name="20% - 强调文字颜色 5 7" xfId="93"/>
-    <cellStyle name="20% - 强调文字颜色 5 8" xfId="94"/>
-    <cellStyle name="20% - 强调文字颜色 5 9" xfId="95"/>
-    <cellStyle name="20% - 强调文字颜色 6 10" xfId="96"/>
-    <cellStyle name="20% - 强调文字颜色 6 11" xfId="97"/>
-    <cellStyle name="20% - 强调文字颜色 6 12" xfId="98"/>
-    <cellStyle name="20% - 强调文字颜色 6 13" xfId="99"/>
-    <cellStyle name="20% - 强调文字颜色 6 14" xfId="100"/>
-    <cellStyle name="20% - 强调文字颜色 6 15" xfId="101"/>
-    <cellStyle name="20% - 强调文字颜色 6 16" xfId="102"/>
-    <cellStyle name="20% - 强调文字颜色 6 17" xfId="103"/>
-    <cellStyle name="20% - 强调文字颜色 6 18" xfId="104"/>
-    <cellStyle name="20% - 强调文字颜色 6 19" xfId="105"/>
-    <cellStyle name="20% - 强调文字颜色 6 2" xfId="106"/>
-    <cellStyle name="20% - 强调文字颜色 6 20" xfId="107"/>
-    <cellStyle name="20% - 强调文字颜色 6 3" xfId="108"/>
-    <cellStyle name="20% - 强调文字颜色 6 4" xfId="109"/>
-    <cellStyle name="20% - 强调文字颜色 6 5" xfId="110"/>
-    <cellStyle name="20% - 强调文字颜色 6 6" xfId="111"/>
-    <cellStyle name="20% - 强调文字颜色 6 7" xfId="112"/>
-    <cellStyle name="20% - 强调文字颜色 6 8" xfId="113"/>
-    <cellStyle name="20% - 强调文字颜色 6 9" xfId="114"/>
-    <cellStyle name="40% - 强调文字颜色 1 10" xfId="115"/>
-    <cellStyle name="40% - 强调文字颜色 1 11" xfId="116"/>
-    <cellStyle name="40% - 强调文字颜色 1 12" xfId="117"/>
-    <cellStyle name="40% - 强调文字颜色 1 13" xfId="118"/>
-    <cellStyle name="40% - 强调文字颜色 1 14" xfId="119"/>
-    <cellStyle name="40% - 强调文字颜色 1 15" xfId="120"/>
-    <cellStyle name="40% - 强调文字颜色 1 16" xfId="121"/>
-    <cellStyle name="40% - 强调文字颜色 1 17" xfId="122"/>
-    <cellStyle name="40% - 强调文字颜色 1 18" xfId="123"/>
-    <cellStyle name="40% - 强调文字颜色 1 19" xfId="124"/>
-    <cellStyle name="40% - 强调文字颜色 1 2" xfId="125"/>
-    <cellStyle name="40% - 强调文字颜色 1 20" xfId="126"/>
-    <cellStyle name="40% - 强调文字颜色 1 3" xfId="127"/>
-    <cellStyle name="40% - 强调文字颜色 1 4" xfId="128"/>
-    <cellStyle name="40% - 强调文字颜色 1 5" xfId="129"/>
-    <cellStyle name="40% - 强调文字颜色 1 6" xfId="130"/>
-    <cellStyle name="40% - 强调文字颜色 1 7" xfId="131"/>
-    <cellStyle name="40% - 强调文字颜色 1 8" xfId="132"/>
-    <cellStyle name="40% - 强调文字颜色 1 9" xfId="133"/>
-    <cellStyle name="40% - 强调文字颜色 2 10" xfId="134"/>
-    <cellStyle name="40% - 强调文字颜色 2 11" xfId="135"/>
-    <cellStyle name="40% - 强调文字颜色 2 12" xfId="136"/>
-    <cellStyle name="40% - 强调文字颜色 2 13" xfId="137"/>
-    <cellStyle name="40% - 强调文字颜色 2 14" xfId="138"/>
-    <cellStyle name="40% - 强调文字颜色 2 15" xfId="139"/>
-    <cellStyle name="40% - 强调文字颜色 2 16" xfId="140"/>
-    <cellStyle name="40% - 强调文字颜色 2 17" xfId="141"/>
-    <cellStyle name="40% - 强调文字颜色 2 18" xfId="142"/>
-    <cellStyle name="40% - 强调文字颜色 2 19" xfId="143"/>
-    <cellStyle name="40% - 强调文字颜色 2 2" xfId="144"/>
-    <cellStyle name="40% - 强调文字颜色 2 20" xfId="145"/>
-    <cellStyle name="40% - 强调文字颜色 2 3" xfId="146"/>
-    <cellStyle name="40% - 强调文字颜色 2 4" xfId="147"/>
-    <cellStyle name="40% - 强调文字颜色 2 5" xfId="148"/>
-    <cellStyle name="40% - 强调文字颜色 2 6" xfId="149"/>
-    <cellStyle name="40% - 强调文字颜色 2 7" xfId="150"/>
-    <cellStyle name="40% - 强调文字颜色 2 8" xfId="151"/>
-    <cellStyle name="40% - 强调文字颜色 2 9" xfId="152"/>
-    <cellStyle name="40% - 强调文字颜色 3 10" xfId="153"/>
-    <cellStyle name="40% - 强调文字颜色 3 11" xfId="154"/>
-    <cellStyle name="40% - 强调文字颜色 3 12" xfId="155"/>
-    <cellStyle name="40% - 强调文字颜色 3 13" xfId="156"/>
-    <cellStyle name="40% - 强调文字颜色 3 14" xfId="157"/>
-    <cellStyle name="40% - 强调文字颜色 3 15" xfId="158"/>
-    <cellStyle name="40% - 强调文字颜色 3 16" xfId="159"/>
-    <cellStyle name="40% - 强调文字颜色 3 17" xfId="160"/>
-    <cellStyle name="40% - 强调文字颜色 3 18" xfId="161"/>
-    <cellStyle name="40% - 强调文字颜色 3 19" xfId="162"/>
-    <cellStyle name="40% - 强调文字颜色 3 2" xfId="163"/>
-    <cellStyle name="40% - 强调文字颜色 3 20" xfId="164"/>
-    <cellStyle name="40% - 强调文字颜色 3 3" xfId="165"/>
-    <cellStyle name="40% - 强调文字颜色 3 4" xfId="166"/>
-    <cellStyle name="40% - 强调文字颜色 3 5" xfId="167"/>
-    <cellStyle name="40% - 强调文字颜色 3 6" xfId="168"/>
-    <cellStyle name="40% - 强调文字颜色 3 7" xfId="169"/>
-    <cellStyle name="40% - 强调文字颜色 3 8" xfId="170"/>
-    <cellStyle name="40% - 强调文字颜色 3 9" xfId="171"/>
-    <cellStyle name="40% - 强调文字颜色 4 10" xfId="172"/>
-    <cellStyle name="40% - 强调文字颜色 4 11" xfId="173"/>
-    <cellStyle name="40% - 强调文字颜色 4 12" xfId="174"/>
-    <cellStyle name="40% - 强调文字颜色 4 13" xfId="175"/>
-    <cellStyle name="40% - 强调文字颜色 4 14" xfId="176"/>
-    <cellStyle name="40% - 强调文字颜色 4 15" xfId="177"/>
-    <cellStyle name="40% - 强调文字颜色 4 16" xfId="178"/>
-    <cellStyle name="40% - 强调文字颜色 4 17" xfId="179"/>
-    <cellStyle name="40% - 强调文字颜色 4 18" xfId="180"/>
-    <cellStyle name="40% - 强调文字颜色 4 19" xfId="181"/>
-    <cellStyle name="40% - 强调文字颜色 4 2" xfId="182"/>
-    <cellStyle name="40% - 强调文字颜色 4 20" xfId="183"/>
-    <cellStyle name="40% - 强调文字颜色 4 3" xfId="184"/>
-    <cellStyle name="40% - 强调文字颜色 4 4" xfId="185"/>
-    <cellStyle name="40% - 强调文字颜色 4 5" xfId="186"/>
-    <cellStyle name="40% - 强调文字颜色 4 6" xfId="187"/>
-    <cellStyle name="40% - 强调文字颜色 4 7" xfId="188"/>
-    <cellStyle name="40% - 强调文字颜色 4 8" xfId="189"/>
-    <cellStyle name="40% - 强调文字颜色 4 9" xfId="190"/>
-    <cellStyle name="40% - 强调文字颜色 5 10" xfId="191"/>
-    <cellStyle name="40% - 强调文字颜色 5 11" xfId="192"/>
-    <cellStyle name="40% - 强调文字颜色 5 12" xfId="193"/>
-    <cellStyle name="40% - 强调文字颜色 5 13" xfId="194"/>
-    <cellStyle name="40% - 强调文字颜色 5 14" xfId="195"/>
-    <cellStyle name="40% - 强调文字颜色 5 15" xfId="196"/>
-    <cellStyle name="40% - 强调文字颜色 5 16" xfId="197"/>
-    <cellStyle name="40% - 强调文字颜色 5 17" xfId="198"/>
-    <cellStyle name="40% - 强调文字颜色 5 18" xfId="199"/>
-    <cellStyle name="40% - 强调文字颜色 5 19" xfId="200"/>
-    <cellStyle name="40% - 强调文字颜色 5 2" xfId="201"/>
-    <cellStyle name="40% - 强调文字颜色 5 20" xfId="202"/>
-    <cellStyle name="40% - 强调文字颜色 5 3" xfId="203"/>
-    <cellStyle name="40% - 强调文字颜色 5 4" xfId="204"/>
-    <cellStyle name="40% - 强调文字颜色 5 5" xfId="205"/>
-    <cellStyle name="40% - 强调文字颜色 5 6" xfId="206"/>
-    <cellStyle name="40% - 强调文字颜色 5 7" xfId="207"/>
-    <cellStyle name="40% - 强调文字颜色 5 8" xfId="208"/>
-    <cellStyle name="40% - 强调文字颜色 5 9" xfId="209"/>
-    <cellStyle name="40% - 强调文字颜色 6 10" xfId="210"/>
-    <cellStyle name="40% - 强调文字颜色 6 11" xfId="211"/>
-    <cellStyle name="40% - 强调文字颜色 6 12" xfId="212"/>
-    <cellStyle name="40% - 强调文字颜色 6 13" xfId="213"/>
-    <cellStyle name="40% - 强调文字颜色 6 14" xfId="214"/>
-    <cellStyle name="40% - 强调文字颜色 6 15" xfId="215"/>
-    <cellStyle name="40% - 强调文字颜色 6 16" xfId="216"/>
-    <cellStyle name="40% - 强调文字颜色 6 17" xfId="217"/>
-    <cellStyle name="40% - 强调文字颜色 6 18" xfId="218"/>
-    <cellStyle name="40% - 强调文字颜色 6 19" xfId="219"/>
-    <cellStyle name="40% - 强调文字颜色 6 2" xfId="220"/>
-    <cellStyle name="40% - 强调文字颜色 6 20" xfId="221"/>
-    <cellStyle name="40% - 强调文字颜色 6 3" xfId="222"/>
-    <cellStyle name="40% - 强调文字颜色 6 4" xfId="223"/>
-    <cellStyle name="40% - 强调文字颜色 6 5" xfId="224"/>
-    <cellStyle name="40% - 强调文字颜色 6 6" xfId="225"/>
-    <cellStyle name="40% - 强调文字颜色 6 7" xfId="226"/>
-    <cellStyle name="40% - 强调文字颜色 6 8" xfId="227"/>
-    <cellStyle name="40% - 强调文字颜色 6 9" xfId="228"/>
-    <cellStyle name="60% - 强调文字颜色 1 10" xfId="229"/>
-    <cellStyle name="60% - 强调文字颜色 1 11" xfId="230"/>
-    <cellStyle name="60% - 强调文字颜色 1 12" xfId="231"/>
-    <cellStyle name="60% - 强调文字颜色 1 13" xfId="232"/>
-    <cellStyle name="60% - 强调文字颜色 1 14" xfId="233"/>
-    <cellStyle name="60% - 强调文字颜色 1 15" xfId="234"/>
-    <cellStyle name="60% - 强调文字颜色 1 16" xfId="235"/>
-    <cellStyle name="60% - 强调文字颜色 1 17" xfId="236"/>
-    <cellStyle name="60% - 强调文字颜色 1 18" xfId="237"/>
-    <cellStyle name="60% - 强调文字颜色 1 19" xfId="238"/>
-    <cellStyle name="60% - 强调文字颜色 1 2" xfId="239"/>
-    <cellStyle name="60% - 强调文字颜色 1 20" xfId="240"/>
-    <cellStyle name="60% - 强调文字颜色 1 3" xfId="241"/>
-    <cellStyle name="60% - 强调文字颜色 1 4" xfId="242"/>
-    <cellStyle name="60% - 强调文字颜色 1 5" xfId="243"/>
-    <cellStyle name="60% - 强调文字颜色 1 6" xfId="244"/>
-    <cellStyle name="60% - 强调文字颜色 1 7" xfId="245"/>
-    <cellStyle name="60% - 强调文字颜色 1 8" xfId="246"/>
-    <cellStyle name="60% - 强调文字颜色 1 9" xfId="247"/>
-    <cellStyle name="60% - 强调文字颜色 2 10" xfId="248"/>
-    <cellStyle name="60% - 强调文字颜色 2 11" xfId="249"/>
-    <cellStyle name="60% - 强调文字颜色 2 12" xfId="250"/>
-    <cellStyle name="60% - 强调文字颜色 2 13" xfId="251"/>
-    <cellStyle name="60% - 强调文字颜色 2 14" xfId="252"/>
-    <cellStyle name="60% - 强调文字颜色 2 15" xfId="253"/>
-    <cellStyle name="60% - 强调文字颜色 2 16" xfId="254"/>
-    <cellStyle name="60% - 强调文字颜色 2 17" xfId="255"/>
-    <cellStyle name="60% - 强调文字颜色 2 18" xfId="256"/>
-    <cellStyle name="60% - 强调文字颜色 2 19" xfId="257"/>
-    <cellStyle name="60% - 强调文字颜色 2 2" xfId="258"/>
-    <cellStyle name="60% - 强调文字颜色 2 20" xfId="259"/>
-    <cellStyle name="60% - 强调文字颜色 2 3" xfId="260"/>
-    <cellStyle name="60% - 强调文字颜色 2 4" xfId="261"/>
-    <cellStyle name="60% - 强调文字颜色 2 5" xfId="262"/>
-    <cellStyle name="60% - 强调文字颜色 2 6" xfId="263"/>
-    <cellStyle name="60% - 强调文字颜色 2 7" xfId="264"/>
-    <cellStyle name="60% - 强调文字颜色 2 8" xfId="265"/>
-    <cellStyle name="60% - 强调文字颜色 2 9" xfId="266"/>
-    <cellStyle name="60% - 强调文字颜色 3 10" xfId="267"/>
-    <cellStyle name="60% - 强调文字颜色 3 11" xfId="268"/>
-    <cellStyle name="60% - 强调文字颜色 3 12" xfId="269"/>
-    <cellStyle name="60% - 强调文字颜色 3 13" xfId="270"/>
-    <cellStyle name="60% - 强调文字颜色 3 14" xfId="271"/>
-    <cellStyle name="60% - 强调文字颜色 3 15" xfId="272"/>
-    <cellStyle name="60% - 强调文字颜色 3 16" xfId="273"/>
-    <cellStyle name="60% - 强调文字颜色 3 17" xfId="274"/>
-    <cellStyle name="60% - 强调文字颜色 3 18" xfId="275"/>
-    <cellStyle name="60% - 强调文字颜色 3 19" xfId="276"/>
-    <cellStyle name="60% - 强调文字颜色 3 2" xfId="277"/>
-    <cellStyle name="60% - 强调文字颜色 3 20" xfId="278"/>
-    <cellStyle name="60% - 强调文字颜色 3 3" xfId="279"/>
-    <cellStyle name="60% - 强调文字颜色 3 4" xfId="280"/>
-    <cellStyle name="60% - 强调文字颜色 3 5" xfId="281"/>
-    <cellStyle name="60% - 强调文字颜色 3 6" xfId="282"/>
-    <cellStyle name="60% - 强调文字颜色 3 7" xfId="283"/>
-    <cellStyle name="60% - 强调文字颜色 3 8" xfId="284"/>
-    <cellStyle name="60% - 强调文字颜色 3 9" xfId="285"/>
-    <cellStyle name="60% - 强调文字颜色 4 10" xfId="286"/>
-    <cellStyle name="60% - 强调文字颜色 4 11" xfId="287"/>
-    <cellStyle name="60% - 强调文字颜色 4 12" xfId="288"/>
-    <cellStyle name="60% - 强调文字颜色 4 13" xfId="289"/>
-    <cellStyle name="60% - 强调文字颜色 4 14" xfId="290"/>
-    <cellStyle name="60% - 强调文字颜色 4 15" xfId="291"/>
-    <cellStyle name="60% - 强调文字颜色 4 16" xfId="292"/>
-    <cellStyle name="60% - 强调文字颜色 4 17" xfId="293"/>
-    <cellStyle name="60% - 强调文字颜色 4 18" xfId="294"/>
-    <cellStyle name="60% - 强调文字颜色 4 19" xfId="295"/>
-    <cellStyle name="60% - 强调文字颜色 4 2" xfId="296"/>
-    <cellStyle name="60% - 强调文字颜色 4 20" xfId="297"/>
-    <cellStyle name="60% - 强调文字颜色 4 3" xfId="298"/>
-    <cellStyle name="60% - 强调文字颜色 4 4" xfId="299"/>
-    <cellStyle name="60% - 强调文字颜色 4 5" xfId="300"/>
-    <cellStyle name="60% - 强调文字颜色 4 6" xfId="301"/>
-    <cellStyle name="60% - 强调文字颜色 4 7" xfId="302"/>
-    <cellStyle name="60% - 强调文字颜色 4 8" xfId="303"/>
-    <cellStyle name="60% - 强调文字颜色 4 9" xfId="304"/>
-    <cellStyle name="60% - 强调文字颜色 5 10" xfId="305"/>
-    <cellStyle name="60% - 强调文字颜色 5 11" xfId="306"/>
-    <cellStyle name="60% - 强调文字颜色 5 12" xfId="307"/>
-    <cellStyle name="60% - 强调文字颜色 5 13" xfId="308"/>
-    <cellStyle name="60% - 强调文字颜色 5 14" xfId="309"/>
-    <cellStyle name="60% - 强调文字颜色 5 15" xfId="310"/>
-    <cellStyle name="60% - 强调文字颜色 5 16" xfId="311"/>
-    <cellStyle name="60% - 强调文字颜色 5 17" xfId="312"/>
-    <cellStyle name="60% - 强调文字颜色 5 18" xfId="313"/>
-    <cellStyle name="60% - 强调文字颜色 5 19" xfId="314"/>
-    <cellStyle name="60% - 强调文字颜色 5 2" xfId="315"/>
-    <cellStyle name="60% - 强调文字颜色 5 20" xfId="316"/>
-    <cellStyle name="60% - 强调文字颜色 5 3" xfId="317"/>
-    <cellStyle name="60% - 强调文字颜色 5 4" xfId="318"/>
-    <cellStyle name="60% - 强调文字颜色 5 5" xfId="319"/>
-    <cellStyle name="60% - 强调文字颜色 5 6" xfId="320"/>
-    <cellStyle name="60% - 强调文字颜色 5 7" xfId="321"/>
-    <cellStyle name="60% - 强调文字颜色 5 8" xfId="322"/>
-    <cellStyle name="60% - 强调文字颜色 5 9" xfId="323"/>
-    <cellStyle name="60% - 强调文字颜色 6 10" xfId="324"/>
-    <cellStyle name="60% - 强调文字颜色 6 11" xfId="325"/>
-    <cellStyle name="60% - 强调文字颜色 6 12" xfId="326"/>
-    <cellStyle name="60% - 强调文字颜色 6 13" xfId="327"/>
-    <cellStyle name="60% - 强调文字颜色 6 14" xfId="328"/>
-    <cellStyle name="60% - 强调文字颜色 6 15" xfId="329"/>
-    <cellStyle name="60% - 强调文字颜色 6 16" xfId="330"/>
-    <cellStyle name="60% - 强调文字颜色 6 17" xfId="331"/>
-    <cellStyle name="60% - 强调文字颜色 6 18" xfId="332"/>
-    <cellStyle name="60% - 强调文字颜色 6 19" xfId="333"/>
-    <cellStyle name="60% - 强调文字颜色 6 2" xfId="334"/>
-    <cellStyle name="60% - 强调文字颜色 6 20" xfId="335"/>
-    <cellStyle name="60% - 强调文字颜色 6 3" xfId="336"/>
-    <cellStyle name="60% - 强调文字颜色 6 4" xfId="337"/>
-    <cellStyle name="60% - 强调文字颜色 6 5" xfId="338"/>
-    <cellStyle name="60% - 强调文字颜色 6 6" xfId="339"/>
-    <cellStyle name="60% - 强调文字颜色 6 7" xfId="340"/>
-    <cellStyle name="60% - 强调文字颜色 6 8" xfId="341"/>
-    <cellStyle name="60% - 强调文字颜色 6 9" xfId="342"/>
+    <cellStyle name="20% - 强调文字颜色 1 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="20% - 强调文字颜色 1 11" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% - 强调文字颜色 1 12" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="20% - 强调文字颜色 1 13" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20% - 强调文字颜色 1 14" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="20% - 强调文字颜色 1 15" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="20% - 强调文字颜色 1 16" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="20% - 强调文字颜色 1 17" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="20% - 强调文字颜色 1 18" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="20% - 强调文字颜色 1 19" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="20% - 强调文字颜色 1 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="20% - 强调文字颜色 1 20" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="20% - 强调文字颜色 1 3" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="20% - 强调文字颜色 1 4" xfId="14" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="20% - 强调文字颜色 1 5" xfId="15" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="20% - 强调文字颜色 1 6" xfId="16" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="20% - 强调文字颜色 1 7" xfId="17" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="20% - 强调文字颜色 1 8" xfId="18" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="20% - 强调文字颜色 1 9" xfId="19" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="20% - 强调文字颜色 2 10" xfId="20" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="20% - 强调文字颜色 2 11" xfId="21" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="20% - 强调文字颜色 2 12" xfId="22" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="20% - 强调文字颜色 2 13" xfId="23" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="20% - 强调文字颜色 2 14" xfId="24" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="20% - 强调文字颜色 2 15" xfId="25" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="20% - 强调文字颜色 2 16" xfId="26" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="20% - 强调文字颜色 2 17" xfId="27" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="20% - 强调文字颜色 2 18" xfId="28" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="20% - 强调文字颜色 2 19" xfId="29" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="20% - 强调文字颜色 2 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="20% - 强调文字颜色 2 20" xfId="31" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="20% - 强调文字颜色 2 3" xfId="32" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="20% - 强调文字颜色 2 4" xfId="33" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="20% - 强调文字颜色 2 5" xfId="34" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="20% - 强调文字颜色 2 6" xfId="35" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="20% - 强调文字颜色 2 7" xfId="36" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="20% - 强调文字颜色 2 8" xfId="37" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="20% - 强调文字颜色 2 9" xfId="38" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="20% - 强调文字颜色 3 10" xfId="39" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="20% - 强调文字颜色 3 11" xfId="40" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="20% - 强调文字颜色 3 12" xfId="41" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="20% - 强调文字颜色 3 13" xfId="42" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="20% - 强调文字颜色 3 14" xfId="43" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="20% - 强调文字颜色 3 15" xfId="44" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="20% - 强调文字颜色 3 16" xfId="45" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="20% - 强调文字颜色 3 17" xfId="46" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="20% - 强调文字颜色 3 18" xfId="47" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="20% - 强调文字颜色 3 19" xfId="48" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="20% - 强调文字颜色 3 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="20% - 强调文字颜色 3 20" xfId="50" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="20% - 强调文字颜色 3 3" xfId="51" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="20% - 强调文字颜色 3 4" xfId="52" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="20% - 强调文字颜色 3 5" xfId="53" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="20% - 强调文字颜色 3 6" xfId="54" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="20% - 强调文字颜色 3 7" xfId="55" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="20% - 强调文字颜色 3 8" xfId="56" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="20% - 强调文字颜色 3 9" xfId="57" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="20% - 强调文字颜色 4 10" xfId="58" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="20% - 强调文字颜色 4 11" xfId="59" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="20% - 强调文字颜色 4 12" xfId="60" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="20% - 强调文字颜色 4 13" xfId="61" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="20% - 强调文字颜色 4 14" xfId="62" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="20% - 强调文字颜色 4 15" xfId="63" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="20% - 强调文字颜色 4 16" xfId="64" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="20% - 强调文字颜色 4 17" xfId="65" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="20% - 强调文字颜色 4 18" xfId="66" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="20% - 强调文字颜色 4 19" xfId="67" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="20% - 强调文字颜色 4 2" xfId="68" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="20% - 强调文字颜色 4 20" xfId="69" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="20% - 强调文字颜色 4 3" xfId="70" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="20% - 强调文字颜色 4 4" xfId="71" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="20% - 强调文字颜色 4 5" xfId="72" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="20% - 强调文字颜色 4 6" xfId="73" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="20% - 强调文字颜色 4 7" xfId="74" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="20% - 强调文字颜色 4 8" xfId="75" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="20% - 强调文字颜色 4 9" xfId="76" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="20% - 强调文字颜色 5 10" xfId="77" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="20% - 强调文字颜色 5 11" xfId="78" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="20% - 强调文字颜色 5 12" xfId="79" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="20% - 强调文字颜色 5 13" xfId="80" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="20% - 强调文字颜色 5 14" xfId="81" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="20% - 强调文字颜色 5 15" xfId="82" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="20% - 强调文字颜色 5 16" xfId="83" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="20% - 强调文字颜色 5 17" xfId="84" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="20% - 强调文字颜色 5 18" xfId="85" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="20% - 强调文字颜色 5 19" xfId="86" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="20% - 强调文字颜色 5 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="20% - 强调文字颜色 5 20" xfId="88" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="20% - 强调文字颜色 5 3" xfId="89" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="20% - 强调文字颜色 5 4" xfId="90" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="20% - 强调文字颜色 5 5" xfId="91" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="20% - 强调文字颜色 5 6" xfId="92" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="20% - 强调文字颜色 5 7" xfId="93" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="20% - 强调文字颜色 5 8" xfId="94" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="20% - 强调文字颜色 5 9" xfId="95" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="20% - 强调文字颜色 6 10" xfId="96" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="20% - 强调文字颜色 6 11" xfId="97" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="20% - 强调文字颜色 6 12" xfId="98" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="20% - 强调文字颜色 6 13" xfId="99" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="20% - 强调文字颜色 6 14" xfId="100" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="20% - 强调文字颜色 6 15" xfId="101" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
+    <cellStyle name="20% - 强调文字颜色 6 16" xfId="102" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="20% - 强调文字颜色 6 17" xfId="103" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
+    <cellStyle name="20% - 强调文字颜色 6 18" xfId="104" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
+    <cellStyle name="20% - 强调文字颜色 6 19" xfId="105" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
+    <cellStyle name="20% - 强调文字颜色 6 2" xfId="106" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
+    <cellStyle name="20% - 强调文字颜色 6 20" xfId="107" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
+    <cellStyle name="20% - 强调文字颜色 6 3" xfId="108" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
+    <cellStyle name="20% - 强调文字颜色 6 4" xfId="109" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
+    <cellStyle name="20% - 强调文字颜色 6 5" xfId="110" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="20% - 强调文字颜色 6 6" xfId="111" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="20% - 强调文字颜色 6 7" xfId="112" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="20% - 强调文字颜色 6 8" xfId="113" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="20% - 强调文字颜色 6 9" xfId="114" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="40% - 强调文字颜色 1 10" xfId="115" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="40% - 强调文字颜色 1 11" xfId="116" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="40% - 强调文字颜色 1 12" xfId="117" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="40% - 强调文字颜色 1 13" xfId="118" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="40% - 强调文字颜色 1 14" xfId="119" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="40% - 强调文字颜色 1 15" xfId="120" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
+    <cellStyle name="40% - 强调文字颜色 1 16" xfId="121" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="40% - 强调文字颜色 1 17" xfId="122" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
+    <cellStyle name="40% - 强调文字颜色 1 18" xfId="123" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
+    <cellStyle name="40% - 强调文字颜色 1 19" xfId="124" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
+    <cellStyle name="40% - 强调文字颜色 1 2" xfId="125" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
+    <cellStyle name="40% - 强调文字颜色 1 20" xfId="126" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
+    <cellStyle name="40% - 强调文字颜色 1 3" xfId="127" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
+    <cellStyle name="40% - 强调文字颜色 1 4" xfId="128" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
+    <cellStyle name="40% - 强调文字颜色 1 5" xfId="129" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
+    <cellStyle name="40% - 强调文字颜色 1 6" xfId="130" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
+    <cellStyle name="40% - 强调文字颜色 1 7" xfId="131" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
+    <cellStyle name="40% - 强调文字颜色 1 8" xfId="132" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
+    <cellStyle name="40% - 强调文字颜色 1 9" xfId="133" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
+    <cellStyle name="40% - 强调文字颜色 2 10" xfId="134" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
+    <cellStyle name="40% - 强调文字颜色 2 11" xfId="135" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
+    <cellStyle name="40% - 强调文字颜色 2 12" xfId="136" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
+    <cellStyle name="40% - 强调文字颜色 2 13" xfId="137" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
+    <cellStyle name="40% - 强调文字颜色 2 14" xfId="138" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
+    <cellStyle name="40% - 强调文字颜色 2 15" xfId="139" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
+    <cellStyle name="40% - 强调文字颜色 2 16" xfId="140" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
+    <cellStyle name="40% - 强调文字颜色 2 17" xfId="141" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
+    <cellStyle name="40% - 强调文字颜色 2 18" xfId="142" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
+    <cellStyle name="40% - 强调文字颜色 2 19" xfId="143" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="40% - 强调文字颜色 2 2" xfId="144" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
+    <cellStyle name="40% - 强调文字颜色 2 20" xfId="145" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
+    <cellStyle name="40% - 强调文字颜色 2 3" xfId="146" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
+    <cellStyle name="40% - 强调文字颜色 2 4" xfId="147" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
+    <cellStyle name="40% - 强调文字颜色 2 5" xfId="148" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
+    <cellStyle name="40% - 强调文字颜色 2 6" xfId="149" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
+    <cellStyle name="40% - 强调文字颜色 2 7" xfId="150" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
+    <cellStyle name="40% - 强调文字颜色 2 8" xfId="151" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
+    <cellStyle name="40% - 强调文字颜色 2 9" xfId="152" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
+    <cellStyle name="40% - 强调文字颜色 3 10" xfId="153" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="40% - 强调文字颜色 3 11" xfId="154" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
+    <cellStyle name="40% - 强调文字颜色 3 12" xfId="155" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
+    <cellStyle name="40% - 强调文字颜色 3 13" xfId="156" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
+    <cellStyle name="40% - 强调文字颜色 3 14" xfId="157" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
+    <cellStyle name="40% - 强调文字颜色 3 15" xfId="158" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
+    <cellStyle name="40% - 强调文字颜色 3 16" xfId="159" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
+    <cellStyle name="40% - 强调文字颜色 3 17" xfId="160" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
+    <cellStyle name="40% - 强调文字颜色 3 18" xfId="161" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
+    <cellStyle name="40% - 强调文字颜色 3 19" xfId="162" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
+    <cellStyle name="40% - 强调文字颜色 3 2" xfId="163" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
+    <cellStyle name="40% - 强调文字颜色 3 20" xfId="164" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
+    <cellStyle name="40% - 强调文字颜色 3 3" xfId="165" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
+    <cellStyle name="40% - 强调文字颜色 3 4" xfId="166" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
+    <cellStyle name="40% - 强调文字颜色 3 5" xfId="167" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
+    <cellStyle name="40% - 强调文字颜色 3 6" xfId="168" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
+    <cellStyle name="40% - 强调文字颜色 3 7" xfId="169" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
+    <cellStyle name="40% - 强调文字颜色 3 8" xfId="170" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
+    <cellStyle name="40% - 强调文字颜色 3 9" xfId="171" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
+    <cellStyle name="40% - 强调文字颜色 4 10" xfId="172" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
+    <cellStyle name="40% - 强调文字颜色 4 11" xfId="173" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
+    <cellStyle name="40% - 强调文字颜色 4 12" xfId="174" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
+    <cellStyle name="40% - 强调文字颜色 4 13" xfId="175" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
+    <cellStyle name="40% - 强调文字颜色 4 14" xfId="176" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
+    <cellStyle name="40% - 强调文字颜色 4 15" xfId="177" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
+    <cellStyle name="40% - 强调文字颜色 4 16" xfId="178" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
+    <cellStyle name="40% - 强调文字颜色 4 17" xfId="179" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
+    <cellStyle name="40% - 强调文字颜色 4 18" xfId="180" xr:uid="{00000000-0005-0000-0000-0000B3000000}"/>
+    <cellStyle name="40% - 强调文字颜色 4 19" xfId="181" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
+    <cellStyle name="40% - 强调文字颜色 4 2" xfId="182" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
+    <cellStyle name="40% - 强调文字颜色 4 20" xfId="183" xr:uid="{00000000-0005-0000-0000-0000B6000000}"/>
+    <cellStyle name="40% - 强调文字颜色 4 3" xfId="184" xr:uid="{00000000-0005-0000-0000-0000B7000000}"/>
+    <cellStyle name="40% - 强调文字颜色 4 4" xfId="185" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
+    <cellStyle name="40% - 强调文字颜色 4 5" xfId="186" xr:uid="{00000000-0005-0000-0000-0000B9000000}"/>
+    <cellStyle name="40% - 强调文字颜色 4 6" xfId="187" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
+    <cellStyle name="40% - 强调文字颜色 4 7" xfId="188" xr:uid="{00000000-0005-0000-0000-0000BB000000}"/>
+    <cellStyle name="40% - 强调文字颜色 4 8" xfId="189" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
+    <cellStyle name="40% - 强调文字颜色 4 9" xfId="190" xr:uid="{00000000-0005-0000-0000-0000BD000000}"/>
+    <cellStyle name="40% - 强调文字颜色 5 10" xfId="191" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
+    <cellStyle name="40% - 强调文字颜色 5 11" xfId="192" xr:uid="{00000000-0005-0000-0000-0000BF000000}"/>
+    <cellStyle name="40% - 强调文字颜色 5 12" xfId="193" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
+    <cellStyle name="40% - 强调文字颜色 5 13" xfId="194" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
+    <cellStyle name="40% - 强调文字颜色 5 14" xfId="195" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
+    <cellStyle name="40% - 强调文字颜色 5 15" xfId="196" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
+    <cellStyle name="40% - 强调文字颜色 5 16" xfId="197" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
+    <cellStyle name="40% - 强调文字颜色 5 17" xfId="198" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
+    <cellStyle name="40% - 强调文字颜色 5 18" xfId="199" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
+    <cellStyle name="40% - 强调文字颜色 5 19" xfId="200" xr:uid="{00000000-0005-0000-0000-0000C7000000}"/>
+    <cellStyle name="40% - 强调文字颜色 5 2" xfId="201" xr:uid="{00000000-0005-0000-0000-0000C8000000}"/>
+    <cellStyle name="40% - 强调文字颜色 5 20" xfId="202" xr:uid="{00000000-0005-0000-0000-0000C9000000}"/>
+    <cellStyle name="40% - 强调文字颜色 5 3" xfId="203" xr:uid="{00000000-0005-0000-0000-0000CA000000}"/>
+    <cellStyle name="40% - 强调文字颜色 5 4" xfId="204" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
+    <cellStyle name="40% - 强调文字颜色 5 5" xfId="205" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
+    <cellStyle name="40% - 强调文字颜色 5 6" xfId="206" xr:uid="{00000000-0005-0000-0000-0000CD000000}"/>
+    <cellStyle name="40% - 强调文字颜色 5 7" xfId="207" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
+    <cellStyle name="40% - 强调文字颜色 5 8" xfId="208" xr:uid="{00000000-0005-0000-0000-0000CF000000}"/>
+    <cellStyle name="40% - 强调文字颜色 5 9" xfId="209" xr:uid="{00000000-0005-0000-0000-0000D0000000}"/>
+    <cellStyle name="40% - 强调文字颜色 6 10" xfId="210" xr:uid="{00000000-0005-0000-0000-0000D1000000}"/>
+    <cellStyle name="40% - 强调文字颜色 6 11" xfId="211" xr:uid="{00000000-0005-0000-0000-0000D2000000}"/>
+    <cellStyle name="40% - 强调文字颜色 6 12" xfId="212" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
+    <cellStyle name="40% - 强调文字颜色 6 13" xfId="213" xr:uid="{00000000-0005-0000-0000-0000D4000000}"/>
+    <cellStyle name="40% - 强调文字颜色 6 14" xfId="214" xr:uid="{00000000-0005-0000-0000-0000D5000000}"/>
+    <cellStyle name="40% - 强调文字颜色 6 15" xfId="215" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
+    <cellStyle name="40% - 强调文字颜色 6 16" xfId="216" xr:uid="{00000000-0005-0000-0000-0000D7000000}"/>
+    <cellStyle name="40% - 强调文字颜色 6 17" xfId="217" xr:uid="{00000000-0005-0000-0000-0000D8000000}"/>
+    <cellStyle name="40% - 强调文字颜色 6 18" xfId="218" xr:uid="{00000000-0005-0000-0000-0000D9000000}"/>
+    <cellStyle name="40% - 强调文字颜色 6 19" xfId="219" xr:uid="{00000000-0005-0000-0000-0000DA000000}"/>
+    <cellStyle name="40% - 强调文字颜色 6 2" xfId="220" xr:uid="{00000000-0005-0000-0000-0000DB000000}"/>
+    <cellStyle name="40% - 强调文字颜色 6 20" xfId="221" xr:uid="{00000000-0005-0000-0000-0000DC000000}"/>
+    <cellStyle name="40% - 强调文字颜色 6 3" xfId="222" xr:uid="{00000000-0005-0000-0000-0000DD000000}"/>
+    <cellStyle name="40% - 强调文字颜色 6 4" xfId="223" xr:uid="{00000000-0005-0000-0000-0000DE000000}"/>
+    <cellStyle name="40% - 强调文字颜色 6 5" xfId="224" xr:uid="{00000000-0005-0000-0000-0000DF000000}"/>
+    <cellStyle name="40% - 强调文字颜色 6 6" xfId="225" xr:uid="{00000000-0005-0000-0000-0000E0000000}"/>
+    <cellStyle name="40% - 强调文字颜色 6 7" xfId="226" xr:uid="{00000000-0005-0000-0000-0000E1000000}"/>
+    <cellStyle name="40% - 强调文字颜色 6 8" xfId="227" xr:uid="{00000000-0005-0000-0000-0000E2000000}"/>
+    <cellStyle name="40% - 强调文字颜色 6 9" xfId="228" xr:uid="{00000000-0005-0000-0000-0000E3000000}"/>
+    <cellStyle name="60% - 强调文字颜色 1 10" xfId="229" xr:uid="{00000000-0005-0000-0000-0000E4000000}"/>
+    <cellStyle name="60% - 强调文字颜色 1 11" xfId="230" xr:uid="{00000000-0005-0000-0000-0000E5000000}"/>
+    <cellStyle name="60% - 强调文字颜色 1 12" xfId="231" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
+    <cellStyle name="60% - 强调文字颜色 1 13" xfId="232" xr:uid="{00000000-0005-0000-0000-0000E7000000}"/>
+    <cellStyle name="60% - 强调文字颜色 1 14" xfId="233" xr:uid="{00000000-0005-0000-0000-0000E8000000}"/>
+    <cellStyle name="60% - 强调文字颜色 1 15" xfId="234" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
+    <cellStyle name="60% - 强调文字颜色 1 16" xfId="235" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
+    <cellStyle name="60% - 强调文字颜色 1 17" xfId="236" xr:uid="{00000000-0005-0000-0000-0000EB000000}"/>
+    <cellStyle name="60% - 强调文字颜色 1 18" xfId="237" xr:uid="{00000000-0005-0000-0000-0000EC000000}"/>
+    <cellStyle name="60% - 强调文字颜色 1 19" xfId="238" xr:uid="{00000000-0005-0000-0000-0000ED000000}"/>
+    <cellStyle name="60% - 强调文字颜色 1 2" xfId="239" xr:uid="{00000000-0005-0000-0000-0000EE000000}"/>
+    <cellStyle name="60% - 强调文字颜色 1 20" xfId="240" xr:uid="{00000000-0005-0000-0000-0000EF000000}"/>
+    <cellStyle name="60% - 强调文字颜色 1 3" xfId="241" xr:uid="{00000000-0005-0000-0000-0000F0000000}"/>
+    <cellStyle name="60% - 强调文字颜色 1 4" xfId="242" xr:uid="{00000000-0005-0000-0000-0000F1000000}"/>
+    <cellStyle name="60% - 强调文字颜色 1 5" xfId="243" xr:uid="{00000000-0005-0000-0000-0000F2000000}"/>
+    <cellStyle name="60% - 强调文字颜色 1 6" xfId="244" xr:uid="{00000000-0005-0000-0000-0000F3000000}"/>
+    <cellStyle name="60% - 强调文字颜色 1 7" xfId="245" xr:uid="{00000000-0005-0000-0000-0000F4000000}"/>
+    <cellStyle name="60% - 强调文字颜色 1 8" xfId="246" xr:uid="{00000000-0005-0000-0000-0000F5000000}"/>
+    <cellStyle name="60% - 强调文字颜色 1 9" xfId="247" xr:uid="{00000000-0005-0000-0000-0000F6000000}"/>
+    <cellStyle name="60% - 强调文字颜色 2 10" xfId="248" xr:uid="{00000000-0005-0000-0000-0000F7000000}"/>
+    <cellStyle name="60% - 强调文字颜色 2 11" xfId="249" xr:uid="{00000000-0005-0000-0000-0000F8000000}"/>
+    <cellStyle name="60% - 强调文字颜色 2 12" xfId="250" xr:uid="{00000000-0005-0000-0000-0000F9000000}"/>
+    <cellStyle name="60% - 强调文字颜色 2 13" xfId="251" xr:uid="{00000000-0005-0000-0000-0000FA000000}"/>
+    <cellStyle name="60% - 强调文字颜色 2 14" xfId="252" xr:uid="{00000000-0005-0000-0000-0000FB000000}"/>
+    <cellStyle name="60% - 强调文字颜色 2 15" xfId="253" xr:uid="{00000000-0005-0000-0000-0000FC000000}"/>
+    <cellStyle name="60% - 强调文字颜色 2 16" xfId="254" xr:uid="{00000000-0005-0000-0000-0000FD000000}"/>
+    <cellStyle name="60% - 强调文字颜色 2 17" xfId="255" xr:uid="{00000000-0005-0000-0000-0000FE000000}"/>
+    <cellStyle name="60% - 强调文字颜色 2 18" xfId="256" xr:uid="{00000000-0005-0000-0000-0000FF000000}"/>
+    <cellStyle name="60% - 强调文字颜色 2 19" xfId="257" xr:uid="{00000000-0005-0000-0000-000000010000}"/>
+    <cellStyle name="60% - 强调文字颜色 2 2" xfId="258" xr:uid="{00000000-0005-0000-0000-000001010000}"/>
+    <cellStyle name="60% - 强调文字颜色 2 20" xfId="259" xr:uid="{00000000-0005-0000-0000-000002010000}"/>
+    <cellStyle name="60% - 强调文字颜色 2 3" xfId="260" xr:uid="{00000000-0005-0000-0000-000003010000}"/>
+    <cellStyle name="60% - 强调文字颜色 2 4" xfId="261" xr:uid="{00000000-0005-0000-0000-000004010000}"/>
+    <cellStyle name="60% - 强调文字颜色 2 5" xfId="262" xr:uid="{00000000-0005-0000-0000-000005010000}"/>
+    <cellStyle name="60% - 强调文字颜色 2 6" xfId="263" xr:uid="{00000000-0005-0000-0000-000006010000}"/>
+    <cellStyle name="60% - 强调文字颜色 2 7" xfId="264" xr:uid="{00000000-0005-0000-0000-000007010000}"/>
+    <cellStyle name="60% - 强调文字颜色 2 8" xfId="265" xr:uid="{00000000-0005-0000-0000-000008010000}"/>
+    <cellStyle name="60% - 强调文字颜色 2 9" xfId="266" xr:uid="{00000000-0005-0000-0000-000009010000}"/>
+    <cellStyle name="60% - 强调文字颜色 3 10" xfId="267" xr:uid="{00000000-0005-0000-0000-00000A010000}"/>
+    <cellStyle name="60% - 强调文字颜色 3 11" xfId="268" xr:uid="{00000000-0005-0000-0000-00000B010000}"/>
+    <cellStyle name="60% - 强调文字颜色 3 12" xfId="269" xr:uid="{00000000-0005-0000-0000-00000C010000}"/>
+    <cellStyle name="60% - 强调文字颜色 3 13" xfId="270" xr:uid="{00000000-0005-0000-0000-00000D010000}"/>
+    <cellStyle name="60% - 强调文字颜色 3 14" xfId="271" xr:uid="{00000000-0005-0000-0000-00000E010000}"/>
+    <cellStyle name="60% - 强调文字颜色 3 15" xfId="272" xr:uid="{00000000-0005-0000-0000-00000F010000}"/>
+    <cellStyle name="60% - 强调文字颜色 3 16" xfId="273" xr:uid="{00000000-0005-0000-0000-000010010000}"/>
+    <cellStyle name="60% - 强调文字颜色 3 17" xfId="274" xr:uid="{00000000-0005-0000-0000-000011010000}"/>
+    <cellStyle name="60% - 强调文字颜色 3 18" xfId="275" xr:uid="{00000000-0005-0000-0000-000012010000}"/>
+    <cellStyle name="60% - 强调文字颜色 3 19" xfId="276" xr:uid="{00000000-0005-0000-0000-000013010000}"/>
+    <cellStyle name="60% - 强调文字颜色 3 2" xfId="277" xr:uid="{00000000-0005-0000-0000-000014010000}"/>
+    <cellStyle name="60% - 强调文字颜色 3 20" xfId="278" xr:uid="{00000000-0005-0000-0000-000015010000}"/>
+    <cellStyle name="60% - 强调文字颜色 3 3" xfId="279" xr:uid="{00000000-0005-0000-0000-000016010000}"/>
+    <cellStyle name="60% - 强调文字颜色 3 4" xfId="280" xr:uid="{00000000-0005-0000-0000-000017010000}"/>
+    <cellStyle name="60% - 强调文字颜色 3 5" xfId="281" xr:uid="{00000000-0005-0000-0000-000018010000}"/>
+    <cellStyle name="60% - 强调文字颜色 3 6" xfId="282" xr:uid="{00000000-0005-0000-0000-000019010000}"/>
+    <cellStyle name="60% - 强调文字颜色 3 7" xfId="283" xr:uid="{00000000-0005-0000-0000-00001A010000}"/>
+    <cellStyle name="60% - 强调文字颜色 3 8" xfId="284" xr:uid="{00000000-0005-0000-0000-00001B010000}"/>
+    <cellStyle name="60% - 强调文字颜色 3 9" xfId="285" xr:uid="{00000000-0005-0000-0000-00001C010000}"/>
+    <cellStyle name="60% - 强调文字颜色 4 10" xfId="286" xr:uid="{00000000-0005-0000-0000-00001D010000}"/>
+    <cellStyle name="60% - 强调文字颜色 4 11" xfId="287" xr:uid="{00000000-0005-0000-0000-00001E010000}"/>
+    <cellStyle name="60% - 强调文字颜色 4 12" xfId="288" xr:uid="{00000000-0005-0000-0000-00001F010000}"/>
+    <cellStyle name="60% - 强调文字颜色 4 13" xfId="289" xr:uid="{00000000-0005-0000-0000-000020010000}"/>
+    <cellStyle name="60% - 强调文字颜色 4 14" xfId="290" xr:uid="{00000000-0005-0000-0000-000021010000}"/>
+    <cellStyle name="60% - 强调文字颜色 4 15" xfId="291" xr:uid="{00000000-0005-0000-0000-000022010000}"/>
+    <cellStyle name="60% - 强调文字颜色 4 16" xfId="292" xr:uid="{00000000-0005-0000-0000-000023010000}"/>
+    <cellStyle name="60% - 强调文字颜色 4 17" xfId="293" xr:uid="{00000000-0005-0000-0000-000024010000}"/>
+    <cellStyle name="60% - 强调文字颜色 4 18" xfId="294" xr:uid="{00000000-0005-0000-0000-000025010000}"/>
+    <cellStyle name="60% - 强调文字颜色 4 19" xfId="295" xr:uid="{00000000-0005-0000-0000-000026010000}"/>
+    <cellStyle name="60% - 强调文字颜色 4 2" xfId="296" xr:uid="{00000000-0005-0000-0000-000027010000}"/>
+    <cellStyle name="60% - 强调文字颜色 4 20" xfId="297" xr:uid="{00000000-0005-0000-0000-000028010000}"/>
+    <cellStyle name="60% - 强调文字颜色 4 3" xfId="298" xr:uid="{00000000-0005-0000-0000-000029010000}"/>
+    <cellStyle name="60% - 强调文字颜色 4 4" xfId="299" xr:uid="{00000000-0005-0000-0000-00002A010000}"/>
+    <cellStyle name="60% - 强调文字颜色 4 5" xfId="300" xr:uid="{00000000-0005-0000-0000-00002B010000}"/>
+    <cellStyle name="60% - 强调文字颜色 4 6" xfId="301" xr:uid="{00000000-0005-0000-0000-00002C010000}"/>
+    <cellStyle name="60% - 强调文字颜色 4 7" xfId="302" xr:uid="{00000000-0005-0000-0000-00002D010000}"/>
+    <cellStyle name="60% - 强调文字颜色 4 8" xfId="303" xr:uid="{00000000-0005-0000-0000-00002E010000}"/>
+    <cellStyle name="60% - 强调文字颜色 4 9" xfId="304" xr:uid="{00000000-0005-0000-0000-00002F010000}"/>
+    <cellStyle name="60% - 强调文字颜色 5 10" xfId="305" xr:uid="{00000000-0005-0000-0000-000030010000}"/>
+    <cellStyle name="60% - 强调文字颜色 5 11" xfId="306" xr:uid="{00000000-0005-0000-0000-000031010000}"/>
+    <cellStyle name="60% - 强调文字颜色 5 12" xfId="307" xr:uid="{00000000-0005-0000-0000-000032010000}"/>
+    <cellStyle name="60% - 强调文字颜色 5 13" xfId="308" xr:uid="{00000000-0005-0000-0000-000033010000}"/>
+    <cellStyle name="60% - 强调文字颜色 5 14" xfId="309" xr:uid="{00000000-0005-0000-0000-000034010000}"/>
+    <cellStyle name="60% - 强调文字颜色 5 15" xfId="310" xr:uid="{00000000-0005-0000-0000-000035010000}"/>
+    <cellStyle name="60% - 强调文字颜色 5 16" xfId="311" xr:uid="{00000000-0005-0000-0000-000036010000}"/>
+    <cellStyle name="60% - 强调文字颜色 5 17" xfId="312" xr:uid="{00000000-0005-0000-0000-000037010000}"/>
+    <cellStyle name="60% - 强调文字颜色 5 18" xfId="313" xr:uid="{00000000-0005-0000-0000-000038010000}"/>
+    <cellStyle name="60% - 强调文字颜色 5 19" xfId="314" xr:uid="{00000000-0005-0000-0000-000039010000}"/>
+    <cellStyle name="60% - 强调文字颜色 5 2" xfId="315" xr:uid="{00000000-0005-0000-0000-00003A010000}"/>
+    <cellStyle name="60% - 强调文字颜色 5 20" xfId="316" xr:uid="{00000000-0005-0000-0000-00003B010000}"/>
+    <cellStyle name="60% - 强调文字颜色 5 3" xfId="317" xr:uid="{00000000-0005-0000-0000-00003C010000}"/>
+    <cellStyle name="60% - 强调文字颜色 5 4" xfId="318" xr:uid="{00000000-0005-0000-0000-00003D010000}"/>
+    <cellStyle name="60% - 强调文字颜色 5 5" xfId="319" xr:uid="{00000000-0005-0000-0000-00003E010000}"/>
+    <cellStyle name="60% - 强调文字颜色 5 6" xfId="320" xr:uid="{00000000-0005-0000-0000-00003F010000}"/>
+    <cellStyle name="60% - 强调文字颜色 5 7" xfId="321" xr:uid="{00000000-0005-0000-0000-000040010000}"/>
+    <cellStyle name="60% - 强调文字颜色 5 8" xfId="322" xr:uid="{00000000-0005-0000-0000-000041010000}"/>
+    <cellStyle name="60% - 强调文字颜色 5 9" xfId="323" xr:uid="{00000000-0005-0000-0000-000042010000}"/>
+    <cellStyle name="60% - 强调文字颜色 6 10" xfId="324" xr:uid="{00000000-0005-0000-0000-000043010000}"/>
+    <cellStyle name="60% - 强调文字颜色 6 11" xfId="325" xr:uid="{00000000-0005-0000-0000-000044010000}"/>
+    <cellStyle name="60% - 强调文字颜色 6 12" xfId="326" xr:uid="{00000000-0005-0000-0000-000045010000}"/>
+    <cellStyle name="60% - 强调文字颜色 6 13" xfId="327" xr:uid="{00000000-0005-0000-0000-000046010000}"/>
+    <cellStyle name="60% - 强调文字颜色 6 14" xfId="328" xr:uid="{00000000-0005-0000-0000-000047010000}"/>
+    <cellStyle name="60% - 强调文字颜色 6 15" xfId="329" xr:uid="{00000000-0005-0000-0000-000048010000}"/>
+    <cellStyle name="60% - 强调文字颜色 6 16" xfId="330" xr:uid="{00000000-0005-0000-0000-000049010000}"/>
+    <cellStyle name="60% - 强调文字颜色 6 17" xfId="331" xr:uid="{00000000-0005-0000-0000-00004A010000}"/>
+    <cellStyle name="60% - 强调文字颜色 6 18" xfId="332" xr:uid="{00000000-0005-0000-0000-00004B010000}"/>
+    <cellStyle name="60% - 强调文字颜色 6 19" xfId="333" xr:uid="{00000000-0005-0000-0000-00004C010000}"/>
+    <cellStyle name="60% - 强调文字颜色 6 2" xfId="334" xr:uid="{00000000-0005-0000-0000-00004D010000}"/>
+    <cellStyle name="60% - 强调文字颜色 6 20" xfId="335" xr:uid="{00000000-0005-0000-0000-00004E010000}"/>
+    <cellStyle name="60% - 强调文字颜色 6 3" xfId="336" xr:uid="{00000000-0005-0000-0000-00004F010000}"/>
+    <cellStyle name="60% - 强调文字颜色 6 4" xfId="337" xr:uid="{00000000-0005-0000-0000-000050010000}"/>
+    <cellStyle name="60% - 强调文字颜色 6 5" xfId="338" xr:uid="{00000000-0005-0000-0000-000051010000}"/>
+    <cellStyle name="60% - 强调文字颜色 6 6" xfId="339" xr:uid="{00000000-0005-0000-0000-000052010000}"/>
+    <cellStyle name="60% - 强调文字颜色 6 7" xfId="340" xr:uid="{00000000-0005-0000-0000-000053010000}"/>
+    <cellStyle name="60% - 强调文字颜色 6 8" xfId="341" xr:uid="{00000000-0005-0000-0000-000054010000}"/>
+    <cellStyle name="60% - 强调文字颜色 6 9" xfId="342" xr:uid="{00000000-0005-0000-0000-000055010000}"/>
     <cellStyle name="标题" xfId="343" builtinId="15" customBuiltin="1"/>
     <cellStyle name="标题 1" xfId="344" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="标题 1 10" xfId="345"/>
-    <cellStyle name="标题 1 11" xfId="346"/>
-    <cellStyle name="标题 1 12" xfId="347"/>
-    <cellStyle name="标题 1 13" xfId="348"/>
-    <cellStyle name="标题 1 14" xfId="349"/>
-    <cellStyle name="标题 1 15" xfId="350"/>
-    <cellStyle name="标题 1 16" xfId="351"/>
-    <cellStyle name="标题 1 17" xfId="352"/>
-    <cellStyle name="标题 1 18" xfId="353"/>
-    <cellStyle name="标题 1 19" xfId="354"/>
-    <cellStyle name="标题 1 2" xfId="355"/>
-    <cellStyle name="标题 1 20" xfId="356"/>
-    <cellStyle name="标题 1 3" xfId="357"/>
-    <cellStyle name="标题 1 4" xfId="358"/>
-    <cellStyle name="标题 1 5" xfId="359"/>
-    <cellStyle name="标题 1 6" xfId="360"/>
-    <cellStyle name="标题 1 7" xfId="361"/>
-    <cellStyle name="标题 1 8" xfId="362"/>
-    <cellStyle name="标题 1 9" xfId="363"/>
-    <cellStyle name="标题 10" xfId="364"/>
-    <cellStyle name="标题 11" xfId="365"/>
-    <cellStyle name="标题 12" xfId="366"/>
-    <cellStyle name="标题 13" xfId="367"/>
-    <cellStyle name="标题 14" xfId="368"/>
-    <cellStyle name="标题 15" xfId="369"/>
-    <cellStyle name="标题 16" xfId="370"/>
-    <cellStyle name="标题 17" xfId="371"/>
-    <cellStyle name="标题 18" xfId="372"/>
-    <cellStyle name="标题 19" xfId="373"/>
+    <cellStyle name="标题 1 10" xfId="345" xr:uid="{00000000-0005-0000-0000-000058010000}"/>
+    <cellStyle name="标题 1 11" xfId="346" xr:uid="{00000000-0005-0000-0000-000059010000}"/>
+    <cellStyle name="标题 1 12" xfId="347" xr:uid="{00000000-0005-0000-0000-00005A010000}"/>
+    <cellStyle name="标题 1 13" xfId="348" xr:uid="{00000000-0005-0000-0000-00005B010000}"/>
+    <cellStyle name="标题 1 14" xfId="349" xr:uid="{00000000-0005-0000-0000-00005C010000}"/>
+    <cellStyle name="标题 1 15" xfId="350" xr:uid="{00000000-0005-0000-0000-00005D010000}"/>
+    <cellStyle name="标题 1 16" xfId="351" xr:uid="{00000000-0005-0000-0000-00005E010000}"/>
+    <cellStyle name="标题 1 17" xfId="352" xr:uid="{00000000-0005-0000-0000-00005F010000}"/>
+    <cellStyle name="标题 1 18" xfId="353" xr:uid="{00000000-0005-0000-0000-000060010000}"/>
+    <cellStyle name="标题 1 19" xfId="354" xr:uid="{00000000-0005-0000-0000-000061010000}"/>
+    <cellStyle name="标题 1 2" xfId="355" xr:uid="{00000000-0005-0000-0000-000062010000}"/>
+    <cellStyle name="标题 1 20" xfId="356" xr:uid="{00000000-0005-0000-0000-000063010000}"/>
+    <cellStyle name="标题 1 3" xfId="357" xr:uid="{00000000-0005-0000-0000-000064010000}"/>
+    <cellStyle name="标题 1 4" xfId="358" xr:uid="{00000000-0005-0000-0000-000065010000}"/>
+    <cellStyle name="标题 1 5" xfId="359" xr:uid="{00000000-0005-0000-0000-000066010000}"/>
+    <cellStyle name="标题 1 6" xfId="360" xr:uid="{00000000-0005-0000-0000-000067010000}"/>
+    <cellStyle name="标题 1 7" xfId="361" xr:uid="{00000000-0005-0000-0000-000068010000}"/>
+    <cellStyle name="标题 1 8" xfId="362" xr:uid="{00000000-0005-0000-0000-000069010000}"/>
+    <cellStyle name="标题 1 9" xfId="363" xr:uid="{00000000-0005-0000-0000-00006A010000}"/>
+    <cellStyle name="标题 10" xfId="364" xr:uid="{00000000-0005-0000-0000-00006B010000}"/>
+    <cellStyle name="标题 11" xfId="365" xr:uid="{00000000-0005-0000-0000-00006C010000}"/>
+    <cellStyle name="标题 12" xfId="366" xr:uid="{00000000-0005-0000-0000-00006D010000}"/>
+    <cellStyle name="标题 13" xfId="367" xr:uid="{00000000-0005-0000-0000-00006E010000}"/>
+    <cellStyle name="标题 14" xfId="368" xr:uid="{00000000-0005-0000-0000-00006F010000}"/>
+    <cellStyle name="标题 15" xfId="369" xr:uid="{00000000-0005-0000-0000-000070010000}"/>
+    <cellStyle name="标题 16" xfId="370" xr:uid="{00000000-0005-0000-0000-000071010000}"/>
+    <cellStyle name="标题 17" xfId="371" xr:uid="{00000000-0005-0000-0000-000072010000}"/>
+    <cellStyle name="标题 18" xfId="372" xr:uid="{00000000-0005-0000-0000-000073010000}"/>
+    <cellStyle name="标题 19" xfId="373" xr:uid="{00000000-0005-0000-0000-000074010000}"/>
     <cellStyle name="标题 2" xfId="374" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="标题 2 10" xfId="375"/>
-    <cellStyle name="标题 2 11" xfId="376"/>
-    <cellStyle name="标题 2 12" xfId="377"/>
-    <cellStyle name="标题 2 13" xfId="378"/>
-    <cellStyle name="标题 2 14" xfId="379"/>
-    <cellStyle name="标题 2 15" xfId="380"/>
-    <cellStyle name="标题 2 16" xfId="381"/>
-    <cellStyle name="标题 2 17" xfId="382"/>
-    <cellStyle name="标题 2 18" xfId="383"/>
-    <cellStyle name="标题 2 19" xfId="384"/>
-    <cellStyle name="标题 2 2" xfId="385"/>
-    <cellStyle name="标题 2 20" xfId="386"/>
-    <cellStyle name="标题 2 3" xfId="387"/>
-    <cellStyle name="标题 2 4" xfId="388"/>
-    <cellStyle name="标题 2 5" xfId="389"/>
-    <cellStyle name="标题 2 6" xfId="390"/>
-    <cellStyle name="标题 2 7" xfId="391"/>
-    <cellStyle name="标题 2 8" xfId="392"/>
-    <cellStyle name="标题 2 9" xfId="393"/>
-    <cellStyle name="标题 20" xfId="394"/>
-    <cellStyle name="标题 21" xfId="395"/>
-    <cellStyle name="标题 22" xfId="396"/>
-    <cellStyle name="标题 23" xfId="397"/>
+    <cellStyle name="标题 2 10" xfId="375" xr:uid="{00000000-0005-0000-0000-000076010000}"/>
+    <cellStyle name="标题 2 11" xfId="376" xr:uid="{00000000-0005-0000-0000-000077010000}"/>
+    <cellStyle name="标题 2 12" xfId="377" xr:uid="{00000000-0005-0000-0000-000078010000}"/>
+    <cellStyle name="标题 2 13" xfId="378" xr:uid="{00000000-0005-0000-0000-000079010000}"/>
+    <cellStyle name="标题 2 14" xfId="379" xr:uid="{00000000-0005-0000-0000-00007A010000}"/>
+    <cellStyle name="标题 2 15" xfId="380" xr:uid="{00000000-0005-0000-0000-00007B010000}"/>
+    <cellStyle name="标题 2 16" xfId="381" xr:uid="{00000000-0005-0000-0000-00007C010000}"/>
+    <cellStyle name="标题 2 17" xfId="382" xr:uid="{00000000-0005-0000-0000-00007D010000}"/>
+    <cellStyle name="标题 2 18" xfId="383" xr:uid="{00000000-0005-0000-0000-00007E010000}"/>
+    <cellStyle name="标题 2 19" xfId="384" xr:uid="{00000000-0005-0000-0000-00007F010000}"/>
+    <cellStyle name="标题 2 2" xfId="385" xr:uid="{00000000-0005-0000-0000-000080010000}"/>
+    <cellStyle name="标题 2 20" xfId="386" xr:uid="{00000000-0005-0000-0000-000081010000}"/>
+    <cellStyle name="标题 2 3" xfId="387" xr:uid="{00000000-0005-0000-0000-000082010000}"/>
+    <cellStyle name="标题 2 4" xfId="388" xr:uid="{00000000-0005-0000-0000-000083010000}"/>
+    <cellStyle name="标题 2 5" xfId="389" xr:uid="{00000000-0005-0000-0000-000084010000}"/>
+    <cellStyle name="标题 2 6" xfId="390" xr:uid="{00000000-0005-0000-0000-000085010000}"/>
+    <cellStyle name="标题 2 7" xfId="391" xr:uid="{00000000-0005-0000-0000-000086010000}"/>
+    <cellStyle name="标题 2 8" xfId="392" xr:uid="{00000000-0005-0000-0000-000087010000}"/>
+    <cellStyle name="标题 2 9" xfId="393" xr:uid="{00000000-0005-0000-0000-000088010000}"/>
+    <cellStyle name="标题 20" xfId="394" xr:uid="{00000000-0005-0000-0000-000089010000}"/>
+    <cellStyle name="标题 21" xfId="395" xr:uid="{00000000-0005-0000-0000-00008A010000}"/>
+    <cellStyle name="标题 22" xfId="396" xr:uid="{00000000-0005-0000-0000-00008B010000}"/>
+    <cellStyle name="标题 23" xfId="397" xr:uid="{00000000-0005-0000-0000-00008C010000}"/>
     <cellStyle name="标题 3" xfId="398" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="标题 3 10" xfId="399"/>
-    <cellStyle name="标题 3 11" xfId="400"/>
-    <cellStyle name="标题 3 12" xfId="401"/>
-    <cellStyle name="标题 3 13" xfId="402"/>
-    <cellStyle name="标题 3 14" xfId="403"/>
-    <cellStyle name="标题 3 15" xfId="404"/>
-    <cellStyle name="标题 3 16" xfId="405"/>
-    <cellStyle name="标题 3 17" xfId="406"/>
-    <cellStyle name="标题 3 18" xfId="407"/>
-    <cellStyle name="标题 3 19" xfId="408"/>
-    <cellStyle name="标题 3 2" xfId="409"/>
-    <cellStyle name="标题 3 20" xfId="410"/>
-    <cellStyle name="标题 3 3" xfId="411"/>
-    <cellStyle name="标题 3 4" xfId="412"/>
-    <cellStyle name="标题 3 5" xfId="413"/>
-    <cellStyle name="标题 3 6" xfId="414"/>
-    <cellStyle name="标题 3 7" xfId="415"/>
-    <cellStyle name="标题 3 8" xfId="416"/>
-    <cellStyle name="标题 3 9" xfId="417"/>
+    <cellStyle name="标题 3 10" xfId="399" xr:uid="{00000000-0005-0000-0000-00008E010000}"/>
+    <cellStyle name="标题 3 11" xfId="400" xr:uid="{00000000-0005-0000-0000-00008F010000}"/>
+    <cellStyle name="标题 3 12" xfId="401" xr:uid="{00000000-0005-0000-0000-000090010000}"/>
+    <cellStyle name="标题 3 13" xfId="402" xr:uid="{00000000-0005-0000-0000-000091010000}"/>
+    <cellStyle name="标题 3 14" xfId="403" xr:uid="{00000000-0005-0000-0000-000092010000}"/>
+    <cellStyle name="标题 3 15" xfId="404" xr:uid="{00000000-0005-0000-0000-000093010000}"/>
+    <cellStyle name="标题 3 16" xfId="405" xr:uid="{00000000-0005-0000-0000-000094010000}"/>
+    <cellStyle name="标题 3 17" xfId="406" xr:uid="{00000000-0005-0000-0000-000095010000}"/>
+    <cellStyle name="标题 3 18" xfId="407" xr:uid="{00000000-0005-0000-0000-000096010000}"/>
+    <cellStyle name="标题 3 19" xfId="408" xr:uid="{00000000-0005-0000-0000-000097010000}"/>
+    <cellStyle name="标题 3 2" xfId="409" xr:uid="{00000000-0005-0000-0000-000098010000}"/>
+    <cellStyle name="标题 3 20" xfId="410" xr:uid="{00000000-0005-0000-0000-000099010000}"/>
+    <cellStyle name="标题 3 3" xfId="411" xr:uid="{00000000-0005-0000-0000-00009A010000}"/>
+    <cellStyle name="标题 3 4" xfId="412" xr:uid="{00000000-0005-0000-0000-00009B010000}"/>
+    <cellStyle name="标题 3 5" xfId="413" xr:uid="{00000000-0005-0000-0000-00009C010000}"/>
+    <cellStyle name="标题 3 6" xfId="414" xr:uid="{00000000-0005-0000-0000-00009D010000}"/>
+    <cellStyle name="标题 3 7" xfId="415" xr:uid="{00000000-0005-0000-0000-00009E010000}"/>
+    <cellStyle name="标题 3 8" xfId="416" xr:uid="{00000000-0005-0000-0000-00009F010000}"/>
+    <cellStyle name="标题 3 9" xfId="417" xr:uid="{00000000-0005-0000-0000-0000A0010000}"/>
     <cellStyle name="标题 4" xfId="418" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="标题 4 10" xfId="419"/>
-    <cellStyle name="标题 4 11" xfId="420"/>
-    <cellStyle name="标题 4 12" xfId="421"/>
-    <cellStyle name="标题 4 13" xfId="422"/>
-    <cellStyle name="标题 4 14" xfId="423"/>
-    <cellStyle name="标题 4 15" xfId="424"/>
-    <cellStyle name="标题 4 16" xfId="425"/>
-    <cellStyle name="标题 4 17" xfId="426"/>
-    <cellStyle name="标题 4 18" xfId="427"/>
-    <cellStyle name="标题 4 19" xfId="428"/>
-    <cellStyle name="标题 4 2" xfId="429"/>
-    <cellStyle name="标题 4 20" xfId="430"/>
-    <cellStyle name="标题 4 3" xfId="431"/>
-    <cellStyle name="标题 4 4" xfId="432"/>
-    <cellStyle name="标题 4 5" xfId="433"/>
-    <cellStyle name="标题 4 6" xfId="434"/>
-    <cellStyle name="标题 4 7" xfId="435"/>
-    <cellStyle name="标题 4 8" xfId="436"/>
-    <cellStyle name="标题 4 9" xfId="437"/>
-    <cellStyle name="标题 5" xfId="438"/>
-    <cellStyle name="标题 6" xfId="439"/>
-    <cellStyle name="标题 7" xfId="440"/>
-    <cellStyle name="标题 8" xfId="441"/>
-    <cellStyle name="标题 9" xfId="442"/>
+    <cellStyle name="标题 4 10" xfId="419" xr:uid="{00000000-0005-0000-0000-0000A2010000}"/>
+    <cellStyle name="标题 4 11" xfId="420" xr:uid="{00000000-0005-0000-0000-0000A3010000}"/>
+    <cellStyle name="标题 4 12" xfId="421" xr:uid="{00000000-0005-0000-0000-0000A4010000}"/>
+    <cellStyle name="标题 4 13" xfId="422" xr:uid="{00000000-0005-0000-0000-0000A5010000}"/>
+    <cellStyle name="标题 4 14" xfId="423" xr:uid="{00000000-0005-0000-0000-0000A6010000}"/>
+    <cellStyle name="标题 4 15" xfId="424" xr:uid="{00000000-0005-0000-0000-0000A7010000}"/>
+    <cellStyle name="标题 4 16" xfId="425" xr:uid="{00000000-0005-0000-0000-0000A8010000}"/>
+    <cellStyle name="标题 4 17" xfId="426" xr:uid="{00000000-0005-0000-0000-0000A9010000}"/>
+    <cellStyle name="标题 4 18" xfId="427" xr:uid="{00000000-0005-0000-0000-0000AA010000}"/>
+    <cellStyle name="标题 4 19" xfId="428" xr:uid="{00000000-0005-0000-0000-0000AB010000}"/>
+    <cellStyle name="标题 4 2" xfId="429" xr:uid="{00000000-0005-0000-0000-0000AC010000}"/>
+    <cellStyle name="标题 4 20" xfId="430" xr:uid="{00000000-0005-0000-0000-0000AD010000}"/>
+    <cellStyle name="标题 4 3" xfId="431" xr:uid="{00000000-0005-0000-0000-0000AE010000}"/>
+    <cellStyle name="标题 4 4" xfId="432" xr:uid="{00000000-0005-0000-0000-0000AF010000}"/>
+    <cellStyle name="标题 4 5" xfId="433" xr:uid="{00000000-0005-0000-0000-0000B0010000}"/>
+    <cellStyle name="标题 4 6" xfId="434" xr:uid="{00000000-0005-0000-0000-0000B1010000}"/>
+    <cellStyle name="标题 4 7" xfId="435" xr:uid="{00000000-0005-0000-0000-0000B2010000}"/>
+    <cellStyle name="标题 4 8" xfId="436" xr:uid="{00000000-0005-0000-0000-0000B3010000}"/>
+    <cellStyle name="标题 4 9" xfId="437" xr:uid="{00000000-0005-0000-0000-0000B4010000}"/>
+    <cellStyle name="标题 5" xfId="438" xr:uid="{00000000-0005-0000-0000-0000B5010000}"/>
+    <cellStyle name="标题 6" xfId="439" xr:uid="{00000000-0005-0000-0000-0000B6010000}"/>
+    <cellStyle name="标题 7" xfId="440" xr:uid="{00000000-0005-0000-0000-0000B7010000}"/>
+    <cellStyle name="标题 8" xfId="441" xr:uid="{00000000-0005-0000-0000-0000B8010000}"/>
+    <cellStyle name="标题 9" xfId="442" xr:uid="{00000000-0005-0000-0000-0000B9010000}"/>
     <cellStyle name="差" xfId="443" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="差 10" xfId="444"/>
-    <cellStyle name="差 11" xfId="445"/>
-    <cellStyle name="差 12" xfId="446"/>
-    <cellStyle name="差 13" xfId="447"/>
-    <cellStyle name="差 14" xfId="448"/>
-    <cellStyle name="差 15" xfId="449"/>
-    <cellStyle name="差 16" xfId="450"/>
-    <cellStyle name="差 17" xfId="451"/>
-    <cellStyle name="差 18" xfId="452"/>
-    <cellStyle name="差 19" xfId="453"/>
-    <cellStyle name="差 2" xfId="454"/>
-    <cellStyle name="差 20" xfId="455"/>
-    <cellStyle name="差 3" xfId="456"/>
-    <cellStyle name="差 4" xfId="457"/>
-    <cellStyle name="差 5" xfId="458"/>
-    <cellStyle name="差 6" xfId="459"/>
-    <cellStyle name="差 7" xfId="460"/>
-    <cellStyle name="差 8" xfId="461"/>
-    <cellStyle name="差 9" xfId="462"/>
+    <cellStyle name="差 10" xfId="444" xr:uid="{00000000-0005-0000-0000-0000BB010000}"/>
+    <cellStyle name="差 11" xfId="445" xr:uid="{00000000-0005-0000-0000-0000BC010000}"/>
+    <cellStyle name="差 12" xfId="446" xr:uid="{00000000-0005-0000-0000-0000BD010000}"/>
+    <cellStyle name="差 13" xfId="447" xr:uid="{00000000-0005-0000-0000-0000BE010000}"/>
+    <cellStyle name="差 14" xfId="448" xr:uid="{00000000-0005-0000-0000-0000BF010000}"/>
+    <cellStyle name="差 15" xfId="449" xr:uid="{00000000-0005-0000-0000-0000C0010000}"/>
+    <cellStyle name="差 16" xfId="450" xr:uid="{00000000-0005-0000-0000-0000C1010000}"/>
+    <cellStyle name="差 17" xfId="451" xr:uid="{00000000-0005-0000-0000-0000C2010000}"/>
+    <cellStyle name="差 18" xfId="452" xr:uid="{00000000-0005-0000-0000-0000C3010000}"/>
+    <cellStyle name="差 19" xfId="453" xr:uid="{00000000-0005-0000-0000-0000C4010000}"/>
+    <cellStyle name="差 2" xfId="454" xr:uid="{00000000-0005-0000-0000-0000C5010000}"/>
+    <cellStyle name="差 20" xfId="455" xr:uid="{00000000-0005-0000-0000-0000C6010000}"/>
+    <cellStyle name="差 3" xfId="456" xr:uid="{00000000-0005-0000-0000-0000C7010000}"/>
+    <cellStyle name="差 4" xfId="457" xr:uid="{00000000-0005-0000-0000-0000C8010000}"/>
+    <cellStyle name="差 5" xfId="458" xr:uid="{00000000-0005-0000-0000-0000C9010000}"/>
+    <cellStyle name="差 6" xfId="459" xr:uid="{00000000-0005-0000-0000-0000CA010000}"/>
+    <cellStyle name="差 7" xfId="460" xr:uid="{00000000-0005-0000-0000-0000CB010000}"/>
+    <cellStyle name="差 8" xfId="461" xr:uid="{00000000-0005-0000-0000-0000CC010000}"/>
+    <cellStyle name="差 9" xfId="462" xr:uid="{00000000-0005-0000-0000-0000CD010000}"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 10" xfId="463"/>
-    <cellStyle name="常规 11" xfId="464"/>
-    <cellStyle name="常规 12" xfId="465"/>
-    <cellStyle name="常规 13" xfId="466"/>
-    <cellStyle name="常规 14" xfId="467"/>
-    <cellStyle name="常规 15" xfId="468"/>
-    <cellStyle name="常规 16" xfId="469"/>
-    <cellStyle name="常规 17" xfId="470"/>
-    <cellStyle name="常规 18" xfId="471"/>
-    <cellStyle name="常规 19" xfId="472"/>
-    <cellStyle name="常规 2" xfId="473"/>
-    <cellStyle name="常规 2 2" xfId="474"/>
-    <cellStyle name="常规 20" xfId="475"/>
-    <cellStyle name="常规 3" xfId="476"/>
-    <cellStyle name="常规 4" xfId="477"/>
-    <cellStyle name="常规 5" xfId="478"/>
-    <cellStyle name="常规 6" xfId="479"/>
-    <cellStyle name="常规 7" xfId="480"/>
-    <cellStyle name="常规 8" xfId="481"/>
-    <cellStyle name="常规 9" xfId="482"/>
+    <cellStyle name="常规 10" xfId="463" xr:uid="{00000000-0005-0000-0000-0000CF010000}"/>
+    <cellStyle name="常规 11" xfId="464" xr:uid="{00000000-0005-0000-0000-0000D0010000}"/>
+    <cellStyle name="常规 12" xfId="465" xr:uid="{00000000-0005-0000-0000-0000D1010000}"/>
+    <cellStyle name="常规 13" xfId="466" xr:uid="{00000000-0005-0000-0000-0000D2010000}"/>
+    <cellStyle name="常规 14" xfId="467" xr:uid="{00000000-0005-0000-0000-0000D3010000}"/>
+    <cellStyle name="常规 15" xfId="468" xr:uid="{00000000-0005-0000-0000-0000D4010000}"/>
+    <cellStyle name="常规 16" xfId="469" xr:uid="{00000000-0005-0000-0000-0000D5010000}"/>
+    <cellStyle name="常规 17" xfId="470" xr:uid="{00000000-0005-0000-0000-0000D6010000}"/>
+    <cellStyle name="常规 18" xfId="471" xr:uid="{00000000-0005-0000-0000-0000D7010000}"/>
+    <cellStyle name="常规 19" xfId="472" xr:uid="{00000000-0005-0000-0000-0000D8010000}"/>
+    <cellStyle name="常规 2" xfId="473" xr:uid="{00000000-0005-0000-0000-0000D9010000}"/>
+    <cellStyle name="常规 2 2" xfId="474" xr:uid="{00000000-0005-0000-0000-0000DA010000}"/>
+    <cellStyle name="常规 20" xfId="475" xr:uid="{00000000-0005-0000-0000-0000DB010000}"/>
+    <cellStyle name="常规 3" xfId="476" xr:uid="{00000000-0005-0000-0000-0000DC010000}"/>
+    <cellStyle name="常规 4" xfId="477" xr:uid="{00000000-0005-0000-0000-0000DD010000}"/>
+    <cellStyle name="常规 5" xfId="478" xr:uid="{00000000-0005-0000-0000-0000DE010000}"/>
+    <cellStyle name="常规 6" xfId="479" xr:uid="{00000000-0005-0000-0000-0000DF010000}"/>
+    <cellStyle name="常规 7" xfId="480" xr:uid="{00000000-0005-0000-0000-0000E0010000}"/>
+    <cellStyle name="常规 8" xfId="481" xr:uid="{00000000-0005-0000-0000-0000E1010000}"/>
+    <cellStyle name="常规 9" xfId="482" xr:uid="{00000000-0005-0000-0000-0000E2010000}"/>
     <cellStyle name="好" xfId="483" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="好 10" xfId="484"/>
-    <cellStyle name="好 11" xfId="485"/>
-    <cellStyle name="好 12" xfId="486"/>
-    <cellStyle name="好 13" xfId="487"/>
-    <cellStyle name="好 14" xfId="488"/>
-    <cellStyle name="好 15" xfId="489"/>
-    <cellStyle name="好 16" xfId="490"/>
-    <cellStyle name="好 17" xfId="491"/>
-    <cellStyle name="好 18" xfId="492"/>
-    <cellStyle name="好 19" xfId="493"/>
-    <cellStyle name="好 2" xfId="494"/>
-    <cellStyle name="好 20" xfId="495"/>
-    <cellStyle name="好 3" xfId="496"/>
-    <cellStyle name="好 4" xfId="497"/>
-    <cellStyle name="好 5" xfId="498"/>
-    <cellStyle name="好 6" xfId="499"/>
-    <cellStyle name="好 7" xfId="500"/>
-    <cellStyle name="好 8" xfId="501"/>
-    <cellStyle name="好 9" xfId="502"/>
+    <cellStyle name="好 10" xfId="484" xr:uid="{00000000-0005-0000-0000-0000E4010000}"/>
+    <cellStyle name="好 11" xfId="485" xr:uid="{00000000-0005-0000-0000-0000E5010000}"/>
+    <cellStyle name="好 12" xfId="486" xr:uid="{00000000-0005-0000-0000-0000E6010000}"/>
+    <cellStyle name="好 13" xfId="487" xr:uid="{00000000-0005-0000-0000-0000E7010000}"/>
+    <cellStyle name="好 14" xfId="488" xr:uid="{00000000-0005-0000-0000-0000E8010000}"/>
+    <cellStyle name="好 15" xfId="489" xr:uid="{00000000-0005-0000-0000-0000E9010000}"/>
+    <cellStyle name="好 16" xfId="490" xr:uid="{00000000-0005-0000-0000-0000EA010000}"/>
+    <cellStyle name="好 17" xfId="491" xr:uid="{00000000-0005-0000-0000-0000EB010000}"/>
+    <cellStyle name="好 18" xfId="492" xr:uid="{00000000-0005-0000-0000-0000EC010000}"/>
+    <cellStyle name="好 19" xfId="493" xr:uid="{00000000-0005-0000-0000-0000ED010000}"/>
+    <cellStyle name="好 2" xfId="494" xr:uid="{00000000-0005-0000-0000-0000EE010000}"/>
+    <cellStyle name="好 20" xfId="495" xr:uid="{00000000-0005-0000-0000-0000EF010000}"/>
+    <cellStyle name="好 3" xfId="496" xr:uid="{00000000-0005-0000-0000-0000F0010000}"/>
+    <cellStyle name="好 4" xfId="497" xr:uid="{00000000-0005-0000-0000-0000F1010000}"/>
+    <cellStyle name="好 5" xfId="498" xr:uid="{00000000-0005-0000-0000-0000F2010000}"/>
+    <cellStyle name="好 6" xfId="499" xr:uid="{00000000-0005-0000-0000-0000F3010000}"/>
+    <cellStyle name="好 7" xfId="500" xr:uid="{00000000-0005-0000-0000-0000F4010000}"/>
+    <cellStyle name="好 8" xfId="501" xr:uid="{00000000-0005-0000-0000-0000F5010000}"/>
+    <cellStyle name="好 9" xfId="502" xr:uid="{00000000-0005-0000-0000-0000F6010000}"/>
     <cellStyle name="汇总" xfId="503" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="汇总 10" xfId="504"/>
-    <cellStyle name="汇总 11" xfId="505"/>
-    <cellStyle name="汇总 12" xfId="506"/>
-    <cellStyle name="汇总 13" xfId="507"/>
-    <cellStyle name="汇总 14" xfId="508"/>
-    <cellStyle name="汇总 15" xfId="509"/>
-    <cellStyle name="汇总 16" xfId="510"/>
-    <cellStyle name="汇总 17" xfId="511"/>
-    <cellStyle name="汇总 18" xfId="512"/>
-    <cellStyle name="汇总 19" xfId="513"/>
-    <cellStyle name="汇总 2" xfId="514"/>
-    <cellStyle name="汇总 20" xfId="515"/>
-    <cellStyle name="汇总 3" xfId="516"/>
-    <cellStyle name="汇总 4" xfId="517"/>
-    <cellStyle name="汇总 5" xfId="518"/>
-    <cellStyle name="汇总 6" xfId="519"/>
-    <cellStyle name="汇总 7" xfId="520"/>
-    <cellStyle name="汇总 8" xfId="521"/>
-    <cellStyle name="汇总 9" xfId="522"/>
+    <cellStyle name="汇总 10" xfId="504" xr:uid="{00000000-0005-0000-0000-0000F8010000}"/>
+    <cellStyle name="汇总 11" xfId="505" xr:uid="{00000000-0005-0000-0000-0000F9010000}"/>
+    <cellStyle name="汇总 12" xfId="506" xr:uid="{00000000-0005-0000-0000-0000FA010000}"/>
+    <cellStyle name="汇总 13" xfId="507" xr:uid="{00000000-0005-0000-0000-0000FB010000}"/>
+    <cellStyle name="汇总 14" xfId="508" xr:uid="{00000000-0005-0000-0000-0000FC010000}"/>
+    <cellStyle name="汇总 15" xfId="509" xr:uid="{00000000-0005-0000-0000-0000FD010000}"/>
+    <cellStyle name="汇总 16" xfId="510" xr:uid="{00000000-0005-0000-0000-0000FE010000}"/>
+    <cellStyle name="汇总 17" xfId="511" xr:uid="{00000000-0005-0000-0000-0000FF010000}"/>
+    <cellStyle name="汇总 18" xfId="512" xr:uid="{00000000-0005-0000-0000-000000020000}"/>
+    <cellStyle name="汇总 19" xfId="513" xr:uid="{00000000-0005-0000-0000-000001020000}"/>
+    <cellStyle name="汇总 2" xfId="514" xr:uid="{00000000-0005-0000-0000-000002020000}"/>
+    <cellStyle name="汇总 20" xfId="515" xr:uid="{00000000-0005-0000-0000-000003020000}"/>
+    <cellStyle name="汇总 3" xfId="516" xr:uid="{00000000-0005-0000-0000-000004020000}"/>
+    <cellStyle name="汇总 4" xfId="517" xr:uid="{00000000-0005-0000-0000-000005020000}"/>
+    <cellStyle name="汇总 5" xfId="518" xr:uid="{00000000-0005-0000-0000-000006020000}"/>
+    <cellStyle name="汇总 6" xfId="519" xr:uid="{00000000-0005-0000-0000-000007020000}"/>
+    <cellStyle name="汇总 7" xfId="520" xr:uid="{00000000-0005-0000-0000-000008020000}"/>
+    <cellStyle name="汇总 8" xfId="521" xr:uid="{00000000-0005-0000-0000-000009020000}"/>
+    <cellStyle name="汇总 9" xfId="522" xr:uid="{00000000-0005-0000-0000-00000A020000}"/>
     <cellStyle name="计算" xfId="523" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="计算 10" xfId="524"/>
-    <cellStyle name="计算 11" xfId="525"/>
-    <cellStyle name="计算 12" xfId="526"/>
-    <cellStyle name="计算 13" xfId="527"/>
-    <cellStyle name="计算 14" xfId="528"/>
-    <cellStyle name="计算 15" xfId="529"/>
-    <cellStyle name="计算 16" xfId="530"/>
-    <cellStyle name="计算 17" xfId="531"/>
-    <cellStyle name="计算 18" xfId="532"/>
-    <cellStyle name="计算 19" xfId="533"/>
-    <cellStyle name="计算 2" xfId="534"/>
-    <cellStyle name="计算 20" xfId="535"/>
-    <cellStyle name="计算 3" xfId="536"/>
-    <cellStyle name="计算 4" xfId="537"/>
-    <cellStyle name="计算 5" xfId="538"/>
-    <cellStyle name="计算 6" xfId="539"/>
-    <cellStyle name="计算 7" xfId="540"/>
-    <cellStyle name="计算 8" xfId="541"/>
-    <cellStyle name="计算 9" xfId="542"/>
+    <cellStyle name="计算 10" xfId="524" xr:uid="{00000000-0005-0000-0000-00000C020000}"/>
+    <cellStyle name="计算 11" xfId="525" xr:uid="{00000000-0005-0000-0000-00000D020000}"/>
+    <cellStyle name="计算 12" xfId="526" xr:uid="{00000000-0005-0000-0000-00000E020000}"/>
+    <cellStyle name="计算 13" xfId="527" xr:uid="{00000000-0005-0000-0000-00000F020000}"/>
+    <cellStyle name="计算 14" xfId="528" xr:uid="{00000000-0005-0000-0000-000010020000}"/>
+    <cellStyle name="计算 15" xfId="529" xr:uid="{00000000-0005-0000-0000-000011020000}"/>
+    <cellStyle name="计算 16" xfId="530" xr:uid="{00000000-0005-0000-0000-000012020000}"/>
+    <cellStyle name="计算 17" xfId="531" xr:uid="{00000000-0005-0000-0000-000013020000}"/>
+    <cellStyle name="计算 18" xfId="532" xr:uid="{00000000-0005-0000-0000-000014020000}"/>
+    <cellStyle name="计算 19" xfId="533" xr:uid="{00000000-0005-0000-0000-000015020000}"/>
+    <cellStyle name="计算 2" xfId="534" xr:uid="{00000000-0005-0000-0000-000016020000}"/>
+    <cellStyle name="计算 20" xfId="535" xr:uid="{00000000-0005-0000-0000-000017020000}"/>
+    <cellStyle name="计算 3" xfId="536" xr:uid="{00000000-0005-0000-0000-000018020000}"/>
+    <cellStyle name="计算 4" xfId="537" xr:uid="{00000000-0005-0000-0000-000019020000}"/>
+    <cellStyle name="计算 5" xfId="538" xr:uid="{00000000-0005-0000-0000-00001A020000}"/>
+    <cellStyle name="计算 6" xfId="539" xr:uid="{00000000-0005-0000-0000-00001B020000}"/>
+    <cellStyle name="计算 7" xfId="540" xr:uid="{00000000-0005-0000-0000-00001C020000}"/>
+    <cellStyle name="计算 8" xfId="541" xr:uid="{00000000-0005-0000-0000-00001D020000}"/>
+    <cellStyle name="计算 9" xfId="542" xr:uid="{00000000-0005-0000-0000-00001E020000}"/>
     <cellStyle name="检查单元格" xfId="543" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="检查单元格 10" xfId="544"/>
-    <cellStyle name="检查单元格 11" xfId="545"/>
-    <cellStyle name="检查单元格 12" xfId="546"/>
-    <cellStyle name="检查单元格 13" xfId="547"/>
-    <cellStyle name="检查单元格 14" xfId="548"/>
-    <cellStyle name="检查单元格 15" xfId="549"/>
-    <cellStyle name="检查单元格 16" xfId="550"/>
-    <cellStyle name="检查单元格 17" xfId="551"/>
-    <cellStyle name="检查单元格 18" xfId="552"/>
-    <cellStyle name="检查单元格 19" xfId="553"/>
-    <cellStyle name="检查单元格 2" xfId="554"/>
-    <cellStyle name="检查单元格 20" xfId="555"/>
-    <cellStyle name="检查单元格 3" xfId="556"/>
-    <cellStyle name="检查单元格 4" xfId="557"/>
-    <cellStyle name="检查单元格 5" xfId="558"/>
-    <cellStyle name="检查单元格 6" xfId="559"/>
-    <cellStyle name="检查单元格 7" xfId="560"/>
-    <cellStyle name="检查单元格 8" xfId="561"/>
-    <cellStyle name="检查单元格 9" xfId="562"/>
+    <cellStyle name="检查单元格 10" xfId="544" xr:uid="{00000000-0005-0000-0000-000020020000}"/>
+    <cellStyle name="检查单元格 11" xfId="545" xr:uid="{00000000-0005-0000-0000-000021020000}"/>
+    <cellStyle name="检查单元格 12" xfId="546" xr:uid="{00000000-0005-0000-0000-000022020000}"/>
+    <cellStyle name="检查单元格 13" xfId="547" xr:uid="{00000000-0005-0000-0000-000023020000}"/>
+    <cellStyle name="检查单元格 14" xfId="548" xr:uid="{00000000-0005-0000-0000-000024020000}"/>
+    <cellStyle name="检查单元格 15" xfId="549" xr:uid="{00000000-0005-0000-0000-000025020000}"/>
+    <cellStyle name="检查单元格 16" xfId="550" xr:uid="{00000000-0005-0000-0000-000026020000}"/>
+    <cellStyle name="检查单元格 17" xfId="551" xr:uid="{00000000-0005-0000-0000-000027020000}"/>
+    <cellStyle name="检查单元格 18" xfId="552" xr:uid="{00000000-0005-0000-0000-000028020000}"/>
+    <cellStyle name="检查单元格 19" xfId="553" xr:uid="{00000000-0005-0000-0000-000029020000}"/>
+    <cellStyle name="检查单元格 2" xfId="554" xr:uid="{00000000-0005-0000-0000-00002A020000}"/>
+    <cellStyle name="检查单元格 20" xfId="555" xr:uid="{00000000-0005-0000-0000-00002B020000}"/>
+    <cellStyle name="检查单元格 3" xfId="556" xr:uid="{00000000-0005-0000-0000-00002C020000}"/>
+    <cellStyle name="检查单元格 4" xfId="557" xr:uid="{00000000-0005-0000-0000-00002D020000}"/>
+    <cellStyle name="检查单元格 5" xfId="558" xr:uid="{00000000-0005-0000-0000-00002E020000}"/>
+    <cellStyle name="检查单元格 6" xfId="559" xr:uid="{00000000-0005-0000-0000-00002F020000}"/>
+    <cellStyle name="检查单元格 7" xfId="560" xr:uid="{00000000-0005-0000-0000-000030020000}"/>
+    <cellStyle name="检查单元格 8" xfId="561" xr:uid="{00000000-0005-0000-0000-000031020000}"/>
+    <cellStyle name="检查单元格 9" xfId="562" xr:uid="{00000000-0005-0000-0000-000032020000}"/>
     <cellStyle name="解释性文本" xfId="563" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="解释性文本 10" xfId="564"/>
-    <cellStyle name="解释性文本 11" xfId="565"/>
-    <cellStyle name="解释性文本 12" xfId="566"/>
-    <cellStyle name="解释性文本 13" xfId="567"/>
-    <cellStyle name="解释性文本 14" xfId="568"/>
-    <cellStyle name="解释性文本 15" xfId="569"/>
-    <cellStyle name="解释性文本 16" xfId="570"/>
-    <cellStyle name="解释性文本 17" xfId="571"/>
-    <cellStyle name="解释性文本 18" xfId="572"/>
-    <cellStyle name="解释性文本 19" xfId="573"/>
-    <cellStyle name="解释性文本 2" xfId="574"/>
-    <cellStyle name="解释性文本 20" xfId="575"/>
-    <cellStyle name="解释性文本 3" xfId="576"/>
-    <cellStyle name="解释性文本 4" xfId="577"/>
-    <cellStyle name="解释性文本 5" xfId="578"/>
-    <cellStyle name="解释性文本 6" xfId="579"/>
-    <cellStyle name="解释性文本 7" xfId="580"/>
-    <cellStyle name="解释性文本 8" xfId="581"/>
-    <cellStyle name="解释性文本 9" xfId="582"/>
+    <cellStyle name="解释性文本 10" xfId="564" xr:uid="{00000000-0005-0000-0000-000034020000}"/>
+    <cellStyle name="解释性文本 11" xfId="565" xr:uid="{00000000-0005-0000-0000-000035020000}"/>
+    <cellStyle name="解释性文本 12" xfId="566" xr:uid="{00000000-0005-0000-0000-000036020000}"/>
+    <cellStyle name="解释性文本 13" xfId="567" xr:uid="{00000000-0005-0000-0000-000037020000}"/>
+    <cellStyle name="解释性文本 14" xfId="568" xr:uid="{00000000-0005-0000-0000-000038020000}"/>
+    <cellStyle name="解释性文本 15" xfId="569" xr:uid="{00000000-0005-0000-0000-000039020000}"/>
+    <cellStyle name="解释性文本 16" xfId="570" xr:uid="{00000000-0005-0000-0000-00003A020000}"/>
+    <cellStyle name="解释性文本 17" xfId="571" xr:uid="{00000000-0005-0000-0000-00003B020000}"/>
+    <cellStyle name="解释性文本 18" xfId="572" xr:uid="{00000000-0005-0000-0000-00003C020000}"/>
+    <cellStyle name="解释性文本 19" xfId="573" xr:uid="{00000000-0005-0000-0000-00003D020000}"/>
+    <cellStyle name="解释性文本 2" xfId="574" xr:uid="{00000000-0005-0000-0000-00003E020000}"/>
+    <cellStyle name="解释性文本 20" xfId="575" xr:uid="{00000000-0005-0000-0000-00003F020000}"/>
+    <cellStyle name="解释性文本 3" xfId="576" xr:uid="{00000000-0005-0000-0000-000040020000}"/>
+    <cellStyle name="解释性文本 4" xfId="577" xr:uid="{00000000-0005-0000-0000-000041020000}"/>
+    <cellStyle name="解释性文本 5" xfId="578" xr:uid="{00000000-0005-0000-0000-000042020000}"/>
+    <cellStyle name="解释性文本 6" xfId="579" xr:uid="{00000000-0005-0000-0000-000043020000}"/>
+    <cellStyle name="解释性文本 7" xfId="580" xr:uid="{00000000-0005-0000-0000-000044020000}"/>
+    <cellStyle name="解释性文本 8" xfId="581" xr:uid="{00000000-0005-0000-0000-000045020000}"/>
+    <cellStyle name="解释性文本 9" xfId="582" xr:uid="{00000000-0005-0000-0000-000046020000}"/>
     <cellStyle name="警告文本" xfId="583" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="警告文本 10" xfId="584"/>
-    <cellStyle name="警告文本 11" xfId="585"/>
-    <cellStyle name="警告文本 12" xfId="586"/>
-    <cellStyle name="警告文本 13" xfId="587"/>
-    <cellStyle name="警告文本 14" xfId="588"/>
-    <cellStyle name="警告文本 15" xfId="589"/>
-    <cellStyle name="警告文本 16" xfId="590"/>
-    <cellStyle name="警告文本 17" xfId="591"/>
-    <cellStyle name="警告文本 18" xfId="592"/>
-    <cellStyle name="警告文本 19" xfId="593"/>
-    <cellStyle name="警告文本 2" xfId="594"/>
-    <cellStyle name="警告文本 20" xfId="595"/>
-    <cellStyle name="警告文本 3" xfId="596"/>
-    <cellStyle name="警告文本 4" xfId="597"/>
-    <cellStyle name="警告文本 5" xfId="598"/>
-    <cellStyle name="警告文本 6" xfId="599"/>
-    <cellStyle name="警告文本 7" xfId="600"/>
-    <cellStyle name="警告文本 8" xfId="601"/>
-    <cellStyle name="警告文本 9" xfId="602"/>
+    <cellStyle name="警告文本 10" xfId="584" xr:uid="{00000000-0005-0000-0000-000048020000}"/>
+    <cellStyle name="警告文本 11" xfId="585" xr:uid="{00000000-0005-0000-0000-000049020000}"/>
+    <cellStyle name="警告文本 12" xfId="586" xr:uid="{00000000-0005-0000-0000-00004A020000}"/>
+    <cellStyle name="警告文本 13" xfId="587" xr:uid="{00000000-0005-0000-0000-00004B020000}"/>
+    <cellStyle name="警告文本 14" xfId="588" xr:uid="{00000000-0005-0000-0000-00004C020000}"/>
+    <cellStyle name="警告文本 15" xfId="589" xr:uid="{00000000-0005-0000-0000-00004D020000}"/>
+    <cellStyle name="警告文本 16" xfId="590" xr:uid="{00000000-0005-0000-0000-00004E020000}"/>
+    <cellStyle name="警告文本 17" xfId="591" xr:uid="{00000000-0005-0000-0000-00004F020000}"/>
+    <cellStyle name="警告文本 18" xfId="592" xr:uid="{00000000-0005-0000-0000-000050020000}"/>
+    <cellStyle name="警告文本 19" xfId="593" xr:uid="{00000000-0005-0000-0000-000051020000}"/>
+    <cellStyle name="警告文本 2" xfId="594" xr:uid="{00000000-0005-0000-0000-000052020000}"/>
+    <cellStyle name="警告文本 20" xfId="595" xr:uid="{00000000-0005-0000-0000-000053020000}"/>
+    <cellStyle name="警告文本 3" xfId="596" xr:uid="{00000000-0005-0000-0000-000054020000}"/>
+    <cellStyle name="警告文本 4" xfId="597" xr:uid="{00000000-0005-0000-0000-000055020000}"/>
+    <cellStyle name="警告文本 5" xfId="598" xr:uid="{00000000-0005-0000-0000-000056020000}"/>
+    <cellStyle name="警告文本 6" xfId="599" xr:uid="{00000000-0005-0000-0000-000057020000}"/>
+    <cellStyle name="警告文本 7" xfId="600" xr:uid="{00000000-0005-0000-0000-000058020000}"/>
+    <cellStyle name="警告文本 8" xfId="601" xr:uid="{00000000-0005-0000-0000-000059020000}"/>
+    <cellStyle name="警告文本 9" xfId="602" xr:uid="{00000000-0005-0000-0000-00005A020000}"/>
     <cellStyle name="链接单元格" xfId="603" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="链接单元格 10" xfId="604"/>
-    <cellStyle name="链接单元格 11" xfId="605"/>
-    <cellStyle name="链接单元格 12" xfId="606"/>
-    <cellStyle name="链接单元格 13" xfId="607"/>
-    <cellStyle name="链接单元格 14" xfId="608"/>
-    <cellStyle name="链接单元格 15" xfId="609"/>
-    <cellStyle name="链接单元格 16" xfId="610"/>
-    <cellStyle name="链接单元格 17" xfId="611"/>
-    <cellStyle name="链接单元格 18" xfId="612"/>
-    <cellStyle name="链接单元格 19" xfId="613"/>
-    <cellStyle name="链接单元格 2" xfId="614"/>
-    <cellStyle name="链接单元格 20" xfId="615"/>
-    <cellStyle name="链接单元格 3" xfId="616"/>
-    <cellStyle name="链接单元格 4" xfId="617"/>
-    <cellStyle name="链接单元格 5" xfId="618"/>
-    <cellStyle name="链接单元格 6" xfId="619"/>
-    <cellStyle name="链接单元格 7" xfId="620"/>
-    <cellStyle name="链接单元格 8" xfId="621"/>
-    <cellStyle name="链接单元格 9" xfId="622"/>
-    <cellStyle name="强调文字颜色 1 10" xfId="623"/>
-    <cellStyle name="强调文字颜色 1 11" xfId="624"/>
-    <cellStyle name="强调文字颜色 1 12" xfId="625"/>
-    <cellStyle name="强调文字颜色 1 13" xfId="626"/>
-    <cellStyle name="强调文字颜色 1 14" xfId="627"/>
-    <cellStyle name="强调文字颜色 1 15" xfId="628"/>
-    <cellStyle name="强调文字颜色 1 16" xfId="629"/>
-    <cellStyle name="强调文字颜色 1 17" xfId="630"/>
-    <cellStyle name="强调文字颜色 1 18" xfId="631"/>
-    <cellStyle name="强调文字颜色 1 19" xfId="632"/>
-    <cellStyle name="强调文字颜色 1 2" xfId="633"/>
-    <cellStyle name="强调文字颜色 1 20" xfId="634"/>
-    <cellStyle name="强调文字颜色 1 3" xfId="635"/>
-    <cellStyle name="强调文字颜色 1 4" xfId="636"/>
-    <cellStyle name="强调文字颜色 1 5" xfId="637"/>
-    <cellStyle name="强调文字颜色 1 6" xfId="638"/>
-    <cellStyle name="强调文字颜色 1 7" xfId="639"/>
-    <cellStyle name="强调文字颜色 1 8" xfId="640"/>
-    <cellStyle name="强调文字颜色 1 9" xfId="641"/>
-    <cellStyle name="强调文字颜色 2 10" xfId="642"/>
-    <cellStyle name="强调文字颜色 2 11" xfId="643"/>
-    <cellStyle name="强调文字颜色 2 12" xfId="644"/>
-    <cellStyle name="强调文字颜色 2 13" xfId="645"/>
-    <cellStyle name="强调文字颜色 2 14" xfId="646"/>
-    <cellStyle name="强调文字颜色 2 15" xfId="647"/>
-    <cellStyle name="强调文字颜色 2 16" xfId="648"/>
-    <cellStyle name="强调文字颜色 2 17" xfId="649"/>
-    <cellStyle name="强调文字颜色 2 18" xfId="650"/>
-    <cellStyle name="强调文字颜色 2 19" xfId="651"/>
-    <cellStyle name="强调文字颜色 2 2" xfId="652"/>
-    <cellStyle name="强调文字颜色 2 20" xfId="653"/>
-    <cellStyle name="强调文字颜色 2 3" xfId="654"/>
-    <cellStyle name="强调文字颜色 2 4" xfId="655"/>
-    <cellStyle name="强调文字颜色 2 5" xfId="656"/>
-    <cellStyle name="强调文字颜色 2 6" xfId="657"/>
-    <cellStyle name="强调文字颜色 2 7" xfId="658"/>
-    <cellStyle name="强调文字颜色 2 8" xfId="659"/>
-    <cellStyle name="强调文字颜色 2 9" xfId="660"/>
-    <cellStyle name="强调文字颜色 3 10" xfId="661"/>
-    <cellStyle name="强调文字颜色 3 11" xfId="662"/>
-    <cellStyle name="强调文字颜色 3 12" xfId="663"/>
-    <cellStyle name="强调文字颜色 3 13" xfId="664"/>
-    <cellStyle name="强调文字颜色 3 14" xfId="665"/>
-    <cellStyle name="强调文字颜色 3 15" xfId="666"/>
-    <cellStyle name="强调文字颜色 3 16" xfId="667"/>
-    <cellStyle name="强调文字颜色 3 17" xfId="668"/>
-    <cellStyle name="强调文字颜色 3 18" xfId="669"/>
-    <cellStyle name="强调文字颜色 3 19" xfId="670"/>
-    <cellStyle name="强调文字颜色 3 2" xfId="671"/>
-    <cellStyle name="强调文字颜色 3 20" xfId="672"/>
-    <cellStyle name="强调文字颜色 3 3" xfId="673"/>
-    <cellStyle name="强调文字颜色 3 4" xfId="674"/>
-    <cellStyle name="强调文字颜色 3 5" xfId="675"/>
-    <cellStyle name="强调文字颜色 3 6" xfId="676"/>
-    <cellStyle name="强调文字颜色 3 7" xfId="677"/>
-    <cellStyle name="强调文字颜色 3 8" xfId="678"/>
-    <cellStyle name="强调文字颜色 3 9" xfId="679"/>
-    <cellStyle name="强调文字颜色 4 10" xfId="680"/>
-    <cellStyle name="强调文字颜色 4 11" xfId="681"/>
-    <cellStyle name="强调文字颜色 4 12" xfId="682"/>
-    <cellStyle name="强调文字颜色 4 13" xfId="683"/>
-    <cellStyle name="强调文字颜色 4 14" xfId="684"/>
-    <cellStyle name="强调文字颜色 4 15" xfId="685"/>
-    <cellStyle name="强调文字颜色 4 16" xfId="686"/>
-    <cellStyle name="强调文字颜色 4 17" xfId="687"/>
-    <cellStyle name="强调文字颜色 4 18" xfId="688"/>
-    <cellStyle name="强调文字颜色 4 19" xfId="689"/>
-    <cellStyle name="强调文字颜色 4 2" xfId="690"/>
-    <cellStyle name="强调文字颜色 4 20" xfId="691"/>
-    <cellStyle name="强调文字颜色 4 3" xfId="692"/>
-    <cellStyle name="强调文字颜色 4 4" xfId="693"/>
-    <cellStyle name="强调文字颜色 4 5" xfId="694"/>
-    <cellStyle name="强调文字颜色 4 6" xfId="695"/>
-    <cellStyle name="强调文字颜色 4 7" xfId="696"/>
-    <cellStyle name="强调文字颜色 4 8" xfId="697"/>
-    <cellStyle name="强调文字颜色 4 9" xfId="698"/>
-    <cellStyle name="强调文字颜色 5 10" xfId="699"/>
-    <cellStyle name="强调文字颜色 5 11" xfId="700"/>
-    <cellStyle name="强调文字颜色 5 12" xfId="701"/>
-    <cellStyle name="强调文字颜色 5 13" xfId="702"/>
-    <cellStyle name="强调文字颜色 5 14" xfId="703"/>
-    <cellStyle name="强调文字颜色 5 15" xfId="704"/>
-    <cellStyle name="强调文字颜色 5 16" xfId="705"/>
-    <cellStyle name="强调文字颜色 5 17" xfId="706"/>
-    <cellStyle name="强调文字颜色 5 18" xfId="707"/>
-    <cellStyle name="强调文字颜色 5 19" xfId="708"/>
-    <cellStyle name="强调文字颜色 5 2" xfId="709"/>
-    <cellStyle name="强调文字颜色 5 20" xfId="710"/>
-    <cellStyle name="强调文字颜色 5 3" xfId="711"/>
-    <cellStyle name="强调文字颜色 5 4" xfId="712"/>
-    <cellStyle name="强调文字颜色 5 5" xfId="713"/>
-    <cellStyle name="强调文字颜色 5 6" xfId="714"/>
-    <cellStyle name="强调文字颜色 5 7" xfId="715"/>
-    <cellStyle name="强调文字颜色 5 8" xfId="716"/>
-    <cellStyle name="强调文字颜色 5 9" xfId="717"/>
-    <cellStyle name="强调文字颜色 6 10" xfId="718"/>
-    <cellStyle name="强调文字颜色 6 11" xfId="719"/>
-    <cellStyle name="强调文字颜色 6 12" xfId="720"/>
-    <cellStyle name="强调文字颜色 6 13" xfId="721"/>
-    <cellStyle name="强调文字颜色 6 14" xfId="722"/>
-    <cellStyle name="强调文字颜色 6 15" xfId="723"/>
-    <cellStyle name="强调文字颜色 6 16" xfId="724"/>
-    <cellStyle name="强调文字颜色 6 17" xfId="725"/>
-    <cellStyle name="强调文字颜色 6 18" xfId="726"/>
-    <cellStyle name="强调文字颜色 6 19" xfId="727"/>
-    <cellStyle name="强调文字颜色 6 2" xfId="728"/>
-    <cellStyle name="强调文字颜色 6 20" xfId="729"/>
-    <cellStyle name="强调文字颜色 6 3" xfId="730"/>
-    <cellStyle name="强调文字颜色 6 4" xfId="731"/>
-    <cellStyle name="强调文字颜色 6 5" xfId="732"/>
-    <cellStyle name="强调文字颜色 6 6" xfId="733"/>
-    <cellStyle name="强调文字颜色 6 7" xfId="734"/>
-    <cellStyle name="强调文字颜色 6 8" xfId="735"/>
-    <cellStyle name="强调文字颜色 6 9" xfId="736"/>
+    <cellStyle name="链接单元格 10" xfId="604" xr:uid="{00000000-0005-0000-0000-00005C020000}"/>
+    <cellStyle name="链接单元格 11" xfId="605" xr:uid="{00000000-0005-0000-0000-00005D020000}"/>
+    <cellStyle name="链接单元格 12" xfId="606" xr:uid="{00000000-0005-0000-0000-00005E020000}"/>
+    <cellStyle name="链接单元格 13" xfId="607" xr:uid="{00000000-0005-0000-0000-00005F020000}"/>
+    <cellStyle name="链接单元格 14" xfId="608" xr:uid="{00000000-0005-0000-0000-000060020000}"/>
+    <cellStyle name="链接单元格 15" xfId="609" xr:uid="{00000000-0005-0000-0000-000061020000}"/>
+    <cellStyle name="链接单元格 16" xfId="610" xr:uid="{00000000-0005-0000-0000-000062020000}"/>
+    <cellStyle name="链接单元格 17" xfId="611" xr:uid="{00000000-0005-0000-0000-000063020000}"/>
+    <cellStyle name="链接单元格 18" xfId="612" xr:uid="{00000000-0005-0000-0000-000064020000}"/>
+    <cellStyle name="链接单元格 19" xfId="613" xr:uid="{00000000-0005-0000-0000-000065020000}"/>
+    <cellStyle name="链接单元格 2" xfId="614" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
+    <cellStyle name="链接单元格 20" xfId="615" xr:uid="{00000000-0005-0000-0000-000067020000}"/>
+    <cellStyle name="链接单元格 3" xfId="616" xr:uid="{00000000-0005-0000-0000-000068020000}"/>
+    <cellStyle name="链接单元格 4" xfId="617" xr:uid="{00000000-0005-0000-0000-000069020000}"/>
+    <cellStyle name="链接单元格 5" xfId="618" xr:uid="{00000000-0005-0000-0000-00006A020000}"/>
+    <cellStyle name="链接单元格 6" xfId="619" xr:uid="{00000000-0005-0000-0000-00006B020000}"/>
+    <cellStyle name="链接单元格 7" xfId="620" xr:uid="{00000000-0005-0000-0000-00006C020000}"/>
+    <cellStyle name="链接单元格 8" xfId="621" xr:uid="{00000000-0005-0000-0000-00006D020000}"/>
+    <cellStyle name="链接单元格 9" xfId="622" xr:uid="{00000000-0005-0000-0000-00006E020000}"/>
+    <cellStyle name="强调文字颜色 1 10" xfId="623" xr:uid="{00000000-0005-0000-0000-00006F020000}"/>
+    <cellStyle name="强调文字颜色 1 11" xfId="624" xr:uid="{00000000-0005-0000-0000-000070020000}"/>
+    <cellStyle name="强调文字颜色 1 12" xfId="625" xr:uid="{00000000-0005-0000-0000-000071020000}"/>
+    <cellStyle name="强调文字颜色 1 13" xfId="626" xr:uid="{00000000-0005-0000-0000-000072020000}"/>
+    <cellStyle name="强调文字颜色 1 14" xfId="627" xr:uid="{00000000-0005-0000-0000-000073020000}"/>
+    <cellStyle name="强调文字颜色 1 15" xfId="628" xr:uid="{00000000-0005-0000-0000-000074020000}"/>
+    <cellStyle name="强调文字颜色 1 16" xfId="629" xr:uid="{00000000-0005-0000-0000-000075020000}"/>
+    <cellStyle name="强调文字颜色 1 17" xfId="630" xr:uid="{00000000-0005-0000-0000-000076020000}"/>
+    <cellStyle name="强调文字颜色 1 18" xfId="631" xr:uid="{00000000-0005-0000-0000-000077020000}"/>
+    <cellStyle name="强调文字颜色 1 19" xfId="632" xr:uid="{00000000-0005-0000-0000-000078020000}"/>
+    <cellStyle name="强调文字颜色 1 2" xfId="633" xr:uid="{00000000-0005-0000-0000-000079020000}"/>
+    <cellStyle name="强调文字颜色 1 20" xfId="634" xr:uid="{00000000-0005-0000-0000-00007A020000}"/>
+    <cellStyle name="强调文字颜色 1 3" xfId="635" xr:uid="{00000000-0005-0000-0000-00007B020000}"/>
+    <cellStyle name="强调文字颜色 1 4" xfId="636" xr:uid="{00000000-0005-0000-0000-00007C020000}"/>
+    <cellStyle name="强调文字颜色 1 5" xfId="637" xr:uid="{00000000-0005-0000-0000-00007D020000}"/>
+    <cellStyle name="强调文字颜色 1 6" xfId="638" xr:uid="{00000000-0005-0000-0000-00007E020000}"/>
+    <cellStyle name="强调文字颜色 1 7" xfId="639" xr:uid="{00000000-0005-0000-0000-00007F020000}"/>
+    <cellStyle name="强调文字颜色 1 8" xfId="640" xr:uid="{00000000-0005-0000-0000-000080020000}"/>
+    <cellStyle name="强调文字颜色 1 9" xfId="641" xr:uid="{00000000-0005-0000-0000-000081020000}"/>
+    <cellStyle name="强调文字颜色 2 10" xfId="642" xr:uid="{00000000-0005-0000-0000-000082020000}"/>
+    <cellStyle name="强调文字颜色 2 11" xfId="643" xr:uid="{00000000-0005-0000-0000-000083020000}"/>
+    <cellStyle name="强调文字颜色 2 12" xfId="644" xr:uid="{00000000-0005-0000-0000-000084020000}"/>
+    <cellStyle name="强调文字颜色 2 13" xfId="645" xr:uid="{00000000-0005-0000-0000-000085020000}"/>
+    <cellStyle name="强调文字颜色 2 14" xfId="646" xr:uid="{00000000-0005-0000-0000-000086020000}"/>
+    <cellStyle name="强调文字颜色 2 15" xfId="647" xr:uid="{00000000-0005-0000-0000-000087020000}"/>
+    <cellStyle name="强调文字颜色 2 16" xfId="648" xr:uid="{00000000-0005-0000-0000-000088020000}"/>
+    <cellStyle name="强调文字颜色 2 17" xfId="649" xr:uid="{00000000-0005-0000-0000-000089020000}"/>
+    <cellStyle name="强调文字颜色 2 18" xfId="650" xr:uid="{00000000-0005-0000-0000-00008A020000}"/>
+    <cellStyle name="强调文字颜色 2 19" xfId="651" xr:uid="{00000000-0005-0000-0000-00008B020000}"/>
+    <cellStyle name="强调文字颜色 2 2" xfId="652" xr:uid="{00000000-0005-0000-0000-00008C020000}"/>
+    <cellStyle name="强调文字颜色 2 20" xfId="653" xr:uid="{00000000-0005-0000-0000-00008D020000}"/>
+    <cellStyle name="强调文字颜色 2 3" xfId="654" xr:uid="{00000000-0005-0000-0000-00008E020000}"/>
+    <cellStyle name="强调文字颜色 2 4" xfId="655" xr:uid="{00000000-0005-0000-0000-00008F020000}"/>
+    <cellStyle name="强调文字颜色 2 5" xfId="656" xr:uid="{00000000-0005-0000-0000-000090020000}"/>
+    <cellStyle name="强调文字颜色 2 6" xfId="657" xr:uid="{00000000-0005-0000-0000-000091020000}"/>
+    <cellStyle name="强调文字颜色 2 7" xfId="658" xr:uid="{00000000-0005-0000-0000-000092020000}"/>
+    <cellStyle name="强调文字颜色 2 8" xfId="659" xr:uid="{00000000-0005-0000-0000-000093020000}"/>
+    <cellStyle name="强调文字颜色 2 9" xfId="660" xr:uid="{00000000-0005-0000-0000-000094020000}"/>
+    <cellStyle name="强调文字颜色 3 10" xfId="661" xr:uid="{00000000-0005-0000-0000-000095020000}"/>
+    <cellStyle name="强调文字颜色 3 11" xfId="662" xr:uid="{00000000-0005-0000-0000-000096020000}"/>
+    <cellStyle name="强调文字颜色 3 12" xfId="663" xr:uid="{00000000-0005-0000-0000-000097020000}"/>
+    <cellStyle name="强调文字颜色 3 13" xfId="664" xr:uid="{00000000-0005-0000-0000-000098020000}"/>
+    <cellStyle name="强调文字颜色 3 14" xfId="665" xr:uid="{00000000-0005-0000-0000-000099020000}"/>
+    <cellStyle name="强调文字颜色 3 15" xfId="666" xr:uid="{00000000-0005-0000-0000-00009A020000}"/>
+    <cellStyle name="强调文字颜色 3 16" xfId="667" xr:uid="{00000000-0005-0000-0000-00009B020000}"/>
+    <cellStyle name="强调文字颜色 3 17" xfId="668" xr:uid="{00000000-0005-0000-0000-00009C020000}"/>
+    <cellStyle name="强调文字颜色 3 18" xfId="669" xr:uid="{00000000-0005-0000-0000-00009D020000}"/>
+    <cellStyle name="强调文字颜色 3 19" xfId="670" xr:uid="{00000000-0005-0000-0000-00009E020000}"/>
+    <cellStyle name="强调文字颜色 3 2" xfId="671" xr:uid="{00000000-0005-0000-0000-00009F020000}"/>
+    <cellStyle name="强调文字颜色 3 20" xfId="672" xr:uid="{00000000-0005-0000-0000-0000A0020000}"/>
+    <cellStyle name="强调文字颜色 3 3" xfId="673" xr:uid="{00000000-0005-0000-0000-0000A1020000}"/>
+    <cellStyle name="强调文字颜色 3 4" xfId="674" xr:uid="{00000000-0005-0000-0000-0000A2020000}"/>
+    <cellStyle name="强调文字颜色 3 5" xfId="675" xr:uid="{00000000-0005-0000-0000-0000A3020000}"/>
+    <cellStyle name="强调文字颜色 3 6" xfId="676" xr:uid="{00000000-0005-0000-0000-0000A4020000}"/>
+    <cellStyle name="强调文字颜色 3 7" xfId="677" xr:uid="{00000000-0005-0000-0000-0000A5020000}"/>
+    <cellStyle name="强调文字颜色 3 8" xfId="678" xr:uid="{00000000-0005-0000-0000-0000A6020000}"/>
+    <cellStyle name="强调文字颜色 3 9" xfId="679" xr:uid="{00000000-0005-0000-0000-0000A7020000}"/>
+    <cellStyle name="强调文字颜色 4 10" xfId="680" xr:uid="{00000000-0005-0000-0000-0000A8020000}"/>
+    <cellStyle name="强调文字颜色 4 11" xfId="681" xr:uid="{00000000-0005-0000-0000-0000A9020000}"/>
+    <cellStyle name="强调文字颜色 4 12" xfId="682" xr:uid="{00000000-0005-0000-0000-0000AA020000}"/>
+    <cellStyle name="强调文字颜色 4 13" xfId="683" xr:uid="{00000000-0005-0000-0000-0000AB020000}"/>
+    <cellStyle name="强调文字颜色 4 14" xfId="684" xr:uid="{00000000-0005-0000-0000-0000AC020000}"/>
+    <cellStyle name="强调文字颜色 4 15" xfId="685" xr:uid="{00000000-0005-0000-0000-0000AD020000}"/>
+    <cellStyle name="强调文字颜色 4 16" xfId="686" xr:uid="{00000000-0005-0000-0000-0000AE020000}"/>
+    <cellStyle name="强调文字颜色 4 17" xfId="687" xr:uid="{00000000-0005-0000-0000-0000AF020000}"/>
+    <cellStyle name="强调文字颜色 4 18" xfId="688" xr:uid="{00000000-0005-0000-0000-0000B0020000}"/>
+    <cellStyle name="强调文字颜色 4 19" xfId="689" xr:uid="{00000000-0005-0000-0000-0000B1020000}"/>
+    <cellStyle name="强调文字颜色 4 2" xfId="690" xr:uid="{00000000-0005-0000-0000-0000B2020000}"/>
+    <cellStyle name="强调文字颜色 4 20" xfId="691" xr:uid="{00000000-0005-0000-0000-0000B3020000}"/>
+    <cellStyle name="强调文字颜色 4 3" xfId="692" xr:uid="{00000000-0005-0000-0000-0000B4020000}"/>
+    <cellStyle name="强调文字颜色 4 4" xfId="693" xr:uid="{00000000-0005-0000-0000-0000B5020000}"/>
+    <cellStyle name="强调文字颜色 4 5" xfId="694" xr:uid="{00000000-0005-0000-0000-0000B6020000}"/>
+    <cellStyle name="强调文字颜色 4 6" xfId="695" xr:uid="{00000000-0005-0000-0000-0000B7020000}"/>
+    <cellStyle name="强调文字颜色 4 7" xfId="696" xr:uid="{00000000-0005-0000-0000-0000B8020000}"/>
+    <cellStyle name="强调文字颜色 4 8" xfId="697" xr:uid="{00000000-0005-0000-0000-0000B9020000}"/>
+    <cellStyle name="强调文字颜色 4 9" xfId="698" xr:uid="{00000000-0005-0000-0000-0000BA020000}"/>
+    <cellStyle name="强调文字颜色 5 10" xfId="699" xr:uid="{00000000-0005-0000-0000-0000BB020000}"/>
+    <cellStyle name="强调文字颜色 5 11" xfId="700" xr:uid="{00000000-0005-0000-0000-0000BC020000}"/>
+    <cellStyle name="强调文字颜色 5 12" xfId="701" xr:uid="{00000000-0005-0000-0000-0000BD020000}"/>
+    <cellStyle name="强调文字颜色 5 13" xfId="702" xr:uid="{00000000-0005-0000-0000-0000BE020000}"/>
+    <cellStyle name="强调文字颜色 5 14" xfId="703" xr:uid="{00000000-0005-0000-0000-0000BF020000}"/>
+    <cellStyle name="强调文字颜色 5 15" xfId="704" xr:uid="{00000000-0005-0000-0000-0000C0020000}"/>
+    <cellStyle name="强调文字颜色 5 16" xfId="705" xr:uid="{00000000-0005-0000-0000-0000C1020000}"/>
+    <cellStyle name="强调文字颜色 5 17" xfId="706" xr:uid="{00000000-0005-0000-0000-0000C2020000}"/>
+    <cellStyle name="强调文字颜色 5 18" xfId="707" xr:uid="{00000000-0005-0000-0000-0000C3020000}"/>
+    <cellStyle name="强调文字颜色 5 19" xfId="708" xr:uid="{00000000-0005-0000-0000-0000C4020000}"/>
+    <cellStyle name="强调文字颜色 5 2" xfId="709" xr:uid="{00000000-0005-0000-0000-0000C5020000}"/>
+    <cellStyle name="强调文字颜色 5 20" xfId="710" xr:uid="{00000000-0005-0000-0000-0000C6020000}"/>
+    <cellStyle name="强调文字颜色 5 3" xfId="711" xr:uid="{00000000-0005-0000-0000-0000C7020000}"/>
+    <cellStyle name="强调文字颜色 5 4" xfId="712" xr:uid="{00000000-0005-0000-0000-0000C8020000}"/>
+    <cellStyle name="强调文字颜色 5 5" xfId="713" xr:uid="{00000000-0005-0000-0000-0000C9020000}"/>
+    <cellStyle name="强调文字颜色 5 6" xfId="714" xr:uid="{00000000-0005-0000-0000-0000CA020000}"/>
+    <cellStyle name="强调文字颜色 5 7" xfId="715" xr:uid="{00000000-0005-0000-0000-0000CB020000}"/>
+    <cellStyle name="强调文字颜色 5 8" xfId="716" xr:uid="{00000000-0005-0000-0000-0000CC020000}"/>
+    <cellStyle name="强调文字颜色 5 9" xfId="717" xr:uid="{00000000-0005-0000-0000-0000CD020000}"/>
+    <cellStyle name="强调文字颜色 6 10" xfId="718" xr:uid="{00000000-0005-0000-0000-0000CE020000}"/>
+    <cellStyle name="强调文字颜色 6 11" xfId="719" xr:uid="{00000000-0005-0000-0000-0000CF020000}"/>
+    <cellStyle name="强调文字颜色 6 12" xfId="720" xr:uid="{00000000-0005-0000-0000-0000D0020000}"/>
+    <cellStyle name="强调文字颜色 6 13" xfId="721" xr:uid="{00000000-0005-0000-0000-0000D1020000}"/>
+    <cellStyle name="强调文字颜色 6 14" xfId="722" xr:uid="{00000000-0005-0000-0000-0000D2020000}"/>
+    <cellStyle name="强调文字颜色 6 15" xfId="723" xr:uid="{00000000-0005-0000-0000-0000D3020000}"/>
+    <cellStyle name="强调文字颜色 6 16" xfId="724" xr:uid="{00000000-0005-0000-0000-0000D4020000}"/>
+    <cellStyle name="强调文字颜色 6 17" xfId="725" xr:uid="{00000000-0005-0000-0000-0000D5020000}"/>
+    <cellStyle name="强调文字颜色 6 18" xfId="726" xr:uid="{00000000-0005-0000-0000-0000D6020000}"/>
+    <cellStyle name="强调文字颜色 6 19" xfId="727" xr:uid="{00000000-0005-0000-0000-0000D7020000}"/>
+    <cellStyle name="强调文字颜色 6 2" xfId="728" xr:uid="{00000000-0005-0000-0000-0000D8020000}"/>
+    <cellStyle name="强调文字颜色 6 20" xfId="729" xr:uid="{00000000-0005-0000-0000-0000D9020000}"/>
+    <cellStyle name="强调文字颜色 6 3" xfId="730" xr:uid="{00000000-0005-0000-0000-0000DA020000}"/>
+    <cellStyle name="强调文字颜色 6 4" xfId="731" xr:uid="{00000000-0005-0000-0000-0000DB020000}"/>
+    <cellStyle name="强调文字颜色 6 5" xfId="732" xr:uid="{00000000-0005-0000-0000-0000DC020000}"/>
+    <cellStyle name="强调文字颜色 6 6" xfId="733" xr:uid="{00000000-0005-0000-0000-0000DD020000}"/>
+    <cellStyle name="强调文字颜色 6 7" xfId="734" xr:uid="{00000000-0005-0000-0000-0000DE020000}"/>
+    <cellStyle name="强调文字颜色 6 8" xfId="735" xr:uid="{00000000-0005-0000-0000-0000DF020000}"/>
+    <cellStyle name="强调文字颜色 6 9" xfId="736" xr:uid="{00000000-0005-0000-0000-0000E0020000}"/>
     <cellStyle name="适中" xfId="737" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="适中 10" xfId="738"/>
-    <cellStyle name="适中 11" xfId="739"/>
-    <cellStyle name="适中 12" xfId="740"/>
-    <cellStyle name="适中 13" xfId="741"/>
-    <cellStyle name="适中 14" xfId="742"/>
-    <cellStyle name="适中 15" xfId="743"/>
-    <cellStyle name="适中 16" xfId="744"/>
-    <cellStyle name="适中 17" xfId="745"/>
-    <cellStyle name="适中 18" xfId="746"/>
-    <cellStyle name="适中 19" xfId="747"/>
-    <cellStyle name="适中 2" xfId="748"/>
-    <cellStyle name="适中 20" xfId="749"/>
-    <cellStyle name="适中 3" xfId="750"/>
-    <cellStyle name="适中 4" xfId="751"/>
-    <cellStyle name="适中 5" xfId="752"/>
-    <cellStyle name="适中 6" xfId="753"/>
-    <cellStyle name="适中 7" xfId="754"/>
-    <cellStyle name="适中 8" xfId="755"/>
-    <cellStyle name="适中 9" xfId="756"/>
+    <cellStyle name="适中 10" xfId="738" xr:uid="{00000000-0005-0000-0000-0000E2020000}"/>
+    <cellStyle name="适中 11" xfId="739" xr:uid="{00000000-0005-0000-0000-0000E3020000}"/>
+    <cellStyle name="适中 12" xfId="740" xr:uid="{00000000-0005-0000-0000-0000E4020000}"/>
+    <cellStyle name="适中 13" xfId="741" xr:uid="{00000000-0005-0000-0000-0000E5020000}"/>
+    <cellStyle name="适中 14" xfId="742" xr:uid="{00000000-0005-0000-0000-0000E6020000}"/>
+    <cellStyle name="适中 15" xfId="743" xr:uid="{00000000-0005-0000-0000-0000E7020000}"/>
+    <cellStyle name="适中 16" xfId="744" xr:uid="{00000000-0005-0000-0000-0000E8020000}"/>
+    <cellStyle name="适中 17" xfId="745" xr:uid="{00000000-0005-0000-0000-0000E9020000}"/>
+    <cellStyle name="适中 18" xfId="746" xr:uid="{00000000-0005-0000-0000-0000EA020000}"/>
+    <cellStyle name="适中 19" xfId="747" xr:uid="{00000000-0005-0000-0000-0000EB020000}"/>
+    <cellStyle name="适中 2" xfId="748" xr:uid="{00000000-0005-0000-0000-0000EC020000}"/>
+    <cellStyle name="适中 20" xfId="749" xr:uid="{00000000-0005-0000-0000-0000ED020000}"/>
+    <cellStyle name="适中 3" xfId="750" xr:uid="{00000000-0005-0000-0000-0000EE020000}"/>
+    <cellStyle name="适中 4" xfId="751" xr:uid="{00000000-0005-0000-0000-0000EF020000}"/>
+    <cellStyle name="适中 5" xfId="752" xr:uid="{00000000-0005-0000-0000-0000F0020000}"/>
+    <cellStyle name="适中 6" xfId="753" xr:uid="{00000000-0005-0000-0000-0000F1020000}"/>
+    <cellStyle name="适中 7" xfId="754" xr:uid="{00000000-0005-0000-0000-0000F2020000}"/>
+    <cellStyle name="适中 8" xfId="755" xr:uid="{00000000-0005-0000-0000-0000F3020000}"/>
+    <cellStyle name="适中 9" xfId="756" xr:uid="{00000000-0005-0000-0000-0000F4020000}"/>
     <cellStyle name="输出" xfId="757" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="输出 10" xfId="758"/>
-    <cellStyle name="输出 11" xfId="759"/>
-    <cellStyle name="输出 12" xfId="760"/>
-    <cellStyle name="输出 13" xfId="761"/>
-    <cellStyle name="输出 14" xfId="762"/>
-    <cellStyle name="输出 15" xfId="763"/>
-    <cellStyle name="输出 16" xfId="764"/>
-    <cellStyle name="输出 17" xfId="765"/>
-    <cellStyle name="输出 18" xfId="766"/>
-    <cellStyle name="输出 19" xfId="767"/>
-    <cellStyle name="输出 2" xfId="768"/>
-    <cellStyle name="输出 20" xfId="769"/>
-    <cellStyle name="输出 3" xfId="770"/>
-    <cellStyle name="输出 4" xfId="771"/>
-    <cellStyle name="输出 5" xfId="772"/>
-    <cellStyle name="输出 6" xfId="773"/>
-    <cellStyle name="输出 7" xfId="774"/>
-    <cellStyle name="输出 8" xfId="775"/>
-    <cellStyle name="输出 9" xfId="776"/>
+    <cellStyle name="输出 10" xfId="758" xr:uid="{00000000-0005-0000-0000-0000F6020000}"/>
+    <cellStyle name="输出 11" xfId="759" xr:uid="{00000000-0005-0000-0000-0000F7020000}"/>
+    <cellStyle name="输出 12" xfId="760" xr:uid="{00000000-0005-0000-0000-0000F8020000}"/>
+    <cellStyle name="输出 13" xfId="761" xr:uid="{00000000-0005-0000-0000-0000F9020000}"/>
+    <cellStyle name="输出 14" xfId="762" xr:uid="{00000000-0005-0000-0000-0000FA020000}"/>
+    <cellStyle name="输出 15" xfId="763" xr:uid="{00000000-0005-0000-0000-0000FB020000}"/>
+    <cellStyle name="输出 16" xfId="764" xr:uid="{00000000-0005-0000-0000-0000FC020000}"/>
+    <cellStyle name="输出 17" xfId="765" xr:uid="{00000000-0005-0000-0000-0000FD020000}"/>
+    <cellStyle name="输出 18" xfId="766" xr:uid="{00000000-0005-0000-0000-0000FE020000}"/>
+    <cellStyle name="输出 19" xfId="767" xr:uid="{00000000-0005-0000-0000-0000FF020000}"/>
+    <cellStyle name="输出 2" xfId="768" xr:uid="{00000000-0005-0000-0000-000000030000}"/>
+    <cellStyle name="输出 20" xfId="769" xr:uid="{00000000-0005-0000-0000-000001030000}"/>
+    <cellStyle name="输出 3" xfId="770" xr:uid="{00000000-0005-0000-0000-000002030000}"/>
+    <cellStyle name="输出 4" xfId="771" xr:uid="{00000000-0005-0000-0000-000003030000}"/>
+    <cellStyle name="输出 5" xfId="772" xr:uid="{00000000-0005-0000-0000-000004030000}"/>
+    <cellStyle name="输出 6" xfId="773" xr:uid="{00000000-0005-0000-0000-000005030000}"/>
+    <cellStyle name="输出 7" xfId="774" xr:uid="{00000000-0005-0000-0000-000006030000}"/>
+    <cellStyle name="输出 8" xfId="775" xr:uid="{00000000-0005-0000-0000-000007030000}"/>
+    <cellStyle name="输出 9" xfId="776" xr:uid="{00000000-0005-0000-0000-000008030000}"/>
     <cellStyle name="输入" xfId="777" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="输入 10" xfId="778"/>
-    <cellStyle name="输入 11" xfId="779"/>
-    <cellStyle name="输入 12" xfId="780"/>
-    <cellStyle name="输入 13" xfId="781"/>
-    <cellStyle name="输入 14" xfId="782"/>
-    <cellStyle name="输入 15" xfId="783"/>
-    <cellStyle name="输入 16" xfId="784"/>
-    <cellStyle name="输入 17" xfId="785"/>
-    <cellStyle name="输入 18" xfId="786"/>
-    <cellStyle name="输入 19" xfId="787"/>
-    <cellStyle name="输入 2" xfId="788"/>
-    <cellStyle name="输入 20" xfId="789"/>
-    <cellStyle name="输入 3" xfId="790"/>
-    <cellStyle name="输入 4" xfId="791"/>
-    <cellStyle name="输入 5" xfId="792"/>
-    <cellStyle name="输入 6" xfId="793"/>
-    <cellStyle name="输入 7" xfId="794"/>
-    <cellStyle name="输入 8" xfId="795"/>
-    <cellStyle name="输入 9" xfId="796"/>
+    <cellStyle name="输入 10" xfId="778" xr:uid="{00000000-0005-0000-0000-00000A030000}"/>
+    <cellStyle name="输入 11" xfId="779" xr:uid="{00000000-0005-0000-0000-00000B030000}"/>
+    <cellStyle name="输入 12" xfId="780" xr:uid="{00000000-0005-0000-0000-00000C030000}"/>
+    <cellStyle name="输入 13" xfId="781" xr:uid="{00000000-0005-0000-0000-00000D030000}"/>
+    <cellStyle name="输入 14" xfId="782" xr:uid="{00000000-0005-0000-0000-00000E030000}"/>
+    <cellStyle name="输入 15" xfId="783" xr:uid="{00000000-0005-0000-0000-00000F030000}"/>
+    <cellStyle name="输入 16" xfId="784" xr:uid="{00000000-0005-0000-0000-000010030000}"/>
+    <cellStyle name="输入 17" xfId="785" xr:uid="{00000000-0005-0000-0000-000011030000}"/>
+    <cellStyle name="输入 18" xfId="786" xr:uid="{00000000-0005-0000-0000-000012030000}"/>
+    <cellStyle name="输入 19" xfId="787" xr:uid="{00000000-0005-0000-0000-000013030000}"/>
+    <cellStyle name="输入 2" xfId="788" xr:uid="{00000000-0005-0000-0000-000014030000}"/>
+    <cellStyle name="输入 20" xfId="789" xr:uid="{00000000-0005-0000-0000-000015030000}"/>
+    <cellStyle name="输入 3" xfId="790" xr:uid="{00000000-0005-0000-0000-000016030000}"/>
+    <cellStyle name="输入 4" xfId="791" xr:uid="{00000000-0005-0000-0000-000017030000}"/>
+    <cellStyle name="输入 5" xfId="792" xr:uid="{00000000-0005-0000-0000-000018030000}"/>
+    <cellStyle name="输入 6" xfId="793" xr:uid="{00000000-0005-0000-0000-000019030000}"/>
+    <cellStyle name="输入 7" xfId="794" xr:uid="{00000000-0005-0000-0000-00001A030000}"/>
+    <cellStyle name="输入 8" xfId="795" xr:uid="{00000000-0005-0000-0000-00001B030000}"/>
+    <cellStyle name="输入 9" xfId="796" xr:uid="{00000000-0005-0000-0000-00001C030000}"/>
     <cellStyle name="注释" xfId="797" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="注释 10" xfId="798"/>
-    <cellStyle name="注释 11" xfId="799"/>
-    <cellStyle name="注释 12" xfId="800"/>
-    <cellStyle name="注释 13" xfId="801"/>
-    <cellStyle name="注释 14" xfId="802"/>
-    <cellStyle name="注释 15" xfId="803"/>
-    <cellStyle name="注释 16" xfId="804"/>
-    <cellStyle name="注释 17" xfId="805"/>
-    <cellStyle name="注释 18" xfId="806"/>
-    <cellStyle name="注释 19" xfId="807"/>
-    <cellStyle name="注释 2" xfId="808"/>
-    <cellStyle name="注释 20" xfId="809"/>
-    <cellStyle name="注释 3" xfId="810"/>
-    <cellStyle name="注释 4" xfId="811"/>
-    <cellStyle name="注释 5" xfId="812"/>
-    <cellStyle name="注释 6" xfId="813"/>
-    <cellStyle name="注释 7" xfId="814"/>
-    <cellStyle name="注释 8" xfId="815"/>
-    <cellStyle name="注释 9" xfId="816"/>
+    <cellStyle name="注释 10" xfId="798" xr:uid="{00000000-0005-0000-0000-00001E030000}"/>
+    <cellStyle name="注释 11" xfId="799" xr:uid="{00000000-0005-0000-0000-00001F030000}"/>
+    <cellStyle name="注释 12" xfId="800" xr:uid="{00000000-0005-0000-0000-000020030000}"/>
+    <cellStyle name="注释 13" xfId="801" xr:uid="{00000000-0005-0000-0000-000021030000}"/>
+    <cellStyle name="注释 14" xfId="802" xr:uid="{00000000-0005-0000-0000-000022030000}"/>
+    <cellStyle name="注释 15" xfId="803" xr:uid="{00000000-0005-0000-0000-000023030000}"/>
+    <cellStyle name="注释 16" xfId="804" xr:uid="{00000000-0005-0000-0000-000024030000}"/>
+    <cellStyle name="注释 17" xfId="805" xr:uid="{00000000-0005-0000-0000-000025030000}"/>
+    <cellStyle name="注释 18" xfId="806" xr:uid="{00000000-0005-0000-0000-000026030000}"/>
+    <cellStyle name="注释 19" xfId="807" xr:uid="{00000000-0005-0000-0000-000027030000}"/>
+    <cellStyle name="注释 2" xfId="808" xr:uid="{00000000-0005-0000-0000-000028030000}"/>
+    <cellStyle name="注释 20" xfId="809" xr:uid="{00000000-0005-0000-0000-000029030000}"/>
+    <cellStyle name="注释 3" xfId="810" xr:uid="{00000000-0005-0000-0000-00002A030000}"/>
+    <cellStyle name="注释 4" xfId="811" xr:uid="{00000000-0005-0000-0000-00002B030000}"/>
+    <cellStyle name="注释 5" xfId="812" xr:uid="{00000000-0005-0000-0000-00002C030000}"/>
+    <cellStyle name="注释 6" xfId="813" xr:uid="{00000000-0005-0000-0000-00002D030000}"/>
+    <cellStyle name="注释 7" xfId="814" xr:uid="{00000000-0005-0000-0000-00002E030000}"/>
+    <cellStyle name="注释 8" xfId="815" xr:uid="{00000000-0005-0000-0000-00002F030000}"/>
+    <cellStyle name="注释 9" xfId="816" xr:uid="{00000000-0005-0000-0000-000030030000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -4028,7 +4216,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4103,6 +4291,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4138,6 +4343,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4313,12 +4535,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4332,14 +4552,15 @@
     <col min="8" max="8" width="22.125" customWidth="1"/>
     <col min="9" max="9" width="22.5" customWidth="1"/>
     <col min="10" max="10" width="21.375" customWidth="1"/>
+    <col min="12" max="13" width="23.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="81" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" ht="81" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
         <v>55</v>
       </c>
@@ -4371,8 +4592,17 @@
       <c r="K2" s="9" t="s">
         <v>64</v>
       </c>
+      <c r="L2" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>54</v>
       </c>
@@ -4404,7 +4634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>800001</v>
       </c>
@@ -4432,14 +4662,23 @@
       <c r="I4">
         <v>0</v>
       </c>
-      <c r="J4">
-        <v>0</v>
+      <c r="J4" s="11" t="s">
+        <v>124</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
+      <c r="L4" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>800002</v>
       </c>
@@ -4473,8 +4712,17 @@
       <c r="K5">
         <v>2</v>
       </c>
+      <c r="L5" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>800005</v>
       </c>
@@ -4508,8 +4756,17 @@
       <c r="K6">
         <v>3</v>
       </c>
+      <c r="L6" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>99</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>800011</v>
       </c>
@@ -4543,8 +4800,17 @@
       <c r="K7">
         <v>1</v>
       </c>
+      <c r="L7" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>800017</v>
       </c>
@@ -4578,8 +4844,17 @@
       <c r="K8">
         <v>2</v>
       </c>
+      <c r="L8" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>800018</v>
       </c>
@@ -4613,8 +4888,17 @@
       <c r="K9">
         <v>3</v>
       </c>
+      <c r="L9" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>800019</v>
       </c>
@@ -4648,8 +4932,17 @@
       <c r="K10">
         <v>1</v>
       </c>
+      <c r="L10" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>103</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>810001</v>
       </c>
@@ -4683,8 +4976,17 @@
       <c r="K11">
         <v>2</v>
       </c>
+      <c r="L11" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>810002</v>
       </c>
@@ -4718,8 +5020,17 @@
       <c r="K12">
         <v>3</v>
       </c>
+      <c r="L12" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="M12" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>810003</v>
       </c>
@@ -4753,8 +5064,17 @@
       <c r="K13">
         <v>1</v>
       </c>
+      <c r="L13" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M13" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="N13" s="10" t="s">
+        <v>106</v>
+      </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>810004</v>
       </c>
@@ -4788,8 +5108,17 @@
       <c r="K14">
         <v>2</v>
       </c>
+      <c r="L14" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="M14" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="N14" s="10" t="s">
+        <v>107</v>
+      </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>810005</v>
       </c>
@@ -4823,8 +5152,17 @@
       <c r="K15">
         <v>3</v>
       </c>
+      <c r="L15" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="M15" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="N15" s="10" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>810006</v>
       </c>
@@ -4858,8 +5196,17 @@
       <c r="K16">
         <v>1</v>
       </c>
+      <c r="L16" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="N16" s="10" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>810007</v>
       </c>
@@ -4893,8 +5240,17 @@
       <c r="K17">
         <v>2</v>
       </c>
+      <c r="L17" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="M17" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="N17" s="10" t="s">
+        <v>110</v>
+      </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>810008</v>
       </c>
@@ -4928,8 +5284,17 @@
       <c r="K18">
         <v>3</v>
       </c>
+      <c r="L18" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="M18" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="N18" s="10" t="s">
+        <v>111</v>
+      </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>810009</v>
       </c>
@@ -4963,8 +5328,17 @@
       <c r="K19">
         <v>1</v>
       </c>
+      <c r="L19" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="M19" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="N19" s="10" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>810010</v>
       </c>
@@ -4998,8 +5372,17 @@
       <c r="K20">
         <v>2</v>
       </c>
+      <c r="L20" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="M20" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="N20" s="10" t="s">
+        <v>113</v>
+      </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>810011</v>
       </c>
@@ -5033,8 +5416,17 @@
       <c r="K21">
         <v>3</v>
       </c>
+      <c r="L21" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="M21" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="N21" s="10" t="s">
+        <v>114</v>
+      </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>810012</v>
       </c>
@@ -5068,8 +5460,17 @@
       <c r="K22">
         <v>1</v>
       </c>
+      <c r="L22" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="M22" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="N22" s="10" t="s">
+        <v>115</v>
+      </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>810013</v>
       </c>
@@ -5103,8 +5504,17 @@
       <c r="K23">
         <v>2</v>
       </c>
+      <c r="L23" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="M23" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="N23" s="10" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>810014</v>
       </c>
@@ -5138,8 +5548,17 @@
       <c r="K24">
         <v>3</v>
       </c>
+      <c r="L24" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M24" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="N24" s="10" t="s">
+        <v>117</v>
+      </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>810015</v>
       </c>
@@ -5173,8 +5592,17 @@
       <c r="K25">
         <v>1</v>
       </c>
+      <c r="L25" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="M25" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="N25" s="10" t="s">
+        <v>118</v>
+      </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>810016</v>
       </c>
@@ -5208,8 +5636,17 @@
       <c r="K26">
         <v>2</v>
       </c>
+      <c r="L26" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="M26" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="N26" s="10" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>810017</v>
       </c>
@@ -5243,8 +5680,17 @@
       <c r="K27">
         <v>3</v>
       </c>
+      <c r="L27" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="M27" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="N27" s="10" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>810018</v>
       </c>
@@ -5278,8 +5724,17 @@
       <c r="K28">
         <v>1</v>
       </c>
+      <c r="L28" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="M28" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="N28" s="10" t="s">
+        <v>121</v>
+      </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>810019</v>
       </c>
@@ -5313,8 +5768,17 @@
       <c r="K29">
         <v>2</v>
       </c>
+      <c r="L29" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="M29" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="N29" s="10" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>810020</v>
       </c>
@@ -5347,6 +5811,15 @@
       </c>
       <c r="K30">
         <v>3</v>
+      </c>
+      <c r="L30" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="M30" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="N30" s="10" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -5358,7 +5831,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5372,7 +5845,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
add c# runtime code
</commit_message>
<xml_diff>
--- a/example/config/BasicItem_Common.xlsx
+++ b/example/config/BasicItem_Common.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\Go\configTool-src\src\github.com\Blizzardx\ConfigProtocol\example\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\porject\GoConfigTool\src\github.com\Blizzardx\ConfigProtocol\example\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1C91DC-4233-4C16-9FE1-5C7787CE5434}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="-225" windowWidth="19440" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5280" yWindow="-225" windowWidth="19440" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -288,10 +287,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>{"type":"map","keyName":"Id","enum":["Quality:yelow=1|blue=2|red=3"]}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>{"type":"Quality",
 "name":"quality1"}</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -489,11 +484,15 @@
     <t>12</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
+  <si>
+    <t>{"type":"list","keyName":"Id","enum":["Quality:yelow=1|blue=2|red=3"]}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3384,823 +3383,823 @@
     </xf>
   </cellXfs>
   <cellStyles count="817">
-    <cellStyle name="20% - 强调文字颜色 1 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 11" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 12" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 13" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 14" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 15" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 16" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 17" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 18" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 19" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 20" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 3" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 4" xfId="14" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 5" xfId="15" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 6" xfId="16" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 7" xfId="17" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 8" xfId="18" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="20% - 强调文字颜色 1 9" xfId="19" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 10" xfId="20" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 11" xfId="21" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 12" xfId="22" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 13" xfId="23" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 14" xfId="24" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 15" xfId="25" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 16" xfId="26" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 17" xfId="27" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 18" xfId="28" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 19" xfId="29" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 20" xfId="31" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 3" xfId="32" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 4" xfId="33" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 5" xfId="34" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 6" xfId="35" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 7" xfId="36" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 8" xfId="37" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="20% - 强调文字颜色 2 9" xfId="38" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 10" xfId="39" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 11" xfId="40" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 12" xfId="41" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 13" xfId="42" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 14" xfId="43" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 15" xfId="44" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 16" xfId="45" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 17" xfId="46" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 18" xfId="47" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 19" xfId="48" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 20" xfId="50" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 3" xfId="51" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 4" xfId="52" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 5" xfId="53" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 6" xfId="54" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 7" xfId="55" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 8" xfId="56" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="20% - 强调文字颜色 3 9" xfId="57" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 10" xfId="58" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 11" xfId="59" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 12" xfId="60" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 13" xfId="61" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 14" xfId="62" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 15" xfId="63" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 16" xfId="64" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 17" xfId="65" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 18" xfId="66" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 19" xfId="67" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 2" xfId="68" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 20" xfId="69" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 3" xfId="70" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 4" xfId="71" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 5" xfId="72" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 6" xfId="73" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 7" xfId="74" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 8" xfId="75" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="20% - 强调文字颜色 4 9" xfId="76" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 10" xfId="77" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 11" xfId="78" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 12" xfId="79" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 13" xfId="80" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 14" xfId="81" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 15" xfId="82" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 16" xfId="83" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 17" xfId="84" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 18" xfId="85" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 19" xfId="86" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 20" xfId="88" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 3" xfId="89" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 4" xfId="90" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 5" xfId="91" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 6" xfId="92" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 7" xfId="93" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 8" xfId="94" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="20% - 强调文字颜色 5 9" xfId="95" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 10" xfId="96" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 11" xfId="97" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 12" xfId="98" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 13" xfId="99" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 14" xfId="100" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 15" xfId="101" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 16" xfId="102" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 17" xfId="103" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 18" xfId="104" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 19" xfId="105" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 2" xfId="106" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 20" xfId="107" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 3" xfId="108" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 4" xfId="109" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 5" xfId="110" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 6" xfId="111" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 7" xfId="112" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 8" xfId="113" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="20% - 强调文字颜色 6 9" xfId="114" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 10" xfId="115" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 11" xfId="116" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 12" xfId="117" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 13" xfId="118" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 14" xfId="119" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 15" xfId="120" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 16" xfId="121" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 17" xfId="122" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 18" xfId="123" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 19" xfId="124" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 2" xfId="125" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 20" xfId="126" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 3" xfId="127" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 4" xfId="128" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 5" xfId="129" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 6" xfId="130" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 7" xfId="131" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 8" xfId="132" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
-    <cellStyle name="40% - 强调文字颜色 1 9" xfId="133" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 10" xfId="134" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 11" xfId="135" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 12" xfId="136" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 13" xfId="137" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 14" xfId="138" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 15" xfId="139" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 16" xfId="140" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 17" xfId="141" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 18" xfId="142" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 19" xfId="143" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 2" xfId="144" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 20" xfId="145" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 3" xfId="146" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 4" xfId="147" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 5" xfId="148" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 6" xfId="149" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 7" xfId="150" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 8" xfId="151" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
-    <cellStyle name="40% - 强调文字颜色 2 9" xfId="152" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 10" xfId="153" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 11" xfId="154" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 12" xfId="155" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 13" xfId="156" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 14" xfId="157" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 15" xfId="158" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 16" xfId="159" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 17" xfId="160" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 18" xfId="161" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 19" xfId="162" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 2" xfId="163" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 20" xfId="164" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 3" xfId="165" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 4" xfId="166" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 5" xfId="167" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 6" xfId="168" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 7" xfId="169" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 8" xfId="170" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
-    <cellStyle name="40% - 强调文字颜色 3 9" xfId="171" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 10" xfId="172" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 11" xfId="173" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 12" xfId="174" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 13" xfId="175" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 14" xfId="176" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 15" xfId="177" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 16" xfId="178" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 17" xfId="179" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 18" xfId="180" xr:uid="{00000000-0005-0000-0000-0000B3000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 19" xfId="181" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 2" xfId="182" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 20" xfId="183" xr:uid="{00000000-0005-0000-0000-0000B6000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 3" xfId="184" xr:uid="{00000000-0005-0000-0000-0000B7000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 4" xfId="185" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 5" xfId="186" xr:uid="{00000000-0005-0000-0000-0000B9000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 6" xfId="187" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 7" xfId="188" xr:uid="{00000000-0005-0000-0000-0000BB000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 8" xfId="189" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
-    <cellStyle name="40% - 强调文字颜色 4 9" xfId="190" xr:uid="{00000000-0005-0000-0000-0000BD000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 10" xfId="191" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 11" xfId="192" xr:uid="{00000000-0005-0000-0000-0000BF000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 12" xfId="193" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 13" xfId="194" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 14" xfId="195" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 15" xfId="196" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 16" xfId="197" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 17" xfId="198" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 18" xfId="199" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 19" xfId="200" xr:uid="{00000000-0005-0000-0000-0000C7000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 2" xfId="201" xr:uid="{00000000-0005-0000-0000-0000C8000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 20" xfId="202" xr:uid="{00000000-0005-0000-0000-0000C9000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 3" xfId="203" xr:uid="{00000000-0005-0000-0000-0000CA000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 4" xfId="204" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 5" xfId="205" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 6" xfId="206" xr:uid="{00000000-0005-0000-0000-0000CD000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 7" xfId="207" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 8" xfId="208" xr:uid="{00000000-0005-0000-0000-0000CF000000}"/>
-    <cellStyle name="40% - 强调文字颜色 5 9" xfId="209" xr:uid="{00000000-0005-0000-0000-0000D0000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 10" xfId="210" xr:uid="{00000000-0005-0000-0000-0000D1000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 11" xfId="211" xr:uid="{00000000-0005-0000-0000-0000D2000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 12" xfId="212" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 13" xfId="213" xr:uid="{00000000-0005-0000-0000-0000D4000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 14" xfId="214" xr:uid="{00000000-0005-0000-0000-0000D5000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 15" xfId="215" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 16" xfId="216" xr:uid="{00000000-0005-0000-0000-0000D7000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 17" xfId="217" xr:uid="{00000000-0005-0000-0000-0000D8000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 18" xfId="218" xr:uid="{00000000-0005-0000-0000-0000D9000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 19" xfId="219" xr:uid="{00000000-0005-0000-0000-0000DA000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 2" xfId="220" xr:uid="{00000000-0005-0000-0000-0000DB000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 20" xfId="221" xr:uid="{00000000-0005-0000-0000-0000DC000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 3" xfId="222" xr:uid="{00000000-0005-0000-0000-0000DD000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 4" xfId="223" xr:uid="{00000000-0005-0000-0000-0000DE000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 5" xfId="224" xr:uid="{00000000-0005-0000-0000-0000DF000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 6" xfId="225" xr:uid="{00000000-0005-0000-0000-0000E0000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 7" xfId="226" xr:uid="{00000000-0005-0000-0000-0000E1000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 8" xfId="227" xr:uid="{00000000-0005-0000-0000-0000E2000000}"/>
-    <cellStyle name="40% - 强调文字颜色 6 9" xfId="228" xr:uid="{00000000-0005-0000-0000-0000E3000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 10" xfId="229" xr:uid="{00000000-0005-0000-0000-0000E4000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 11" xfId="230" xr:uid="{00000000-0005-0000-0000-0000E5000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 12" xfId="231" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 13" xfId="232" xr:uid="{00000000-0005-0000-0000-0000E7000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 14" xfId="233" xr:uid="{00000000-0005-0000-0000-0000E8000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 15" xfId="234" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 16" xfId="235" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 17" xfId="236" xr:uid="{00000000-0005-0000-0000-0000EB000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 18" xfId="237" xr:uid="{00000000-0005-0000-0000-0000EC000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 19" xfId="238" xr:uid="{00000000-0005-0000-0000-0000ED000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 2" xfId="239" xr:uid="{00000000-0005-0000-0000-0000EE000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 20" xfId="240" xr:uid="{00000000-0005-0000-0000-0000EF000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 3" xfId="241" xr:uid="{00000000-0005-0000-0000-0000F0000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 4" xfId="242" xr:uid="{00000000-0005-0000-0000-0000F1000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 5" xfId="243" xr:uid="{00000000-0005-0000-0000-0000F2000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 6" xfId="244" xr:uid="{00000000-0005-0000-0000-0000F3000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 7" xfId="245" xr:uid="{00000000-0005-0000-0000-0000F4000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 8" xfId="246" xr:uid="{00000000-0005-0000-0000-0000F5000000}"/>
-    <cellStyle name="60% - 强调文字颜色 1 9" xfId="247" xr:uid="{00000000-0005-0000-0000-0000F6000000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 10" xfId="248" xr:uid="{00000000-0005-0000-0000-0000F7000000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 11" xfId="249" xr:uid="{00000000-0005-0000-0000-0000F8000000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 12" xfId="250" xr:uid="{00000000-0005-0000-0000-0000F9000000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 13" xfId="251" xr:uid="{00000000-0005-0000-0000-0000FA000000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 14" xfId="252" xr:uid="{00000000-0005-0000-0000-0000FB000000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 15" xfId="253" xr:uid="{00000000-0005-0000-0000-0000FC000000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 16" xfId="254" xr:uid="{00000000-0005-0000-0000-0000FD000000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 17" xfId="255" xr:uid="{00000000-0005-0000-0000-0000FE000000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 18" xfId="256" xr:uid="{00000000-0005-0000-0000-0000FF000000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 19" xfId="257" xr:uid="{00000000-0005-0000-0000-000000010000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 2" xfId="258" xr:uid="{00000000-0005-0000-0000-000001010000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 20" xfId="259" xr:uid="{00000000-0005-0000-0000-000002010000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 3" xfId="260" xr:uid="{00000000-0005-0000-0000-000003010000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 4" xfId="261" xr:uid="{00000000-0005-0000-0000-000004010000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 5" xfId="262" xr:uid="{00000000-0005-0000-0000-000005010000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 6" xfId="263" xr:uid="{00000000-0005-0000-0000-000006010000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 7" xfId="264" xr:uid="{00000000-0005-0000-0000-000007010000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 8" xfId="265" xr:uid="{00000000-0005-0000-0000-000008010000}"/>
-    <cellStyle name="60% - 强调文字颜色 2 9" xfId="266" xr:uid="{00000000-0005-0000-0000-000009010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 10" xfId="267" xr:uid="{00000000-0005-0000-0000-00000A010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 11" xfId="268" xr:uid="{00000000-0005-0000-0000-00000B010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 12" xfId="269" xr:uid="{00000000-0005-0000-0000-00000C010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 13" xfId="270" xr:uid="{00000000-0005-0000-0000-00000D010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 14" xfId="271" xr:uid="{00000000-0005-0000-0000-00000E010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 15" xfId="272" xr:uid="{00000000-0005-0000-0000-00000F010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 16" xfId="273" xr:uid="{00000000-0005-0000-0000-000010010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 17" xfId="274" xr:uid="{00000000-0005-0000-0000-000011010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 18" xfId="275" xr:uid="{00000000-0005-0000-0000-000012010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 19" xfId="276" xr:uid="{00000000-0005-0000-0000-000013010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 2" xfId="277" xr:uid="{00000000-0005-0000-0000-000014010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 20" xfId="278" xr:uid="{00000000-0005-0000-0000-000015010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 3" xfId="279" xr:uid="{00000000-0005-0000-0000-000016010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 4" xfId="280" xr:uid="{00000000-0005-0000-0000-000017010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 5" xfId="281" xr:uid="{00000000-0005-0000-0000-000018010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 6" xfId="282" xr:uid="{00000000-0005-0000-0000-000019010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 7" xfId="283" xr:uid="{00000000-0005-0000-0000-00001A010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 8" xfId="284" xr:uid="{00000000-0005-0000-0000-00001B010000}"/>
-    <cellStyle name="60% - 强调文字颜色 3 9" xfId="285" xr:uid="{00000000-0005-0000-0000-00001C010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 10" xfId="286" xr:uid="{00000000-0005-0000-0000-00001D010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 11" xfId="287" xr:uid="{00000000-0005-0000-0000-00001E010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 12" xfId="288" xr:uid="{00000000-0005-0000-0000-00001F010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 13" xfId="289" xr:uid="{00000000-0005-0000-0000-000020010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 14" xfId="290" xr:uid="{00000000-0005-0000-0000-000021010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 15" xfId="291" xr:uid="{00000000-0005-0000-0000-000022010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 16" xfId="292" xr:uid="{00000000-0005-0000-0000-000023010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 17" xfId="293" xr:uid="{00000000-0005-0000-0000-000024010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 18" xfId="294" xr:uid="{00000000-0005-0000-0000-000025010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 19" xfId="295" xr:uid="{00000000-0005-0000-0000-000026010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 2" xfId="296" xr:uid="{00000000-0005-0000-0000-000027010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 20" xfId="297" xr:uid="{00000000-0005-0000-0000-000028010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 3" xfId="298" xr:uid="{00000000-0005-0000-0000-000029010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 4" xfId="299" xr:uid="{00000000-0005-0000-0000-00002A010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 5" xfId="300" xr:uid="{00000000-0005-0000-0000-00002B010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 6" xfId="301" xr:uid="{00000000-0005-0000-0000-00002C010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 7" xfId="302" xr:uid="{00000000-0005-0000-0000-00002D010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 8" xfId="303" xr:uid="{00000000-0005-0000-0000-00002E010000}"/>
-    <cellStyle name="60% - 强调文字颜色 4 9" xfId="304" xr:uid="{00000000-0005-0000-0000-00002F010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 10" xfId="305" xr:uid="{00000000-0005-0000-0000-000030010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 11" xfId="306" xr:uid="{00000000-0005-0000-0000-000031010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 12" xfId="307" xr:uid="{00000000-0005-0000-0000-000032010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 13" xfId="308" xr:uid="{00000000-0005-0000-0000-000033010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 14" xfId="309" xr:uid="{00000000-0005-0000-0000-000034010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 15" xfId="310" xr:uid="{00000000-0005-0000-0000-000035010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 16" xfId="311" xr:uid="{00000000-0005-0000-0000-000036010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 17" xfId="312" xr:uid="{00000000-0005-0000-0000-000037010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 18" xfId="313" xr:uid="{00000000-0005-0000-0000-000038010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 19" xfId="314" xr:uid="{00000000-0005-0000-0000-000039010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 2" xfId="315" xr:uid="{00000000-0005-0000-0000-00003A010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 20" xfId="316" xr:uid="{00000000-0005-0000-0000-00003B010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 3" xfId="317" xr:uid="{00000000-0005-0000-0000-00003C010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 4" xfId="318" xr:uid="{00000000-0005-0000-0000-00003D010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 5" xfId="319" xr:uid="{00000000-0005-0000-0000-00003E010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 6" xfId="320" xr:uid="{00000000-0005-0000-0000-00003F010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 7" xfId="321" xr:uid="{00000000-0005-0000-0000-000040010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 8" xfId="322" xr:uid="{00000000-0005-0000-0000-000041010000}"/>
-    <cellStyle name="60% - 强调文字颜色 5 9" xfId="323" xr:uid="{00000000-0005-0000-0000-000042010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 10" xfId="324" xr:uid="{00000000-0005-0000-0000-000043010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 11" xfId="325" xr:uid="{00000000-0005-0000-0000-000044010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 12" xfId="326" xr:uid="{00000000-0005-0000-0000-000045010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 13" xfId="327" xr:uid="{00000000-0005-0000-0000-000046010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 14" xfId="328" xr:uid="{00000000-0005-0000-0000-000047010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 15" xfId="329" xr:uid="{00000000-0005-0000-0000-000048010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 16" xfId="330" xr:uid="{00000000-0005-0000-0000-000049010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 17" xfId="331" xr:uid="{00000000-0005-0000-0000-00004A010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 18" xfId="332" xr:uid="{00000000-0005-0000-0000-00004B010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 19" xfId="333" xr:uid="{00000000-0005-0000-0000-00004C010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 2" xfId="334" xr:uid="{00000000-0005-0000-0000-00004D010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 20" xfId="335" xr:uid="{00000000-0005-0000-0000-00004E010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 3" xfId="336" xr:uid="{00000000-0005-0000-0000-00004F010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 4" xfId="337" xr:uid="{00000000-0005-0000-0000-000050010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 5" xfId="338" xr:uid="{00000000-0005-0000-0000-000051010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 6" xfId="339" xr:uid="{00000000-0005-0000-0000-000052010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 7" xfId="340" xr:uid="{00000000-0005-0000-0000-000053010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 8" xfId="341" xr:uid="{00000000-0005-0000-0000-000054010000}"/>
-    <cellStyle name="60% - 强调文字颜色 6 9" xfId="342" xr:uid="{00000000-0005-0000-0000-000055010000}"/>
+    <cellStyle name="20% - 强调文字颜色 1 10" xfId="1"/>
+    <cellStyle name="20% - 强调文字颜色 1 11" xfId="2"/>
+    <cellStyle name="20% - 强调文字颜色 1 12" xfId="3"/>
+    <cellStyle name="20% - 强调文字颜色 1 13" xfId="4"/>
+    <cellStyle name="20% - 强调文字颜色 1 14" xfId="5"/>
+    <cellStyle name="20% - 强调文字颜色 1 15" xfId="6"/>
+    <cellStyle name="20% - 强调文字颜色 1 16" xfId="7"/>
+    <cellStyle name="20% - 强调文字颜色 1 17" xfId="8"/>
+    <cellStyle name="20% - 强调文字颜色 1 18" xfId="9"/>
+    <cellStyle name="20% - 强调文字颜色 1 19" xfId="10"/>
+    <cellStyle name="20% - 强调文字颜色 1 2" xfId="11"/>
+    <cellStyle name="20% - 强调文字颜色 1 20" xfId="12"/>
+    <cellStyle name="20% - 强调文字颜色 1 3" xfId="13"/>
+    <cellStyle name="20% - 强调文字颜色 1 4" xfId="14"/>
+    <cellStyle name="20% - 强调文字颜色 1 5" xfId="15"/>
+    <cellStyle name="20% - 强调文字颜色 1 6" xfId="16"/>
+    <cellStyle name="20% - 强调文字颜色 1 7" xfId="17"/>
+    <cellStyle name="20% - 强调文字颜色 1 8" xfId="18"/>
+    <cellStyle name="20% - 强调文字颜色 1 9" xfId="19"/>
+    <cellStyle name="20% - 强调文字颜色 2 10" xfId="20"/>
+    <cellStyle name="20% - 强调文字颜色 2 11" xfId="21"/>
+    <cellStyle name="20% - 强调文字颜色 2 12" xfId="22"/>
+    <cellStyle name="20% - 强调文字颜色 2 13" xfId="23"/>
+    <cellStyle name="20% - 强调文字颜色 2 14" xfId="24"/>
+    <cellStyle name="20% - 强调文字颜色 2 15" xfId="25"/>
+    <cellStyle name="20% - 强调文字颜色 2 16" xfId="26"/>
+    <cellStyle name="20% - 强调文字颜色 2 17" xfId="27"/>
+    <cellStyle name="20% - 强调文字颜色 2 18" xfId="28"/>
+    <cellStyle name="20% - 强调文字颜色 2 19" xfId="29"/>
+    <cellStyle name="20% - 强调文字颜色 2 2" xfId="30"/>
+    <cellStyle name="20% - 强调文字颜色 2 20" xfId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2 3" xfId="32"/>
+    <cellStyle name="20% - 强调文字颜色 2 4" xfId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2 5" xfId="34"/>
+    <cellStyle name="20% - 强调文字颜色 2 6" xfId="35"/>
+    <cellStyle name="20% - 强调文字颜色 2 7" xfId="36"/>
+    <cellStyle name="20% - 强调文字颜色 2 8" xfId="37"/>
+    <cellStyle name="20% - 强调文字颜色 2 9" xfId="38"/>
+    <cellStyle name="20% - 强调文字颜色 3 10" xfId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3 11" xfId="40"/>
+    <cellStyle name="20% - 强调文字颜色 3 12" xfId="41"/>
+    <cellStyle name="20% - 强调文字颜色 3 13" xfId="42"/>
+    <cellStyle name="20% - 强调文字颜色 3 14" xfId="43"/>
+    <cellStyle name="20% - 强调文字颜色 3 15" xfId="44"/>
+    <cellStyle name="20% - 强调文字颜色 3 16" xfId="45"/>
+    <cellStyle name="20% - 强调文字颜色 3 17" xfId="46"/>
+    <cellStyle name="20% - 强调文字颜色 3 18" xfId="47"/>
+    <cellStyle name="20% - 强调文字颜色 3 19" xfId="48"/>
+    <cellStyle name="20% - 强调文字颜色 3 2" xfId="49"/>
+    <cellStyle name="20% - 强调文字颜色 3 20" xfId="50"/>
+    <cellStyle name="20% - 强调文字颜色 3 3" xfId="51"/>
+    <cellStyle name="20% - 强调文字颜色 3 4" xfId="52"/>
+    <cellStyle name="20% - 强调文字颜色 3 5" xfId="53"/>
+    <cellStyle name="20% - 强调文字颜色 3 6" xfId="54"/>
+    <cellStyle name="20% - 强调文字颜色 3 7" xfId="55"/>
+    <cellStyle name="20% - 强调文字颜色 3 8" xfId="56"/>
+    <cellStyle name="20% - 强调文字颜色 3 9" xfId="57"/>
+    <cellStyle name="20% - 强调文字颜色 4 10" xfId="58"/>
+    <cellStyle name="20% - 强调文字颜色 4 11" xfId="59"/>
+    <cellStyle name="20% - 强调文字颜色 4 12" xfId="60"/>
+    <cellStyle name="20% - 强调文字颜色 4 13" xfId="61"/>
+    <cellStyle name="20% - 强调文字颜色 4 14" xfId="62"/>
+    <cellStyle name="20% - 强调文字颜色 4 15" xfId="63"/>
+    <cellStyle name="20% - 强调文字颜色 4 16" xfId="64"/>
+    <cellStyle name="20% - 强调文字颜色 4 17" xfId="65"/>
+    <cellStyle name="20% - 强调文字颜色 4 18" xfId="66"/>
+    <cellStyle name="20% - 强调文字颜色 4 19" xfId="67"/>
+    <cellStyle name="20% - 强调文字颜色 4 2" xfId="68"/>
+    <cellStyle name="20% - 强调文字颜色 4 20" xfId="69"/>
+    <cellStyle name="20% - 强调文字颜色 4 3" xfId="70"/>
+    <cellStyle name="20% - 强调文字颜色 4 4" xfId="71"/>
+    <cellStyle name="20% - 强调文字颜色 4 5" xfId="72"/>
+    <cellStyle name="20% - 强调文字颜色 4 6" xfId="73"/>
+    <cellStyle name="20% - 强调文字颜色 4 7" xfId="74"/>
+    <cellStyle name="20% - 强调文字颜色 4 8" xfId="75"/>
+    <cellStyle name="20% - 强调文字颜色 4 9" xfId="76"/>
+    <cellStyle name="20% - 强调文字颜色 5 10" xfId="77"/>
+    <cellStyle name="20% - 强调文字颜色 5 11" xfId="78"/>
+    <cellStyle name="20% - 强调文字颜色 5 12" xfId="79"/>
+    <cellStyle name="20% - 强调文字颜色 5 13" xfId="80"/>
+    <cellStyle name="20% - 强调文字颜色 5 14" xfId="81"/>
+    <cellStyle name="20% - 强调文字颜色 5 15" xfId="82"/>
+    <cellStyle name="20% - 强调文字颜色 5 16" xfId="83"/>
+    <cellStyle name="20% - 强调文字颜色 5 17" xfId="84"/>
+    <cellStyle name="20% - 强调文字颜色 5 18" xfId="85"/>
+    <cellStyle name="20% - 强调文字颜色 5 19" xfId="86"/>
+    <cellStyle name="20% - 强调文字颜色 5 2" xfId="87"/>
+    <cellStyle name="20% - 强调文字颜色 5 20" xfId="88"/>
+    <cellStyle name="20% - 强调文字颜色 5 3" xfId="89"/>
+    <cellStyle name="20% - 强调文字颜色 5 4" xfId="90"/>
+    <cellStyle name="20% - 强调文字颜色 5 5" xfId="91"/>
+    <cellStyle name="20% - 强调文字颜色 5 6" xfId="92"/>
+    <cellStyle name="20% - 强调文字颜色 5 7" xfId="93"/>
+    <cellStyle name="20% - 强调文字颜色 5 8" xfId="94"/>
+    <cellStyle name="20% - 强调文字颜色 5 9" xfId="95"/>
+    <cellStyle name="20% - 强调文字颜色 6 10" xfId="96"/>
+    <cellStyle name="20% - 强调文字颜色 6 11" xfId="97"/>
+    <cellStyle name="20% - 强调文字颜色 6 12" xfId="98"/>
+    <cellStyle name="20% - 强调文字颜色 6 13" xfId="99"/>
+    <cellStyle name="20% - 强调文字颜色 6 14" xfId="100"/>
+    <cellStyle name="20% - 强调文字颜色 6 15" xfId="101"/>
+    <cellStyle name="20% - 强调文字颜色 6 16" xfId="102"/>
+    <cellStyle name="20% - 强调文字颜色 6 17" xfId="103"/>
+    <cellStyle name="20% - 强调文字颜色 6 18" xfId="104"/>
+    <cellStyle name="20% - 强调文字颜色 6 19" xfId="105"/>
+    <cellStyle name="20% - 强调文字颜色 6 2" xfId="106"/>
+    <cellStyle name="20% - 强调文字颜色 6 20" xfId="107"/>
+    <cellStyle name="20% - 强调文字颜色 6 3" xfId="108"/>
+    <cellStyle name="20% - 强调文字颜色 6 4" xfId="109"/>
+    <cellStyle name="20% - 强调文字颜色 6 5" xfId="110"/>
+    <cellStyle name="20% - 强调文字颜色 6 6" xfId="111"/>
+    <cellStyle name="20% - 强调文字颜色 6 7" xfId="112"/>
+    <cellStyle name="20% - 强调文字颜色 6 8" xfId="113"/>
+    <cellStyle name="20% - 强调文字颜色 6 9" xfId="114"/>
+    <cellStyle name="40% - 强调文字颜色 1 10" xfId="115"/>
+    <cellStyle name="40% - 强调文字颜色 1 11" xfId="116"/>
+    <cellStyle name="40% - 强调文字颜色 1 12" xfId="117"/>
+    <cellStyle name="40% - 强调文字颜色 1 13" xfId="118"/>
+    <cellStyle name="40% - 强调文字颜色 1 14" xfId="119"/>
+    <cellStyle name="40% - 强调文字颜色 1 15" xfId="120"/>
+    <cellStyle name="40% - 强调文字颜色 1 16" xfId="121"/>
+    <cellStyle name="40% - 强调文字颜色 1 17" xfId="122"/>
+    <cellStyle name="40% - 强调文字颜色 1 18" xfId="123"/>
+    <cellStyle name="40% - 强调文字颜色 1 19" xfId="124"/>
+    <cellStyle name="40% - 强调文字颜色 1 2" xfId="125"/>
+    <cellStyle name="40% - 强调文字颜色 1 20" xfId="126"/>
+    <cellStyle name="40% - 强调文字颜色 1 3" xfId="127"/>
+    <cellStyle name="40% - 强调文字颜色 1 4" xfId="128"/>
+    <cellStyle name="40% - 强调文字颜色 1 5" xfId="129"/>
+    <cellStyle name="40% - 强调文字颜色 1 6" xfId="130"/>
+    <cellStyle name="40% - 强调文字颜色 1 7" xfId="131"/>
+    <cellStyle name="40% - 强调文字颜色 1 8" xfId="132"/>
+    <cellStyle name="40% - 强调文字颜色 1 9" xfId="133"/>
+    <cellStyle name="40% - 强调文字颜色 2 10" xfId="134"/>
+    <cellStyle name="40% - 强调文字颜色 2 11" xfId="135"/>
+    <cellStyle name="40% - 强调文字颜色 2 12" xfId="136"/>
+    <cellStyle name="40% - 强调文字颜色 2 13" xfId="137"/>
+    <cellStyle name="40% - 强调文字颜色 2 14" xfId="138"/>
+    <cellStyle name="40% - 强调文字颜色 2 15" xfId="139"/>
+    <cellStyle name="40% - 强调文字颜色 2 16" xfId="140"/>
+    <cellStyle name="40% - 强调文字颜色 2 17" xfId="141"/>
+    <cellStyle name="40% - 强调文字颜色 2 18" xfId="142"/>
+    <cellStyle name="40% - 强调文字颜色 2 19" xfId="143"/>
+    <cellStyle name="40% - 强调文字颜色 2 2" xfId="144"/>
+    <cellStyle name="40% - 强调文字颜色 2 20" xfId="145"/>
+    <cellStyle name="40% - 强调文字颜色 2 3" xfId="146"/>
+    <cellStyle name="40% - 强调文字颜色 2 4" xfId="147"/>
+    <cellStyle name="40% - 强调文字颜色 2 5" xfId="148"/>
+    <cellStyle name="40% - 强调文字颜色 2 6" xfId="149"/>
+    <cellStyle name="40% - 强调文字颜色 2 7" xfId="150"/>
+    <cellStyle name="40% - 强调文字颜色 2 8" xfId="151"/>
+    <cellStyle name="40% - 强调文字颜色 2 9" xfId="152"/>
+    <cellStyle name="40% - 强调文字颜色 3 10" xfId="153"/>
+    <cellStyle name="40% - 强调文字颜色 3 11" xfId="154"/>
+    <cellStyle name="40% - 强调文字颜色 3 12" xfId="155"/>
+    <cellStyle name="40% - 强调文字颜色 3 13" xfId="156"/>
+    <cellStyle name="40% - 强调文字颜色 3 14" xfId="157"/>
+    <cellStyle name="40% - 强调文字颜色 3 15" xfId="158"/>
+    <cellStyle name="40% - 强调文字颜色 3 16" xfId="159"/>
+    <cellStyle name="40% - 强调文字颜色 3 17" xfId="160"/>
+    <cellStyle name="40% - 强调文字颜色 3 18" xfId="161"/>
+    <cellStyle name="40% - 强调文字颜色 3 19" xfId="162"/>
+    <cellStyle name="40% - 强调文字颜色 3 2" xfId="163"/>
+    <cellStyle name="40% - 强调文字颜色 3 20" xfId="164"/>
+    <cellStyle name="40% - 强调文字颜色 3 3" xfId="165"/>
+    <cellStyle name="40% - 强调文字颜色 3 4" xfId="166"/>
+    <cellStyle name="40% - 强调文字颜色 3 5" xfId="167"/>
+    <cellStyle name="40% - 强调文字颜色 3 6" xfId="168"/>
+    <cellStyle name="40% - 强调文字颜色 3 7" xfId="169"/>
+    <cellStyle name="40% - 强调文字颜色 3 8" xfId="170"/>
+    <cellStyle name="40% - 强调文字颜色 3 9" xfId="171"/>
+    <cellStyle name="40% - 强调文字颜色 4 10" xfId="172"/>
+    <cellStyle name="40% - 强调文字颜色 4 11" xfId="173"/>
+    <cellStyle name="40% - 强调文字颜色 4 12" xfId="174"/>
+    <cellStyle name="40% - 强调文字颜色 4 13" xfId="175"/>
+    <cellStyle name="40% - 强调文字颜色 4 14" xfId="176"/>
+    <cellStyle name="40% - 强调文字颜色 4 15" xfId="177"/>
+    <cellStyle name="40% - 强调文字颜色 4 16" xfId="178"/>
+    <cellStyle name="40% - 强调文字颜色 4 17" xfId="179"/>
+    <cellStyle name="40% - 强调文字颜色 4 18" xfId="180"/>
+    <cellStyle name="40% - 强调文字颜色 4 19" xfId="181"/>
+    <cellStyle name="40% - 强调文字颜色 4 2" xfId="182"/>
+    <cellStyle name="40% - 强调文字颜色 4 20" xfId="183"/>
+    <cellStyle name="40% - 强调文字颜色 4 3" xfId="184"/>
+    <cellStyle name="40% - 强调文字颜色 4 4" xfId="185"/>
+    <cellStyle name="40% - 强调文字颜色 4 5" xfId="186"/>
+    <cellStyle name="40% - 强调文字颜色 4 6" xfId="187"/>
+    <cellStyle name="40% - 强调文字颜色 4 7" xfId="188"/>
+    <cellStyle name="40% - 强调文字颜色 4 8" xfId="189"/>
+    <cellStyle name="40% - 强调文字颜色 4 9" xfId="190"/>
+    <cellStyle name="40% - 强调文字颜色 5 10" xfId="191"/>
+    <cellStyle name="40% - 强调文字颜色 5 11" xfId="192"/>
+    <cellStyle name="40% - 强调文字颜色 5 12" xfId="193"/>
+    <cellStyle name="40% - 强调文字颜色 5 13" xfId="194"/>
+    <cellStyle name="40% - 强调文字颜色 5 14" xfId="195"/>
+    <cellStyle name="40% - 强调文字颜色 5 15" xfId="196"/>
+    <cellStyle name="40% - 强调文字颜色 5 16" xfId="197"/>
+    <cellStyle name="40% - 强调文字颜色 5 17" xfId="198"/>
+    <cellStyle name="40% - 强调文字颜色 5 18" xfId="199"/>
+    <cellStyle name="40% - 强调文字颜色 5 19" xfId="200"/>
+    <cellStyle name="40% - 强调文字颜色 5 2" xfId="201"/>
+    <cellStyle name="40% - 强调文字颜色 5 20" xfId="202"/>
+    <cellStyle name="40% - 强调文字颜色 5 3" xfId="203"/>
+    <cellStyle name="40% - 强调文字颜色 5 4" xfId="204"/>
+    <cellStyle name="40% - 强调文字颜色 5 5" xfId="205"/>
+    <cellStyle name="40% - 强调文字颜色 5 6" xfId="206"/>
+    <cellStyle name="40% - 强调文字颜色 5 7" xfId="207"/>
+    <cellStyle name="40% - 强调文字颜色 5 8" xfId="208"/>
+    <cellStyle name="40% - 强调文字颜色 5 9" xfId="209"/>
+    <cellStyle name="40% - 强调文字颜色 6 10" xfId="210"/>
+    <cellStyle name="40% - 强调文字颜色 6 11" xfId="211"/>
+    <cellStyle name="40% - 强调文字颜色 6 12" xfId="212"/>
+    <cellStyle name="40% - 强调文字颜色 6 13" xfId="213"/>
+    <cellStyle name="40% - 强调文字颜色 6 14" xfId="214"/>
+    <cellStyle name="40% - 强调文字颜色 6 15" xfId="215"/>
+    <cellStyle name="40% - 强调文字颜色 6 16" xfId="216"/>
+    <cellStyle name="40% - 强调文字颜色 6 17" xfId="217"/>
+    <cellStyle name="40% - 强调文字颜色 6 18" xfId="218"/>
+    <cellStyle name="40% - 强调文字颜色 6 19" xfId="219"/>
+    <cellStyle name="40% - 强调文字颜色 6 2" xfId="220"/>
+    <cellStyle name="40% - 强调文字颜色 6 20" xfId="221"/>
+    <cellStyle name="40% - 强调文字颜色 6 3" xfId="222"/>
+    <cellStyle name="40% - 强调文字颜色 6 4" xfId="223"/>
+    <cellStyle name="40% - 强调文字颜色 6 5" xfId="224"/>
+    <cellStyle name="40% - 强调文字颜色 6 6" xfId="225"/>
+    <cellStyle name="40% - 强调文字颜色 6 7" xfId="226"/>
+    <cellStyle name="40% - 强调文字颜色 6 8" xfId="227"/>
+    <cellStyle name="40% - 强调文字颜色 6 9" xfId="228"/>
+    <cellStyle name="60% - 强调文字颜色 1 10" xfId="229"/>
+    <cellStyle name="60% - 强调文字颜色 1 11" xfId="230"/>
+    <cellStyle name="60% - 强调文字颜色 1 12" xfId="231"/>
+    <cellStyle name="60% - 强调文字颜色 1 13" xfId="232"/>
+    <cellStyle name="60% - 强调文字颜色 1 14" xfId="233"/>
+    <cellStyle name="60% - 强调文字颜色 1 15" xfId="234"/>
+    <cellStyle name="60% - 强调文字颜色 1 16" xfId="235"/>
+    <cellStyle name="60% - 强调文字颜色 1 17" xfId="236"/>
+    <cellStyle name="60% - 强调文字颜色 1 18" xfId="237"/>
+    <cellStyle name="60% - 强调文字颜色 1 19" xfId="238"/>
+    <cellStyle name="60% - 强调文字颜色 1 2" xfId="239"/>
+    <cellStyle name="60% - 强调文字颜色 1 20" xfId="240"/>
+    <cellStyle name="60% - 强调文字颜色 1 3" xfId="241"/>
+    <cellStyle name="60% - 强调文字颜色 1 4" xfId="242"/>
+    <cellStyle name="60% - 强调文字颜色 1 5" xfId="243"/>
+    <cellStyle name="60% - 强调文字颜色 1 6" xfId="244"/>
+    <cellStyle name="60% - 强调文字颜色 1 7" xfId="245"/>
+    <cellStyle name="60% - 强调文字颜色 1 8" xfId="246"/>
+    <cellStyle name="60% - 强调文字颜色 1 9" xfId="247"/>
+    <cellStyle name="60% - 强调文字颜色 2 10" xfId="248"/>
+    <cellStyle name="60% - 强调文字颜色 2 11" xfId="249"/>
+    <cellStyle name="60% - 强调文字颜色 2 12" xfId="250"/>
+    <cellStyle name="60% - 强调文字颜色 2 13" xfId="251"/>
+    <cellStyle name="60% - 强调文字颜色 2 14" xfId="252"/>
+    <cellStyle name="60% - 强调文字颜色 2 15" xfId="253"/>
+    <cellStyle name="60% - 强调文字颜色 2 16" xfId="254"/>
+    <cellStyle name="60% - 强调文字颜色 2 17" xfId="255"/>
+    <cellStyle name="60% - 强调文字颜色 2 18" xfId="256"/>
+    <cellStyle name="60% - 强调文字颜色 2 19" xfId="257"/>
+    <cellStyle name="60% - 强调文字颜色 2 2" xfId="258"/>
+    <cellStyle name="60% - 强调文字颜色 2 20" xfId="259"/>
+    <cellStyle name="60% - 强调文字颜色 2 3" xfId="260"/>
+    <cellStyle name="60% - 强调文字颜色 2 4" xfId="261"/>
+    <cellStyle name="60% - 强调文字颜色 2 5" xfId="262"/>
+    <cellStyle name="60% - 强调文字颜色 2 6" xfId="263"/>
+    <cellStyle name="60% - 强调文字颜色 2 7" xfId="264"/>
+    <cellStyle name="60% - 强调文字颜色 2 8" xfId="265"/>
+    <cellStyle name="60% - 强调文字颜色 2 9" xfId="266"/>
+    <cellStyle name="60% - 强调文字颜色 3 10" xfId="267"/>
+    <cellStyle name="60% - 强调文字颜色 3 11" xfId="268"/>
+    <cellStyle name="60% - 强调文字颜色 3 12" xfId="269"/>
+    <cellStyle name="60% - 强调文字颜色 3 13" xfId="270"/>
+    <cellStyle name="60% - 强调文字颜色 3 14" xfId="271"/>
+    <cellStyle name="60% - 强调文字颜色 3 15" xfId="272"/>
+    <cellStyle name="60% - 强调文字颜色 3 16" xfId="273"/>
+    <cellStyle name="60% - 强调文字颜色 3 17" xfId="274"/>
+    <cellStyle name="60% - 强调文字颜色 3 18" xfId="275"/>
+    <cellStyle name="60% - 强调文字颜色 3 19" xfId="276"/>
+    <cellStyle name="60% - 强调文字颜色 3 2" xfId="277"/>
+    <cellStyle name="60% - 强调文字颜色 3 20" xfId="278"/>
+    <cellStyle name="60% - 强调文字颜色 3 3" xfId="279"/>
+    <cellStyle name="60% - 强调文字颜色 3 4" xfId="280"/>
+    <cellStyle name="60% - 强调文字颜色 3 5" xfId="281"/>
+    <cellStyle name="60% - 强调文字颜色 3 6" xfId="282"/>
+    <cellStyle name="60% - 强调文字颜色 3 7" xfId="283"/>
+    <cellStyle name="60% - 强调文字颜色 3 8" xfId="284"/>
+    <cellStyle name="60% - 强调文字颜色 3 9" xfId="285"/>
+    <cellStyle name="60% - 强调文字颜色 4 10" xfId="286"/>
+    <cellStyle name="60% - 强调文字颜色 4 11" xfId="287"/>
+    <cellStyle name="60% - 强调文字颜色 4 12" xfId="288"/>
+    <cellStyle name="60% - 强调文字颜色 4 13" xfId="289"/>
+    <cellStyle name="60% - 强调文字颜色 4 14" xfId="290"/>
+    <cellStyle name="60% - 强调文字颜色 4 15" xfId="291"/>
+    <cellStyle name="60% - 强调文字颜色 4 16" xfId="292"/>
+    <cellStyle name="60% - 强调文字颜色 4 17" xfId="293"/>
+    <cellStyle name="60% - 强调文字颜色 4 18" xfId="294"/>
+    <cellStyle name="60% - 强调文字颜色 4 19" xfId="295"/>
+    <cellStyle name="60% - 强调文字颜色 4 2" xfId="296"/>
+    <cellStyle name="60% - 强调文字颜色 4 20" xfId="297"/>
+    <cellStyle name="60% - 强调文字颜色 4 3" xfId="298"/>
+    <cellStyle name="60% - 强调文字颜色 4 4" xfId="299"/>
+    <cellStyle name="60% - 强调文字颜色 4 5" xfId="300"/>
+    <cellStyle name="60% - 强调文字颜色 4 6" xfId="301"/>
+    <cellStyle name="60% - 强调文字颜色 4 7" xfId="302"/>
+    <cellStyle name="60% - 强调文字颜色 4 8" xfId="303"/>
+    <cellStyle name="60% - 强调文字颜色 4 9" xfId="304"/>
+    <cellStyle name="60% - 强调文字颜色 5 10" xfId="305"/>
+    <cellStyle name="60% - 强调文字颜色 5 11" xfId="306"/>
+    <cellStyle name="60% - 强调文字颜色 5 12" xfId="307"/>
+    <cellStyle name="60% - 强调文字颜色 5 13" xfId="308"/>
+    <cellStyle name="60% - 强调文字颜色 5 14" xfId="309"/>
+    <cellStyle name="60% - 强调文字颜色 5 15" xfId="310"/>
+    <cellStyle name="60% - 强调文字颜色 5 16" xfId="311"/>
+    <cellStyle name="60% - 强调文字颜色 5 17" xfId="312"/>
+    <cellStyle name="60% - 强调文字颜色 5 18" xfId="313"/>
+    <cellStyle name="60% - 强调文字颜色 5 19" xfId="314"/>
+    <cellStyle name="60% - 强调文字颜色 5 2" xfId="315"/>
+    <cellStyle name="60% - 强调文字颜色 5 20" xfId="316"/>
+    <cellStyle name="60% - 强调文字颜色 5 3" xfId="317"/>
+    <cellStyle name="60% - 强调文字颜色 5 4" xfId="318"/>
+    <cellStyle name="60% - 强调文字颜色 5 5" xfId="319"/>
+    <cellStyle name="60% - 强调文字颜色 5 6" xfId="320"/>
+    <cellStyle name="60% - 强调文字颜色 5 7" xfId="321"/>
+    <cellStyle name="60% - 强调文字颜色 5 8" xfId="322"/>
+    <cellStyle name="60% - 强调文字颜色 5 9" xfId="323"/>
+    <cellStyle name="60% - 强调文字颜色 6 10" xfId="324"/>
+    <cellStyle name="60% - 强调文字颜色 6 11" xfId="325"/>
+    <cellStyle name="60% - 强调文字颜色 6 12" xfId="326"/>
+    <cellStyle name="60% - 强调文字颜色 6 13" xfId="327"/>
+    <cellStyle name="60% - 强调文字颜色 6 14" xfId="328"/>
+    <cellStyle name="60% - 强调文字颜色 6 15" xfId="329"/>
+    <cellStyle name="60% - 强调文字颜色 6 16" xfId="330"/>
+    <cellStyle name="60% - 强调文字颜色 6 17" xfId="331"/>
+    <cellStyle name="60% - 强调文字颜色 6 18" xfId="332"/>
+    <cellStyle name="60% - 强调文字颜色 6 19" xfId="333"/>
+    <cellStyle name="60% - 强调文字颜色 6 2" xfId="334"/>
+    <cellStyle name="60% - 强调文字颜色 6 20" xfId="335"/>
+    <cellStyle name="60% - 强调文字颜色 6 3" xfId="336"/>
+    <cellStyle name="60% - 强调文字颜色 6 4" xfId="337"/>
+    <cellStyle name="60% - 强调文字颜色 6 5" xfId="338"/>
+    <cellStyle name="60% - 强调文字颜色 6 6" xfId="339"/>
+    <cellStyle name="60% - 强调文字颜色 6 7" xfId="340"/>
+    <cellStyle name="60% - 强调文字颜色 6 8" xfId="341"/>
+    <cellStyle name="60% - 强调文字颜色 6 9" xfId="342"/>
     <cellStyle name="标题" xfId="343" builtinId="15" customBuiltin="1"/>
     <cellStyle name="标题 1" xfId="344" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="标题 1 10" xfId="345" xr:uid="{00000000-0005-0000-0000-000058010000}"/>
-    <cellStyle name="标题 1 11" xfId="346" xr:uid="{00000000-0005-0000-0000-000059010000}"/>
-    <cellStyle name="标题 1 12" xfId="347" xr:uid="{00000000-0005-0000-0000-00005A010000}"/>
-    <cellStyle name="标题 1 13" xfId="348" xr:uid="{00000000-0005-0000-0000-00005B010000}"/>
-    <cellStyle name="标题 1 14" xfId="349" xr:uid="{00000000-0005-0000-0000-00005C010000}"/>
-    <cellStyle name="标题 1 15" xfId="350" xr:uid="{00000000-0005-0000-0000-00005D010000}"/>
-    <cellStyle name="标题 1 16" xfId="351" xr:uid="{00000000-0005-0000-0000-00005E010000}"/>
-    <cellStyle name="标题 1 17" xfId="352" xr:uid="{00000000-0005-0000-0000-00005F010000}"/>
-    <cellStyle name="标题 1 18" xfId="353" xr:uid="{00000000-0005-0000-0000-000060010000}"/>
-    <cellStyle name="标题 1 19" xfId="354" xr:uid="{00000000-0005-0000-0000-000061010000}"/>
-    <cellStyle name="标题 1 2" xfId="355" xr:uid="{00000000-0005-0000-0000-000062010000}"/>
-    <cellStyle name="标题 1 20" xfId="356" xr:uid="{00000000-0005-0000-0000-000063010000}"/>
-    <cellStyle name="标题 1 3" xfId="357" xr:uid="{00000000-0005-0000-0000-000064010000}"/>
-    <cellStyle name="标题 1 4" xfId="358" xr:uid="{00000000-0005-0000-0000-000065010000}"/>
-    <cellStyle name="标题 1 5" xfId="359" xr:uid="{00000000-0005-0000-0000-000066010000}"/>
-    <cellStyle name="标题 1 6" xfId="360" xr:uid="{00000000-0005-0000-0000-000067010000}"/>
-    <cellStyle name="标题 1 7" xfId="361" xr:uid="{00000000-0005-0000-0000-000068010000}"/>
-    <cellStyle name="标题 1 8" xfId="362" xr:uid="{00000000-0005-0000-0000-000069010000}"/>
-    <cellStyle name="标题 1 9" xfId="363" xr:uid="{00000000-0005-0000-0000-00006A010000}"/>
-    <cellStyle name="标题 10" xfId="364" xr:uid="{00000000-0005-0000-0000-00006B010000}"/>
-    <cellStyle name="标题 11" xfId="365" xr:uid="{00000000-0005-0000-0000-00006C010000}"/>
-    <cellStyle name="标题 12" xfId="366" xr:uid="{00000000-0005-0000-0000-00006D010000}"/>
-    <cellStyle name="标题 13" xfId="367" xr:uid="{00000000-0005-0000-0000-00006E010000}"/>
-    <cellStyle name="标题 14" xfId="368" xr:uid="{00000000-0005-0000-0000-00006F010000}"/>
-    <cellStyle name="标题 15" xfId="369" xr:uid="{00000000-0005-0000-0000-000070010000}"/>
-    <cellStyle name="标题 16" xfId="370" xr:uid="{00000000-0005-0000-0000-000071010000}"/>
-    <cellStyle name="标题 17" xfId="371" xr:uid="{00000000-0005-0000-0000-000072010000}"/>
-    <cellStyle name="标题 18" xfId="372" xr:uid="{00000000-0005-0000-0000-000073010000}"/>
-    <cellStyle name="标题 19" xfId="373" xr:uid="{00000000-0005-0000-0000-000074010000}"/>
+    <cellStyle name="标题 1 10" xfId="345"/>
+    <cellStyle name="标题 1 11" xfId="346"/>
+    <cellStyle name="标题 1 12" xfId="347"/>
+    <cellStyle name="标题 1 13" xfId="348"/>
+    <cellStyle name="标题 1 14" xfId="349"/>
+    <cellStyle name="标题 1 15" xfId="350"/>
+    <cellStyle name="标题 1 16" xfId="351"/>
+    <cellStyle name="标题 1 17" xfId="352"/>
+    <cellStyle name="标题 1 18" xfId="353"/>
+    <cellStyle name="标题 1 19" xfId="354"/>
+    <cellStyle name="标题 1 2" xfId="355"/>
+    <cellStyle name="标题 1 20" xfId="356"/>
+    <cellStyle name="标题 1 3" xfId="357"/>
+    <cellStyle name="标题 1 4" xfId="358"/>
+    <cellStyle name="标题 1 5" xfId="359"/>
+    <cellStyle name="标题 1 6" xfId="360"/>
+    <cellStyle name="标题 1 7" xfId="361"/>
+    <cellStyle name="标题 1 8" xfId="362"/>
+    <cellStyle name="标题 1 9" xfId="363"/>
+    <cellStyle name="标题 10" xfId="364"/>
+    <cellStyle name="标题 11" xfId="365"/>
+    <cellStyle name="标题 12" xfId="366"/>
+    <cellStyle name="标题 13" xfId="367"/>
+    <cellStyle name="标题 14" xfId="368"/>
+    <cellStyle name="标题 15" xfId="369"/>
+    <cellStyle name="标题 16" xfId="370"/>
+    <cellStyle name="标题 17" xfId="371"/>
+    <cellStyle name="标题 18" xfId="372"/>
+    <cellStyle name="标题 19" xfId="373"/>
     <cellStyle name="标题 2" xfId="374" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="标题 2 10" xfId="375" xr:uid="{00000000-0005-0000-0000-000076010000}"/>
-    <cellStyle name="标题 2 11" xfId="376" xr:uid="{00000000-0005-0000-0000-000077010000}"/>
-    <cellStyle name="标题 2 12" xfId="377" xr:uid="{00000000-0005-0000-0000-000078010000}"/>
-    <cellStyle name="标题 2 13" xfId="378" xr:uid="{00000000-0005-0000-0000-000079010000}"/>
-    <cellStyle name="标题 2 14" xfId="379" xr:uid="{00000000-0005-0000-0000-00007A010000}"/>
-    <cellStyle name="标题 2 15" xfId="380" xr:uid="{00000000-0005-0000-0000-00007B010000}"/>
-    <cellStyle name="标题 2 16" xfId="381" xr:uid="{00000000-0005-0000-0000-00007C010000}"/>
-    <cellStyle name="标题 2 17" xfId="382" xr:uid="{00000000-0005-0000-0000-00007D010000}"/>
-    <cellStyle name="标题 2 18" xfId="383" xr:uid="{00000000-0005-0000-0000-00007E010000}"/>
-    <cellStyle name="标题 2 19" xfId="384" xr:uid="{00000000-0005-0000-0000-00007F010000}"/>
-    <cellStyle name="标题 2 2" xfId="385" xr:uid="{00000000-0005-0000-0000-000080010000}"/>
-    <cellStyle name="标题 2 20" xfId="386" xr:uid="{00000000-0005-0000-0000-000081010000}"/>
-    <cellStyle name="标题 2 3" xfId="387" xr:uid="{00000000-0005-0000-0000-000082010000}"/>
-    <cellStyle name="标题 2 4" xfId="388" xr:uid="{00000000-0005-0000-0000-000083010000}"/>
-    <cellStyle name="标题 2 5" xfId="389" xr:uid="{00000000-0005-0000-0000-000084010000}"/>
-    <cellStyle name="标题 2 6" xfId="390" xr:uid="{00000000-0005-0000-0000-000085010000}"/>
-    <cellStyle name="标题 2 7" xfId="391" xr:uid="{00000000-0005-0000-0000-000086010000}"/>
-    <cellStyle name="标题 2 8" xfId="392" xr:uid="{00000000-0005-0000-0000-000087010000}"/>
-    <cellStyle name="标题 2 9" xfId="393" xr:uid="{00000000-0005-0000-0000-000088010000}"/>
-    <cellStyle name="标题 20" xfId="394" xr:uid="{00000000-0005-0000-0000-000089010000}"/>
-    <cellStyle name="标题 21" xfId="395" xr:uid="{00000000-0005-0000-0000-00008A010000}"/>
-    <cellStyle name="标题 22" xfId="396" xr:uid="{00000000-0005-0000-0000-00008B010000}"/>
-    <cellStyle name="标题 23" xfId="397" xr:uid="{00000000-0005-0000-0000-00008C010000}"/>
+    <cellStyle name="标题 2 10" xfId="375"/>
+    <cellStyle name="标题 2 11" xfId="376"/>
+    <cellStyle name="标题 2 12" xfId="377"/>
+    <cellStyle name="标题 2 13" xfId="378"/>
+    <cellStyle name="标题 2 14" xfId="379"/>
+    <cellStyle name="标题 2 15" xfId="380"/>
+    <cellStyle name="标题 2 16" xfId="381"/>
+    <cellStyle name="标题 2 17" xfId="382"/>
+    <cellStyle name="标题 2 18" xfId="383"/>
+    <cellStyle name="标题 2 19" xfId="384"/>
+    <cellStyle name="标题 2 2" xfId="385"/>
+    <cellStyle name="标题 2 20" xfId="386"/>
+    <cellStyle name="标题 2 3" xfId="387"/>
+    <cellStyle name="标题 2 4" xfId="388"/>
+    <cellStyle name="标题 2 5" xfId="389"/>
+    <cellStyle name="标题 2 6" xfId="390"/>
+    <cellStyle name="标题 2 7" xfId="391"/>
+    <cellStyle name="标题 2 8" xfId="392"/>
+    <cellStyle name="标题 2 9" xfId="393"/>
+    <cellStyle name="标题 20" xfId="394"/>
+    <cellStyle name="标题 21" xfId="395"/>
+    <cellStyle name="标题 22" xfId="396"/>
+    <cellStyle name="标题 23" xfId="397"/>
     <cellStyle name="标题 3" xfId="398" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="标题 3 10" xfId="399" xr:uid="{00000000-0005-0000-0000-00008E010000}"/>
-    <cellStyle name="标题 3 11" xfId="400" xr:uid="{00000000-0005-0000-0000-00008F010000}"/>
-    <cellStyle name="标题 3 12" xfId="401" xr:uid="{00000000-0005-0000-0000-000090010000}"/>
-    <cellStyle name="标题 3 13" xfId="402" xr:uid="{00000000-0005-0000-0000-000091010000}"/>
-    <cellStyle name="标题 3 14" xfId="403" xr:uid="{00000000-0005-0000-0000-000092010000}"/>
-    <cellStyle name="标题 3 15" xfId="404" xr:uid="{00000000-0005-0000-0000-000093010000}"/>
-    <cellStyle name="标题 3 16" xfId="405" xr:uid="{00000000-0005-0000-0000-000094010000}"/>
-    <cellStyle name="标题 3 17" xfId="406" xr:uid="{00000000-0005-0000-0000-000095010000}"/>
-    <cellStyle name="标题 3 18" xfId="407" xr:uid="{00000000-0005-0000-0000-000096010000}"/>
-    <cellStyle name="标题 3 19" xfId="408" xr:uid="{00000000-0005-0000-0000-000097010000}"/>
-    <cellStyle name="标题 3 2" xfId="409" xr:uid="{00000000-0005-0000-0000-000098010000}"/>
-    <cellStyle name="标题 3 20" xfId="410" xr:uid="{00000000-0005-0000-0000-000099010000}"/>
-    <cellStyle name="标题 3 3" xfId="411" xr:uid="{00000000-0005-0000-0000-00009A010000}"/>
-    <cellStyle name="标题 3 4" xfId="412" xr:uid="{00000000-0005-0000-0000-00009B010000}"/>
-    <cellStyle name="标题 3 5" xfId="413" xr:uid="{00000000-0005-0000-0000-00009C010000}"/>
-    <cellStyle name="标题 3 6" xfId="414" xr:uid="{00000000-0005-0000-0000-00009D010000}"/>
-    <cellStyle name="标题 3 7" xfId="415" xr:uid="{00000000-0005-0000-0000-00009E010000}"/>
-    <cellStyle name="标题 3 8" xfId="416" xr:uid="{00000000-0005-0000-0000-00009F010000}"/>
-    <cellStyle name="标题 3 9" xfId="417" xr:uid="{00000000-0005-0000-0000-0000A0010000}"/>
+    <cellStyle name="标题 3 10" xfId="399"/>
+    <cellStyle name="标题 3 11" xfId="400"/>
+    <cellStyle name="标题 3 12" xfId="401"/>
+    <cellStyle name="标题 3 13" xfId="402"/>
+    <cellStyle name="标题 3 14" xfId="403"/>
+    <cellStyle name="标题 3 15" xfId="404"/>
+    <cellStyle name="标题 3 16" xfId="405"/>
+    <cellStyle name="标题 3 17" xfId="406"/>
+    <cellStyle name="标题 3 18" xfId="407"/>
+    <cellStyle name="标题 3 19" xfId="408"/>
+    <cellStyle name="标题 3 2" xfId="409"/>
+    <cellStyle name="标题 3 20" xfId="410"/>
+    <cellStyle name="标题 3 3" xfId="411"/>
+    <cellStyle name="标题 3 4" xfId="412"/>
+    <cellStyle name="标题 3 5" xfId="413"/>
+    <cellStyle name="标题 3 6" xfId="414"/>
+    <cellStyle name="标题 3 7" xfId="415"/>
+    <cellStyle name="标题 3 8" xfId="416"/>
+    <cellStyle name="标题 3 9" xfId="417"/>
     <cellStyle name="标题 4" xfId="418" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="标题 4 10" xfId="419" xr:uid="{00000000-0005-0000-0000-0000A2010000}"/>
-    <cellStyle name="标题 4 11" xfId="420" xr:uid="{00000000-0005-0000-0000-0000A3010000}"/>
-    <cellStyle name="标题 4 12" xfId="421" xr:uid="{00000000-0005-0000-0000-0000A4010000}"/>
-    <cellStyle name="标题 4 13" xfId="422" xr:uid="{00000000-0005-0000-0000-0000A5010000}"/>
-    <cellStyle name="标题 4 14" xfId="423" xr:uid="{00000000-0005-0000-0000-0000A6010000}"/>
-    <cellStyle name="标题 4 15" xfId="424" xr:uid="{00000000-0005-0000-0000-0000A7010000}"/>
-    <cellStyle name="标题 4 16" xfId="425" xr:uid="{00000000-0005-0000-0000-0000A8010000}"/>
-    <cellStyle name="标题 4 17" xfId="426" xr:uid="{00000000-0005-0000-0000-0000A9010000}"/>
-    <cellStyle name="标题 4 18" xfId="427" xr:uid="{00000000-0005-0000-0000-0000AA010000}"/>
-    <cellStyle name="标题 4 19" xfId="428" xr:uid="{00000000-0005-0000-0000-0000AB010000}"/>
-    <cellStyle name="标题 4 2" xfId="429" xr:uid="{00000000-0005-0000-0000-0000AC010000}"/>
-    <cellStyle name="标题 4 20" xfId="430" xr:uid="{00000000-0005-0000-0000-0000AD010000}"/>
-    <cellStyle name="标题 4 3" xfId="431" xr:uid="{00000000-0005-0000-0000-0000AE010000}"/>
-    <cellStyle name="标题 4 4" xfId="432" xr:uid="{00000000-0005-0000-0000-0000AF010000}"/>
-    <cellStyle name="标题 4 5" xfId="433" xr:uid="{00000000-0005-0000-0000-0000B0010000}"/>
-    <cellStyle name="标题 4 6" xfId="434" xr:uid="{00000000-0005-0000-0000-0000B1010000}"/>
-    <cellStyle name="标题 4 7" xfId="435" xr:uid="{00000000-0005-0000-0000-0000B2010000}"/>
-    <cellStyle name="标题 4 8" xfId="436" xr:uid="{00000000-0005-0000-0000-0000B3010000}"/>
-    <cellStyle name="标题 4 9" xfId="437" xr:uid="{00000000-0005-0000-0000-0000B4010000}"/>
-    <cellStyle name="标题 5" xfId="438" xr:uid="{00000000-0005-0000-0000-0000B5010000}"/>
-    <cellStyle name="标题 6" xfId="439" xr:uid="{00000000-0005-0000-0000-0000B6010000}"/>
-    <cellStyle name="标题 7" xfId="440" xr:uid="{00000000-0005-0000-0000-0000B7010000}"/>
-    <cellStyle name="标题 8" xfId="441" xr:uid="{00000000-0005-0000-0000-0000B8010000}"/>
-    <cellStyle name="标题 9" xfId="442" xr:uid="{00000000-0005-0000-0000-0000B9010000}"/>
+    <cellStyle name="标题 4 10" xfId="419"/>
+    <cellStyle name="标题 4 11" xfId="420"/>
+    <cellStyle name="标题 4 12" xfId="421"/>
+    <cellStyle name="标题 4 13" xfId="422"/>
+    <cellStyle name="标题 4 14" xfId="423"/>
+    <cellStyle name="标题 4 15" xfId="424"/>
+    <cellStyle name="标题 4 16" xfId="425"/>
+    <cellStyle name="标题 4 17" xfId="426"/>
+    <cellStyle name="标题 4 18" xfId="427"/>
+    <cellStyle name="标题 4 19" xfId="428"/>
+    <cellStyle name="标题 4 2" xfId="429"/>
+    <cellStyle name="标题 4 20" xfId="430"/>
+    <cellStyle name="标题 4 3" xfId="431"/>
+    <cellStyle name="标题 4 4" xfId="432"/>
+    <cellStyle name="标题 4 5" xfId="433"/>
+    <cellStyle name="标题 4 6" xfId="434"/>
+    <cellStyle name="标题 4 7" xfId="435"/>
+    <cellStyle name="标题 4 8" xfId="436"/>
+    <cellStyle name="标题 4 9" xfId="437"/>
+    <cellStyle name="标题 5" xfId="438"/>
+    <cellStyle name="标题 6" xfId="439"/>
+    <cellStyle name="标题 7" xfId="440"/>
+    <cellStyle name="标题 8" xfId="441"/>
+    <cellStyle name="标题 9" xfId="442"/>
     <cellStyle name="差" xfId="443" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="差 10" xfId="444" xr:uid="{00000000-0005-0000-0000-0000BB010000}"/>
-    <cellStyle name="差 11" xfId="445" xr:uid="{00000000-0005-0000-0000-0000BC010000}"/>
-    <cellStyle name="差 12" xfId="446" xr:uid="{00000000-0005-0000-0000-0000BD010000}"/>
-    <cellStyle name="差 13" xfId="447" xr:uid="{00000000-0005-0000-0000-0000BE010000}"/>
-    <cellStyle name="差 14" xfId="448" xr:uid="{00000000-0005-0000-0000-0000BF010000}"/>
-    <cellStyle name="差 15" xfId="449" xr:uid="{00000000-0005-0000-0000-0000C0010000}"/>
-    <cellStyle name="差 16" xfId="450" xr:uid="{00000000-0005-0000-0000-0000C1010000}"/>
-    <cellStyle name="差 17" xfId="451" xr:uid="{00000000-0005-0000-0000-0000C2010000}"/>
-    <cellStyle name="差 18" xfId="452" xr:uid="{00000000-0005-0000-0000-0000C3010000}"/>
-    <cellStyle name="差 19" xfId="453" xr:uid="{00000000-0005-0000-0000-0000C4010000}"/>
-    <cellStyle name="差 2" xfId="454" xr:uid="{00000000-0005-0000-0000-0000C5010000}"/>
-    <cellStyle name="差 20" xfId="455" xr:uid="{00000000-0005-0000-0000-0000C6010000}"/>
-    <cellStyle name="差 3" xfId="456" xr:uid="{00000000-0005-0000-0000-0000C7010000}"/>
-    <cellStyle name="差 4" xfId="457" xr:uid="{00000000-0005-0000-0000-0000C8010000}"/>
-    <cellStyle name="差 5" xfId="458" xr:uid="{00000000-0005-0000-0000-0000C9010000}"/>
-    <cellStyle name="差 6" xfId="459" xr:uid="{00000000-0005-0000-0000-0000CA010000}"/>
-    <cellStyle name="差 7" xfId="460" xr:uid="{00000000-0005-0000-0000-0000CB010000}"/>
-    <cellStyle name="差 8" xfId="461" xr:uid="{00000000-0005-0000-0000-0000CC010000}"/>
-    <cellStyle name="差 9" xfId="462" xr:uid="{00000000-0005-0000-0000-0000CD010000}"/>
+    <cellStyle name="差 10" xfId="444"/>
+    <cellStyle name="差 11" xfId="445"/>
+    <cellStyle name="差 12" xfId="446"/>
+    <cellStyle name="差 13" xfId="447"/>
+    <cellStyle name="差 14" xfId="448"/>
+    <cellStyle name="差 15" xfId="449"/>
+    <cellStyle name="差 16" xfId="450"/>
+    <cellStyle name="差 17" xfId="451"/>
+    <cellStyle name="差 18" xfId="452"/>
+    <cellStyle name="差 19" xfId="453"/>
+    <cellStyle name="差 2" xfId="454"/>
+    <cellStyle name="差 20" xfId="455"/>
+    <cellStyle name="差 3" xfId="456"/>
+    <cellStyle name="差 4" xfId="457"/>
+    <cellStyle name="差 5" xfId="458"/>
+    <cellStyle name="差 6" xfId="459"/>
+    <cellStyle name="差 7" xfId="460"/>
+    <cellStyle name="差 8" xfId="461"/>
+    <cellStyle name="差 9" xfId="462"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 10" xfId="463" xr:uid="{00000000-0005-0000-0000-0000CF010000}"/>
-    <cellStyle name="常规 11" xfId="464" xr:uid="{00000000-0005-0000-0000-0000D0010000}"/>
-    <cellStyle name="常规 12" xfId="465" xr:uid="{00000000-0005-0000-0000-0000D1010000}"/>
-    <cellStyle name="常规 13" xfId="466" xr:uid="{00000000-0005-0000-0000-0000D2010000}"/>
-    <cellStyle name="常规 14" xfId="467" xr:uid="{00000000-0005-0000-0000-0000D3010000}"/>
-    <cellStyle name="常规 15" xfId="468" xr:uid="{00000000-0005-0000-0000-0000D4010000}"/>
-    <cellStyle name="常规 16" xfId="469" xr:uid="{00000000-0005-0000-0000-0000D5010000}"/>
-    <cellStyle name="常规 17" xfId="470" xr:uid="{00000000-0005-0000-0000-0000D6010000}"/>
-    <cellStyle name="常规 18" xfId="471" xr:uid="{00000000-0005-0000-0000-0000D7010000}"/>
-    <cellStyle name="常规 19" xfId="472" xr:uid="{00000000-0005-0000-0000-0000D8010000}"/>
-    <cellStyle name="常规 2" xfId="473" xr:uid="{00000000-0005-0000-0000-0000D9010000}"/>
-    <cellStyle name="常规 2 2" xfId="474" xr:uid="{00000000-0005-0000-0000-0000DA010000}"/>
-    <cellStyle name="常规 20" xfId="475" xr:uid="{00000000-0005-0000-0000-0000DB010000}"/>
-    <cellStyle name="常规 3" xfId="476" xr:uid="{00000000-0005-0000-0000-0000DC010000}"/>
-    <cellStyle name="常规 4" xfId="477" xr:uid="{00000000-0005-0000-0000-0000DD010000}"/>
-    <cellStyle name="常规 5" xfId="478" xr:uid="{00000000-0005-0000-0000-0000DE010000}"/>
-    <cellStyle name="常规 6" xfId="479" xr:uid="{00000000-0005-0000-0000-0000DF010000}"/>
-    <cellStyle name="常规 7" xfId="480" xr:uid="{00000000-0005-0000-0000-0000E0010000}"/>
-    <cellStyle name="常规 8" xfId="481" xr:uid="{00000000-0005-0000-0000-0000E1010000}"/>
-    <cellStyle name="常规 9" xfId="482" xr:uid="{00000000-0005-0000-0000-0000E2010000}"/>
+    <cellStyle name="常规 10" xfId="463"/>
+    <cellStyle name="常规 11" xfId="464"/>
+    <cellStyle name="常规 12" xfId="465"/>
+    <cellStyle name="常规 13" xfId="466"/>
+    <cellStyle name="常规 14" xfId="467"/>
+    <cellStyle name="常规 15" xfId="468"/>
+    <cellStyle name="常规 16" xfId="469"/>
+    <cellStyle name="常规 17" xfId="470"/>
+    <cellStyle name="常规 18" xfId="471"/>
+    <cellStyle name="常规 19" xfId="472"/>
+    <cellStyle name="常规 2" xfId="473"/>
+    <cellStyle name="常规 2 2" xfId="474"/>
+    <cellStyle name="常规 20" xfId="475"/>
+    <cellStyle name="常规 3" xfId="476"/>
+    <cellStyle name="常规 4" xfId="477"/>
+    <cellStyle name="常规 5" xfId="478"/>
+    <cellStyle name="常规 6" xfId="479"/>
+    <cellStyle name="常规 7" xfId="480"/>
+    <cellStyle name="常规 8" xfId="481"/>
+    <cellStyle name="常规 9" xfId="482"/>
     <cellStyle name="好" xfId="483" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="好 10" xfId="484" xr:uid="{00000000-0005-0000-0000-0000E4010000}"/>
-    <cellStyle name="好 11" xfId="485" xr:uid="{00000000-0005-0000-0000-0000E5010000}"/>
-    <cellStyle name="好 12" xfId="486" xr:uid="{00000000-0005-0000-0000-0000E6010000}"/>
-    <cellStyle name="好 13" xfId="487" xr:uid="{00000000-0005-0000-0000-0000E7010000}"/>
-    <cellStyle name="好 14" xfId="488" xr:uid="{00000000-0005-0000-0000-0000E8010000}"/>
-    <cellStyle name="好 15" xfId="489" xr:uid="{00000000-0005-0000-0000-0000E9010000}"/>
-    <cellStyle name="好 16" xfId="490" xr:uid="{00000000-0005-0000-0000-0000EA010000}"/>
-    <cellStyle name="好 17" xfId="491" xr:uid="{00000000-0005-0000-0000-0000EB010000}"/>
-    <cellStyle name="好 18" xfId="492" xr:uid="{00000000-0005-0000-0000-0000EC010000}"/>
-    <cellStyle name="好 19" xfId="493" xr:uid="{00000000-0005-0000-0000-0000ED010000}"/>
-    <cellStyle name="好 2" xfId="494" xr:uid="{00000000-0005-0000-0000-0000EE010000}"/>
-    <cellStyle name="好 20" xfId="495" xr:uid="{00000000-0005-0000-0000-0000EF010000}"/>
-    <cellStyle name="好 3" xfId="496" xr:uid="{00000000-0005-0000-0000-0000F0010000}"/>
-    <cellStyle name="好 4" xfId="497" xr:uid="{00000000-0005-0000-0000-0000F1010000}"/>
-    <cellStyle name="好 5" xfId="498" xr:uid="{00000000-0005-0000-0000-0000F2010000}"/>
-    <cellStyle name="好 6" xfId="499" xr:uid="{00000000-0005-0000-0000-0000F3010000}"/>
-    <cellStyle name="好 7" xfId="500" xr:uid="{00000000-0005-0000-0000-0000F4010000}"/>
-    <cellStyle name="好 8" xfId="501" xr:uid="{00000000-0005-0000-0000-0000F5010000}"/>
-    <cellStyle name="好 9" xfId="502" xr:uid="{00000000-0005-0000-0000-0000F6010000}"/>
+    <cellStyle name="好 10" xfId="484"/>
+    <cellStyle name="好 11" xfId="485"/>
+    <cellStyle name="好 12" xfId="486"/>
+    <cellStyle name="好 13" xfId="487"/>
+    <cellStyle name="好 14" xfId="488"/>
+    <cellStyle name="好 15" xfId="489"/>
+    <cellStyle name="好 16" xfId="490"/>
+    <cellStyle name="好 17" xfId="491"/>
+    <cellStyle name="好 18" xfId="492"/>
+    <cellStyle name="好 19" xfId="493"/>
+    <cellStyle name="好 2" xfId="494"/>
+    <cellStyle name="好 20" xfId="495"/>
+    <cellStyle name="好 3" xfId="496"/>
+    <cellStyle name="好 4" xfId="497"/>
+    <cellStyle name="好 5" xfId="498"/>
+    <cellStyle name="好 6" xfId="499"/>
+    <cellStyle name="好 7" xfId="500"/>
+    <cellStyle name="好 8" xfId="501"/>
+    <cellStyle name="好 9" xfId="502"/>
     <cellStyle name="汇总" xfId="503" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="汇总 10" xfId="504" xr:uid="{00000000-0005-0000-0000-0000F8010000}"/>
-    <cellStyle name="汇总 11" xfId="505" xr:uid="{00000000-0005-0000-0000-0000F9010000}"/>
-    <cellStyle name="汇总 12" xfId="506" xr:uid="{00000000-0005-0000-0000-0000FA010000}"/>
-    <cellStyle name="汇总 13" xfId="507" xr:uid="{00000000-0005-0000-0000-0000FB010000}"/>
-    <cellStyle name="汇总 14" xfId="508" xr:uid="{00000000-0005-0000-0000-0000FC010000}"/>
-    <cellStyle name="汇总 15" xfId="509" xr:uid="{00000000-0005-0000-0000-0000FD010000}"/>
-    <cellStyle name="汇总 16" xfId="510" xr:uid="{00000000-0005-0000-0000-0000FE010000}"/>
-    <cellStyle name="汇总 17" xfId="511" xr:uid="{00000000-0005-0000-0000-0000FF010000}"/>
-    <cellStyle name="汇总 18" xfId="512" xr:uid="{00000000-0005-0000-0000-000000020000}"/>
-    <cellStyle name="汇总 19" xfId="513" xr:uid="{00000000-0005-0000-0000-000001020000}"/>
-    <cellStyle name="汇总 2" xfId="514" xr:uid="{00000000-0005-0000-0000-000002020000}"/>
-    <cellStyle name="汇总 20" xfId="515" xr:uid="{00000000-0005-0000-0000-000003020000}"/>
-    <cellStyle name="汇总 3" xfId="516" xr:uid="{00000000-0005-0000-0000-000004020000}"/>
-    <cellStyle name="汇总 4" xfId="517" xr:uid="{00000000-0005-0000-0000-000005020000}"/>
-    <cellStyle name="汇总 5" xfId="518" xr:uid="{00000000-0005-0000-0000-000006020000}"/>
-    <cellStyle name="汇总 6" xfId="519" xr:uid="{00000000-0005-0000-0000-000007020000}"/>
-    <cellStyle name="汇总 7" xfId="520" xr:uid="{00000000-0005-0000-0000-000008020000}"/>
-    <cellStyle name="汇总 8" xfId="521" xr:uid="{00000000-0005-0000-0000-000009020000}"/>
-    <cellStyle name="汇总 9" xfId="522" xr:uid="{00000000-0005-0000-0000-00000A020000}"/>
+    <cellStyle name="汇总 10" xfId="504"/>
+    <cellStyle name="汇总 11" xfId="505"/>
+    <cellStyle name="汇总 12" xfId="506"/>
+    <cellStyle name="汇总 13" xfId="507"/>
+    <cellStyle name="汇总 14" xfId="508"/>
+    <cellStyle name="汇总 15" xfId="509"/>
+    <cellStyle name="汇总 16" xfId="510"/>
+    <cellStyle name="汇总 17" xfId="511"/>
+    <cellStyle name="汇总 18" xfId="512"/>
+    <cellStyle name="汇总 19" xfId="513"/>
+    <cellStyle name="汇总 2" xfId="514"/>
+    <cellStyle name="汇总 20" xfId="515"/>
+    <cellStyle name="汇总 3" xfId="516"/>
+    <cellStyle name="汇总 4" xfId="517"/>
+    <cellStyle name="汇总 5" xfId="518"/>
+    <cellStyle name="汇总 6" xfId="519"/>
+    <cellStyle name="汇总 7" xfId="520"/>
+    <cellStyle name="汇总 8" xfId="521"/>
+    <cellStyle name="汇总 9" xfId="522"/>
     <cellStyle name="计算" xfId="523" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="计算 10" xfId="524" xr:uid="{00000000-0005-0000-0000-00000C020000}"/>
-    <cellStyle name="计算 11" xfId="525" xr:uid="{00000000-0005-0000-0000-00000D020000}"/>
-    <cellStyle name="计算 12" xfId="526" xr:uid="{00000000-0005-0000-0000-00000E020000}"/>
-    <cellStyle name="计算 13" xfId="527" xr:uid="{00000000-0005-0000-0000-00000F020000}"/>
-    <cellStyle name="计算 14" xfId="528" xr:uid="{00000000-0005-0000-0000-000010020000}"/>
-    <cellStyle name="计算 15" xfId="529" xr:uid="{00000000-0005-0000-0000-000011020000}"/>
-    <cellStyle name="计算 16" xfId="530" xr:uid="{00000000-0005-0000-0000-000012020000}"/>
-    <cellStyle name="计算 17" xfId="531" xr:uid="{00000000-0005-0000-0000-000013020000}"/>
-    <cellStyle name="计算 18" xfId="532" xr:uid="{00000000-0005-0000-0000-000014020000}"/>
-    <cellStyle name="计算 19" xfId="533" xr:uid="{00000000-0005-0000-0000-000015020000}"/>
-    <cellStyle name="计算 2" xfId="534" xr:uid="{00000000-0005-0000-0000-000016020000}"/>
-    <cellStyle name="计算 20" xfId="535" xr:uid="{00000000-0005-0000-0000-000017020000}"/>
-    <cellStyle name="计算 3" xfId="536" xr:uid="{00000000-0005-0000-0000-000018020000}"/>
-    <cellStyle name="计算 4" xfId="537" xr:uid="{00000000-0005-0000-0000-000019020000}"/>
-    <cellStyle name="计算 5" xfId="538" xr:uid="{00000000-0005-0000-0000-00001A020000}"/>
-    <cellStyle name="计算 6" xfId="539" xr:uid="{00000000-0005-0000-0000-00001B020000}"/>
-    <cellStyle name="计算 7" xfId="540" xr:uid="{00000000-0005-0000-0000-00001C020000}"/>
-    <cellStyle name="计算 8" xfId="541" xr:uid="{00000000-0005-0000-0000-00001D020000}"/>
-    <cellStyle name="计算 9" xfId="542" xr:uid="{00000000-0005-0000-0000-00001E020000}"/>
+    <cellStyle name="计算 10" xfId="524"/>
+    <cellStyle name="计算 11" xfId="525"/>
+    <cellStyle name="计算 12" xfId="526"/>
+    <cellStyle name="计算 13" xfId="527"/>
+    <cellStyle name="计算 14" xfId="528"/>
+    <cellStyle name="计算 15" xfId="529"/>
+    <cellStyle name="计算 16" xfId="530"/>
+    <cellStyle name="计算 17" xfId="531"/>
+    <cellStyle name="计算 18" xfId="532"/>
+    <cellStyle name="计算 19" xfId="533"/>
+    <cellStyle name="计算 2" xfId="534"/>
+    <cellStyle name="计算 20" xfId="535"/>
+    <cellStyle name="计算 3" xfId="536"/>
+    <cellStyle name="计算 4" xfId="537"/>
+    <cellStyle name="计算 5" xfId="538"/>
+    <cellStyle name="计算 6" xfId="539"/>
+    <cellStyle name="计算 7" xfId="540"/>
+    <cellStyle name="计算 8" xfId="541"/>
+    <cellStyle name="计算 9" xfId="542"/>
     <cellStyle name="检查单元格" xfId="543" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="检查单元格 10" xfId="544" xr:uid="{00000000-0005-0000-0000-000020020000}"/>
-    <cellStyle name="检查单元格 11" xfId="545" xr:uid="{00000000-0005-0000-0000-000021020000}"/>
-    <cellStyle name="检查单元格 12" xfId="546" xr:uid="{00000000-0005-0000-0000-000022020000}"/>
-    <cellStyle name="检查单元格 13" xfId="547" xr:uid="{00000000-0005-0000-0000-000023020000}"/>
-    <cellStyle name="检查单元格 14" xfId="548" xr:uid="{00000000-0005-0000-0000-000024020000}"/>
-    <cellStyle name="检查单元格 15" xfId="549" xr:uid="{00000000-0005-0000-0000-000025020000}"/>
-    <cellStyle name="检查单元格 16" xfId="550" xr:uid="{00000000-0005-0000-0000-000026020000}"/>
-    <cellStyle name="检查单元格 17" xfId="551" xr:uid="{00000000-0005-0000-0000-000027020000}"/>
-    <cellStyle name="检查单元格 18" xfId="552" xr:uid="{00000000-0005-0000-0000-000028020000}"/>
-    <cellStyle name="检查单元格 19" xfId="553" xr:uid="{00000000-0005-0000-0000-000029020000}"/>
-    <cellStyle name="检查单元格 2" xfId="554" xr:uid="{00000000-0005-0000-0000-00002A020000}"/>
-    <cellStyle name="检查单元格 20" xfId="555" xr:uid="{00000000-0005-0000-0000-00002B020000}"/>
-    <cellStyle name="检查单元格 3" xfId="556" xr:uid="{00000000-0005-0000-0000-00002C020000}"/>
-    <cellStyle name="检查单元格 4" xfId="557" xr:uid="{00000000-0005-0000-0000-00002D020000}"/>
-    <cellStyle name="检查单元格 5" xfId="558" xr:uid="{00000000-0005-0000-0000-00002E020000}"/>
-    <cellStyle name="检查单元格 6" xfId="559" xr:uid="{00000000-0005-0000-0000-00002F020000}"/>
-    <cellStyle name="检查单元格 7" xfId="560" xr:uid="{00000000-0005-0000-0000-000030020000}"/>
-    <cellStyle name="检查单元格 8" xfId="561" xr:uid="{00000000-0005-0000-0000-000031020000}"/>
-    <cellStyle name="检查单元格 9" xfId="562" xr:uid="{00000000-0005-0000-0000-000032020000}"/>
+    <cellStyle name="检查单元格 10" xfId="544"/>
+    <cellStyle name="检查单元格 11" xfId="545"/>
+    <cellStyle name="检查单元格 12" xfId="546"/>
+    <cellStyle name="检查单元格 13" xfId="547"/>
+    <cellStyle name="检查单元格 14" xfId="548"/>
+    <cellStyle name="检查单元格 15" xfId="549"/>
+    <cellStyle name="检查单元格 16" xfId="550"/>
+    <cellStyle name="检查单元格 17" xfId="551"/>
+    <cellStyle name="检查单元格 18" xfId="552"/>
+    <cellStyle name="检查单元格 19" xfId="553"/>
+    <cellStyle name="检查单元格 2" xfId="554"/>
+    <cellStyle name="检查单元格 20" xfId="555"/>
+    <cellStyle name="检查单元格 3" xfId="556"/>
+    <cellStyle name="检查单元格 4" xfId="557"/>
+    <cellStyle name="检查单元格 5" xfId="558"/>
+    <cellStyle name="检查单元格 6" xfId="559"/>
+    <cellStyle name="检查单元格 7" xfId="560"/>
+    <cellStyle name="检查单元格 8" xfId="561"/>
+    <cellStyle name="检查单元格 9" xfId="562"/>
     <cellStyle name="解释性文本" xfId="563" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="解释性文本 10" xfId="564" xr:uid="{00000000-0005-0000-0000-000034020000}"/>
-    <cellStyle name="解释性文本 11" xfId="565" xr:uid="{00000000-0005-0000-0000-000035020000}"/>
-    <cellStyle name="解释性文本 12" xfId="566" xr:uid="{00000000-0005-0000-0000-000036020000}"/>
-    <cellStyle name="解释性文本 13" xfId="567" xr:uid="{00000000-0005-0000-0000-000037020000}"/>
-    <cellStyle name="解释性文本 14" xfId="568" xr:uid="{00000000-0005-0000-0000-000038020000}"/>
-    <cellStyle name="解释性文本 15" xfId="569" xr:uid="{00000000-0005-0000-0000-000039020000}"/>
-    <cellStyle name="解释性文本 16" xfId="570" xr:uid="{00000000-0005-0000-0000-00003A020000}"/>
-    <cellStyle name="解释性文本 17" xfId="571" xr:uid="{00000000-0005-0000-0000-00003B020000}"/>
-    <cellStyle name="解释性文本 18" xfId="572" xr:uid="{00000000-0005-0000-0000-00003C020000}"/>
-    <cellStyle name="解释性文本 19" xfId="573" xr:uid="{00000000-0005-0000-0000-00003D020000}"/>
-    <cellStyle name="解释性文本 2" xfId="574" xr:uid="{00000000-0005-0000-0000-00003E020000}"/>
-    <cellStyle name="解释性文本 20" xfId="575" xr:uid="{00000000-0005-0000-0000-00003F020000}"/>
-    <cellStyle name="解释性文本 3" xfId="576" xr:uid="{00000000-0005-0000-0000-000040020000}"/>
-    <cellStyle name="解释性文本 4" xfId="577" xr:uid="{00000000-0005-0000-0000-000041020000}"/>
-    <cellStyle name="解释性文本 5" xfId="578" xr:uid="{00000000-0005-0000-0000-000042020000}"/>
-    <cellStyle name="解释性文本 6" xfId="579" xr:uid="{00000000-0005-0000-0000-000043020000}"/>
-    <cellStyle name="解释性文本 7" xfId="580" xr:uid="{00000000-0005-0000-0000-000044020000}"/>
-    <cellStyle name="解释性文本 8" xfId="581" xr:uid="{00000000-0005-0000-0000-000045020000}"/>
-    <cellStyle name="解释性文本 9" xfId="582" xr:uid="{00000000-0005-0000-0000-000046020000}"/>
+    <cellStyle name="解释性文本 10" xfId="564"/>
+    <cellStyle name="解释性文本 11" xfId="565"/>
+    <cellStyle name="解释性文本 12" xfId="566"/>
+    <cellStyle name="解释性文本 13" xfId="567"/>
+    <cellStyle name="解释性文本 14" xfId="568"/>
+    <cellStyle name="解释性文本 15" xfId="569"/>
+    <cellStyle name="解释性文本 16" xfId="570"/>
+    <cellStyle name="解释性文本 17" xfId="571"/>
+    <cellStyle name="解释性文本 18" xfId="572"/>
+    <cellStyle name="解释性文本 19" xfId="573"/>
+    <cellStyle name="解释性文本 2" xfId="574"/>
+    <cellStyle name="解释性文本 20" xfId="575"/>
+    <cellStyle name="解释性文本 3" xfId="576"/>
+    <cellStyle name="解释性文本 4" xfId="577"/>
+    <cellStyle name="解释性文本 5" xfId="578"/>
+    <cellStyle name="解释性文本 6" xfId="579"/>
+    <cellStyle name="解释性文本 7" xfId="580"/>
+    <cellStyle name="解释性文本 8" xfId="581"/>
+    <cellStyle name="解释性文本 9" xfId="582"/>
     <cellStyle name="警告文本" xfId="583" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="警告文本 10" xfId="584" xr:uid="{00000000-0005-0000-0000-000048020000}"/>
-    <cellStyle name="警告文本 11" xfId="585" xr:uid="{00000000-0005-0000-0000-000049020000}"/>
-    <cellStyle name="警告文本 12" xfId="586" xr:uid="{00000000-0005-0000-0000-00004A020000}"/>
-    <cellStyle name="警告文本 13" xfId="587" xr:uid="{00000000-0005-0000-0000-00004B020000}"/>
-    <cellStyle name="警告文本 14" xfId="588" xr:uid="{00000000-0005-0000-0000-00004C020000}"/>
-    <cellStyle name="警告文本 15" xfId="589" xr:uid="{00000000-0005-0000-0000-00004D020000}"/>
-    <cellStyle name="警告文本 16" xfId="590" xr:uid="{00000000-0005-0000-0000-00004E020000}"/>
-    <cellStyle name="警告文本 17" xfId="591" xr:uid="{00000000-0005-0000-0000-00004F020000}"/>
-    <cellStyle name="警告文本 18" xfId="592" xr:uid="{00000000-0005-0000-0000-000050020000}"/>
-    <cellStyle name="警告文本 19" xfId="593" xr:uid="{00000000-0005-0000-0000-000051020000}"/>
-    <cellStyle name="警告文本 2" xfId="594" xr:uid="{00000000-0005-0000-0000-000052020000}"/>
-    <cellStyle name="警告文本 20" xfId="595" xr:uid="{00000000-0005-0000-0000-000053020000}"/>
-    <cellStyle name="警告文本 3" xfId="596" xr:uid="{00000000-0005-0000-0000-000054020000}"/>
-    <cellStyle name="警告文本 4" xfId="597" xr:uid="{00000000-0005-0000-0000-000055020000}"/>
-    <cellStyle name="警告文本 5" xfId="598" xr:uid="{00000000-0005-0000-0000-000056020000}"/>
-    <cellStyle name="警告文本 6" xfId="599" xr:uid="{00000000-0005-0000-0000-000057020000}"/>
-    <cellStyle name="警告文本 7" xfId="600" xr:uid="{00000000-0005-0000-0000-000058020000}"/>
-    <cellStyle name="警告文本 8" xfId="601" xr:uid="{00000000-0005-0000-0000-000059020000}"/>
-    <cellStyle name="警告文本 9" xfId="602" xr:uid="{00000000-0005-0000-0000-00005A020000}"/>
+    <cellStyle name="警告文本 10" xfId="584"/>
+    <cellStyle name="警告文本 11" xfId="585"/>
+    <cellStyle name="警告文本 12" xfId="586"/>
+    <cellStyle name="警告文本 13" xfId="587"/>
+    <cellStyle name="警告文本 14" xfId="588"/>
+    <cellStyle name="警告文本 15" xfId="589"/>
+    <cellStyle name="警告文本 16" xfId="590"/>
+    <cellStyle name="警告文本 17" xfId="591"/>
+    <cellStyle name="警告文本 18" xfId="592"/>
+    <cellStyle name="警告文本 19" xfId="593"/>
+    <cellStyle name="警告文本 2" xfId="594"/>
+    <cellStyle name="警告文本 20" xfId="595"/>
+    <cellStyle name="警告文本 3" xfId="596"/>
+    <cellStyle name="警告文本 4" xfId="597"/>
+    <cellStyle name="警告文本 5" xfId="598"/>
+    <cellStyle name="警告文本 6" xfId="599"/>
+    <cellStyle name="警告文本 7" xfId="600"/>
+    <cellStyle name="警告文本 8" xfId="601"/>
+    <cellStyle name="警告文本 9" xfId="602"/>
     <cellStyle name="链接单元格" xfId="603" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="链接单元格 10" xfId="604" xr:uid="{00000000-0005-0000-0000-00005C020000}"/>
-    <cellStyle name="链接单元格 11" xfId="605" xr:uid="{00000000-0005-0000-0000-00005D020000}"/>
-    <cellStyle name="链接单元格 12" xfId="606" xr:uid="{00000000-0005-0000-0000-00005E020000}"/>
-    <cellStyle name="链接单元格 13" xfId="607" xr:uid="{00000000-0005-0000-0000-00005F020000}"/>
-    <cellStyle name="链接单元格 14" xfId="608" xr:uid="{00000000-0005-0000-0000-000060020000}"/>
-    <cellStyle name="链接单元格 15" xfId="609" xr:uid="{00000000-0005-0000-0000-000061020000}"/>
-    <cellStyle name="链接单元格 16" xfId="610" xr:uid="{00000000-0005-0000-0000-000062020000}"/>
-    <cellStyle name="链接单元格 17" xfId="611" xr:uid="{00000000-0005-0000-0000-000063020000}"/>
-    <cellStyle name="链接单元格 18" xfId="612" xr:uid="{00000000-0005-0000-0000-000064020000}"/>
-    <cellStyle name="链接单元格 19" xfId="613" xr:uid="{00000000-0005-0000-0000-000065020000}"/>
-    <cellStyle name="链接单元格 2" xfId="614" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
-    <cellStyle name="链接单元格 20" xfId="615" xr:uid="{00000000-0005-0000-0000-000067020000}"/>
-    <cellStyle name="链接单元格 3" xfId="616" xr:uid="{00000000-0005-0000-0000-000068020000}"/>
-    <cellStyle name="链接单元格 4" xfId="617" xr:uid="{00000000-0005-0000-0000-000069020000}"/>
-    <cellStyle name="链接单元格 5" xfId="618" xr:uid="{00000000-0005-0000-0000-00006A020000}"/>
-    <cellStyle name="链接单元格 6" xfId="619" xr:uid="{00000000-0005-0000-0000-00006B020000}"/>
-    <cellStyle name="链接单元格 7" xfId="620" xr:uid="{00000000-0005-0000-0000-00006C020000}"/>
-    <cellStyle name="链接单元格 8" xfId="621" xr:uid="{00000000-0005-0000-0000-00006D020000}"/>
-    <cellStyle name="链接单元格 9" xfId="622" xr:uid="{00000000-0005-0000-0000-00006E020000}"/>
-    <cellStyle name="强调文字颜色 1 10" xfId="623" xr:uid="{00000000-0005-0000-0000-00006F020000}"/>
-    <cellStyle name="强调文字颜色 1 11" xfId="624" xr:uid="{00000000-0005-0000-0000-000070020000}"/>
-    <cellStyle name="强调文字颜色 1 12" xfId="625" xr:uid="{00000000-0005-0000-0000-000071020000}"/>
-    <cellStyle name="强调文字颜色 1 13" xfId="626" xr:uid="{00000000-0005-0000-0000-000072020000}"/>
-    <cellStyle name="强调文字颜色 1 14" xfId="627" xr:uid="{00000000-0005-0000-0000-000073020000}"/>
-    <cellStyle name="强调文字颜色 1 15" xfId="628" xr:uid="{00000000-0005-0000-0000-000074020000}"/>
-    <cellStyle name="强调文字颜色 1 16" xfId="629" xr:uid="{00000000-0005-0000-0000-000075020000}"/>
-    <cellStyle name="强调文字颜色 1 17" xfId="630" xr:uid="{00000000-0005-0000-0000-000076020000}"/>
-    <cellStyle name="强调文字颜色 1 18" xfId="631" xr:uid="{00000000-0005-0000-0000-000077020000}"/>
-    <cellStyle name="强调文字颜色 1 19" xfId="632" xr:uid="{00000000-0005-0000-0000-000078020000}"/>
-    <cellStyle name="强调文字颜色 1 2" xfId="633" xr:uid="{00000000-0005-0000-0000-000079020000}"/>
-    <cellStyle name="强调文字颜色 1 20" xfId="634" xr:uid="{00000000-0005-0000-0000-00007A020000}"/>
-    <cellStyle name="强调文字颜色 1 3" xfId="635" xr:uid="{00000000-0005-0000-0000-00007B020000}"/>
-    <cellStyle name="强调文字颜色 1 4" xfId="636" xr:uid="{00000000-0005-0000-0000-00007C020000}"/>
-    <cellStyle name="强调文字颜色 1 5" xfId="637" xr:uid="{00000000-0005-0000-0000-00007D020000}"/>
-    <cellStyle name="强调文字颜色 1 6" xfId="638" xr:uid="{00000000-0005-0000-0000-00007E020000}"/>
-    <cellStyle name="强调文字颜色 1 7" xfId="639" xr:uid="{00000000-0005-0000-0000-00007F020000}"/>
-    <cellStyle name="强调文字颜色 1 8" xfId="640" xr:uid="{00000000-0005-0000-0000-000080020000}"/>
-    <cellStyle name="强调文字颜色 1 9" xfId="641" xr:uid="{00000000-0005-0000-0000-000081020000}"/>
-    <cellStyle name="强调文字颜色 2 10" xfId="642" xr:uid="{00000000-0005-0000-0000-000082020000}"/>
-    <cellStyle name="强调文字颜色 2 11" xfId="643" xr:uid="{00000000-0005-0000-0000-000083020000}"/>
-    <cellStyle name="强调文字颜色 2 12" xfId="644" xr:uid="{00000000-0005-0000-0000-000084020000}"/>
-    <cellStyle name="强调文字颜色 2 13" xfId="645" xr:uid="{00000000-0005-0000-0000-000085020000}"/>
-    <cellStyle name="强调文字颜色 2 14" xfId="646" xr:uid="{00000000-0005-0000-0000-000086020000}"/>
-    <cellStyle name="强调文字颜色 2 15" xfId="647" xr:uid="{00000000-0005-0000-0000-000087020000}"/>
-    <cellStyle name="强调文字颜色 2 16" xfId="648" xr:uid="{00000000-0005-0000-0000-000088020000}"/>
-    <cellStyle name="强调文字颜色 2 17" xfId="649" xr:uid="{00000000-0005-0000-0000-000089020000}"/>
-    <cellStyle name="强调文字颜色 2 18" xfId="650" xr:uid="{00000000-0005-0000-0000-00008A020000}"/>
-    <cellStyle name="强调文字颜色 2 19" xfId="651" xr:uid="{00000000-0005-0000-0000-00008B020000}"/>
-    <cellStyle name="强调文字颜色 2 2" xfId="652" xr:uid="{00000000-0005-0000-0000-00008C020000}"/>
-    <cellStyle name="强调文字颜色 2 20" xfId="653" xr:uid="{00000000-0005-0000-0000-00008D020000}"/>
-    <cellStyle name="强调文字颜色 2 3" xfId="654" xr:uid="{00000000-0005-0000-0000-00008E020000}"/>
-    <cellStyle name="强调文字颜色 2 4" xfId="655" xr:uid="{00000000-0005-0000-0000-00008F020000}"/>
-    <cellStyle name="强调文字颜色 2 5" xfId="656" xr:uid="{00000000-0005-0000-0000-000090020000}"/>
-    <cellStyle name="强调文字颜色 2 6" xfId="657" xr:uid="{00000000-0005-0000-0000-000091020000}"/>
-    <cellStyle name="强调文字颜色 2 7" xfId="658" xr:uid="{00000000-0005-0000-0000-000092020000}"/>
-    <cellStyle name="强调文字颜色 2 8" xfId="659" xr:uid="{00000000-0005-0000-0000-000093020000}"/>
-    <cellStyle name="强调文字颜色 2 9" xfId="660" xr:uid="{00000000-0005-0000-0000-000094020000}"/>
-    <cellStyle name="强调文字颜色 3 10" xfId="661" xr:uid="{00000000-0005-0000-0000-000095020000}"/>
-    <cellStyle name="强调文字颜色 3 11" xfId="662" xr:uid="{00000000-0005-0000-0000-000096020000}"/>
-    <cellStyle name="强调文字颜色 3 12" xfId="663" xr:uid="{00000000-0005-0000-0000-000097020000}"/>
-    <cellStyle name="强调文字颜色 3 13" xfId="664" xr:uid="{00000000-0005-0000-0000-000098020000}"/>
-    <cellStyle name="强调文字颜色 3 14" xfId="665" xr:uid="{00000000-0005-0000-0000-000099020000}"/>
-    <cellStyle name="强调文字颜色 3 15" xfId="666" xr:uid="{00000000-0005-0000-0000-00009A020000}"/>
-    <cellStyle name="强调文字颜色 3 16" xfId="667" xr:uid="{00000000-0005-0000-0000-00009B020000}"/>
-    <cellStyle name="强调文字颜色 3 17" xfId="668" xr:uid="{00000000-0005-0000-0000-00009C020000}"/>
-    <cellStyle name="强调文字颜色 3 18" xfId="669" xr:uid="{00000000-0005-0000-0000-00009D020000}"/>
-    <cellStyle name="强调文字颜色 3 19" xfId="670" xr:uid="{00000000-0005-0000-0000-00009E020000}"/>
-    <cellStyle name="强调文字颜色 3 2" xfId="671" xr:uid="{00000000-0005-0000-0000-00009F020000}"/>
-    <cellStyle name="强调文字颜色 3 20" xfId="672" xr:uid="{00000000-0005-0000-0000-0000A0020000}"/>
-    <cellStyle name="强调文字颜色 3 3" xfId="673" xr:uid="{00000000-0005-0000-0000-0000A1020000}"/>
-    <cellStyle name="强调文字颜色 3 4" xfId="674" xr:uid="{00000000-0005-0000-0000-0000A2020000}"/>
-    <cellStyle name="强调文字颜色 3 5" xfId="675" xr:uid="{00000000-0005-0000-0000-0000A3020000}"/>
-    <cellStyle name="强调文字颜色 3 6" xfId="676" xr:uid="{00000000-0005-0000-0000-0000A4020000}"/>
-    <cellStyle name="强调文字颜色 3 7" xfId="677" xr:uid="{00000000-0005-0000-0000-0000A5020000}"/>
-    <cellStyle name="强调文字颜色 3 8" xfId="678" xr:uid="{00000000-0005-0000-0000-0000A6020000}"/>
-    <cellStyle name="强调文字颜色 3 9" xfId="679" xr:uid="{00000000-0005-0000-0000-0000A7020000}"/>
-    <cellStyle name="强调文字颜色 4 10" xfId="680" xr:uid="{00000000-0005-0000-0000-0000A8020000}"/>
-    <cellStyle name="强调文字颜色 4 11" xfId="681" xr:uid="{00000000-0005-0000-0000-0000A9020000}"/>
-    <cellStyle name="强调文字颜色 4 12" xfId="682" xr:uid="{00000000-0005-0000-0000-0000AA020000}"/>
-    <cellStyle name="强调文字颜色 4 13" xfId="683" xr:uid="{00000000-0005-0000-0000-0000AB020000}"/>
-    <cellStyle name="强调文字颜色 4 14" xfId="684" xr:uid="{00000000-0005-0000-0000-0000AC020000}"/>
-    <cellStyle name="强调文字颜色 4 15" xfId="685" xr:uid="{00000000-0005-0000-0000-0000AD020000}"/>
-    <cellStyle name="强调文字颜色 4 16" xfId="686" xr:uid="{00000000-0005-0000-0000-0000AE020000}"/>
-    <cellStyle name="强调文字颜色 4 17" xfId="687" xr:uid="{00000000-0005-0000-0000-0000AF020000}"/>
-    <cellStyle name="强调文字颜色 4 18" xfId="688" xr:uid="{00000000-0005-0000-0000-0000B0020000}"/>
-    <cellStyle name="强调文字颜色 4 19" xfId="689" xr:uid="{00000000-0005-0000-0000-0000B1020000}"/>
-    <cellStyle name="强调文字颜色 4 2" xfId="690" xr:uid="{00000000-0005-0000-0000-0000B2020000}"/>
-    <cellStyle name="强调文字颜色 4 20" xfId="691" xr:uid="{00000000-0005-0000-0000-0000B3020000}"/>
-    <cellStyle name="强调文字颜色 4 3" xfId="692" xr:uid="{00000000-0005-0000-0000-0000B4020000}"/>
-    <cellStyle name="强调文字颜色 4 4" xfId="693" xr:uid="{00000000-0005-0000-0000-0000B5020000}"/>
-    <cellStyle name="强调文字颜色 4 5" xfId="694" xr:uid="{00000000-0005-0000-0000-0000B6020000}"/>
-    <cellStyle name="强调文字颜色 4 6" xfId="695" xr:uid="{00000000-0005-0000-0000-0000B7020000}"/>
-    <cellStyle name="强调文字颜色 4 7" xfId="696" xr:uid="{00000000-0005-0000-0000-0000B8020000}"/>
-    <cellStyle name="强调文字颜色 4 8" xfId="697" xr:uid="{00000000-0005-0000-0000-0000B9020000}"/>
-    <cellStyle name="强调文字颜色 4 9" xfId="698" xr:uid="{00000000-0005-0000-0000-0000BA020000}"/>
-    <cellStyle name="强调文字颜色 5 10" xfId="699" xr:uid="{00000000-0005-0000-0000-0000BB020000}"/>
-    <cellStyle name="强调文字颜色 5 11" xfId="700" xr:uid="{00000000-0005-0000-0000-0000BC020000}"/>
-    <cellStyle name="强调文字颜色 5 12" xfId="701" xr:uid="{00000000-0005-0000-0000-0000BD020000}"/>
-    <cellStyle name="强调文字颜色 5 13" xfId="702" xr:uid="{00000000-0005-0000-0000-0000BE020000}"/>
-    <cellStyle name="强调文字颜色 5 14" xfId="703" xr:uid="{00000000-0005-0000-0000-0000BF020000}"/>
-    <cellStyle name="强调文字颜色 5 15" xfId="704" xr:uid="{00000000-0005-0000-0000-0000C0020000}"/>
-    <cellStyle name="强调文字颜色 5 16" xfId="705" xr:uid="{00000000-0005-0000-0000-0000C1020000}"/>
-    <cellStyle name="强调文字颜色 5 17" xfId="706" xr:uid="{00000000-0005-0000-0000-0000C2020000}"/>
-    <cellStyle name="强调文字颜色 5 18" xfId="707" xr:uid="{00000000-0005-0000-0000-0000C3020000}"/>
-    <cellStyle name="强调文字颜色 5 19" xfId="708" xr:uid="{00000000-0005-0000-0000-0000C4020000}"/>
-    <cellStyle name="强调文字颜色 5 2" xfId="709" xr:uid="{00000000-0005-0000-0000-0000C5020000}"/>
-    <cellStyle name="强调文字颜色 5 20" xfId="710" xr:uid="{00000000-0005-0000-0000-0000C6020000}"/>
-    <cellStyle name="强调文字颜色 5 3" xfId="711" xr:uid="{00000000-0005-0000-0000-0000C7020000}"/>
-    <cellStyle name="强调文字颜色 5 4" xfId="712" xr:uid="{00000000-0005-0000-0000-0000C8020000}"/>
-    <cellStyle name="强调文字颜色 5 5" xfId="713" xr:uid="{00000000-0005-0000-0000-0000C9020000}"/>
-    <cellStyle name="强调文字颜色 5 6" xfId="714" xr:uid="{00000000-0005-0000-0000-0000CA020000}"/>
-    <cellStyle name="强调文字颜色 5 7" xfId="715" xr:uid="{00000000-0005-0000-0000-0000CB020000}"/>
-    <cellStyle name="强调文字颜色 5 8" xfId="716" xr:uid="{00000000-0005-0000-0000-0000CC020000}"/>
-    <cellStyle name="强调文字颜色 5 9" xfId="717" xr:uid="{00000000-0005-0000-0000-0000CD020000}"/>
-    <cellStyle name="强调文字颜色 6 10" xfId="718" xr:uid="{00000000-0005-0000-0000-0000CE020000}"/>
-    <cellStyle name="强调文字颜色 6 11" xfId="719" xr:uid="{00000000-0005-0000-0000-0000CF020000}"/>
-    <cellStyle name="强调文字颜色 6 12" xfId="720" xr:uid="{00000000-0005-0000-0000-0000D0020000}"/>
-    <cellStyle name="强调文字颜色 6 13" xfId="721" xr:uid="{00000000-0005-0000-0000-0000D1020000}"/>
-    <cellStyle name="强调文字颜色 6 14" xfId="722" xr:uid="{00000000-0005-0000-0000-0000D2020000}"/>
-    <cellStyle name="强调文字颜色 6 15" xfId="723" xr:uid="{00000000-0005-0000-0000-0000D3020000}"/>
-    <cellStyle name="强调文字颜色 6 16" xfId="724" xr:uid="{00000000-0005-0000-0000-0000D4020000}"/>
-    <cellStyle name="强调文字颜色 6 17" xfId="725" xr:uid="{00000000-0005-0000-0000-0000D5020000}"/>
-    <cellStyle name="强调文字颜色 6 18" xfId="726" xr:uid="{00000000-0005-0000-0000-0000D6020000}"/>
-    <cellStyle name="强调文字颜色 6 19" xfId="727" xr:uid="{00000000-0005-0000-0000-0000D7020000}"/>
-    <cellStyle name="强调文字颜色 6 2" xfId="728" xr:uid="{00000000-0005-0000-0000-0000D8020000}"/>
-    <cellStyle name="强调文字颜色 6 20" xfId="729" xr:uid="{00000000-0005-0000-0000-0000D9020000}"/>
-    <cellStyle name="强调文字颜色 6 3" xfId="730" xr:uid="{00000000-0005-0000-0000-0000DA020000}"/>
-    <cellStyle name="强调文字颜色 6 4" xfId="731" xr:uid="{00000000-0005-0000-0000-0000DB020000}"/>
-    <cellStyle name="强调文字颜色 6 5" xfId="732" xr:uid="{00000000-0005-0000-0000-0000DC020000}"/>
-    <cellStyle name="强调文字颜色 6 6" xfId="733" xr:uid="{00000000-0005-0000-0000-0000DD020000}"/>
-    <cellStyle name="强调文字颜色 6 7" xfId="734" xr:uid="{00000000-0005-0000-0000-0000DE020000}"/>
-    <cellStyle name="强调文字颜色 6 8" xfId="735" xr:uid="{00000000-0005-0000-0000-0000DF020000}"/>
-    <cellStyle name="强调文字颜色 6 9" xfId="736" xr:uid="{00000000-0005-0000-0000-0000E0020000}"/>
+    <cellStyle name="链接单元格 10" xfId="604"/>
+    <cellStyle name="链接单元格 11" xfId="605"/>
+    <cellStyle name="链接单元格 12" xfId="606"/>
+    <cellStyle name="链接单元格 13" xfId="607"/>
+    <cellStyle name="链接单元格 14" xfId="608"/>
+    <cellStyle name="链接单元格 15" xfId="609"/>
+    <cellStyle name="链接单元格 16" xfId="610"/>
+    <cellStyle name="链接单元格 17" xfId="611"/>
+    <cellStyle name="链接单元格 18" xfId="612"/>
+    <cellStyle name="链接单元格 19" xfId="613"/>
+    <cellStyle name="链接单元格 2" xfId="614"/>
+    <cellStyle name="链接单元格 20" xfId="615"/>
+    <cellStyle name="链接单元格 3" xfId="616"/>
+    <cellStyle name="链接单元格 4" xfId="617"/>
+    <cellStyle name="链接单元格 5" xfId="618"/>
+    <cellStyle name="链接单元格 6" xfId="619"/>
+    <cellStyle name="链接单元格 7" xfId="620"/>
+    <cellStyle name="链接单元格 8" xfId="621"/>
+    <cellStyle name="链接单元格 9" xfId="622"/>
+    <cellStyle name="强调文字颜色 1 10" xfId="623"/>
+    <cellStyle name="强调文字颜色 1 11" xfId="624"/>
+    <cellStyle name="强调文字颜色 1 12" xfId="625"/>
+    <cellStyle name="强调文字颜色 1 13" xfId="626"/>
+    <cellStyle name="强调文字颜色 1 14" xfId="627"/>
+    <cellStyle name="强调文字颜色 1 15" xfId="628"/>
+    <cellStyle name="强调文字颜色 1 16" xfId="629"/>
+    <cellStyle name="强调文字颜色 1 17" xfId="630"/>
+    <cellStyle name="强调文字颜色 1 18" xfId="631"/>
+    <cellStyle name="强调文字颜色 1 19" xfId="632"/>
+    <cellStyle name="强调文字颜色 1 2" xfId="633"/>
+    <cellStyle name="强调文字颜色 1 20" xfId="634"/>
+    <cellStyle name="强调文字颜色 1 3" xfId="635"/>
+    <cellStyle name="强调文字颜色 1 4" xfId="636"/>
+    <cellStyle name="强调文字颜色 1 5" xfId="637"/>
+    <cellStyle name="强调文字颜色 1 6" xfId="638"/>
+    <cellStyle name="强调文字颜色 1 7" xfId="639"/>
+    <cellStyle name="强调文字颜色 1 8" xfId="640"/>
+    <cellStyle name="强调文字颜色 1 9" xfId="641"/>
+    <cellStyle name="强调文字颜色 2 10" xfId="642"/>
+    <cellStyle name="强调文字颜色 2 11" xfId="643"/>
+    <cellStyle name="强调文字颜色 2 12" xfId="644"/>
+    <cellStyle name="强调文字颜色 2 13" xfId="645"/>
+    <cellStyle name="强调文字颜色 2 14" xfId="646"/>
+    <cellStyle name="强调文字颜色 2 15" xfId="647"/>
+    <cellStyle name="强调文字颜色 2 16" xfId="648"/>
+    <cellStyle name="强调文字颜色 2 17" xfId="649"/>
+    <cellStyle name="强调文字颜色 2 18" xfId="650"/>
+    <cellStyle name="强调文字颜色 2 19" xfId="651"/>
+    <cellStyle name="强调文字颜色 2 2" xfId="652"/>
+    <cellStyle name="强调文字颜色 2 20" xfId="653"/>
+    <cellStyle name="强调文字颜色 2 3" xfId="654"/>
+    <cellStyle name="强调文字颜色 2 4" xfId="655"/>
+    <cellStyle name="强调文字颜色 2 5" xfId="656"/>
+    <cellStyle name="强调文字颜色 2 6" xfId="657"/>
+    <cellStyle name="强调文字颜色 2 7" xfId="658"/>
+    <cellStyle name="强调文字颜色 2 8" xfId="659"/>
+    <cellStyle name="强调文字颜色 2 9" xfId="660"/>
+    <cellStyle name="强调文字颜色 3 10" xfId="661"/>
+    <cellStyle name="强调文字颜色 3 11" xfId="662"/>
+    <cellStyle name="强调文字颜色 3 12" xfId="663"/>
+    <cellStyle name="强调文字颜色 3 13" xfId="664"/>
+    <cellStyle name="强调文字颜色 3 14" xfId="665"/>
+    <cellStyle name="强调文字颜色 3 15" xfId="666"/>
+    <cellStyle name="强调文字颜色 3 16" xfId="667"/>
+    <cellStyle name="强调文字颜色 3 17" xfId="668"/>
+    <cellStyle name="强调文字颜色 3 18" xfId="669"/>
+    <cellStyle name="强调文字颜色 3 19" xfId="670"/>
+    <cellStyle name="强调文字颜色 3 2" xfId="671"/>
+    <cellStyle name="强调文字颜色 3 20" xfId="672"/>
+    <cellStyle name="强调文字颜色 3 3" xfId="673"/>
+    <cellStyle name="强调文字颜色 3 4" xfId="674"/>
+    <cellStyle name="强调文字颜色 3 5" xfId="675"/>
+    <cellStyle name="强调文字颜色 3 6" xfId="676"/>
+    <cellStyle name="强调文字颜色 3 7" xfId="677"/>
+    <cellStyle name="强调文字颜色 3 8" xfId="678"/>
+    <cellStyle name="强调文字颜色 3 9" xfId="679"/>
+    <cellStyle name="强调文字颜色 4 10" xfId="680"/>
+    <cellStyle name="强调文字颜色 4 11" xfId="681"/>
+    <cellStyle name="强调文字颜色 4 12" xfId="682"/>
+    <cellStyle name="强调文字颜色 4 13" xfId="683"/>
+    <cellStyle name="强调文字颜色 4 14" xfId="684"/>
+    <cellStyle name="强调文字颜色 4 15" xfId="685"/>
+    <cellStyle name="强调文字颜色 4 16" xfId="686"/>
+    <cellStyle name="强调文字颜色 4 17" xfId="687"/>
+    <cellStyle name="强调文字颜色 4 18" xfId="688"/>
+    <cellStyle name="强调文字颜色 4 19" xfId="689"/>
+    <cellStyle name="强调文字颜色 4 2" xfId="690"/>
+    <cellStyle name="强调文字颜色 4 20" xfId="691"/>
+    <cellStyle name="强调文字颜色 4 3" xfId="692"/>
+    <cellStyle name="强调文字颜色 4 4" xfId="693"/>
+    <cellStyle name="强调文字颜色 4 5" xfId="694"/>
+    <cellStyle name="强调文字颜色 4 6" xfId="695"/>
+    <cellStyle name="强调文字颜色 4 7" xfId="696"/>
+    <cellStyle name="强调文字颜色 4 8" xfId="697"/>
+    <cellStyle name="强调文字颜色 4 9" xfId="698"/>
+    <cellStyle name="强调文字颜色 5 10" xfId="699"/>
+    <cellStyle name="强调文字颜色 5 11" xfId="700"/>
+    <cellStyle name="强调文字颜色 5 12" xfId="701"/>
+    <cellStyle name="强调文字颜色 5 13" xfId="702"/>
+    <cellStyle name="强调文字颜色 5 14" xfId="703"/>
+    <cellStyle name="强调文字颜色 5 15" xfId="704"/>
+    <cellStyle name="强调文字颜色 5 16" xfId="705"/>
+    <cellStyle name="强调文字颜色 5 17" xfId="706"/>
+    <cellStyle name="强调文字颜色 5 18" xfId="707"/>
+    <cellStyle name="强调文字颜色 5 19" xfId="708"/>
+    <cellStyle name="强调文字颜色 5 2" xfId="709"/>
+    <cellStyle name="强调文字颜色 5 20" xfId="710"/>
+    <cellStyle name="强调文字颜色 5 3" xfId="711"/>
+    <cellStyle name="强调文字颜色 5 4" xfId="712"/>
+    <cellStyle name="强调文字颜色 5 5" xfId="713"/>
+    <cellStyle name="强调文字颜色 5 6" xfId="714"/>
+    <cellStyle name="强调文字颜色 5 7" xfId="715"/>
+    <cellStyle name="强调文字颜色 5 8" xfId="716"/>
+    <cellStyle name="强调文字颜色 5 9" xfId="717"/>
+    <cellStyle name="强调文字颜色 6 10" xfId="718"/>
+    <cellStyle name="强调文字颜色 6 11" xfId="719"/>
+    <cellStyle name="强调文字颜色 6 12" xfId="720"/>
+    <cellStyle name="强调文字颜色 6 13" xfId="721"/>
+    <cellStyle name="强调文字颜色 6 14" xfId="722"/>
+    <cellStyle name="强调文字颜色 6 15" xfId="723"/>
+    <cellStyle name="强调文字颜色 6 16" xfId="724"/>
+    <cellStyle name="强调文字颜色 6 17" xfId="725"/>
+    <cellStyle name="强调文字颜色 6 18" xfId="726"/>
+    <cellStyle name="强调文字颜色 6 19" xfId="727"/>
+    <cellStyle name="强调文字颜色 6 2" xfId="728"/>
+    <cellStyle name="强调文字颜色 6 20" xfId="729"/>
+    <cellStyle name="强调文字颜色 6 3" xfId="730"/>
+    <cellStyle name="强调文字颜色 6 4" xfId="731"/>
+    <cellStyle name="强调文字颜色 6 5" xfId="732"/>
+    <cellStyle name="强调文字颜色 6 6" xfId="733"/>
+    <cellStyle name="强调文字颜色 6 7" xfId="734"/>
+    <cellStyle name="强调文字颜色 6 8" xfId="735"/>
+    <cellStyle name="强调文字颜色 6 9" xfId="736"/>
     <cellStyle name="适中" xfId="737" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="适中 10" xfId="738" xr:uid="{00000000-0005-0000-0000-0000E2020000}"/>
-    <cellStyle name="适中 11" xfId="739" xr:uid="{00000000-0005-0000-0000-0000E3020000}"/>
-    <cellStyle name="适中 12" xfId="740" xr:uid="{00000000-0005-0000-0000-0000E4020000}"/>
-    <cellStyle name="适中 13" xfId="741" xr:uid="{00000000-0005-0000-0000-0000E5020000}"/>
-    <cellStyle name="适中 14" xfId="742" xr:uid="{00000000-0005-0000-0000-0000E6020000}"/>
-    <cellStyle name="适中 15" xfId="743" xr:uid="{00000000-0005-0000-0000-0000E7020000}"/>
-    <cellStyle name="适中 16" xfId="744" xr:uid="{00000000-0005-0000-0000-0000E8020000}"/>
-    <cellStyle name="适中 17" xfId="745" xr:uid="{00000000-0005-0000-0000-0000E9020000}"/>
-    <cellStyle name="适中 18" xfId="746" xr:uid="{00000000-0005-0000-0000-0000EA020000}"/>
-    <cellStyle name="适中 19" xfId="747" xr:uid="{00000000-0005-0000-0000-0000EB020000}"/>
-    <cellStyle name="适中 2" xfId="748" xr:uid="{00000000-0005-0000-0000-0000EC020000}"/>
-    <cellStyle name="适中 20" xfId="749" xr:uid="{00000000-0005-0000-0000-0000ED020000}"/>
-    <cellStyle name="适中 3" xfId="750" xr:uid="{00000000-0005-0000-0000-0000EE020000}"/>
-    <cellStyle name="适中 4" xfId="751" xr:uid="{00000000-0005-0000-0000-0000EF020000}"/>
-    <cellStyle name="适中 5" xfId="752" xr:uid="{00000000-0005-0000-0000-0000F0020000}"/>
-    <cellStyle name="适中 6" xfId="753" xr:uid="{00000000-0005-0000-0000-0000F1020000}"/>
-    <cellStyle name="适中 7" xfId="754" xr:uid="{00000000-0005-0000-0000-0000F2020000}"/>
-    <cellStyle name="适中 8" xfId="755" xr:uid="{00000000-0005-0000-0000-0000F3020000}"/>
-    <cellStyle name="适中 9" xfId="756" xr:uid="{00000000-0005-0000-0000-0000F4020000}"/>
+    <cellStyle name="适中 10" xfId="738"/>
+    <cellStyle name="适中 11" xfId="739"/>
+    <cellStyle name="适中 12" xfId="740"/>
+    <cellStyle name="适中 13" xfId="741"/>
+    <cellStyle name="适中 14" xfId="742"/>
+    <cellStyle name="适中 15" xfId="743"/>
+    <cellStyle name="适中 16" xfId="744"/>
+    <cellStyle name="适中 17" xfId="745"/>
+    <cellStyle name="适中 18" xfId="746"/>
+    <cellStyle name="适中 19" xfId="747"/>
+    <cellStyle name="适中 2" xfId="748"/>
+    <cellStyle name="适中 20" xfId="749"/>
+    <cellStyle name="适中 3" xfId="750"/>
+    <cellStyle name="适中 4" xfId="751"/>
+    <cellStyle name="适中 5" xfId="752"/>
+    <cellStyle name="适中 6" xfId="753"/>
+    <cellStyle name="适中 7" xfId="754"/>
+    <cellStyle name="适中 8" xfId="755"/>
+    <cellStyle name="适中 9" xfId="756"/>
     <cellStyle name="输出" xfId="757" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="输出 10" xfId="758" xr:uid="{00000000-0005-0000-0000-0000F6020000}"/>
-    <cellStyle name="输出 11" xfId="759" xr:uid="{00000000-0005-0000-0000-0000F7020000}"/>
-    <cellStyle name="输出 12" xfId="760" xr:uid="{00000000-0005-0000-0000-0000F8020000}"/>
-    <cellStyle name="输出 13" xfId="761" xr:uid="{00000000-0005-0000-0000-0000F9020000}"/>
-    <cellStyle name="输出 14" xfId="762" xr:uid="{00000000-0005-0000-0000-0000FA020000}"/>
-    <cellStyle name="输出 15" xfId="763" xr:uid="{00000000-0005-0000-0000-0000FB020000}"/>
-    <cellStyle name="输出 16" xfId="764" xr:uid="{00000000-0005-0000-0000-0000FC020000}"/>
-    <cellStyle name="输出 17" xfId="765" xr:uid="{00000000-0005-0000-0000-0000FD020000}"/>
-    <cellStyle name="输出 18" xfId="766" xr:uid="{00000000-0005-0000-0000-0000FE020000}"/>
-    <cellStyle name="输出 19" xfId="767" xr:uid="{00000000-0005-0000-0000-0000FF020000}"/>
-    <cellStyle name="输出 2" xfId="768" xr:uid="{00000000-0005-0000-0000-000000030000}"/>
-    <cellStyle name="输出 20" xfId="769" xr:uid="{00000000-0005-0000-0000-000001030000}"/>
-    <cellStyle name="输出 3" xfId="770" xr:uid="{00000000-0005-0000-0000-000002030000}"/>
-    <cellStyle name="输出 4" xfId="771" xr:uid="{00000000-0005-0000-0000-000003030000}"/>
-    <cellStyle name="输出 5" xfId="772" xr:uid="{00000000-0005-0000-0000-000004030000}"/>
-    <cellStyle name="输出 6" xfId="773" xr:uid="{00000000-0005-0000-0000-000005030000}"/>
-    <cellStyle name="输出 7" xfId="774" xr:uid="{00000000-0005-0000-0000-000006030000}"/>
-    <cellStyle name="输出 8" xfId="775" xr:uid="{00000000-0005-0000-0000-000007030000}"/>
-    <cellStyle name="输出 9" xfId="776" xr:uid="{00000000-0005-0000-0000-000008030000}"/>
+    <cellStyle name="输出 10" xfId="758"/>
+    <cellStyle name="输出 11" xfId="759"/>
+    <cellStyle name="输出 12" xfId="760"/>
+    <cellStyle name="输出 13" xfId="761"/>
+    <cellStyle name="输出 14" xfId="762"/>
+    <cellStyle name="输出 15" xfId="763"/>
+    <cellStyle name="输出 16" xfId="764"/>
+    <cellStyle name="输出 17" xfId="765"/>
+    <cellStyle name="输出 18" xfId="766"/>
+    <cellStyle name="输出 19" xfId="767"/>
+    <cellStyle name="输出 2" xfId="768"/>
+    <cellStyle name="输出 20" xfId="769"/>
+    <cellStyle name="输出 3" xfId="770"/>
+    <cellStyle name="输出 4" xfId="771"/>
+    <cellStyle name="输出 5" xfId="772"/>
+    <cellStyle name="输出 6" xfId="773"/>
+    <cellStyle name="输出 7" xfId="774"/>
+    <cellStyle name="输出 8" xfId="775"/>
+    <cellStyle name="输出 9" xfId="776"/>
     <cellStyle name="输入" xfId="777" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="输入 10" xfId="778" xr:uid="{00000000-0005-0000-0000-00000A030000}"/>
-    <cellStyle name="输入 11" xfId="779" xr:uid="{00000000-0005-0000-0000-00000B030000}"/>
-    <cellStyle name="输入 12" xfId="780" xr:uid="{00000000-0005-0000-0000-00000C030000}"/>
-    <cellStyle name="输入 13" xfId="781" xr:uid="{00000000-0005-0000-0000-00000D030000}"/>
-    <cellStyle name="输入 14" xfId="782" xr:uid="{00000000-0005-0000-0000-00000E030000}"/>
-    <cellStyle name="输入 15" xfId="783" xr:uid="{00000000-0005-0000-0000-00000F030000}"/>
-    <cellStyle name="输入 16" xfId="784" xr:uid="{00000000-0005-0000-0000-000010030000}"/>
-    <cellStyle name="输入 17" xfId="785" xr:uid="{00000000-0005-0000-0000-000011030000}"/>
-    <cellStyle name="输入 18" xfId="786" xr:uid="{00000000-0005-0000-0000-000012030000}"/>
-    <cellStyle name="输入 19" xfId="787" xr:uid="{00000000-0005-0000-0000-000013030000}"/>
-    <cellStyle name="输入 2" xfId="788" xr:uid="{00000000-0005-0000-0000-000014030000}"/>
-    <cellStyle name="输入 20" xfId="789" xr:uid="{00000000-0005-0000-0000-000015030000}"/>
-    <cellStyle name="输入 3" xfId="790" xr:uid="{00000000-0005-0000-0000-000016030000}"/>
-    <cellStyle name="输入 4" xfId="791" xr:uid="{00000000-0005-0000-0000-000017030000}"/>
-    <cellStyle name="输入 5" xfId="792" xr:uid="{00000000-0005-0000-0000-000018030000}"/>
-    <cellStyle name="输入 6" xfId="793" xr:uid="{00000000-0005-0000-0000-000019030000}"/>
-    <cellStyle name="输入 7" xfId="794" xr:uid="{00000000-0005-0000-0000-00001A030000}"/>
-    <cellStyle name="输入 8" xfId="795" xr:uid="{00000000-0005-0000-0000-00001B030000}"/>
-    <cellStyle name="输入 9" xfId="796" xr:uid="{00000000-0005-0000-0000-00001C030000}"/>
+    <cellStyle name="输入 10" xfId="778"/>
+    <cellStyle name="输入 11" xfId="779"/>
+    <cellStyle name="输入 12" xfId="780"/>
+    <cellStyle name="输入 13" xfId="781"/>
+    <cellStyle name="输入 14" xfId="782"/>
+    <cellStyle name="输入 15" xfId="783"/>
+    <cellStyle name="输入 16" xfId="784"/>
+    <cellStyle name="输入 17" xfId="785"/>
+    <cellStyle name="输入 18" xfId="786"/>
+    <cellStyle name="输入 19" xfId="787"/>
+    <cellStyle name="输入 2" xfId="788"/>
+    <cellStyle name="输入 20" xfId="789"/>
+    <cellStyle name="输入 3" xfId="790"/>
+    <cellStyle name="输入 4" xfId="791"/>
+    <cellStyle name="输入 5" xfId="792"/>
+    <cellStyle name="输入 6" xfId="793"/>
+    <cellStyle name="输入 7" xfId="794"/>
+    <cellStyle name="输入 8" xfId="795"/>
+    <cellStyle name="输入 9" xfId="796"/>
     <cellStyle name="注释" xfId="797" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="注释 10" xfId="798" xr:uid="{00000000-0005-0000-0000-00001E030000}"/>
-    <cellStyle name="注释 11" xfId="799" xr:uid="{00000000-0005-0000-0000-00001F030000}"/>
-    <cellStyle name="注释 12" xfId="800" xr:uid="{00000000-0005-0000-0000-000020030000}"/>
-    <cellStyle name="注释 13" xfId="801" xr:uid="{00000000-0005-0000-0000-000021030000}"/>
-    <cellStyle name="注释 14" xfId="802" xr:uid="{00000000-0005-0000-0000-000022030000}"/>
-    <cellStyle name="注释 15" xfId="803" xr:uid="{00000000-0005-0000-0000-000023030000}"/>
-    <cellStyle name="注释 16" xfId="804" xr:uid="{00000000-0005-0000-0000-000024030000}"/>
-    <cellStyle name="注释 17" xfId="805" xr:uid="{00000000-0005-0000-0000-000025030000}"/>
-    <cellStyle name="注释 18" xfId="806" xr:uid="{00000000-0005-0000-0000-000026030000}"/>
-    <cellStyle name="注释 19" xfId="807" xr:uid="{00000000-0005-0000-0000-000027030000}"/>
-    <cellStyle name="注释 2" xfId="808" xr:uid="{00000000-0005-0000-0000-000028030000}"/>
-    <cellStyle name="注释 20" xfId="809" xr:uid="{00000000-0005-0000-0000-000029030000}"/>
-    <cellStyle name="注释 3" xfId="810" xr:uid="{00000000-0005-0000-0000-00002A030000}"/>
-    <cellStyle name="注释 4" xfId="811" xr:uid="{00000000-0005-0000-0000-00002B030000}"/>
-    <cellStyle name="注释 5" xfId="812" xr:uid="{00000000-0005-0000-0000-00002C030000}"/>
-    <cellStyle name="注释 6" xfId="813" xr:uid="{00000000-0005-0000-0000-00002D030000}"/>
-    <cellStyle name="注释 7" xfId="814" xr:uid="{00000000-0005-0000-0000-00002E030000}"/>
-    <cellStyle name="注释 8" xfId="815" xr:uid="{00000000-0005-0000-0000-00002F030000}"/>
-    <cellStyle name="注释 9" xfId="816" xr:uid="{00000000-0005-0000-0000-000030030000}"/>
+    <cellStyle name="注释 10" xfId="798"/>
+    <cellStyle name="注释 11" xfId="799"/>
+    <cellStyle name="注释 12" xfId="800"/>
+    <cellStyle name="注释 13" xfId="801"/>
+    <cellStyle name="注释 14" xfId="802"/>
+    <cellStyle name="注释 15" xfId="803"/>
+    <cellStyle name="注释 16" xfId="804"/>
+    <cellStyle name="注释 17" xfId="805"/>
+    <cellStyle name="注释 18" xfId="806"/>
+    <cellStyle name="注释 19" xfId="807"/>
+    <cellStyle name="注释 2" xfId="808"/>
+    <cellStyle name="注释 20" xfId="809"/>
+    <cellStyle name="注释 3" xfId="810"/>
+    <cellStyle name="注释 4" xfId="811"/>
+    <cellStyle name="注释 5" xfId="812"/>
+    <cellStyle name="注释 6" xfId="813"/>
+    <cellStyle name="注释 7" xfId="814"/>
+    <cellStyle name="注释 8" xfId="815"/>
+    <cellStyle name="注释 9" xfId="816"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -4216,7 +4215,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4291,23 +4290,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4343,23 +4325,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4535,7 +4500,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -4557,7 +4522,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
-        <v>63</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="81" x14ac:dyDescent="0.15">
@@ -4575,7 +4540,7 @@
         <v>57</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>58</v>
@@ -4590,16 +4555,16 @@
         <v>60</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L2" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>95</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.15">
@@ -4651,7 +4616,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>19</v>
@@ -4663,19 +4628,19 @@
         <v>0</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.15">
@@ -4713,13 +4678,13 @@
         <v>2</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.15">
@@ -4757,13 +4722,13 @@
         <v>3</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.15">
@@ -4801,13 +4766,13 @@
         <v>1</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.15">
@@ -4845,13 +4810,13 @@
         <v>2</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N8" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.15">
@@ -4889,13 +4854,13 @@
         <v>3</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N9" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.15">
@@ -4933,13 +4898,13 @@
         <v>1</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N10" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.15">
@@ -4977,13 +4942,13 @@
         <v>2</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N11" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
@@ -5021,13 +4986,13 @@
         <v>3</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N12" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.15">
@@ -5065,13 +5030,13 @@
         <v>1</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N13" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.15">
@@ -5109,13 +5074,13 @@
         <v>2</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.15">
@@ -5153,13 +5118,13 @@
         <v>3</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M15" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N15" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.15">
@@ -5197,13 +5162,13 @@
         <v>1</v>
       </c>
       <c r="L16" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M16" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N16" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.15">
@@ -5241,13 +5206,13 @@
         <v>2</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M17" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N17" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.15">
@@ -5285,13 +5250,13 @@
         <v>3</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M18" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N18" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.15">
@@ -5329,13 +5294,13 @@
         <v>1</v>
       </c>
       <c r="L19" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M19" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N19" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.15">
@@ -5373,13 +5338,13 @@
         <v>2</v>
       </c>
       <c r="L20" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M20" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N20" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.15">
@@ -5417,13 +5382,13 @@
         <v>3</v>
       </c>
       <c r="L21" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M21" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N21" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.15">
@@ -5461,13 +5426,13 @@
         <v>1</v>
       </c>
       <c r="L22" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M22" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N22" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.15">
@@ -5505,13 +5470,13 @@
         <v>2</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N23" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.15">
@@ -5549,13 +5514,13 @@
         <v>3</v>
       </c>
       <c r="L24" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M24" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N24" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.15">
@@ -5593,13 +5558,13 @@
         <v>1</v>
       </c>
       <c r="L25" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M25" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N25" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.15">
@@ -5637,13 +5602,13 @@
         <v>2</v>
       </c>
       <c r="L26" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M26" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N26" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.15">
@@ -5681,13 +5646,13 @@
         <v>3</v>
       </c>
       <c r="L27" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M27" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N27" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.15">
@@ -5725,13 +5690,13 @@
         <v>1</v>
       </c>
       <c r="L28" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M28" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N28" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.15">
@@ -5769,13 +5734,13 @@
         <v>2</v>
       </c>
       <c r="L29" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M29" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N29" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.15">
@@ -5813,13 +5778,13 @@
         <v>3</v>
       </c>
       <c r="L30" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M30" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N30" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -5831,7 +5796,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5845,7 +5810,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
add ts runtime ( cocos creator example )
</commit_message>
<xml_diff>
--- a/example/config/BasicItem_Common.xlsx
+++ b/example/config/BasicItem_Common.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\Go\configTool-src\src\github.com\Blizzardx\ConfigProtocol\example\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C9FB40-ED05-497F-91C0-254436F15FB2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBF1C48-8457-40DA-8588-E54B323D80BA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5280" yWindow="-225" windowWidth="19440" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="123">
   <si>
     <t>道具图标：直接调用美术资源图名</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>icon100005</t>
-  </si>
-  <si>
-    <t>{}</t>
   </si>
   <si>
     <t>显示用金钱</t>
@@ -67,10 +64,6 @@
   </si>
   <si>
     <t>改名牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>{}</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -4559,54 +4552,54 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="81" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>63</v>
-      </c>
       <c r="L2" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="N2" s="9" t="s">
         <v>93</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -4624,7 +4617,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H3" t="s">
         <v>5</v>
@@ -4641,10 +4634,10 @@
         <v>800001</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -4653,31 +4646,28 @@
         <v>10</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.15">
@@ -4685,10 +4675,10 @@
         <v>800002</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -4700,10 +4690,7 @@
         <v>999</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -4715,13 +4702,13 @@
         <v>2</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.15">
@@ -4732,7 +4719,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -4744,10 +4731,7 @@
         <v>9999</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -4759,27 +4743,27 @@
         <v>3</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7">
-        <v>800011</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -4788,10 +4772,7 @@
         <v>999</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -4803,13 +4784,13 @@
         <v>1</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.15">
@@ -4817,10 +4798,10 @@
         <v>800017</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -4832,10 +4813,7 @@
         <v>999</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -4847,13 +4825,13 @@
         <v>2</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N8" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.15">
@@ -4861,10 +4839,10 @@
         <v>800018</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -4876,10 +4854,7 @@
         <v>9999</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -4891,13 +4866,13 @@
         <v>3</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N9" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.15">
@@ -4905,10 +4880,10 @@
         <v>800019</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -4920,10 +4895,7 @@
         <v>999</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -4935,13 +4907,13 @@
         <v>1</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="N10" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.15">
@@ -4949,10 +4921,10 @@
         <v>810001</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -4964,10 +4936,7 @@
         <v>999</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -4979,13 +4948,13 @@
         <v>2</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N11" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
@@ -4993,10 +4962,10 @@
         <v>810002</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -5008,10 +4977,7 @@
         <v>999</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -5023,13 +4989,13 @@
         <v>3</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="N12" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.15">
@@ -5037,10 +5003,10 @@
         <v>810003</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D13" s="4">
         <v>2</v>
@@ -5052,10 +5018,7 @@
         <v>999</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -5067,13 +5030,13 @@
         <v>1</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N13" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.15">
@@ -5081,10 +5044,10 @@
         <v>810004</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D14" s="4">
         <v>2</v>
@@ -5096,10 +5059,7 @@
         <v>999</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -5111,13 +5071,13 @@
         <v>2</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.15">
@@ -5125,10 +5085,10 @@
         <v>810005</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D15" s="4">
         <v>2</v>
@@ -5140,10 +5100,7 @@
         <v>999</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -5155,13 +5112,13 @@
         <v>3</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M15" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="N15" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.15">
@@ -5169,10 +5126,10 @@
         <v>810006</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D16" s="4">
         <v>3</v>
@@ -5184,10 +5141,7 @@
         <v>999</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -5199,13 +5153,13 @@
         <v>1</v>
       </c>
       <c r="L16" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M16" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N16" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.15">
@@ -5213,10 +5167,10 @@
         <v>810007</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D17" s="4">
         <v>3</v>
@@ -5228,10 +5182,7 @@
         <v>999</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -5243,13 +5194,13 @@
         <v>2</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M17" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="N17" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.15">
@@ -5257,10 +5208,10 @@
         <v>810008</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D18" s="4">
         <v>3</v>
@@ -5272,10 +5223,7 @@
         <v>999</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -5287,13 +5235,13 @@
         <v>3</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M18" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="N18" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.15">
@@ -5301,10 +5249,10 @@
         <v>810009</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D19" s="4">
         <v>3</v>
@@ -5316,10 +5264,7 @@
         <v>999</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -5331,13 +5276,13 @@
         <v>1</v>
       </c>
       <c r="L19" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M19" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="N19" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.15">
@@ -5345,10 +5290,10 @@
         <v>810010</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D20" s="4">
         <v>4</v>
@@ -5360,10 +5305,7 @@
         <v>999</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -5375,13 +5317,13 @@
         <v>2</v>
       </c>
       <c r="L20" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M20" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="N20" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.15">
@@ -5389,10 +5331,10 @@
         <v>810011</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D21" s="4">
         <v>4</v>
@@ -5404,10 +5346,7 @@
         <v>999</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -5419,13 +5358,13 @@
         <v>3</v>
       </c>
       <c r="L21" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M21" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="N21" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.15">
@@ -5433,10 +5372,10 @@
         <v>810012</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D22" s="7">
         <v>4</v>
@@ -5448,10 +5387,7 @@
         <v>999</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -5463,13 +5399,13 @@
         <v>1</v>
       </c>
       <c r="L22" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M22" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N22" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.15">
@@ -5477,10 +5413,10 @@
         <v>810013</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D23" s="4">
         <v>4</v>
@@ -5492,10 +5428,7 @@
         <v>999</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H23" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -5507,13 +5440,13 @@
         <v>2</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="N23" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.15">
@@ -5521,10 +5454,10 @@
         <v>810014</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D24" s="4">
         <v>4</v>
@@ -5536,10 +5469,7 @@
         <v>999</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -5551,13 +5481,13 @@
         <v>3</v>
       </c>
       <c r="L24" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M24" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N24" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.15">
@@ -5565,10 +5495,10 @@
         <v>810015</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D25" s="4">
         <v>5</v>
@@ -5580,10 +5510,7 @@
         <v>999</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -5595,13 +5522,13 @@
         <v>1</v>
       </c>
       <c r="L25" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M25" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="N25" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.15">
@@ -5609,10 +5536,10 @@
         <v>810016</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D26" s="4">
         <v>5</v>
@@ -5624,10 +5551,7 @@
         <v>999</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -5639,13 +5563,13 @@
         <v>2</v>
       </c>
       <c r="L26" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M26" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N26" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.15">
@@ -5653,10 +5577,10 @@
         <v>810017</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D27" s="4">
         <v>5</v>
@@ -5668,10 +5592,7 @@
         <v>999</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H27" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -5683,13 +5604,13 @@
         <v>3</v>
       </c>
       <c r="L27" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M27" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N27" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.15">
@@ -5697,10 +5618,10 @@
         <v>810018</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D28" s="4">
         <v>5</v>
@@ -5712,10 +5633,7 @@
         <v>999</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H28" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -5727,13 +5645,13 @@
         <v>1</v>
       </c>
       <c r="L28" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M28" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="N28" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.15">
@@ -5741,10 +5659,10 @@
         <v>810019</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D29" s="4">
         <v>5</v>
@@ -5756,10 +5674,7 @@
         <v>999</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H29" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -5771,13 +5686,13 @@
         <v>2</v>
       </c>
       <c r="L29" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M29" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N29" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.15">
@@ -5785,10 +5700,10 @@
         <v>810020</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D30" s="4">
         <v>5</v>
@@ -5800,10 +5715,7 @@
         <v>999</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H30" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -5815,13 +5727,13 @@
         <v>3</v>
       </c>
       <c r="L30" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M30" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="N30" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>